<commit_message>
Added table on units of analysis
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="9" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="11" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId1"/>
@@ -28,9 +28,11 @@
     <sheet name="Figure - Theory the Org" sheetId="15" r:id="rId14"/>
     <sheet name="Figure - Conceptual Framework" sheetId="9" r:id="rId15"/>
     <sheet name="Figure - Literature Landscape" sheetId="14" r:id="rId16"/>
+    <sheet name="Table - Unit of Analysis" sheetId="17" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Table - Determinants Examined'!$3:$4</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="16">'Table - Unit of Analysis'!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="380">
   <si>
     <t>Total</t>
   </si>
@@ -1317,6 +1319,193 @@
   </si>
   <si>
     <t>Research Cycle</t>
+  </si>
+  <si>
+    <t>Organizations</t>
+  </si>
+  <si>
+    <t>Individuals</t>
+  </si>
+  <si>
+    <t>Does technology maturity level influence an organizations willingness to acquire a given technology?</t>
+  </si>
+  <si>
+    <t>Technology maturity level</t>
+  </si>
+  <si>
+    <t>Individuals grouped by organization</t>
+  </si>
+  <si>
+    <t>Organizations were 50 percent more likely to have a majority of technology transfer decision-makers favor adding the technology to the decision agenda when it was a high maturity level than when it was the low maturity level.</t>
+  </si>
+  <si>
+    <t>Does technology maturity level influence a demand-side technology transfer decision-maker's willingness to pursue a given technology?</t>
+  </si>
+  <si>
+    <t>A higher percentage of private sector organizations in the life sciences sector acquired technology at a high maturity level than private sector organizations in all other sectors.</t>
+  </si>
+  <si>
+    <t>Survey</t>
+  </si>
+  <si>
+    <t>Content analysis</t>
+  </si>
+  <si>
+    <t>Documents</t>
+  </si>
+  <si>
+    <t>Decision premise statements about technology maturity in company records
+Statements indicating technology maturity level in Univesity-owned patents</t>
+  </si>
+  <si>
+    <t>Fifty percent (50%) of the private sector organizations used a decision premise that a technology had to have attained a minimum maturity level that was higher than the average maturity level of technologies available from universities.</t>
+  </si>
+  <si>
+    <t>Responses about decision premises by demand-side organization members.
+Responses about technology maturity level at time of patenting by supply-side organization members.</t>
+  </si>
+  <si>
+    <t>When making decisions about whether to acquire a technology, do most private sector organizations use a decision premise that a technology must have a minimum maturity level that happens to be higher than the typical maturity level of technologies available from universities?</t>
+  </si>
+  <si>
+    <t>Fifty percent (50%) of the private sector organizations used a decision premise that a technology had to have attained a minimum maturity level that was higher than the average maturity level of technologies at the time of patent application by universities.</t>
+  </si>
+  <si>
+    <t>Response choice of whether to acquire the technology.</t>
+  </si>
+  <si>
+    <t>Statements about the maturity level of technology acquired by the organization.</t>
+  </si>
+  <si>
+    <t>Do certain types of private sector organizations acquire more technology at higher maturity levels than others?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Data Description
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The kind of data collected.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Data Collection
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>How the data to perform the study is obtained.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Unit of Observation
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The item (or items) is actually observed, measured, or collected.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Unit of Analysis
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The unit about which one would like to make a generalizing statement.</t>
+    </r>
+  </si>
+  <si>
+    <t>Research Question</t>
+  </si>
+  <si>
+    <t>Responses about the maturity level of technology the organization has acquired.</t>
+  </si>
+  <si>
+    <t>Experiment using demand-side technology transfer decision-makers as subjects.  Random assignment to comparison or treatment case by inidividual. Comparison group presented with case where technology maturity level is low.  Treatment group presented with case where technology maturity level is high.  All other aspects of the case are the same.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Example Statement of Findings
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>For illustrative purposes only.</t>
+    </r>
+  </si>
+  <si>
+    <t>Experiment using demand-side technology transfer decision-makers as subjects.  Random assignment to comparison or treatment group by individual. Comparison group presented with case where technology maturity level is low.  Treatment group presented with case where technology maturity level is high.  All other aspects of the case are the same.</t>
+  </si>
+  <si>
+    <t>Experiment using demand-side technology transfer decision-makers as subjects.  Random assignment to comparison or treatment group by organization afflication.  Comparison group presented with case where technology maturity level is low.  Treatment group presented with case where technology maturity level is high.  All other aspects of the case are the same.</t>
+  </si>
+  <si>
+    <t>Subjects chose to acquite the technology at the high maturity level twice as often as the technology at the low maturity level.</t>
+  </si>
+  <si>
+    <t>Are technologies at a high maturity level more likely to be acquired by private sector organizations than technologies at a low maturity level?</t>
+  </si>
+  <si>
+    <t>Documents (news releases)
+Individuals</t>
+  </si>
+  <si>
+    <t>Content analysis
+Interviews or surveys</t>
+  </si>
+  <si>
+    <t>Interviews</t>
+  </si>
+  <si>
+    <t>Statements about decision premises by demand-side organization members.
+Statements about technology maturity level at time of patenting by supply-side organization members.</t>
+  </si>
+  <si>
+    <t>Are demand-side technology transfer decision-makers more apt to consider acquiring a technology the higher the technology maturity level?</t>
+  </si>
+  <si>
+    <t>Subjects chose to acquire the technology at the high maturity level twice as often as the technology at the low maturity level.</t>
+  </si>
+  <si>
+    <t>Subjects were 50 percent more likely to add the technology to the decision agenda when it was a high maturity level than when it was the low maturity level.</t>
+  </si>
+  <si>
+    <t>Subjects were 50 percent more likely to consider acquiring the high maturity level technology than the low maturity level technology.</t>
   </si>
 </sst>
 </file>
@@ -1419,15 +1608,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -1649,13 +1844,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -1979,6 +2185,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2005,6 +2217,30 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -11914,18 +12150,15 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Development stage of </a:t>
+            <a:t>Options</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1200">
+            <a:rPr lang="en-US" sz="1200" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>the  technology</a:t>
+            <a:t> of technologies available for acquisition</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -15275,7 +15508,7 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -15300,7 +15533,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -15346,6 +15581,356 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="82" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.7109375" style="112" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" style="111" customWidth="1"/>
+    <col min="3" max="3" width="1.7109375" style="111" customWidth="1"/>
+    <col min="4" max="4" width="24" style="111" customWidth="1"/>
+    <col min="5" max="5" width="1.7109375" style="111" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" style="111" customWidth="1"/>
+    <col min="7" max="7" width="1.7109375" style="111" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" style="111" customWidth="1"/>
+    <col min="9" max="9" width="1.7109375" style="111" customWidth="1"/>
+    <col min="10" max="10" width="25.7109375" style="111" customWidth="1"/>
+    <col min="11" max="11" width="1.7109375" style="111" customWidth="1"/>
+    <col min="12" max="12" width="50.7109375" style="111" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="111"/>
+    <col min="14" max="14" width="62" style="111" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="111"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="125"/>
+      <c r="B1" s="124" t="s">
+        <v>364</v>
+      </c>
+      <c r="C1" s="124"/>
+      <c r="D1" s="124" t="s">
+        <v>363</v>
+      </c>
+      <c r="E1" s="124"/>
+      <c r="F1" s="124" t="s">
+        <v>361</v>
+      </c>
+      <c r="G1" s="124"/>
+      <c r="H1" s="124" t="s">
+        <v>360</v>
+      </c>
+      <c r="I1" s="124"/>
+      <c r="J1" s="124" t="s">
+        <v>362</v>
+      </c>
+      <c r="K1" s="124"/>
+      <c r="L1" s="124" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+      <c r="A2" s="130">
+        <v>1</v>
+      </c>
+      <c r="B2" s="131" t="s">
+        <v>347</v>
+      </c>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131" t="s">
+        <v>342</v>
+      </c>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131" t="s">
+        <v>366</v>
+      </c>
+      <c r="G2" s="131"/>
+      <c r="H2" s="131" t="s">
+        <v>357</v>
+      </c>
+      <c r="I2" s="131"/>
+      <c r="J2" s="131" t="s">
+        <v>342</v>
+      </c>
+      <c r="K2" s="131"/>
+      <c r="L2" s="131" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+      <c r="A3" s="83">
+        <v>2</v>
+      </c>
+      <c r="B3" s="84" t="s">
+        <v>343</v>
+      </c>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84" t="s">
+        <v>341</v>
+      </c>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84" t="s">
+        <v>369</v>
+      </c>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84" t="s">
+        <v>357</v>
+      </c>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84" t="s">
+        <v>345</v>
+      </c>
+      <c r="K3" s="84"/>
+      <c r="L3" s="84" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A4" s="83">
+        <v>3</v>
+      </c>
+      <c r="B4" s="84" t="s">
+        <v>355</v>
+      </c>
+      <c r="C4" s="84"/>
+      <c r="D4" s="84" t="s">
+        <v>341</v>
+      </c>
+      <c r="E4" s="84"/>
+      <c r="F4" s="84" t="s">
+        <v>350</v>
+      </c>
+      <c r="G4" s="84"/>
+      <c r="H4" s="84" t="s">
+        <v>352</v>
+      </c>
+      <c r="I4" s="84"/>
+      <c r="J4" s="84" t="s">
+        <v>351</v>
+      </c>
+      <c r="K4" s="84"/>
+      <c r="L4" s="84" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A5" s="83">
+        <v>4</v>
+      </c>
+      <c r="B5" s="84" t="s">
+        <v>355</v>
+      </c>
+      <c r="C5" s="84"/>
+      <c r="D5" s="84" t="s">
+        <v>341</v>
+      </c>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84" t="s">
+        <v>349</v>
+      </c>
+      <c r="G5" s="84"/>
+      <c r="H5" s="84" t="s">
+        <v>354</v>
+      </c>
+      <c r="I5" s="84"/>
+      <c r="J5" s="84" t="s">
+        <v>345</v>
+      </c>
+      <c r="K5" s="84"/>
+      <c r="L5" s="84" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A6" s="83">
+        <v>5</v>
+      </c>
+      <c r="B6" s="84" t="s">
+        <v>355</v>
+      </c>
+      <c r="C6" s="84"/>
+      <c r="D6" s="84" t="s">
+        <v>341</v>
+      </c>
+      <c r="E6" s="84"/>
+      <c r="F6" s="84" t="s">
+        <v>374</v>
+      </c>
+      <c r="G6" s="84"/>
+      <c r="H6" s="84" t="s">
+        <v>375</v>
+      </c>
+      <c r="I6" s="84"/>
+      <c r="J6" s="84" t="s">
+        <v>345</v>
+      </c>
+      <c r="K6" s="84"/>
+      <c r="L6" s="84" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="83">
+        <v>6</v>
+      </c>
+      <c r="B7" s="84" t="s">
+        <v>359</v>
+      </c>
+      <c r="C7" s="84"/>
+      <c r="D7" s="84" t="s">
+        <v>341</v>
+      </c>
+      <c r="E7" s="84"/>
+      <c r="F7" s="84" t="s">
+        <v>349</v>
+      </c>
+      <c r="G7" s="84"/>
+      <c r="H7" s="84" t="s">
+        <v>365</v>
+      </c>
+      <c r="I7" s="84"/>
+      <c r="J7" s="84" t="s">
+        <v>342</v>
+      </c>
+      <c r="K7" s="84"/>
+      <c r="L7" s="84" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="83">
+        <v>7</v>
+      </c>
+      <c r="B8" s="84" t="s">
+        <v>359</v>
+      </c>
+      <c r="C8" s="84"/>
+      <c r="D8" s="84" t="s">
+        <v>341</v>
+      </c>
+      <c r="E8" s="84"/>
+      <c r="F8" s="84" t="s">
+        <v>350</v>
+      </c>
+      <c r="G8" s="84"/>
+      <c r="H8" s="84" t="s">
+        <v>358</v>
+      </c>
+      <c r="I8" s="84"/>
+      <c r="J8" s="84" t="s">
+        <v>351</v>
+      </c>
+      <c r="K8" s="84"/>
+      <c r="L8" s="84" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+      <c r="A9" s="126">
+        <v>8</v>
+      </c>
+      <c r="B9" s="127" t="s">
+        <v>371</v>
+      </c>
+      <c r="C9" s="127"/>
+      <c r="D9" s="127" t="s">
+        <v>344</v>
+      </c>
+      <c r="E9" s="127"/>
+      <c r="F9" s="127" t="s">
+        <v>368</v>
+      </c>
+      <c r="G9" s="127"/>
+      <c r="H9" s="127" t="s">
+        <v>357</v>
+      </c>
+      <c r="I9" s="127"/>
+      <c r="J9" s="127" t="s">
+        <v>342</v>
+      </c>
+      <c r="K9" s="127"/>
+      <c r="L9" s="127" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="128">
+        <v>9</v>
+      </c>
+      <c r="B10" s="129" t="s">
+        <v>371</v>
+      </c>
+      <c r="C10" s="129"/>
+      <c r="D10" s="129" t="s">
+        <v>344</v>
+      </c>
+      <c r="E10" s="129"/>
+      <c r="F10" s="129" t="s">
+        <v>373</v>
+      </c>
+      <c r="G10" s="129"/>
+      <c r="H10" s="129" t="s">
+        <v>358</v>
+      </c>
+      <c r="I10" s="129"/>
+      <c r="J10" s="129" t="s">
+        <v>372</v>
+      </c>
+      <c r="K10" s="129"/>
+      <c r="L10" s="129" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+      <c r="A11" s="128">
+        <v>10</v>
+      </c>
+      <c r="B11" s="129" t="s">
+        <v>376</v>
+      </c>
+      <c r="C11" s="129"/>
+      <c r="D11" s="129" t="s">
+        <v>342</v>
+      </c>
+      <c r="E11" s="129"/>
+      <c r="F11" s="129" t="s">
+        <v>368</v>
+      </c>
+      <c r="G11" s="129"/>
+      <c r="H11" s="129" t="s">
+        <v>357</v>
+      </c>
+      <c r="I11" s="129"/>
+      <c r="J11" s="129" t="s">
+        <v>342</v>
+      </c>
+      <c r="K11" s="129"/>
+      <c r="L11" s="129" t="s">
+        <v>379</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="55" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;LTable 
+Potential research questions based by unit of analysis, data collection method, and unit of observation</oddHeader>
+    <oddFooter>&amp;CPage &amp;P of &amp;N</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -15712,54 +16297,54 @@
       <c r="H20" s="109"/>
     </row>
     <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="111" t="s">
+      <c r="A21" s="113" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="111"/>
-      <c r="C21" s="111"/>
-      <c r="D21" s="111"/>
-      <c r="E21" s="111"/>
-      <c r="F21" s="111"/>
+      <c r="B21" s="113"/>
+      <c r="C21" s="113"/>
+      <c r="D21" s="113"/>
+      <c r="E21" s="113"/>
+      <c r="F21" s="113"/>
     </row>
     <row r="22" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="112" t="s">
+      <c r="A22" s="114" t="s">
         <v>179</v>
       </c>
-      <c r="B22" s="112"/>
-      <c r="C22" s="112"/>
-      <c r="D22" s="112"/>
-      <c r="E22" s="112"/>
-      <c r="F22" s="112"/>
+      <c r="B22" s="114"/>
+      <c r="C22" s="114"/>
+      <c r="D22" s="114"/>
+      <c r="E22" s="114"/>
+      <c r="F22" s="114"/>
     </row>
     <row r="23" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="111" t="s">
+      <c r="A23" s="113" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="111"/>
-      <c r="C23" s="111"/>
-      <c r="D23" s="111"/>
-      <c r="E23" s="111"/>
-      <c r="F23" s="111"/>
+      <c r="B23" s="113"/>
+      <c r="C23" s="113"/>
+      <c r="D23" s="113"/>
+      <c r="E23" s="113"/>
+      <c r="F23" s="113"/>
     </row>
     <row r="24" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="111" t="s">
+      <c r="A24" s="113" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="111"/>
-      <c r="C24" s="111"/>
-      <c r="D24" s="111"/>
-      <c r="E24" s="111"/>
-      <c r="F24" s="111"/>
+      <c r="B24" s="113"/>
+      <c r="C24" s="113"/>
+      <c r="D24" s="113"/>
+      <c r="E24" s="113"/>
+      <c r="F24" s="113"/>
     </row>
     <row r="25" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="111" t="s">
+      <c r="A25" s="113" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="111"/>
-      <c r="C25" s="111"/>
-      <c r="D25" s="111"/>
-      <c r="E25" s="111"/>
-      <c r="F25" s="111"/>
+      <c r="B25" s="113"/>
+      <c r="C25" s="113"/>
+      <c r="D25" s="113"/>
+      <c r="E25" s="113"/>
+      <c r="F25" s="113"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="30"/>
@@ -15943,38 +16528,38 @@
       <c r="B3" s="69"/>
       <c r="C3" s="70"/>
       <c r="D3" s="71"/>
-      <c r="E3" s="116" t="s">
+      <c r="E3" s="118" t="s">
         <v>276</v>
       </c>
-      <c r="F3" s="117"/>
-      <c r="G3" s="117"/>
-      <c r="H3" s="114"/>
-      <c r="I3" s="113" t="s">
+      <c r="F3" s="119"/>
+      <c r="G3" s="119"/>
+      <c r="H3" s="116"/>
+      <c r="I3" s="115" t="s">
         <v>304</v>
       </c>
-      <c r="J3" s="114"/>
-      <c r="K3" s="113" t="s">
+      <c r="J3" s="116"/>
+      <c r="K3" s="115" t="s">
         <v>305</v>
       </c>
-      <c r="L3" s="115"/>
-      <c r="M3" s="116" t="s">
+      <c r="L3" s="117"/>
+      <c r="M3" s="118" t="s">
         <v>292</v>
       </c>
-      <c r="N3" s="117"/>
-      <c r="O3" s="114"/>
-      <c r="P3" s="118" t="s">
+      <c r="N3" s="119"/>
+      <c r="O3" s="116"/>
+      <c r="P3" s="120" t="s">
         <v>257</v>
       </c>
-      <c r="Q3" s="117"/>
-      <c r="R3" s="117"/>
-      <c r="S3" s="117"/>
-      <c r="T3" s="117"/>
-      <c r="U3" s="117"/>
-      <c r="V3" s="117"/>
-      <c r="W3" s="117"/>
-      <c r="X3" s="117"/>
-      <c r="Y3" s="117"/>
-      <c r="Z3" s="119"/>
+      <c r="Q3" s="119"/>
+      <c r="R3" s="119"/>
+      <c r="S3" s="119"/>
+      <c r="T3" s="119"/>
+      <c r="U3" s="119"/>
+      <c r="V3" s="119"/>
+      <c r="W3" s="119"/>
+      <c r="X3" s="119"/>
+      <c r="Y3" s="119"/>
+      <c r="Z3" s="121"/>
       <c r="AA3" s="90"/>
     </row>
     <row r="4" spans="1:27" ht="170.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -19250,10 +19835,10 @@
       <c r="A3" s="69"/>
       <c r="B3" s="70"/>
       <c r="C3" s="71"/>
-      <c r="D3" s="116" t="s">
+      <c r="D3" s="118" t="s">
         <v>202</v>
       </c>
-      <c r="E3" s="114"/>
+      <c r="E3" s="116"/>
       <c r="F3" s="73"/>
     </row>
     <row r="4" spans="1:6" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -19513,32 +20098,32 @@
       <c r="F23" s="59"/>
     </row>
     <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="111"/>
-      <c r="B24" s="111"/>
-      <c r="C24" s="111"/>
-      <c r="D24" s="111"/>
-      <c r="E24" s="111"/>
+      <c r="A24" s="113"/>
+      <c r="B24" s="113"/>
+      <c r="C24" s="113"/>
+      <c r="D24" s="113"/>
+      <c r="E24" s="113"/>
     </row>
     <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="111"/>
-      <c r="B25" s="111"/>
-      <c r="C25" s="111"/>
-      <c r="D25" s="111"/>
-      <c r="E25" s="111"/>
+      <c r="A25" s="113"/>
+      <c r="B25" s="113"/>
+      <c r="C25" s="113"/>
+      <c r="D25" s="113"/>
+      <c r="E25" s="113"/>
     </row>
     <row r="26" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="111"/>
-      <c r="B26" s="111"/>
-      <c r="C26" s="111"/>
-      <c r="D26" s="111"/>
-      <c r="E26" s="111"/>
+      <c r="A26" s="113"/>
+      <c r="B26" s="113"/>
+      <c r="C26" s="113"/>
+      <c r="D26" s="113"/>
+      <c r="E26" s="113"/>
     </row>
     <row r="27" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="111"/>
-      <c r="B27" s="111"/>
-      <c r="C27" s="111"/>
-      <c r="D27" s="111"/>
-      <c r="E27" s="111"/>
+      <c r="A27" s="113"/>
+      <c r="B27" s="113"/>
+      <c r="C27" s="113"/>
+      <c r="D27" s="113"/>
+      <c r="E27" s="113"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="60"/>
@@ -20340,27 +20925,27 @@
       <c r="H16" s="32"/>
     </row>
     <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="111"/>
-      <c r="B17" s="111"/>
-      <c r="C17" s="111"/>
+      <c r="A17" s="113"/>
+      <c r="B17" s="113"/>
+      <c r="C17" s="113"/>
       <c r="D17" s="32"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="111"/>
-      <c r="B18" s="111"/>
-      <c r="C18" s="111"/>
+      <c r="A18" s="113"/>
+      <c r="B18" s="113"/>
+      <c r="C18" s="113"/>
       <c r="D18" s="32"/>
       <c r="E18" s="32"/>
       <c r="F18" s="32"/>
       <c r="H18" s="32"/>
     </row>
     <row r="19" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="111"/>
-      <c r="B19" s="111"/>
-      <c r="C19" s="111"/>
+      <c r="A19" s="113"/>
+      <c r="B19" s="113"/>
+      <c r="C19" s="113"/>
       <c r="D19" s="32"/>
       <c r="E19" s="32"/>
       <c r="F19" s="32"/>
@@ -20799,30 +21384,30 @@
       <c r="C41" s="52"/>
     </row>
     <row r="42" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="120" t="s">
+      <c r="A42" s="122" t="s">
         <v>174</v>
       </c>
-      <c r="B42" s="120"/>
-      <c r="C42" s="120"/>
+      <c r="B42" s="122"/>
+      <c r="C42" s="122"/>
     </row>
     <row r="43" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="121" t="s">
+      <c r="A43" s="123" t="s">
         <v>175</v>
       </c>
-      <c r="B43" s="121"/>
-      <c r="C43" s="121"/>
+      <c r="B43" s="123"/>
+      <c r="C43" s="123"/>
     </row>
     <row r="44" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="120" t="s">
+      <c r="A44" s="122" t="s">
         <v>176</v>
       </c>
-      <c r="B44" s="120"/>
-      <c r="C44" s="120"/>
+      <c r="B44" s="122"/>
+      <c r="C44" s="122"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="111"/>
-      <c r="B45" s="111"/>
-      <c r="C45" s="111"/>
+      <c r="A45" s="113"/>
+      <c r="B45" s="113"/>
+      <c r="C45" s="113"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="37"/>

</xml_diff>

<commit_message>
Added content to table on unit of analysis options
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="392">
   <si>
     <t>Total</t>
   </si>
@@ -1506,6 +1506,43 @@
   </si>
   <si>
     <t>Subjects were 50 percent more likely to consider acquiring the high maturity level technology than the low maturity level technology.</t>
+  </si>
+  <si>
+    <t>Do technology transfer decision-makers at private sector organizations disfavor low maturity level technologies?</t>
+  </si>
+  <si>
+    <t>Only 20 percent of subjects chose to pursue the low maturity level technology where 50 percent of subjects chose to pursue the high maturity level technology.</t>
+  </si>
+  <si>
+    <t>Do demand-side private sector organizations disfavor low maturity level technologies?</t>
+  </si>
+  <si>
+    <t>Experiment using demand-side technology transfer decision-makers as subjects.  Random assignment to comparison or treatment group by individual.  Comparison group presented with case where technology maturity level is low.  Treatment group presented with case where technology maturity level is high.  All other aspects of the case are the same.</t>
+  </si>
+  <si>
+    <t>Only 20 percent of organizations had a majority of respondents choose to pursue the low maturity level technology where 50 percent of organizations had a majority of subjects choose to pursue the high maturity level technology.</t>
+  </si>
+  <si>
+    <t>Data about the most recent decision about whether to pursue a university technology.</t>
+  </si>
+  <si>
+    <t>Only 20 percent of organizations chose to pursue a low maturity level technology where 80 percent of organizations chose to pursue a high maturity level technology.</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>Observations of discussions about technology acquisition opportunties
+Statements about technology transfer decisions.</t>
+  </si>
+  <si>
+    <t>Statements about technology transfer decisions.</t>
+  </si>
+  <si>
+    <t>Organizations chose to pursue a low maturity level technology only 20 percent of the time.</t>
+  </si>
+  <si>
+    <t>Data about technology transfer decisions.</t>
   </si>
 </sst>
 </file>
@@ -1861,7 +1898,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -2188,6 +2225,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2218,28 +2282,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -15589,13 +15632,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15618,56 +15661,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="125"/>
-      <c r="B1" s="124" t="s">
+      <c r="A1" s="115"/>
+      <c r="B1" s="114" t="s">
         <v>364</v>
       </c>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124" t="s">
+      <c r="C1" s="114"/>
+      <c r="D1" s="114" t="s">
         <v>363</v>
       </c>
-      <c r="E1" s="124"/>
-      <c r="F1" s="124" t="s">
+      <c r="E1" s="114"/>
+      <c r="F1" s="114" t="s">
         <v>361</v>
       </c>
-      <c r="G1" s="124"/>
-      <c r="H1" s="124" t="s">
+      <c r="G1" s="114"/>
+      <c r="H1" s="114" t="s">
         <v>360</v>
       </c>
-      <c r="I1" s="124"/>
-      <c r="J1" s="124" t="s">
+      <c r="I1" s="114"/>
+      <c r="J1" s="114" t="s">
         <v>362</v>
       </c>
-      <c r="K1" s="124"/>
-      <c r="L1" s="124" t="s">
+      <c r="K1" s="114"/>
+      <c r="L1" s="114" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="180" x14ac:dyDescent="0.25">
-      <c r="A2" s="130">
+      <c r="A2" s="120">
         <v>1</v>
       </c>
-      <c r="B2" s="131" t="s">
+      <c r="B2" s="121" t="s">
         <v>347</v>
       </c>
-      <c r="C2" s="131"/>
-      <c r="D2" s="131" t="s">
+      <c r="C2" s="121"/>
+      <c r="D2" s="121" t="s">
         <v>342</v>
       </c>
-      <c r="E2" s="131"/>
-      <c r="F2" s="131" t="s">
+      <c r="E2" s="121"/>
+      <c r="F2" s="121" t="s">
         <v>366</v>
       </c>
-      <c r="G2" s="131"/>
-      <c r="H2" s="131" t="s">
+      <c r="G2" s="121"/>
+      <c r="H2" s="121" t="s">
         <v>357</v>
       </c>
-      <c r="I2" s="131"/>
-      <c r="J2" s="131" t="s">
+      <c r="I2" s="121"/>
+      <c r="J2" s="121" t="s">
         <v>342</v>
       </c>
-      <c r="K2" s="131"/>
-      <c r="L2" s="131" t="s">
+      <c r="K2" s="121"/>
+      <c r="L2" s="121" t="s">
         <v>378</v>
       </c>
     </row>
@@ -15699,227 +15742,395 @@
         <v>346</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="135" x14ac:dyDescent="0.25">
-      <c r="A4" s="83">
+    <row r="4" spans="1:12" s="113" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A4" s="116">
         <v>3</v>
       </c>
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="117" t="s">
+        <v>380</v>
+      </c>
+      <c r="C4" s="117"/>
+      <c r="D4" s="117" t="s">
+        <v>342</v>
+      </c>
+      <c r="E4" s="117"/>
+      <c r="F4" s="117" t="s">
+        <v>383</v>
+      </c>
+      <c r="G4" s="117"/>
+      <c r="H4" s="117" t="s">
+        <v>357</v>
+      </c>
+      <c r="I4" s="117"/>
+      <c r="J4" s="117" t="s">
+        <v>342</v>
+      </c>
+      <c r="K4" s="117"/>
+      <c r="L4" s="117" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="133" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A5" s="118">
+        <v>4</v>
+      </c>
+      <c r="B5" s="119" t="s">
+        <v>382</v>
+      </c>
+      <c r="C5" s="119"/>
+      <c r="D5" s="119" t="s">
+        <v>341</v>
+      </c>
+      <c r="E5" s="119"/>
+      <c r="F5" s="119" t="s">
+        <v>369</v>
+      </c>
+      <c r="G5" s="119"/>
+      <c r="H5" s="119" t="s">
+        <v>357</v>
+      </c>
+      <c r="I5" s="119"/>
+      <c r="J5" s="119" t="s">
+        <v>345</v>
+      </c>
+      <c r="K5" s="119"/>
+      <c r="L5" s="119" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="133" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="118">
+        <v>5</v>
+      </c>
+      <c r="B6" s="119" t="s">
+        <v>382</v>
+      </c>
+      <c r="C6" s="119"/>
+      <c r="D6" s="119" t="s">
+        <v>341</v>
+      </c>
+      <c r="E6" s="119"/>
+      <c r="F6" s="119" t="s">
+        <v>349</v>
+      </c>
+      <c r="G6" s="119"/>
+      <c r="H6" s="119" t="s">
+        <v>385</v>
+      </c>
+      <c r="I6" s="119"/>
+      <c r="J6" s="119" t="s">
+        <v>342</v>
+      </c>
+      <c r="K6" s="119"/>
+      <c r="L6" s="119" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="133" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A7" s="118">
+        <v>6</v>
+      </c>
+      <c r="B7" s="119" t="s">
+        <v>382</v>
+      </c>
+      <c r="C7" s="119"/>
+      <c r="D7" s="119" t="s">
+        <v>341</v>
+      </c>
+      <c r="E7" s="119"/>
+      <c r="F7" s="119" t="s">
+        <v>387</v>
+      </c>
+      <c r="G7" s="119"/>
+      <c r="H7" s="119" t="s">
+        <v>388</v>
+      </c>
+      <c r="I7" s="119"/>
+      <c r="J7" s="119" t="s">
+        <v>342</v>
+      </c>
+      <c r="K7" s="119"/>
+      <c r="L7" s="119" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="133" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="118">
+        <v>7</v>
+      </c>
+      <c r="B8" s="119" t="s">
+        <v>382</v>
+      </c>
+      <c r="C8" s="119"/>
+      <c r="D8" s="119" t="s">
+        <v>341</v>
+      </c>
+      <c r="E8" s="119"/>
+      <c r="F8" s="119" t="s">
+        <v>350</v>
+      </c>
+      <c r="G8" s="119"/>
+      <c r="H8" s="119" t="s">
+        <v>389</v>
+      </c>
+      <c r="I8" s="119"/>
+      <c r="J8" s="119" t="s">
+        <v>351</v>
+      </c>
+      <c r="K8" s="119"/>
+      <c r="L8" s="119" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="133" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="118">
+        <v>8</v>
+      </c>
+      <c r="B9" s="119" t="s">
+        <v>382</v>
+      </c>
+      <c r="C9" s="119"/>
+      <c r="D9" s="119" t="s">
+        <v>341</v>
+      </c>
+      <c r="E9" s="119"/>
+      <c r="F9" s="119" t="s">
+        <v>374</v>
+      </c>
+      <c r="G9" s="119"/>
+      <c r="H9" s="119" t="s">
+        <v>391</v>
+      </c>
+      <c r="I9" s="119"/>
+      <c r="J9" s="119" t="s">
+        <v>342</v>
+      </c>
+      <c r="K9" s="119"/>
+      <c r="L9" s="119" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A10" s="83">
+        <v>9</v>
+      </c>
+      <c r="B10" s="84" t="s">
         <v>355</v>
       </c>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84" t="s">
+      <c r="C10" s="84"/>
+      <c r="D10" s="84" t="s">
         <v>341</v>
       </c>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84" t="s">
+      <c r="E10" s="84"/>
+      <c r="F10" s="84" t="s">
         <v>350</v>
       </c>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84" t="s">
+      <c r="G10" s="84"/>
+      <c r="H10" s="84" t="s">
         <v>352</v>
       </c>
-      <c r="I4" s="84"/>
-      <c r="J4" s="84" t="s">
+      <c r="I10" s="84"/>
+      <c r="J10" s="84" t="s">
         <v>351</v>
       </c>
-      <c r="K4" s="84"/>
-      <c r="L4" s="84" t="s">
+      <c r="K10" s="84"/>
+      <c r="L10" s="84" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="135" x14ac:dyDescent="0.25">
-      <c r="A5" s="83">
-        <v>4</v>
-      </c>
-      <c r="B5" s="84" t="s">
+    <row r="11" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A11" s="83">
+        <v>10</v>
+      </c>
+      <c r="B11" s="84" t="s">
         <v>355</v>
       </c>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84" t="s">
+      <c r="C11" s="84"/>
+      <c r="D11" s="84" t="s">
         <v>341</v>
       </c>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84" t="s">
+      <c r="E11" s="84"/>
+      <c r="F11" s="84" t="s">
         <v>349</v>
       </c>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84" t="s">
+      <c r="G11" s="84"/>
+      <c r="H11" s="84" t="s">
         <v>354</v>
       </c>
-      <c r="I5" s="84"/>
-      <c r="J5" s="84" t="s">
+      <c r="I11" s="84"/>
+      <c r="J11" s="84" t="s">
         <v>345</v>
       </c>
-      <c r="K5" s="84"/>
-      <c r="L5" s="84" t="s">
+      <c r="K11" s="84"/>
+      <c r="L11" s="84" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="135" x14ac:dyDescent="0.25">
-      <c r="A6" s="83">
-        <v>5</v>
-      </c>
-      <c r="B6" s="84" t="s">
+    <row r="12" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A12" s="83">
+        <v>11</v>
+      </c>
+      <c r="B12" s="84" t="s">
         <v>355</v>
       </c>
-      <c r="C6" s="84"/>
-      <c r="D6" s="84" t="s">
+      <c r="C12" s="84"/>
+      <c r="D12" s="84" t="s">
         <v>341</v>
       </c>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84" t="s">
+      <c r="E12" s="84"/>
+      <c r="F12" s="84" t="s">
         <v>374</v>
       </c>
-      <c r="G6" s="84"/>
-      <c r="H6" s="84" t="s">
+      <c r="G12" s="84"/>
+      <c r="H12" s="84" t="s">
         <v>375</v>
       </c>
-      <c r="I6" s="84"/>
-      <c r="J6" s="84" t="s">
+      <c r="I12" s="84"/>
+      <c r="J12" s="84" t="s">
         <v>345</v>
       </c>
-      <c r="K6" s="84"/>
-      <c r="L6" s="84" t="s">
+      <c r="K12" s="84"/>
+      <c r="L12" s="84" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="83">
-        <v>6</v>
-      </c>
-      <c r="B7" s="84" t="s">
+    <row r="13" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="83">
+        <v>12</v>
+      </c>
+      <c r="B13" s="84" t="s">
         <v>359</v>
       </c>
-      <c r="C7" s="84"/>
-      <c r="D7" s="84" t="s">
+      <c r="C13" s="84"/>
+      <c r="D13" s="84" t="s">
         <v>341</v>
       </c>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84" t="s">
+      <c r="E13" s="84"/>
+      <c r="F13" s="84" t="s">
         <v>349</v>
       </c>
-      <c r="G7" s="84"/>
-      <c r="H7" s="84" t="s">
+      <c r="G13" s="84"/>
+      <c r="H13" s="84" t="s">
         <v>365</v>
       </c>
-      <c r="I7" s="84"/>
-      <c r="J7" s="84" t="s">
+      <c r="I13" s="84"/>
+      <c r="J13" s="84" t="s">
         <v>342</v>
       </c>
-      <c r="K7" s="84"/>
-      <c r="L7" s="84" t="s">
+      <c r="K13" s="84"/>
+      <c r="L13" s="84" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="83">
-        <v>7</v>
-      </c>
-      <c r="B8" s="84" t="s">
+    <row r="14" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="83">
+        <v>13</v>
+      </c>
+      <c r="B14" s="84" t="s">
         <v>359</v>
       </c>
-      <c r="C8" s="84"/>
-      <c r="D8" s="84" t="s">
+      <c r="C14" s="84"/>
+      <c r="D14" s="84" t="s">
         <v>341</v>
       </c>
-      <c r="E8" s="84"/>
-      <c r="F8" s="84" t="s">
+      <c r="E14" s="84"/>
+      <c r="F14" s="84" t="s">
         <v>350</v>
       </c>
-      <c r="G8" s="84"/>
-      <c r="H8" s="84" t="s">
+      <c r="G14" s="84"/>
+      <c r="H14" s="84" t="s">
         <v>358</v>
       </c>
-      <c r="I8" s="84"/>
-      <c r="J8" s="84" t="s">
+      <c r="I14" s="84"/>
+      <c r="J14" s="84" t="s">
         <v>351</v>
       </c>
-      <c r="K8" s="84"/>
-      <c r="L8" s="84" t="s">
+      <c r="K14" s="84"/>
+      <c r="L14" s="84" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="180" x14ac:dyDescent="0.25">
-      <c r="A9" s="126">
-        <v>8</v>
-      </c>
-      <c r="B9" s="127" t="s">
+    <row r="15" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+      <c r="A15" s="116">
+        <v>14</v>
+      </c>
+      <c r="B15" s="117" t="s">
         <v>371</v>
       </c>
-      <c r="C9" s="127"/>
-      <c r="D9" s="127" t="s">
+      <c r="C15" s="117"/>
+      <c r="D15" s="117" t="s">
         <v>344</v>
       </c>
-      <c r="E9" s="127"/>
-      <c r="F9" s="127" t="s">
+      <c r="E15" s="117"/>
+      <c r="F15" s="117" t="s">
         <v>368</v>
       </c>
-      <c r="G9" s="127"/>
-      <c r="H9" s="127" t="s">
+      <c r="G15" s="117"/>
+      <c r="H15" s="117" t="s">
         <v>357</v>
       </c>
-      <c r="I9" s="127"/>
-      <c r="J9" s="127" t="s">
+      <c r="I15" s="117"/>
+      <c r="J15" s="117" t="s">
         <v>342</v>
       </c>
-      <c r="K9" s="127"/>
-      <c r="L9" s="127" t="s">
+      <c r="K15" s="117"/>
+      <c r="L15" s="117" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="128">
-        <v>9</v>
-      </c>
-      <c r="B10" s="129" t="s">
+    <row r="16" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="118">
+        <v>15</v>
+      </c>
+      <c r="B16" s="119" t="s">
         <v>371</v>
       </c>
-      <c r="C10" s="129"/>
-      <c r="D10" s="129" t="s">
+      <c r="C16" s="119"/>
+      <c r="D16" s="119" t="s">
         <v>344</v>
       </c>
-      <c r="E10" s="129"/>
-      <c r="F10" s="129" t="s">
+      <c r="E16" s="119"/>
+      <c r="F16" s="119" t="s">
         <v>373</v>
       </c>
-      <c r="G10" s="129"/>
-      <c r="H10" s="129" t="s">
+      <c r="G16" s="119"/>
+      <c r="H16" s="119" t="s">
         <v>358</v>
       </c>
-      <c r="I10" s="129"/>
-      <c r="J10" s="129" t="s">
+      <c r="I16" s="119"/>
+      <c r="J16" s="119" t="s">
         <v>372</v>
       </c>
-      <c r="K10" s="129"/>
-      <c r="L10" s="129" t="s">
+      <c r="K16" s="119"/>
+      <c r="L16" s="119" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="180" x14ac:dyDescent="0.25">
-      <c r="A11" s="128">
-        <v>10</v>
-      </c>
-      <c r="B11" s="129" t="s">
+    <row r="17" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+      <c r="A17" s="118">
+        <v>16</v>
+      </c>
+      <c r="B17" s="119" t="s">
         <v>376</v>
       </c>
-      <c r="C11" s="129"/>
-      <c r="D11" s="129" t="s">
+      <c r="C17" s="119"/>
+      <c r="D17" s="119" t="s">
         <v>342</v>
       </c>
-      <c r="E11" s="129"/>
-      <c r="F11" s="129" t="s">
+      <c r="E17" s="119"/>
+      <c r="F17" s="119" t="s">
         <v>368</v>
       </c>
-      <c r="G11" s="129"/>
-      <c r="H11" s="129" t="s">
+      <c r="G17" s="119"/>
+      <c r="H17" s="119" t="s">
         <v>357</v>
       </c>
-      <c r="I11" s="129"/>
-      <c r="J11" s="129" t="s">
+      <c r="I17" s="119"/>
+      <c r="J17" s="119" t="s">
         <v>342</v>
       </c>
-      <c r="K11" s="129"/>
-      <c r="L11" s="129" t="s">
+      <c r="K17" s="119"/>
+      <c r="L17" s="119" t="s">
         <v>379</v>
       </c>
     </row>
@@ -16297,54 +16508,54 @@
       <c r="H20" s="109"/>
     </row>
     <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="113" t="s">
+      <c r="A21" s="122" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="113"/>
-      <c r="C21" s="113"/>
-      <c r="D21" s="113"/>
-      <c r="E21" s="113"/>
-      <c r="F21" s="113"/>
+      <c r="B21" s="122"/>
+      <c r="C21" s="122"/>
+      <c r="D21" s="122"/>
+      <c r="E21" s="122"/>
+      <c r="F21" s="122"/>
     </row>
     <row r="22" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="114" t="s">
+      <c r="A22" s="123" t="s">
         <v>179</v>
       </c>
-      <c r="B22" s="114"/>
-      <c r="C22" s="114"/>
-      <c r="D22" s="114"/>
-      <c r="E22" s="114"/>
-      <c r="F22" s="114"/>
+      <c r="B22" s="123"/>
+      <c r="C22" s="123"/>
+      <c r="D22" s="123"/>
+      <c r="E22" s="123"/>
+      <c r="F22" s="123"/>
     </row>
     <row r="23" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="113" t="s">
+      <c r="A23" s="122" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="113"/>
-      <c r="C23" s="113"/>
-      <c r="D23" s="113"/>
-      <c r="E23" s="113"/>
-      <c r="F23" s="113"/>
+      <c r="B23" s="122"/>
+      <c r="C23" s="122"/>
+      <c r="D23" s="122"/>
+      <c r="E23" s="122"/>
+      <c r="F23" s="122"/>
     </row>
     <row r="24" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="113" t="s">
+      <c r="A24" s="122" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="113"/>
-      <c r="C24" s="113"/>
-      <c r="D24" s="113"/>
-      <c r="E24" s="113"/>
-      <c r="F24" s="113"/>
+      <c r="B24" s="122"/>
+      <c r="C24" s="122"/>
+      <c r="D24" s="122"/>
+      <c r="E24" s="122"/>
+      <c r="F24" s="122"/>
     </row>
     <row r="25" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="113" t="s">
+      <c r="A25" s="122" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="113"/>
-      <c r="C25" s="113"/>
-      <c r="D25" s="113"/>
-      <c r="E25" s="113"/>
-      <c r="F25" s="113"/>
+      <c r="B25" s="122"/>
+      <c r="C25" s="122"/>
+      <c r="D25" s="122"/>
+      <c r="E25" s="122"/>
+      <c r="F25" s="122"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="30"/>
@@ -16528,38 +16739,38 @@
       <c r="B3" s="69"/>
       <c r="C3" s="70"/>
       <c r="D3" s="71"/>
-      <c r="E3" s="118" t="s">
+      <c r="E3" s="127" t="s">
         <v>276</v>
       </c>
-      <c r="F3" s="119"/>
-      <c r="G3" s="119"/>
-      <c r="H3" s="116"/>
-      <c r="I3" s="115" t="s">
+      <c r="F3" s="128"/>
+      <c r="G3" s="128"/>
+      <c r="H3" s="125"/>
+      <c r="I3" s="124" t="s">
         <v>304</v>
       </c>
-      <c r="J3" s="116"/>
-      <c r="K3" s="115" t="s">
+      <c r="J3" s="125"/>
+      <c r="K3" s="124" t="s">
         <v>305</v>
       </c>
-      <c r="L3" s="117"/>
-      <c r="M3" s="118" t="s">
+      <c r="L3" s="126"/>
+      <c r="M3" s="127" t="s">
         <v>292</v>
       </c>
-      <c r="N3" s="119"/>
-      <c r="O3" s="116"/>
-      <c r="P3" s="120" t="s">
+      <c r="N3" s="128"/>
+      <c r="O3" s="125"/>
+      <c r="P3" s="129" t="s">
         <v>257</v>
       </c>
-      <c r="Q3" s="119"/>
-      <c r="R3" s="119"/>
-      <c r="S3" s="119"/>
-      <c r="T3" s="119"/>
-      <c r="U3" s="119"/>
-      <c r="V3" s="119"/>
-      <c r="W3" s="119"/>
-      <c r="X3" s="119"/>
-      <c r="Y3" s="119"/>
-      <c r="Z3" s="121"/>
+      <c r="Q3" s="128"/>
+      <c r="R3" s="128"/>
+      <c r="S3" s="128"/>
+      <c r="T3" s="128"/>
+      <c r="U3" s="128"/>
+      <c r="V3" s="128"/>
+      <c r="W3" s="128"/>
+      <c r="X3" s="128"/>
+      <c r="Y3" s="128"/>
+      <c r="Z3" s="130"/>
       <c r="AA3" s="90"/>
     </row>
     <row r="4" spans="1:27" ht="170.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -19835,10 +20046,10 @@
       <c r="A3" s="69"/>
       <c r="B3" s="70"/>
       <c r="C3" s="71"/>
-      <c r="D3" s="118" t="s">
+      <c r="D3" s="127" t="s">
         <v>202</v>
       </c>
-      <c r="E3" s="116"/>
+      <c r="E3" s="125"/>
       <c r="F3" s="73"/>
     </row>
     <row r="4" spans="1:6" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20098,32 +20309,32 @@
       <c r="F23" s="59"/>
     </row>
     <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="113"/>
-      <c r="B24" s="113"/>
-      <c r="C24" s="113"/>
-      <c r="D24" s="113"/>
-      <c r="E24" s="113"/>
+      <c r="A24" s="122"/>
+      <c r="B24" s="122"/>
+      <c r="C24" s="122"/>
+      <c r="D24" s="122"/>
+      <c r="E24" s="122"/>
     </row>
     <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="113"/>
-      <c r="B25" s="113"/>
-      <c r="C25" s="113"/>
-      <c r="D25" s="113"/>
-      <c r="E25" s="113"/>
+      <c r="A25" s="122"/>
+      <c r="B25" s="122"/>
+      <c r="C25" s="122"/>
+      <c r="D25" s="122"/>
+      <c r="E25" s="122"/>
     </row>
     <row r="26" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="113"/>
-      <c r="B26" s="113"/>
-      <c r="C26" s="113"/>
-      <c r="D26" s="113"/>
-      <c r="E26" s="113"/>
+      <c r="A26" s="122"/>
+      <c r="B26" s="122"/>
+      <c r="C26" s="122"/>
+      <c r="D26" s="122"/>
+      <c r="E26" s="122"/>
     </row>
     <row r="27" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="113"/>
-      <c r="B27" s="113"/>
-      <c r="C27" s="113"/>
-      <c r="D27" s="113"/>
-      <c r="E27" s="113"/>
+      <c r="A27" s="122"/>
+      <c r="B27" s="122"/>
+      <c r="C27" s="122"/>
+      <c r="D27" s="122"/>
+      <c r="E27" s="122"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="60"/>
@@ -20925,27 +21136,27 @@
       <c r="H16" s="32"/>
     </row>
     <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="113"/>
-      <c r="B17" s="113"/>
-      <c r="C17" s="113"/>
+      <c r="A17" s="122"/>
+      <c r="B17" s="122"/>
+      <c r="C17" s="122"/>
       <c r="D17" s="32"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="113"/>
-      <c r="B18" s="113"/>
-      <c r="C18" s="113"/>
+      <c r="A18" s="122"/>
+      <c r="B18" s="122"/>
+      <c r="C18" s="122"/>
       <c r="D18" s="32"/>
       <c r="E18" s="32"/>
       <c r="F18" s="32"/>
       <c r="H18" s="32"/>
     </row>
     <row r="19" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="113"/>
-      <c r="B19" s="113"/>
-      <c r="C19" s="113"/>
+      <c r="A19" s="122"/>
+      <c r="B19" s="122"/>
+      <c r="C19" s="122"/>
       <c r="D19" s="32"/>
       <c r="E19" s="32"/>
       <c r="F19" s="32"/>
@@ -21384,30 +21595,30 @@
       <c r="C41" s="52"/>
     </row>
     <row r="42" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="122" t="s">
+      <c r="A42" s="131" t="s">
         <v>174</v>
       </c>
-      <c r="B42" s="122"/>
-      <c r="C42" s="122"/>
+      <c r="B42" s="131"/>
+      <c r="C42" s="131"/>
     </row>
     <row r="43" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="123" t="s">
+      <c r="A43" s="132" t="s">
         <v>175</v>
       </c>
-      <c r="B43" s="123"/>
-      <c r="C43" s="123"/>
+      <c r="B43" s="132"/>
+      <c r="C43" s="132"/>
     </row>
     <row r="44" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="122" t="s">
+      <c r="A44" s="131" t="s">
         <v>176</v>
       </c>
-      <c r="B44" s="122"/>
-      <c r="C44" s="122"/>
+      <c r="B44" s="131"/>
+      <c r="C44" s="131"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="113"/>
-      <c r="B45" s="113"/>
-      <c r="C45" s="113"/>
+      <c r="A45" s="122"/>
+      <c r="B45" s="122"/>
+      <c r="C45" s="122"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="37"/>

</xml_diff>

<commit_message>
Updated table on units of analysis and figure on research questions
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="14" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938"/>
   </bookViews>
   <sheets>
     <sheet name="Table - Unit of Analysis" sheetId="17" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="421">
   <si>
     <t>Total</t>
   </si>
@@ -1328,16 +1328,10 @@
     <t>Individuals</t>
   </si>
   <si>
-    <t>Does technology maturity level influence an organizations willingness to acquire a given technology?</t>
-  </si>
-  <si>
     <t>Technology maturity level</t>
   </si>
   <si>
     <t>Individuals grouped by organization</t>
-  </si>
-  <si>
-    <t>Organizations were 50 percent more likely to have a majority of technology transfer decision-makers favor adding the technology to the decision agenda when it was a high maturity level than when it was the low maturity level.</t>
   </si>
   <si>
     <t>Does technology maturity level influence a demand-side technology transfer decision-maker's willingness to pursue a given technology?</t>
@@ -1414,22 +1408,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Unit of Observation
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The item (or items) is actually observed, measured, or collected.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Unit of Analysis
 </t>
     </r>
@@ -1509,9 +1487,6 @@
     <t>Subjects were 50 percent more likely to consider acquiring the high maturity level technology than the low maturity level technology.</t>
   </si>
   <si>
-    <t>Do technology transfer decision-makers at private sector organizations disfavor low maturity level technologies?</t>
-  </si>
-  <si>
     <t>Only 20 percent of subjects chose to pursue the low maturity level technology where 50 percent of subjects chose to pursue the high maturity level technology.</t>
   </si>
   <si>
@@ -1550,9 +1525,6 @@
   </si>
   <si>
     <t>Fifty percent (50%) of organizations used technology maturity as a factor in determining the uncertainty associated with a technology being considered for acquisition.</t>
-  </si>
-  <si>
-    <t>Response about how organization assesses the uncertainty of a technology being considered for acquisition.</t>
   </si>
   <si>
     <t>Policy Problem:</t>
@@ -1624,6 +1596,87 @@
       </rPr>
       <t xml:space="preserve"> (See attached)</t>
     </r>
+  </si>
+  <si>
+    <t>Organizations were 50 percent more likely to have a majority of technology transfer decision-makers favor acquiring the technology when it was a high maturity level than when it was the low maturity level.</t>
+  </si>
+  <si>
+    <t>Does technology maturity level influence a demand-side organization's willingness to acquire a given technology?</t>
+  </si>
+  <si>
+    <t>Do technology transfer decision-makers at demand-side private sector organizations disfavor low maturity level technologies?</t>
+  </si>
+  <si>
+    <t>Information about licensing deals</t>
+  </si>
+  <si>
+    <t>Content analysis
+Interviews</t>
+  </si>
+  <si>
+    <t>Documents (news releases about licensing deals)
+Individuals</t>
+  </si>
+  <si>
+    <t>2b</t>
+  </si>
+  <si>
+    <t>2a</t>
+  </si>
+  <si>
+    <t>4a</t>
+  </si>
+  <si>
+    <t>4b</t>
+  </si>
+  <si>
+    <t>4c</t>
+  </si>
+  <si>
+    <t>4d</t>
+  </si>
+  <si>
+    <t>4e</t>
+  </si>
+  <si>
+    <t>5a</t>
+  </si>
+  <si>
+    <t>5b</t>
+  </si>
+  <si>
+    <t>5c</t>
+  </si>
+  <si>
+    <t>6a</t>
+  </si>
+  <si>
+    <t>6b</t>
+  </si>
+  <si>
+    <t>7a</t>
+  </si>
+  <si>
+    <t>7b</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Unit of Observation
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The item (or items) actually observed, measured, or collected.</t>
+    </r>
+  </si>
+  <si>
+    <t>Responses about how organizations assess the uncertainty of a technology being considered for acquisition.</t>
   </si>
 </sst>
 </file>
@@ -1987,7 +2040,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -2347,6 +2400,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2373,12 +2441,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -6690,177 +6752,700 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>325755</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>59054</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>441960</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Oval 2">
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="34" name="Group 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD233C43-0F9D-4ACF-B636-472C0AE35751}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{445C3D5D-4683-47A0-A2CC-EE65C8C4CC81}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4105275" y="3362324"/>
-          <a:ext cx="1097280" cy="1097280"/>
+          <a:off x="1657350" y="3219450"/>
+          <a:ext cx="5090160" cy="4175760"/>
+          <a:chOff x="2352675" y="3219450"/>
+          <a:chExt cx="5090160" cy="4175760"/>
         </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Research Focus</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6AD26590-3F4B-4518-A25D-3E8963C124F0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2486025" y="3486150"/>
-          <a:ext cx="1457325" cy="276225"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="34925">
-          <a:solidFill>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6AD26590-3F4B-4518-A25D-3E8963C124F0}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2695575" y="5048250"/>
+            <a:ext cx="1457325" cy="276225"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="34925">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="med" len="lg"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
             <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="med" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>504826</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBBBD7A6-E6EF-4DEC-B3DB-176C513D51C6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="5381626" y="4086225"/>
-          <a:ext cx="1523999" cy="361950"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="34925">
-          <a:solidFill>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBBBD7A6-E6EF-4DEC-B3DB-176C513D51C6}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1" flipV="1">
+            <a:off x="5591176" y="5648325"/>
+            <a:ext cx="1523999" cy="361950"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="34925">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="med" len="lg"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
             <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="med" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1611748-3DDB-4C42-92FF-7505F3012EEE}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="5419727" y="4305300"/>
+            <a:ext cx="1152523" cy="809625"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="34925">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="med" len="lg"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CA98F22-A31E-448B-87FD-5DBAA15050F6}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="3038475" y="5972175"/>
+            <a:ext cx="1323975" cy="1019176"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="34925">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="med" len="lg"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{619AAA80-B249-445A-9685-B64A206D56BA}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1" flipV="1">
+            <a:off x="4905375" y="6153150"/>
+            <a:ext cx="9525" cy="847725"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="34925">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="med" len="lg"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="21" name="Straight Arrow Connector 20">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B14EE800-C54E-4B20-824B-9CEC9CD0CE97}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4838700" y="3562350"/>
+            <a:ext cx="9525" cy="1238250"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="34925">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="med" len="lg"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="24" name="TextBox 23">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9E98AA5-91EB-475C-8446-6875CBF3D5C6}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4657725" y="3219450"/>
+            <a:ext cx="365760" cy="327660"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200"/>
+              <a:t>R</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="-25000"/>
+              <a:t>1</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="28" name="TextBox 27">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5434548E-348E-441C-88A2-445469707225}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2352675" y="4781550"/>
+            <a:ext cx="365760" cy="365760"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200"/>
+              <a:t>R</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="-25000"/>
+              <a:t>2</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="29" name="TextBox 28">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42003440-D0E8-46C3-B8F6-D84718F56B60}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2705100" y="6905625"/>
+            <a:ext cx="365760" cy="365760"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200"/>
+              <a:t>R</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="-25000"/>
+              <a:t>3</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="30" name="TextBox 29">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2548F813-3D6D-42DB-B234-071B6A03A4F9}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4724400" y="7029450"/>
+            <a:ext cx="365760" cy="365760"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200"/>
+              <a:t>R</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="-25000"/>
+              <a:t>4</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="31" name="TextBox 30">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4084328A-9E0B-4C7D-9CC2-11A6A177D9A1}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7077075" y="5848350"/>
+            <a:ext cx="365760" cy="365760"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200"/>
+              <a:t>R</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="-25000"/>
+              <a:t>5</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="32" name="TextBox 31">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7121D022-EE9C-4216-B8D3-37A5DA51708B}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6562725" y="4067175"/>
+            <a:ext cx="365760" cy="365760"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200"/>
+              <a:t>R</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="-25000"/>
+              <a:t>n</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="37" name="Picture 36">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD30540C-FC92-438C-A4D0-FC40CAD63B18}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill rotWithShape="1">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect t="2288" r="8230" b="4271"/>
+          <a:stretch/>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4324352" y="4943475"/>
+            <a:ext cx="1070142" cy="1097280"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="39" name="TextBox 38">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC5FA382-E1CC-4624-A42E-6483FEEA17D6}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4438650" y="5248275"/>
+            <a:ext cx="822960" cy="514350"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Research Focus</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1200" baseline="-25000">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -14859,18 +15444,18 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J17" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A19" sqref="A19"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="112" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="112" customWidth="1"/>
     <col min="2" max="2" width="50.7109375" style="111" customWidth="1"/>
     <col min="3" max="3" width="1.7109375" style="111" customWidth="1"/>
     <col min="4" max="4" width="24" style="111" customWidth="1"/>
@@ -14890,27 +15475,27 @@
     <row r="1" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="115"/>
       <c r="B1" s="114" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C1" s="114"/>
       <c r="D1" s="114" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="E1" s="114"/>
       <c r="F1" s="114" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G1" s="114"/>
       <c r="H1" s="114" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="I1" s="114"/>
       <c r="J1" s="114" t="s">
-        <v>362</v>
+        <v>419</v>
       </c>
       <c r="K1" s="114"/>
       <c r="L1" s="114" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="180" x14ac:dyDescent="0.25">
@@ -14918,7 +15503,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="121" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C2" s="121"/>
       <c r="D2" s="121" t="s">
@@ -14926,11 +15511,11 @@
       </c>
       <c r="E2" s="121"/>
       <c r="F2" s="121" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="G2" s="121"/>
       <c r="H2" s="121" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="I2" s="121"/>
       <c r="J2" s="121" t="s">
@@ -14938,15 +15523,15 @@
       </c>
       <c r="K2" s="121"/>
       <c r="L2" s="121" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="180" x14ac:dyDescent="0.25">
-      <c r="A3" s="83">
-        <v>2</v>
+      <c r="A3" s="83" t="s">
+        <v>406</v>
       </c>
       <c r="B3" s="84" t="s">
-        <v>343</v>
+        <v>400</v>
       </c>
       <c r="C3" s="84"/>
       <c r="D3" s="84" t="s">
@@ -14954,83 +15539,83 @@
       </c>
       <c r="E3" s="84"/>
       <c r="F3" s="84" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="G3" s="84"/>
       <c r="H3" s="84" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="I3" s="84"/>
       <c r="J3" s="84" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K3" s="84"/>
       <c r="L3" s="84" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="113" customFormat="1" ht="180" x14ac:dyDescent="0.25">
-      <c r="A4" s="116">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="123" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="83" t="s">
+        <v>405</v>
+      </c>
+      <c r="B4" s="84" t="s">
+        <v>400</v>
+      </c>
+      <c r="C4" s="84"/>
+      <c r="D4" s="84" t="s">
+        <v>341</v>
+      </c>
+      <c r="E4" s="84"/>
+      <c r="F4" s="84" t="s">
+        <v>403</v>
+      </c>
+      <c r="G4" s="84"/>
+      <c r="H4" s="84" t="s">
+        <v>402</v>
+      </c>
+      <c r="I4" s="84"/>
+      <c r="J4" s="84" t="s">
+        <v>404</v>
+      </c>
+      <c r="K4" s="84"/>
+      <c r="L4" s="84" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="113" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A5" s="116">
         <v>3</v>
       </c>
-      <c r="B4" s="117" t="s">
-        <v>380</v>
-      </c>
-      <c r="C4" s="117"/>
-      <c r="D4" s="117" t="s">
+      <c r="B5" s="117" t="s">
+        <v>401</v>
+      </c>
+      <c r="C5" s="117"/>
+      <c r="D5" s="117" t="s">
         <v>342</v>
       </c>
-      <c r="E4" s="117"/>
-      <c r="F4" s="117" t="s">
-        <v>383</v>
-      </c>
-      <c r="G4" s="117"/>
-      <c r="H4" s="117" t="s">
-        <v>357</v>
-      </c>
-      <c r="I4" s="117"/>
-      <c r="J4" s="117" t="s">
+      <c r="E5" s="117"/>
+      <c r="F5" s="117" t="s">
+        <v>379</v>
+      </c>
+      <c r="G5" s="117"/>
+      <c r="H5" s="117" t="s">
+        <v>355</v>
+      </c>
+      <c r="I5" s="117"/>
+      <c r="J5" s="117" t="s">
         <v>342</v>
       </c>
-      <c r="K4" s="117"/>
-      <c r="L4" s="117" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="122" customFormat="1" ht="180" x14ac:dyDescent="0.25">
-      <c r="A5" s="118">
-        <v>4</v>
-      </c>
-      <c r="B5" s="119" t="s">
-        <v>382</v>
-      </c>
-      <c r="C5" s="119"/>
-      <c r="D5" s="119" t="s">
-        <v>341</v>
-      </c>
-      <c r="E5" s="119"/>
-      <c r="F5" s="119" t="s">
-        <v>369</v>
-      </c>
-      <c r="G5" s="119"/>
-      <c r="H5" s="119" t="s">
-        <v>357</v>
-      </c>
-      <c r="I5" s="119"/>
-      <c r="J5" s="119" t="s">
-        <v>345</v>
-      </c>
-      <c r="K5" s="119"/>
-      <c r="L5" s="119" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="122" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="118">
-        <v>5</v>
+      <c r="K5" s="117"/>
+      <c r="L5" s="117" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="122" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A6" s="118" t="s">
+        <v>407</v>
       </c>
       <c r="B6" s="119" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="C6" s="119"/>
       <c r="D6" s="119" t="s">
@@ -15038,27 +15623,27 @@
       </c>
       <c r="E6" s="119"/>
       <c r="F6" s="119" t="s">
-        <v>349</v>
+        <v>366</v>
       </c>
       <c r="G6" s="119"/>
       <c r="H6" s="119" t="s">
-        <v>385</v>
+        <v>355</v>
       </c>
       <c r="I6" s="119"/>
       <c r="J6" s="119" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="K6" s="119"/>
       <c r="L6" s="119" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="122" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A7" s="118">
-        <v>6</v>
+        <v>380</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="122" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="118" t="s">
+        <v>408</v>
       </c>
       <c r="B7" s="119" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="C7" s="119"/>
       <c r="D7" s="119" t="s">
@@ -15066,11 +15651,11 @@
       </c>
       <c r="E7" s="119"/>
       <c r="F7" s="119" t="s">
-        <v>387</v>
+        <v>347</v>
       </c>
       <c r="G7" s="119"/>
       <c r="H7" s="119" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="I7" s="119"/>
       <c r="J7" s="119" t="s">
@@ -15078,15 +15663,15 @@
       </c>
       <c r="K7" s="119"/>
       <c r="L7" s="119" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="122" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="118">
-        <v>7</v>
+        <v>382</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="122" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A8" s="118" t="s">
+        <v>409</v>
       </c>
       <c r="B8" s="119" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="C8" s="119"/>
       <c r="D8" s="119" t="s">
@@ -15094,27 +15679,27 @@
       </c>
       <c r="E8" s="119"/>
       <c r="F8" s="119" t="s">
-        <v>350</v>
+        <v>383</v>
       </c>
       <c r="G8" s="119"/>
       <c r="H8" s="119" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="I8" s="119"/>
       <c r="J8" s="119" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="K8" s="119"/>
       <c r="L8" s="119" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="122" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="118">
-        <v>8</v>
+        <v>382</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="122" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="118" t="s">
+        <v>410</v>
       </c>
       <c r="B9" s="119" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="C9" s="119"/>
       <c r="D9" s="119" t="s">
@@ -15122,55 +15707,55 @@
       </c>
       <c r="E9" s="119"/>
       <c r="F9" s="119" t="s">
-        <v>374</v>
+        <v>348</v>
       </c>
       <c r="G9" s="119"/>
       <c r="H9" s="119" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="I9" s="119"/>
       <c r="J9" s="119" t="s">
-        <v>342</v>
+        <v>349</v>
       </c>
       <c r="K9" s="119"/>
       <c r="L9" s="119" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="135" x14ac:dyDescent="0.25">
-      <c r="A10" s="83">
-        <v>9</v>
-      </c>
-      <c r="B10" s="84" t="s">
-        <v>355</v>
-      </c>
-      <c r="C10" s="84"/>
-      <c r="D10" s="84" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="122" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="118" t="s">
+        <v>411</v>
+      </c>
+      <c r="B10" s="119" t="s">
+        <v>378</v>
+      </c>
+      <c r="C10" s="119"/>
+      <c r="D10" s="119" t="s">
         <v>341</v>
       </c>
-      <c r="E10" s="84"/>
-      <c r="F10" s="84" t="s">
-        <v>350</v>
-      </c>
-      <c r="G10" s="84"/>
-      <c r="H10" s="84" t="s">
-        <v>352</v>
-      </c>
-      <c r="I10" s="84"/>
-      <c r="J10" s="84" t="s">
-        <v>351</v>
-      </c>
-      <c r="K10" s="84"/>
-      <c r="L10" s="84" t="s">
+      <c r="E10" s="119"/>
+      <c r="F10" s="119" t="s">
+        <v>371</v>
+      </c>
+      <c r="G10" s="119"/>
+      <c r="H10" s="119" t="s">
+        <v>387</v>
+      </c>
+      <c r="I10" s="119"/>
+      <c r="J10" s="119" t="s">
+        <v>342</v>
+      </c>
+      <c r="K10" s="119"/>
+      <c r="L10" s="119" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A11" s="83" t="s">
+        <v>412</v>
+      </c>
+      <c r="B11" s="84" t="s">
         <v>353</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="135" x14ac:dyDescent="0.25">
-      <c r="A11" s="83">
-        <v>10</v>
-      </c>
-      <c r="B11" s="84" t="s">
-        <v>355</v>
       </c>
       <c r="C11" s="84"/>
       <c r="D11" s="84" t="s">
@@ -15178,27 +15763,27 @@
       </c>
       <c r="E11" s="84"/>
       <c r="F11" s="84" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G11" s="84"/>
       <c r="H11" s="84" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="I11" s="84"/>
       <c r="J11" s="84" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="K11" s="84"/>
       <c r="L11" s="84" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="135" x14ac:dyDescent="0.25">
-      <c r="A12" s="83">
-        <v>11</v>
+      <c r="A12" s="83" t="s">
+        <v>413</v>
       </c>
       <c r="B12" s="84" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C12" s="84"/>
       <c r="D12" s="84" t="s">
@@ -15206,27 +15791,27 @@
       </c>
       <c r="E12" s="84"/>
       <c r="F12" s="84" t="s">
-        <v>374</v>
+        <v>347</v>
       </c>
       <c r="G12" s="84"/>
       <c r="H12" s="84" t="s">
-        <v>375</v>
+        <v>352</v>
       </c>
       <c r="I12" s="84"/>
       <c r="J12" s="84" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K12" s="84"/>
       <c r="L12" s="84" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="83">
-        <v>12</v>
+        <v>354</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A13" s="83" t="s">
+        <v>414</v>
       </c>
       <c r="B13" s="84" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="C13" s="84"/>
       <c r="D13" s="84" t="s">
@@ -15234,27 +15819,27 @@
       </c>
       <c r="E13" s="84"/>
       <c r="F13" s="84" t="s">
-        <v>349</v>
+        <v>371</v>
       </c>
       <c r="G13" s="84"/>
       <c r="H13" s="84" t="s">
-        <v>365</v>
+        <v>372</v>
       </c>
       <c r="I13" s="84"/>
       <c r="J13" s="84" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="K13" s="84"/>
       <c r="L13" s="84" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="83">
-        <v>13</v>
+      <c r="A14" s="83" t="s">
+        <v>415</v>
       </c>
       <c r="B14" s="84" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C14" s="84"/>
       <c r="D14" s="84" t="s">
@@ -15262,126 +15847,159 @@
       </c>
       <c r="E14" s="84"/>
       <c r="F14" s="84" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="G14" s="84"/>
       <c r="H14" s="84" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="I14" s="84"/>
       <c r="J14" s="84" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="K14" s="84"/>
       <c r="L14" s="84" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="83" t="s">
+        <v>416</v>
+      </c>
+      <c r="B15" s="84" t="s">
+        <v>357</v>
+      </c>
+      <c r="C15" s="84"/>
+      <c r="D15" s="84" t="s">
+        <v>341</v>
+      </c>
+      <c r="E15" s="84"/>
+      <c r="F15" s="84" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="180" x14ac:dyDescent="0.25">
-      <c r="A15" s="116">
-        <v>14</v>
-      </c>
-      <c r="B15" s="117" t="s">
-        <v>371</v>
-      </c>
-      <c r="C15" s="117"/>
-      <c r="D15" s="117" t="s">
-        <v>344</v>
-      </c>
-      <c r="E15" s="117"/>
-      <c r="F15" s="117" t="s">
+      <c r="G15" s="84"/>
+      <c r="H15" s="84" t="s">
+        <v>356</v>
+      </c>
+      <c r="I15" s="84"/>
+      <c r="J15" s="84" t="s">
+        <v>349</v>
+      </c>
+      <c r="K15" s="84"/>
+      <c r="L15" s="84" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+      <c r="A16" s="116" t="s">
+        <v>417</v>
+      </c>
+      <c r="B16" s="117" t="s">
         <v>368</v>
       </c>
-      <c r="G15" s="117"/>
-      <c r="H15" s="117" t="s">
-        <v>357</v>
-      </c>
-      <c r="I15" s="117"/>
-      <c r="J15" s="117" t="s">
+      <c r="C16" s="117"/>
+      <c r="D16" s="117" t="s">
+        <v>343</v>
+      </c>
+      <c r="E16" s="117"/>
+      <c r="F16" s="117" t="s">
+        <v>365</v>
+      </c>
+      <c r="G16" s="117"/>
+      <c r="H16" s="117" t="s">
+        <v>355</v>
+      </c>
+      <c r="I16" s="117"/>
+      <c r="J16" s="117" t="s">
         <v>342</v>
       </c>
-      <c r="K15" s="117"/>
-      <c r="L15" s="117" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="118">
-        <v>15</v>
-      </c>
-      <c r="B16" s="119" t="s">
-        <v>371</v>
-      </c>
-      <c r="C16" s="119"/>
-      <c r="D16" s="119" t="s">
-        <v>344</v>
-      </c>
-      <c r="E16" s="119"/>
-      <c r="F16" s="119" t="s">
-        <v>373</v>
-      </c>
-      <c r="G16" s="119"/>
-      <c r="H16" s="119" t="s">
-        <v>358</v>
-      </c>
-      <c r="I16" s="119"/>
-      <c r="J16" s="119" t="s">
-        <v>372</v>
-      </c>
-      <c r="K16" s="119"/>
-      <c r="L16" s="119" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="180" x14ac:dyDescent="0.25">
-      <c r="A17" s="118">
-        <v>16</v>
+      <c r="K16" s="117"/>
+      <c r="L16" s="117" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="118" t="s">
+        <v>418</v>
       </c>
       <c r="B17" s="119" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="C17" s="119"/>
       <c r="D17" s="119" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E17" s="119"/>
       <c r="F17" s="119" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="G17" s="119"/>
       <c r="H17" s="119" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I17" s="119"/>
       <c r="J17" s="119" t="s">
-        <v>342</v>
+        <v>369</v>
       </c>
       <c r="K17" s="119"/>
       <c r="L17" s="119" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="112">
-        <v>17</v>
-      </c>
-      <c r="B18" s="111" t="s">
-        <v>392</v>
-      </c>
-      <c r="D18" s="111" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+      <c r="A18" s="116">
+        <v>8</v>
+      </c>
+      <c r="B18" s="117" t="s">
+        <v>373</v>
+      </c>
+      <c r="C18" s="117"/>
+      <c r="D18" s="117" t="s">
+        <v>342</v>
+      </c>
+      <c r="E18" s="117"/>
+      <c r="F18" s="117" t="s">
+        <v>365</v>
+      </c>
+      <c r="G18" s="117"/>
+      <c r="H18" s="117" t="s">
+        <v>355</v>
+      </c>
+      <c r="I18" s="117"/>
+      <c r="J18" s="117" t="s">
+        <v>342</v>
+      </c>
+      <c r="K18" s="117"/>
+      <c r="L18" s="117" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="83">
+        <v>9</v>
+      </c>
+      <c r="B19" s="84" t="s">
+        <v>388</v>
+      </c>
+      <c r="C19" s="84"/>
+      <c r="D19" s="84" t="s">
         <v>341</v>
       </c>
-      <c r="F18" s="111" t="s">
-        <v>349</v>
-      </c>
-      <c r="H18" s="111" t="s">
-        <v>394</v>
-      </c>
-      <c r="J18" s="111" t="s">
+      <c r="E19" s="84"/>
+      <c r="F19" s="84" t="s">
+        <v>347</v>
+      </c>
+      <c r="G19" s="84"/>
+      <c r="H19" s="84" t="s">
+        <v>420</v>
+      </c>
+      <c r="I19" s="84"/>
+      <c r="J19" s="84" t="s">
         <v>342</v>
       </c>
-      <c r="L18" s="111" t="s">
-        <v>393</v>
+      <c r="K19" s="84"/>
+      <c r="L19" s="84" t="s">
+        <v>389</v>
       </c>
     </row>
   </sheetData>
@@ -15389,7 +16007,7 @@
   <pageSetup scale="55" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;LTable 
-Potential research questions based by unit of analysis, data collection method, and unit of observation</oddHeader>
+&amp;"-,Italic"Potential research questions by unit of analysis and data collection method</oddHeader>
     <oddFooter>&amp;CPage &amp;P of &amp;N</oddFooter>
   </headerFooter>
 </worksheet>
@@ -16847,9 +17465,14 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16858,71 +17481,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="125" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="135" t="s">
-        <v>401</v>
+      <c r="A3" s="126" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="136" t="s">
+      <c r="A6" s="139" t="s">
+        <v>390</v>
+      </c>
+      <c r="B6" s="139"/>
+      <c r="C6" s="129" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6" s="129"/>
+      <c r="E6" s="129"/>
+      <c r="F6" s="129"/>
+      <c r="G6" s="129"/>
+      <c r="H6" s="129"/>
+      <c r="I6" s="129"/>
+      <c r="J6" s="129"/>
+      <c r="K6" s="129"/>
+      <c r="L6" s="129"/>
+      <c r="M6" s="129"/>
+      <c r="N6" s="129"/>
+    </row>
+    <row r="8" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="139" t="s">
+        <v>391</v>
+      </c>
+      <c r="B8" s="139"/>
+      <c r="C8" s="129" t="s">
+        <v>392</v>
+      </c>
+      <c r="D8" s="129"/>
+      <c r="E8" s="129"/>
+      <c r="F8" s="129"/>
+      <c r="G8" s="129"/>
+      <c r="H8" s="129"/>
+      <c r="I8" s="129"/>
+      <c r="J8" s="129"/>
+      <c r="K8" s="129"/>
+      <c r="L8" s="129"/>
+      <c r="M8" s="129"/>
+      <c r="N8" s="129"/>
+    </row>
+    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="127"/>
+      <c r="B9" s="127"/>
+      <c r="C9" s="124"/>
+      <c r="D9" s="124"/>
+      <c r="E9" s="124"/>
+      <c r="F9" s="124"/>
+      <c r="G9" s="124"/>
+      <c r="H9" s="124"/>
+      <c r="I9" s="124"/>
+      <c r="J9" s="124"/>
+      <c r="K9" s="124"/>
+      <c r="L9" s="124"/>
+      <c r="M9" s="124"/>
+      <c r="N9" s="124"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="139" t="s">
         <v>395</v>
       </c>
-      <c r="B6" s="136"/>
-      <c r="C6" s="124" t="s">
+      <c r="B10" s="139"/>
+      <c r="C10" s="23" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="139" t="s">
+        <v>397</v>
+      </c>
+      <c r="B12" s="139"/>
+      <c r="C12" s="23" t="s">
         <v>398</v>
-      </c>
-      <c r="D6" s="124"/>
-      <c r="E6" s="124"/>
-      <c r="F6" s="124"/>
-      <c r="G6" s="124"/>
-      <c r="H6" s="124"/>
-      <c r="I6" s="124"/>
-      <c r="J6" s="124"/>
-      <c r="K6" s="124"/>
-      <c r="L6" s="124"/>
-      <c r="M6" s="124"/>
-      <c r="N6" s="124"/>
-    </row>
-    <row r="8" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="136" t="s">
-        <v>396</v>
-      </c>
-      <c r="B8" s="136"/>
-      <c r="C8" s="124" t="s">
-        <v>397</v>
-      </c>
-      <c r="D8" s="124"/>
-      <c r="E8" s="124"/>
-      <c r="F8" s="124"/>
-      <c r="G8" s="124"/>
-      <c r="H8" s="124"/>
-      <c r="I8" s="124"/>
-      <c r="J8" s="124"/>
-      <c r="K8" s="124"/>
-      <c r="L8" s="124"/>
-      <c r="M8" s="124"/>
-      <c r="N8" s="124"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="136" t="s">
-        <v>400</v>
-      </c>
-      <c r="B10" s="136"/>
-      <c r="C10" s="23" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="18" x14ac:dyDescent="0.25">
-      <c r="A12" s="136" t="s">
-        <v>402</v>
-      </c>
-      <c r="B12" s="136"/>
-      <c r="C12" s="23" t="s">
-        <v>403</v>
       </c>
     </row>
   </sheetData>
@@ -16935,7 +17574,7 @@
     <mergeCell ref="C8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="68" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -17760,54 +18399,54 @@
       <c r="H20" s="109"/>
     </row>
     <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="123" t="s">
+      <c r="A21" s="128" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="123"/>
-      <c r="C21" s="123"/>
-      <c r="D21" s="123"/>
-      <c r="E21" s="123"/>
-      <c r="F21" s="123"/>
+      <c r="B21" s="128"/>
+      <c r="C21" s="128"/>
+      <c r="D21" s="128"/>
+      <c r="E21" s="128"/>
+      <c r="F21" s="128"/>
     </row>
     <row r="22" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="124" t="s">
+      <c r="A22" s="129" t="s">
         <v>179</v>
       </c>
-      <c r="B22" s="124"/>
-      <c r="C22" s="124"/>
-      <c r="D22" s="124"/>
-      <c r="E22" s="124"/>
-      <c r="F22" s="124"/>
+      <c r="B22" s="129"/>
+      <c r="C22" s="129"/>
+      <c r="D22" s="129"/>
+      <c r="E22" s="129"/>
+      <c r="F22" s="129"/>
     </row>
     <row r="23" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="123" t="s">
+      <c r="A23" s="128" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="123"/>
-      <c r="C23" s="123"/>
-      <c r="D23" s="123"/>
-      <c r="E23" s="123"/>
-      <c r="F23" s="123"/>
+      <c r="B23" s="128"/>
+      <c r="C23" s="128"/>
+      <c r="D23" s="128"/>
+      <c r="E23" s="128"/>
+      <c r="F23" s="128"/>
     </row>
     <row r="24" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="123" t="s">
+      <c r="A24" s="128" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="123"/>
-      <c r="C24" s="123"/>
-      <c r="D24" s="123"/>
-      <c r="E24" s="123"/>
-      <c r="F24" s="123"/>
+      <c r="B24" s="128"/>
+      <c r="C24" s="128"/>
+      <c r="D24" s="128"/>
+      <c r="E24" s="128"/>
+      <c r="F24" s="128"/>
     </row>
     <row r="25" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="123" t="s">
+      <c r="A25" s="128" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="123"/>
-      <c r="C25" s="123"/>
-      <c r="D25" s="123"/>
-      <c r="E25" s="123"/>
-      <c r="F25" s="123"/>
+      <c r="B25" s="128"/>
+      <c r="C25" s="128"/>
+      <c r="D25" s="128"/>
+      <c r="E25" s="128"/>
+      <c r="F25" s="128"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="30"/>
@@ -17991,38 +18630,38 @@
       <c r="B3" s="69"/>
       <c r="C3" s="70"/>
       <c r="D3" s="71"/>
-      <c r="E3" s="128" t="s">
+      <c r="E3" s="133" t="s">
         <v>276</v>
       </c>
-      <c r="F3" s="129"/>
-      <c r="G3" s="129"/>
-      <c r="H3" s="126"/>
-      <c r="I3" s="125" t="s">
+      <c r="F3" s="134"/>
+      <c r="G3" s="134"/>
+      <c r="H3" s="131"/>
+      <c r="I3" s="130" t="s">
         <v>304</v>
       </c>
-      <c r="J3" s="126"/>
-      <c r="K3" s="125" t="s">
+      <c r="J3" s="131"/>
+      <c r="K3" s="130" t="s">
         <v>305</v>
       </c>
-      <c r="L3" s="127"/>
-      <c r="M3" s="128" t="s">
+      <c r="L3" s="132"/>
+      <c r="M3" s="133" t="s">
         <v>292</v>
       </c>
-      <c r="N3" s="129"/>
-      <c r="O3" s="126"/>
-      <c r="P3" s="130" t="s">
+      <c r="N3" s="134"/>
+      <c r="O3" s="131"/>
+      <c r="P3" s="135" t="s">
         <v>257</v>
       </c>
-      <c r="Q3" s="129"/>
-      <c r="R3" s="129"/>
-      <c r="S3" s="129"/>
-      <c r="T3" s="129"/>
-      <c r="U3" s="129"/>
-      <c r="V3" s="129"/>
-      <c r="W3" s="129"/>
-      <c r="X3" s="129"/>
-      <c r="Y3" s="129"/>
-      <c r="Z3" s="131"/>
+      <c r="Q3" s="134"/>
+      <c r="R3" s="134"/>
+      <c r="S3" s="134"/>
+      <c r="T3" s="134"/>
+      <c r="U3" s="134"/>
+      <c r="V3" s="134"/>
+      <c r="W3" s="134"/>
+      <c r="X3" s="134"/>
+      <c r="Y3" s="134"/>
+      <c r="Z3" s="136"/>
       <c r="AA3" s="90"/>
     </row>
     <row r="4" spans="1:27" ht="170.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -21298,10 +21937,10 @@
       <c r="A3" s="69"/>
       <c r="B3" s="70"/>
       <c r="C3" s="71"/>
-      <c r="D3" s="128" t="s">
+      <c r="D3" s="133" t="s">
         <v>202</v>
       </c>
-      <c r="E3" s="126"/>
+      <c r="E3" s="131"/>
       <c r="F3" s="73"/>
     </row>
     <row r="4" spans="1:6" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -21561,32 +22200,32 @@
       <c r="F23" s="59"/>
     </row>
     <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="123"/>
-      <c r="B24" s="123"/>
-      <c r="C24" s="123"/>
-      <c r="D24" s="123"/>
-      <c r="E24" s="123"/>
+      <c r="A24" s="128"/>
+      <c r="B24" s="128"/>
+      <c r="C24" s="128"/>
+      <c r="D24" s="128"/>
+      <c r="E24" s="128"/>
     </row>
     <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="123"/>
-      <c r="B25" s="123"/>
-      <c r="C25" s="123"/>
-      <c r="D25" s="123"/>
-      <c r="E25" s="123"/>
+      <c r="A25" s="128"/>
+      <c r="B25" s="128"/>
+      <c r="C25" s="128"/>
+      <c r="D25" s="128"/>
+      <c r="E25" s="128"/>
     </row>
     <row r="26" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="123"/>
-      <c r="B26" s="123"/>
-      <c r="C26" s="123"/>
-      <c r="D26" s="123"/>
-      <c r="E26" s="123"/>
+      <c r="A26" s="128"/>
+      <c r="B26" s="128"/>
+      <c r="C26" s="128"/>
+      <c r="D26" s="128"/>
+      <c r="E26" s="128"/>
     </row>
     <row r="27" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="123"/>
-      <c r="B27" s="123"/>
-      <c r="C27" s="123"/>
-      <c r="D27" s="123"/>
-      <c r="E27" s="123"/>
+      <c r="A27" s="128"/>
+      <c r="B27" s="128"/>
+      <c r="C27" s="128"/>
+      <c r="D27" s="128"/>
+      <c r="E27" s="128"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="60"/>
@@ -22388,27 +23027,27 @@
       <c r="H16" s="32"/>
     </row>
     <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="123"/>
-      <c r="B17" s="123"/>
-      <c r="C17" s="123"/>
+      <c r="A17" s="128"/>
+      <c r="B17" s="128"/>
+      <c r="C17" s="128"/>
       <c r="D17" s="32"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="123"/>
-      <c r="B18" s="123"/>
-      <c r="C18" s="123"/>
+      <c r="A18" s="128"/>
+      <c r="B18" s="128"/>
+      <c r="C18" s="128"/>
       <c r="D18" s="32"/>
       <c r="E18" s="32"/>
       <c r="F18" s="32"/>
       <c r="H18" s="32"/>
     </row>
     <row r="19" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="123"/>
-      <c r="B19" s="123"/>
-      <c r="C19" s="123"/>
+      <c r="A19" s="128"/>
+      <c r="B19" s="128"/>
+      <c r="C19" s="128"/>
       <c r="D19" s="32"/>
       <c r="E19" s="32"/>
       <c r="F19" s="32"/>
@@ -22847,30 +23486,30 @@
       <c r="C41" s="52"/>
     </row>
     <row r="42" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="132" t="s">
+      <c r="A42" s="137" t="s">
         <v>174</v>
       </c>
-      <c r="B42" s="132"/>
-      <c r="C42" s="132"/>
+      <c r="B42" s="137"/>
+      <c r="C42" s="137"/>
     </row>
     <row r="43" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="133" t="s">
+      <c r="A43" s="138" t="s">
         <v>175</v>
       </c>
-      <c r="B43" s="133"/>
-      <c r="C43" s="133"/>
+      <c r="B43" s="138"/>
+      <c r="C43" s="138"/>
     </row>
     <row r="44" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="132" t="s">
+      <c r="A44" s="137" t="s">
         <v>176</v>
       </c>
-      <c r="B44" s="132"/>
-      <c r="C44" s="132"/>
+      <c r="B44" s="137"/>
+      <c r="C44" s="137"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="123"/>
-      <c r="B45" s="123"/>
-      <c r="C45" s="123"/>
+      <c r="A45" s="128"/>
+      <c r="B45" s="128"/>
+      <c r="C45" s="128"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="37"/>

</xml_diff>

<commit_message>
Added cases to the table on units of analysis
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938"/>
   </bookViews>
   <sheets>
-    <sheet name="Table - Unit of Analysis" sheetId="17" r:id="rId1"/>
+    <sheet name="Table - Units of Analysis" sheetId="17" r:id="rId1"/>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId2"/>
     <sheet name="Table - Tech Tran Policies" sheetId="5" r:id="rId3"/>
     <sheet name="Table - Determinants Examined" sheetId="6" r:id="rId4"/>
@@ -33,7 +33,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">'Table - Determinants Examined'!$3:$4</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Table - Unit of Analysis'!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Table - Units of Analysis'!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="429">
   <si>
     <t>Total</t>
   </si>
@@ -1334,9 +1334,6 @@
     <t>Individuals grouped by organization</t>
   </si>
   <si>
-    <t>Does technology maturity level influence a demand-side technology transfer decision-maker's willingness to pursue a given technology?</t>
-  </si>
-  <si>
     <t>A higher percentage of private sector organizations in the life sciences sector acquired technology at a high maturity level than private sector organizations in all other sectors.</t>
   </si>
   <si>
@@ -1454,18 +1451,7 @@
     <t>Experiment using demand-side technology transfer decision-makers as subjects.  Random assignment to comparison or treatment group by organization afflication.  Comparison group presented with case where technology maturity level is low.  Treatment group presented with case where technology maturity level is high.  All other aspects of the case are the same.</t>
   </si>
   <si>
-    <t>Subjects chose to acquite the technology at the high maturity level twice as often as the technology at the low maturity level.</t>
-  </si>
-  <si>
     <t>Are technologies at a high maturity level more likely to be acquired by private sector organizations than technologies at a low maturity level?</t>
-  </si>
-  <si>
-    <t>Documents (news releases)
-Individuals</t>
-  </si>
-  <si>
-    <t>Content analysis
-Interviews or surveys</t>
   </si>
   <si>
     <t>Interviews</t>
@@ -1478,18 +1464,6 @@
     <t>Are demand-side technology transfer decision-makers more apt to consider acquiring a technology the higher the technology maturity level?</t>
   </si>
   <si>
-    <t>Subjects chose to acquire the technology at the high maturity level twice as often as the technology at the low maturity level.</t>
-  </si>
-  <si>
-    <t>Subjects were 50 percent more likely to add the technology to the decision agenda when it was a high maturity level than when it was the low maturity level.</t>
-  </si>
-  <si>
-    <t>Subjects were 50 percent more likely to consider acquiring the high maturity level technology than the low maturity level technology.</t>
-  </si>
-  <si>
-    <t>Only 20 percent of subjects chose to pursue the low maturity level technology where 50 percent of subjects chose to pursue the high maturity level technology.</t>
-  </si>
-  <si>
     <t>Do demand-side private sector organizations disfavor low maturity level technologies?</t>
   </si>
   <si>
@@ -1515,9 +1489,6 @@
     <t>Statements about technology transfer decisions.</t>
   </si>
   <si>
-    <t>Organizations chose to pursue a low maturity level technology only 20 percent of the time.</t>
-  </si>
-  <si>
     <t>Data about technology transfer decisions.</t>
   </si>
   <si>
@@ -1543,9 +1514,6 @@
   </si>
   <si>
     <t>Research Focus:</t>
-  </si>
-  <si>
-    <t>Isolating the Research Question</t>
   </si>
   <si>
     <t xml:space="preserve">Research Question(s): </t>
@@ -1610,14 +1578,6 @@
     <t>Information about licensing deals</t>
   </si>
   <si>
-    <t>Content analysis
-Interviews</t>
-  </si>
-  <si>
-    <t>Documents (news releases about licensing deals)
-Individuals</t>
-  </si>
-  <si>
     <t>2b</t>
   </si>
   <si>
@@ -1658,6 +1618,15 @@
   </si>
   <si>
     <t>7b</t>
+  </si>
+  <si>
+    <t>Responses about how organizations assess the uncertainty of a technology being considered for acquisition.</t>
+  </si>
+  <si>
+    <t>Conceptualization of the Proposed Study</t>
+  </si>
+  <si>
+    <t>Does technology maturity level influence a demand-side technology transfer decision-maker's willingness to acquire a given technology?</t>
   </si>
   <si>
     <r>
@@ -1672,11 +1641,65 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>The item (or items) actually observed, measured, or collected.</t>
+      <t>The item(s) actually observed, measured, or collected.</t>
     </r>
   </si>
   <si>
-    <t>Responses about how organizations assess the uncertainty of a technology being considered for acquisition.</t>
+    <t>Organizations demonstrated an unwillingness to acquire low maturity level technologies.</t>
+  </si>
+  <si>
+    <t>Documents (news releases and organization records); 
+Individuals</t>
+  </si>
+  <si>
+    <t>Content analysis; 
+Interviews or surveys</t>
+  </si>
+  <si>
+    <t>Content analysis; 
+Interviews</t>
+  </si>
+  <si>
+    <t>High maturity level technologies were pursued twice as often a low matruity levl technologies.</t>
+  </si>
+  <si>
+    <t>Organizations demonstrated a tendency not to pursue low maturity level technologies.</t>
+  </si>
+  <si>
+    <t>Organizations chose to pursue a low maturity level technology in only 20 percent of the cases.</t>
+  </si>
+  <si>
+    <t>Do demand-side technology transfer decision makers in private sector organizations use technology maturity level in their sensemaking and sensegiving communications?</t>
+  </si>
+  <si>
+    <t>Ethnographic study</t>
+  </si>
+  <si>
+    <t>Sensemaking and sensegiving communications.</t>
+  </si>
+  <si>
+    <t>Fifty percent (50%) of technology transfer decision-makers in private sector organizations studied used technology maturity level in their sensemaking and sensegiving communications.</t>
+  </si>
+  <si>
+    <t>Is technology maturity level used the sensemaking and sensegiving communications of demand-side private sector organizations?</t>
+  </si>
+  <si>
+    <t>Individuals (interpersonal interactions)</t>
+  </si>
+  <si>
+    <t>Technology maturity level was regularly incorporated into the sensemaking and sensegiving communications of private sector organizations.</t>
+  </si>
+  <si>
+    <t>Subjects were 50 percent more likely to acquire a high maturity level technology than a low maturity level.</t>
+  </si>
+  <si>
+    <t>Only 20 percent of subjects chose to pursue the low maturity level technology whereas 50 percent of subjects chose to pursue the high maturity level technology.</t>
+  </si>
+  <si>
+    <t>Subjects chose to acquire the high maturity level technology twice as often the low maturity level technology.</t>
+  </si>
+  <si>
+    <t>Subjects were 50 percent more likely to acquire the high maturity level technology than the low maturity level technology.</t>
   </si>
 </sst>
 </file>
@@ -2040,7 +2063,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -2408,6 +2431,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -15444,7 +15470,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
@@ -15456,54 +15482,54 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" style="112" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" style="111" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" style="111" customWidth="1"/>
     <col min="3" max="3" width="1.7109375" style="111" customWidth="1"/>
-    <col min="4" max="4" width="24" style="111" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="111" customWidth="1"/>
     <col min="5" max="5" width="1.7109375" style="111" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" style="111" customWidth="1"/>
+    <col min="6" max="6" width="40.7109375" style="111" customWidth="1"/>
     <col min="7" max="7" width="1.7109375" style="111" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" style="111" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" style="111" customWidth="1"/>
     <col min="9" max="9" width="1.7109375" style="111" customWidth="1"/>
-    <col min="10" max="10" width="25.7109375" style="111" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" style="111" customWidth="1"/>
     <col min="11" max="11" width="1.7109375" style="111" customWidth="1"/>
-    <col min="12" max="12" width="50.7109375" style="111" customWidth="1"/>
+    <col min="12" max="12" width="40.7109375" style="111" customWidth="1"/>
     <col min="13" max="13" width="9.140625" style="111"/>
     <col min="14" max="14" width="62" style="111" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="111"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="115"/>
       <c r="B1" s="114" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C1" s="114"/>
       <c r="D1" s="114" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E1" s="114"/>
       <c r="F1" s="114" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G1" s="114"/>
       <c r="H1" s="114" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I1" s="114"/>
       <c r="J1" s="114" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="K1" s="114"/>
       <c r="L1" s="114" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="120">
         <v>1</v>
       </c>
       <c r="B2" s="121" t="s">
-        <v>345</v>
+        <v>409</v>
       </c>
       <c r="C2" s="121"/>
       <c r="D2" s="121" t="s">
@@ -15511,11 +15537,11 @@
       </c>
       <c r="E2" s="121"/>
       <c r="F2" s="121" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G2" s="121"/>
       <c r="H2" s="121" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I2" s="121"/>
       <c r="J2" s="121" t="s">
@@ -15523,15 +15549,15 @@
       </c>
       <c r="K2" s="121"/>
       <c r="L2" s="121" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="83" t="s">
-        <v>406</v>
+        <v>394</v>
       </c>
       <c r="B3" s="84" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="C3" s="84"/>
       <c r="D3" s="84" t="s">
@@ -15539,11 +15565,11 @@
       </c>
       <c r="E3" s="84"/>
       <c r="F3" s="84" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G3" s="84"/>
       <c r="H3" s="84" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I3" s="84"/>
       <c r="J3" s="84" t="s">
@@ -15551,15 +15577,15 @@
       </c>
       <c r="K3" s="84"/>
       <c r="L3" s="84" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="123" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="83" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
       <c r="B4" s="84" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="C4" s="84"/>
       <c r="D4" s="84" t="s">
@@ -15567,27 +15593,27 @@
       </c>
       <c r="E4" s="84"/>
       <c r="F4" s="84" t="s">
-        <v>403</v>
+        <v>414</v>
       </c>
       <c r="G4" s="84"/>
       <c r="H4" s="84" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
       <c r="I4" s="84"/>
       <c r="J4" s="84" t="s">
-        <v>404</v>
+        <v>412</v>
       </c>
       <c r="K4" s="84"/>
       <c r="L4" s="84" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="113" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="113" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="116">
         <v>3</v>
       </c>
       <c r="B5" s="117" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="C5" s="117"/>
       <c r="D5" s="117" t="s">
@@ -15595,11 +15621,11 @@
       </c>
       <c r="E5" s="117"/>
       <c r="F5" s="117" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="G5" s="117"/>
       <c r="H5" s="117" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I5" s="117"/>
       <c r="J5" s="117" t="s">
@@ -15607,15 +15633,15 @@
       </c>
       <c r="K5" s="117"/>
       <c r="L5" s="117" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="122" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="122" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="118" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="B6" s="119" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="C6" s="119"/>
       <c r="D6" s="119" t="s">
@@ -15623,11 +15649,11 @@
       </c>
       <c r="E6" s="119"/>
       <c r="F6" s="119" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G6" s="119"/>
       <c r="H6" s="119" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I6" s="119"/>
       <c r="J6" s="119" t="s">
@@ -15635,15 +15661,15 @@
       </c>
       <c r="K6" s="119"/>
       <c r="L6" s="119" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="122" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="118" t="s">
-        <v>408</v>
+        <v>396</v>
       </c>
       <c r="B7" s="119" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="C7" s="119"/>
       <c r="D7" s="119" t="s">
@@ -15651,11 +15677,11 @@
       </c>
       <c r="E7" s="119"/>
       <c r="F7" s="119" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G7" s="119"/>
       <c r="H7" s="119" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="I7" s="119"/>
       <c r="J7" s="119" t="s">
@@ -15663,15 +15689,15 @@
       </c>
       <c r="K7" s="119"/>
       <c r="L7" s="119" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="122" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="118" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
       <c r="B8" s="119" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="C8" s="119"/>
       <c r="D8" s="119" t="s">
@@ -15679,11 +15705,11 @@
       </c>
       <c r="E8" s="119"/>
       <c r="F8" s="119" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="G8" s="119"/>
       <c r="H8" s="119" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="I8" s="119"/>
       <c r="J8" s="119" t="s">
@@ -15691,15 +15717,15 @@
       </c>
       <c r="K8" s="119"/>
       <c r="L8" s="119" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="122" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="118" t="s">
-        <v>410</v>
+        <v>398</v>
       </c>
       <c r="B9" s="119" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="C9" s="119"/>
       <c r="D9" s="119" t="s">
@@ -15707,27 +15733,27 @@
       </c>
       <c r="E9" s="119"/>
       <c r="F9" s="119" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G9" s="119"/>
       <c r="H9" s="119" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="I9" s="119"/>
       <c r="J9" s="119" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K9" s="119"/>
       <c r="L9" s="119" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="122" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="122" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="118" t="s">
-        <v>411</v>
+        <v>399</v>
       </c>
       <c r="B10" s="119" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="C10" s="119"/>
       <c r="D10" s="119" t="s">
@@ -15735,11 +15761,11 @@
       </c>
       <c r="E10" s="119"/>
       <c r="F10" s="119" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="G10" s="119"/>
       <c r="H10" s="119" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="I10" s="119"/>
       <c r="J10" s="119" t="s">
@@ -15747,15 +15773,15 @@
       </c>
       <c r="K10" s="119"/>
       <c r="L10" s="119" t="s">
-        <v>386</v>
+        <v>416</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A11" s="83" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="B11" s="84" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C11" s="84"/>
       <c r="D11" s="84" t="s">
@@ -15763,27 +15789,27 @@
       </c>
       <c r="E11" s="84"/>
       <c r="F11" s="84" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G11" s="84"/>
       <c r="H11" s="84" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="I11" s="84"/>
       <c r="J11" s="84" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K11" s="84"/>
       <c r="L11" s="84" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A12" s="83" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
       <c r="B12" s="84" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C12" s="84"/>
       <c r="D12" s="84" t="s">
@@ -15791,11 +15817,11 @@
       </c>
       <c r="E12" s="84"/>
       <c r="F12" s="84" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G12" s="84"/>
       <c r="H12" s="84" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="I12" s="84"/>
       <c r="J12" s="84" t="s">
@@ -15803,15 +15829,15 @@
       </c>
       <c r="K12" s="84"/>
       <c r="L12" s="84" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A13" s="83" t="s">
-        <v>414</v>
+        <v>402</v>
       </c>
       <c r="B13" s="84" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C13" s="84"/>
       <c r="D13" s="84" t="s">
@@ -15819,11 +15845,11 @@
       </c>
       <c r="E13" s="84"/>
       <c r="F13" s="84" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="G13" s="84"/>
       <c r="H13" s="84" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="I13" s="84"/>
       <c r="J13" s="84" t="s">
@@ -15831,15 +15857,15 @@
       </c>
       <c r="K13" s="84"/>
       <c r="L13" s="84" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="83" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
       <c r="B14" s="84" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C14" s="84"/>
       <c r="D14" s="84" t="s">
@@ -15847,11 +15873,11 @@
       </c>
       <c r="E14" s="84"/>
       <c r="F14" s="84" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G14" s="84"/>
       <c r="H14" s="84" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I14" s="84"/>
       <c r="J14" s="84" t="s">
@@ -15859,15 +15885,15 @@
       </c>
       <c r="K14" s="84"/>
       <c r="L14" s="84" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="83" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
       <c r="B15" s="84" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C15" s="84"/>
       <c r="D15" s="84" t="s">
@@ -15875,27 +15901,27 @@
       </c>
       <c r="E15" s="84"/>
       <c r="F15" s="84" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G15" s="84"/>
       <c r="H15" s="84" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I15" s="84"/>
       <c r="J15" s="84" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K15" s="84"/>
       <c r="L15" s="84" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A16" s="116" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
       <c r="B16" s="117" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C16" s="117"/>
       <c r="D16" s="117" t="s">
@@ -15903,11 +15929,11 @@
       </c>
       <c r="E16" s="117"/>
       <c r="F16" s="117" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G16" s="117"/>
       <c r="H16" s="117" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I16" s="117"/>
       <c r="J16" s="117" t="s">
@@ -15915,15 +15941,15 @@
       </c>
       <c r="K16" s="117"/>
       <c r="L16" s="117" t="s">
-        <v>374</v>
+        <v>427</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="118" t="s">
-        <v>418</v>
+        <v>406</v>
       </c>
       <c r="B17" s="119" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C17" s="119"/>
       <c r="D17" s="119" t="s">
@@ -15931,27 +15957,27 @@
       </c>
       <c r="E17" s="119"/>
       <c r="F17" s="119" t="s">
-        <v>370</v>
+        <v>413</v>
       </c>
       <c r="G17" s="119"/>
       <c r="H17" s="119" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I17" s="119"/>
       <c r="J17" s="119" t="s">
-        <v>369</v>
+        <v>412</v>
       </c>
       <c r="K17" s="119"/>
       <c r="L17" s="119" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" s="116">
         <v>8</v>
       </c>
       <c r="B18" s="117" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="C18" s="117"/>
       <c r="D18" s="117" t="s">
@@ -15959,11 +15985,11 @@
       </c>
       <c r="E18" s="117"/>
       <c r="F18" s="117" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G18" s="117"/>
       <c r="H18" s="117" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I18" s="117"/>
       <c r="J18" s="117" t="s">
@@ -15971,15 +15997,15 @@
       </c>
       <c r="K18" s="117"/>
       <c r="L18" s="117" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="83">
         <v>9</v>
       </c>
       <c r="B19" s="84" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="C19" s="84"/>
       <c r="D19" s="84" t="s">
@@ -15987,11 +16013,11 @@
       </c>
       <c r="E19" s="84"/>
       <c r="F19" s="84" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G19" s="84"/>
       <c r="H19" s="84" t="s">
-        <v>420</v>
+        <v>407</v>
       </c>
       <c r="I19" s="84"/>
       <c r="J19" s="84" t="s">
@@ -15999,12 +16025,68 @@
       </c>
       <c r="K19" s="84"/>
       <c r="L19" s="84" t="s">
-        <v>389</v>
+        <v>380</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="128" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="83">
+        <v>10</v>
+      </c>
+      <c r="B20" s="84" t="s">
+        <v>418</v>
+      </c>
+      <c r="C20" s="84"/>
+      <c r="D20" s="84" t="s">
+        <v>342</v>
+      </c>
+      <c r="E20" s="84"/>
+      <c r="F20" s="84" t="s">
+        <v>419</v>
+      </c>
+      <c r="G20" s="84"/>
+      <c r="H20" s="84" t="s">
+        <v>420</v>
+      </c>
+      <c r="I20" s="84"/>
+      <c r="J20" s="84" t="s">
+        <v>342</v>
+      </c>
+      <c r="K20" s="84"/>
+      <c r="L20" s="84" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" s="128" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="83">
+        <v>11</v>
+      </c>
+      <c r="B21" s="84" t="s">
+        <v>422</v>
+      </c>
+      <c r="C21" s="84"/>
+      <c r="D21" s="84" t="s">
+        <v>341</v>
+      </c>
+      <c r="E21" s="84"/>
+      <c r="F21" s="84" t="s">
+        <v>419</v>
+      </c>
+      <c r="G21" s="84"/>
+      <c r="H21" s="84" t="s">
+        <v>420</v>
+      </c>
+      <c r="I21" s="84"/>
+      <c r="J21" s="84" t="s">
+        <v>423</v>
+      </c>
+      <c r="K21" s="84"/>
+      <c r="L21" s="84" t="s">
+        <v>424</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="55" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="61" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;LTable 
 &amp;"-,Italic"Potential research questions by unit of analysis and data collection method</oddHeader>
@@ -17470,9 +17552,7 @@
   </sheetPr>
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17487,48 +17567,48 @@
     </row>
     <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="126" t="s">
-        <v>396</v>
+        <v>408</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="139" t="s">
-        <v>390</v>
-      </c>
-      <c r="B6" s="139"/>
-      <c r="C6" s="129" t="s">
-        <v>393</v>
-      </c>
-      <c r="D6" s="129"/>
-      <c r="E6" s="129"/>
-      <c r="F6" s="129"/>
-      <c r="G6" s="129"/>
-      <c r="H6" s="129"/>
-      <c r="I6" s="129"/>
-      <c r="J6" s="129"/>
-      <c r="K6" s="129"/>
-      <c r="L6" s="129"/>
-      <c r="M6" s="129"/>
-      <c r="N6" s="129"/>
+      <c r="A6" s="140" t="s">
+        <v>381</v>
+      </c>
+      <c r="B6" s="140"/>
+      <c r="C6" s="130" t="s">
+        <v>384</v>
+      </c>
+      <c r="D6" s="130"/>
+      <c r="E6" s="130"/>
+      <c r="F6" s="130"/>
+      <c r="G6" s="130"/>
+      <c r="H6" s="130"/>
+      <c r="I6" s="130"/>
+      <c r="J6" s="130"/>
+      <c r="K6" s="130"/>
+      <c r="L6" s="130"/>
+      <c r="M6" s="130"/>
+      <c r="N6" s="130"/>
     </row>
     <row r="8" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="139" t="s">
-        <v>391</v>
-      </c>
-      <c r="B8" s="139"/>
-      <c r="C8" s="129" t="s">
-        <v>392</v>
-      </c>
-      <c r="D8" s="129"/>
-      <c r="E8" s="129"/>
-      <c r="F8" s="129"/>
-      <c r="G8" s="129"/>
-      <c r="H8" s="129"/>
-      <c r="I8" s="129"/>
-      <c r="J8" s="129"/>
-      <c r="K8" s="129"/>
-      <c r="L8" s="129"/>
-      <c r="M8" s="129"/>
-      <c r="N8" s="129"/>
+      <c r="A8" s="140" t="s">
+        <v>382</v>
+      </c>
+      <c r="B8" s="140"/>
+      <c r="C8" s="130" t="s">
+        <v>383</v>
+      </c>
+      <c r="D8" s="130"/>
+      <c r="E8" s="130"/>
+      <c r="F8" s="130"/>
+      <c r="G8" s="130"/>
+      <c r="H8" s="130"/>
+      <c r="I8" s="130"/>
+      <c r="J8" s="130"/>
+      <c r="K8" s="130"/>
+      <c r="L8" s="130"/>
+      <c r="M8" s="130"/>
+      <c r="N8" s="130"/>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="127"/>
@@ -17547,21 +17627,21 @@
       <c r="N9" s="124"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="139" t="s">
-        <v>395</v>
-      </c>
-      <c r="B10" s="139"/>
+      <c r="A10" s="140" t="s">
+        <v>386</v>
+      </c>
+      <c r="B10" s="140"/>
       <c r="C10" s="23" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="18" x14ac:dyDescent="0.25">
-      <c r="A12" s="139" t="s">
-        <v>397</v>
-      </c>
-      <c r="B12" s="139"/>
+      <c r="A12" s="140" t="s">
+        <v>387</v>
+      </c>
+      <c r="B12" s="140"/>
       <c r="C12" s="23" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -18399,54 +18479,54 @@
       <c r="H20" s="109"/>
     </row>
     <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="128" t="s">
+      <c r="A21" s="129" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="128"/>
-      <c r="C21" s="128"/>
-      <c r="D21" s="128"/>
-      <c r="E21" s="128"/>
-      <c r="F21" s="128"/>
+      <c r="B21" s="129"/>
+      <c r="C21" s="129"/>
+      <c r="D21" s="129"/>
+      <c r="E21" s="129"/>
+      <c r="F21" s="129"/>
     </row>
     <row r="22" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="129" t="s">
+      <c r="A22" s="130" t="s">
         <v>179</v>
       </c>
-      <c r="B22" s="129"/>
-      <c r="C22" s="129"/>
-      <c r="D22" s="129"/>
-      <c r="E22" s="129"/>
-      <c r="F22" s="129"/>
+      <c r="B22" s="130"/>
+      <c r="C22" s="130"/>
+      <c r="D22" s="130"/>
+      <c r="E22" s="130"/>
+      <c r="F22" s="130"/>
     </row>
     <row r="23" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="128" t="s">
+      <c r="A23" s="129" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="128"/>
-      <c r="C23" s="128"/>
-      <c r="D23" s="128"/>
-      <c r="E23" s="128"/>
-      <c r="F23" s="128"/>
+      <c r="B23" s="129"/>
+      <c r="C23" s="129"/>
+      <c r="D23" s="129"/>
+      <c r="E23" s="129"/>
+      <c r="F23" s="129"/>
     </row>
     <row r="24" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="128" t="s">
+      <c r="A24" s="129" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="128"/>
-      <c r="C24" s="128"/>
-      <c r="D24" s="128"/>
-      <c r="E24" s="128"/>
-      <c r="F24" s="128"/>
+      <c r="B24" s="129"/>
+      <c r="C24" s="129"/>
+      <c r="D24" s="129"/>
+      <c r="E24" s="129"/>
+      <c r="F24" s="129"/>
     </row>
     <row r="25" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="128" t="s">
+      <c r="A25" s="129" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="128"/>
-      <c r="C25" s="128"/>
-      <c r="D25" s="128"/>
-      <c r="E25" s="128"/>
-      <c r="F25" s="128"/>
+      <c r="B25" s="129"/>
+      <c r="C25" s="129"/>
+      <c r="D25" s="129"/>
+      <c r="E25" s="129"/>
+      <c r="F25" s="129"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="30"/>
@@ -18630,38 +18710,38 @@
       <c r="B3" s="69"/>
       <c r="C3" s="70"/>
       <c r="D3" s="71"/>
-      <c r="E3" s="133" t="s">
+      <c r="E3" s="134" t="s">
         <v>276</v>
       </c>
-      <c r="F3" s="134"/>
-      <c r="G3" s="134"/>
-      <c r="H3" s="131"/>
-      <c r="I3" s="130" t="s">
+      <c r="F3" s="135"/>
+      <c r="G3" s="135"/>
+      <c r="H3" s="132"/>
+      <c r="I3" s="131" t="s">
         <v>304</v>
       </c>
-      <c r="J3" s="131"/>
-      <c r="K3" s="130" t="s">
+      <c r="J3" s="132"/>
+      <c r="K3" s="131" t="s">
         <v>305</v>
       </c>
-      <c r="L3" s="132"/>
-      <c r="M3" s="133" t="s">
+      <c r="L3" s="133"/>
+      <c r="M3" s="134" t="s">
         <v>292</v>
       </c>
-      <c r="N3" s="134"/>
-      <c r="O3" s="131"/>
-      <c r="P3" s="135" t="s">
+      <c r="N3" s="135"/>
+      <c r="O3" s="132"/>
+      <c r="P3" s="136" t="s">
         <v>257</v>
       </c>
-      <c r="Q3" s="134"/>
-      <c r="R3" s="134"/>
-      <c r="S3" s="134"/>
-      <c r="T3" s="134"/>
-      <c r="U3" s="134"/>
-      <c r="V3" s="134"/>
-      <c r="W3" s="134"/>
-      <c r="X3" s="134"/>
-      <c r="Y3" s="134"/>
-      <c r="Z3" s="136"/>
+      <c r="Q3" s="135"/>
+      <c r="R3" s="135"/>
+      <c r="S3" s="135"/>
+      <c r="T3" s="135"/>
+      <c r="U3" s="135"/>
+      <c r="V3" s="135"/>
+      <c r="W3" s="135"/>
+      <c r="X3" s="135"/>
+      <c r="Y3" s="135"/>
+      <c r="Z3" s="137"/>
       <c r="AA3" s="90"/>
     </row>
     <row r="4" spans="1:27" ht="170.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -21937,10 +22017,10 @@
       <c r="A3" s="69"/>
       <c r="B3" s="70"/>
       <c r="C3" s="71"/>
-      <c r="D3" s="133" t="s">
+      <c r="D3" s="134" t="s">
         <v>202</v>
       </c>
-      <c r="E3" s="131"/>
+      <c r="E3" s="132"/>
       <c r="F3" s="73"/>
     </row>
     <row r="4" spans="1:6" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -22200,32 +22280,32 @@
       <c r="F23" s="59"/>
     </row>
     <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="128"/>
-      <c r="B24" s="128"/>
-      <c r="C24" s="128"/>
-      <c r="D24" s="128"/>
-      <c r="E24" s="128"/>
+      <c r="A24" s="129"/>
+      <c r="B24" s="129"/>
+      <c r="C24" s="129"/>
+      <c r="D24" s="129"/>
+      <c r="E24" s="129"/>
     </row>
     <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="128"/>
-      <c r="B25" s="128"/>
-      <c r="C25" s="128"/>
-      <c r="D25" s="128"/>
-      <c r="E25" s="128"/>
+      <c r="A25" s="129"/>
+      <c r="B25" s="129"/>
+      <c r="C25" s="129"/>
+      <c r="D25" s="129"/>
+      <c r="E25" s="129"/>
     </row>
     <row r="26" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="128"/>
-      <c r="B26" s="128"/>
-      <c r="C26" s="128"/>
-      <c r="D26" s="128"/>
-      <c r="E26" s="128"/>
+      <c r="A26" s="129"/>
+      <c r="B26" s="129"/>
+      <c r="C26" s="129"/>
+      <c r="D26" s="129"/>
+      <c r="E26" s="129"/>
     </row>
     <row r="27" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="128"/>
-      <c r="B27" s="128"/>
-      <c r="C27" s="128"/>
-      <c r="D27" s="128"/>
-      <c r="E27" s="128"/>
+      <c r="A27" s="129"/>
+      <c r="B27" s="129"/>
+      <c r="C27" s="129"/>
+      <c r="D27" s="129"/>
+      <c r="E27" s="129"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="60"/>
@@ -23027,27 +23107,27 @@
       <c r="H16" s="32"/>
     </row>
     <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="128"/>
-      <c r="B17" s="128"/>
-      <c r="C17" s="128"/>
+      <c r="A17" s="129"/>
+      <c r="B17" s="129"/>
+      <c r="C17" s="129"/>
       <c r="D17" s="32"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="128"/>
-      <c r="B18" s="128"/>
-      <c r="C18" s="128"/>
+      <c r="A18" s="129"/>
+      <c r="B18" s="129"/>
+      <c r="C18" s="129"/>
       <c r="D18" s="32"/>
       <c r="E18" s="32"/>
       <c r="F18" s="32"/>
       <c r="H18" s="32"/>
     </row>
     <row r="19" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="128"/>
-      <c r="B19" s="128"/>
-      <c r="C19" s="128"/>
+      <c r="A19" s="129"/>
+      <c r="B19" s="129"/>
+      <c r="C19" s="129"/>
       <c r="D19" s="32"/>
       <c r="E19" s="32"/>
       <c r="F19" s="32"/>
@@ -23486,30 +23566,30 @@
       <c r="C41" s="52"/>
     </row>
     <row r="42" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="137" t="s">
+      <c r="A42" s="138" t="s">
         <v>174</v>
       </c>
-      <c r="B42" s="137"/>
-      <c r="C42" s="137"/>
+      <c r="B42" s="138"/>
+      <c r="C42" s="138"/>
     </row>
     <row r="43" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="138" t="s">
+      <c r="A43" s="139" t="s">
         <v>175</v>
       </c>
-      <c r="B43" s="138"/>
-      <c r="C43" s="138"/>
+      <c r="B43" s="139"/>
+      <c r="C43" s="139"/>
     </row>
     <row r="44" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="137" t="s">
+      <c r="A44" s="138" t="s">
         <v>176</v>
       </c>
-      <c r="B44" s="137"/>
-      <c r="C44" s="137"/>
+      <c r="B44" s="138"/>
+      <c r="C44" s="138"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="128"/>
-      <c r="B45" s="128"/>
-      <c r="C45" s="128"/>
+      <c r="A45" s="129"/>
+      <c r="B45" s="129"/>
+      <c r="C45" s="129"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="37"/>

</xml_diff>

<commit_message>
Minor edit to figure on research approach
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
@@ -1506,9 +1506,6 @@
     <t>Why is such a low percentage of technologies derived from federally-funded research and development transferred to the private sector for use that benefits the public interest?</t>
   </si>
   <si>
-    <t>How does technology maturity level influence the technology transfer activities of private sector organizations?</t>
-  </si>
-  <si>
     <t>Organizations were 50 percent more likely to have a majority of technology transfer decision-makers favor acquiring the technology when it was a high maturity level than when it was the low maturity level.</t>
   </si>
   <si>
@@ -1735,6 +1732,9 @@
   </si>
   <si>
     <t xml:space="preserve">Potential Research Question(s):  </t>
+  </si>
+  <si>
+    <t>How does technology maturity level influence the technology transfer priorities and intentions of demand-side private sector organizations?</t>
   </si>
 </sst>
 </file>
@@ -2482,6 +2482,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2514,9 +2517,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -6849,7 +6849,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2705100" y="3181350"/>
+          <a:off x="2705100" y="3371850"/>
           <a:ext cx="5090160" cy="4175760"/>
           <a:chOff x="2352675" y="3219450"/>
           <a:chExt cx="5090160" cy="4175760"/>
@@ -15552,7 +15552,7 @@
       </c>
       <c r="C1" s="114"/>
       <c r="D1" s="114" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E1" s="114"/>
       <c r="F1" s="114" t="s">
@@ -15564,7 +15564,7 @@
       </c>
       <c r="I1" s="114"/>
       <c r="J1" s="114" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="K1" s="114"/>
       <c r="L1" s="114" t="s">
@@ -15573,7 +15573,7 @@
     </row>
     <row r="2" spans="1:14" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="116" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B2" s="117" t="s">
         <v>343</v>
@@ -15596,12 +15596,12 @@
       </c>
       <c r="K2" s="117"/>
       <c r="L2" s="117" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="118" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B3" s="119" t="s">
         <v>343</v>
@@ -15612,7 +15612,7 @@
       </c>
       <c r="E3" s="119"/>
       <c r="F3" s="119" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G3" s="119"/>
       <c r="H3" s="119" t="s">
@@ -15620,11 +15620,11 @@
       </c>
       <c r="I3" s="119"/>
       <c r="J3" s="119" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="K3" s="119"/>
       <c r="L3" s="119" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="135" x14ac:dyDescent="0.25">
@@ -15636,7 +15636,7 @@
       </c>
       <c r="C4" s="121"/>
       <c r="D4" s="121" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E4" s="121"/>
       <c r="F4" s="121" t="s">
@@ -15652,7 +15652,7 @@
       </c>
       <c r="K4" s="121"/>
       <c r="L4" s="121" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="135" x14ac:dyDescent="0.25">
@@ -15664,7 +15664,7 @@
       </c>
       <c r="C5" s="117"/>
       <c r="D5" s="117" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E5" s="117"/>
       <c r="F5" s="117" t="s">
@@ -15680,7 +15680,7 @@
       </c>
       <c r="K5" s="117"/>
       <c r="L5" s="117" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="135" x14ac:dyDescent="0.25">
@@ -15708,7 +15708,7 @@
       </c>
       <c r="K6" s="117"/>
       <c r="L6" s="117" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="75" x14ac:dyDescent="0.25">
@@ -15720,15 +15720,15 @@
       </c>
       <c r="C7" s="84"/>
       <c r="D7" s="84" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E7" s="84"/>
       <c r="F7" s="84" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G7" s="84"/>
       <c r="H7" s="84" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="I7" s="84"/>
       <c r="J7" s="84" t="s">
@@ -15736,19 +15736,19 @@
       </c>
       <c r="K7" s="84"/>
       <c r="L7" s="84" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="122" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="83" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B8" s="84" t="s">
         <v>341</v>
       </c>
       <c r="C8" s="84"/>
       <c r="D8" s="84" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E8" s="84"/>
       <c r="F8" s="84" t="s">
@@ -15764,44 +15764,44 @@
       </c>
       <c r="K8" s="84"/>
       <c r="L8" s="84" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="M8" s="129"/>
       <c r="N8" s="129"/>
     </row>
     <row r="9" spans="1:14" s="122" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="83" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B9" s="84" t="s">
         <v>341</v>
       </c>
       <c r="C9" s="84"/>
       <c r="D9" s="84" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E9" s="84"/>
       <c r="F9" s="84" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G9" s="84"/>
       <c r="H9" s="84" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I9" s="84"/>
       <c r="J9" s="84" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="K9" s="84"/>
       <c r="L9" s="84" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="M9" s="129"/>
       <c r="N9" s="129"/>
     </row>
     <row r="10" spans="1:14" s="122" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="118" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B10" s="119" t="s">
         <v>341</v>
@@ -15829,7 +15829,7 @@
     </row>
     <row r="11" spans="1:14" s="122" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="118" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B11" s="119" t="s">
         <v>341</v>
@@ -15857,7 +15857,7 @@
     </row>
     <row r="12" spans="1:14" s="122" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A12" s="118" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B12" s="119" t="s">
         <v>341</v>
@@ -15885,7 +15885,7 @@
     </row>
     <row r="13" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="118" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B13" s="119" t="s">
         <v>341</v>
@@ -15908,14 +15908,14 @@
       </c>
       <c r="K13" s="119"/>
       <c r="L13" s="119" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="M13" s="122"/>
       <c r="N13" s="122"/>
     </row>
     <row r="14" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="118" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B14" s="119" t="s">
         <v>341</v>
@@ -15938,14 +15938,14 @@
       </c>
       <c r="K14" s="119"/>
       <c r="L14" s="119" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="M14" s="122"/>
       <c r="N14" s="122"/>
     </row>
     <row r="15" spans="1:14" ht="135" x14ac:dyDescent="0.25">
       <c r="A15" s="83" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B15" s="84" t="s">
         <v>341</v>
@@ -15973,7 +15973,7 @@
     </row>
     <row r="16" spans="1:14" ht="180" x14ac:dyDescent="0.25">
       <c r="A16" s="83" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B16" s="84" t="s">
         <v>341</v>
@@ -16001,7 +16001,7 @@
     </row>
     <row r="17" spans="1:12" ht="180" x14ac:dyDescent="0.25">
       <c r="A17" s="83" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B17" s="84" t="s">
         <v>341</v>
@@ -16029,7 +16029,7 @@
     </row>
     <row r="18" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="83" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B18" s="84" t="s">
         <v>341</v>
@@ -16057,7 +16057,7 @@
     </row>
     <row r="19" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="83" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B19" s="84" t="s">
         <v>341</v>
@@ -16100,7 +16100,7 @@
       </c>
       <c r="G20" s="84"/>
       <c r="H20" s="84" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I20" s="84"/>
       <c r="J20" s="84" t="s">
@@ -16120,23 +16120,23 @@
       </c>
       <c r="C21" s="84"/>
       <c r="D21" s="84" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E21" s="84"/>
       <c r="F21" s="84" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G21" s="84"/>
       <c r="H21" s="84" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="I21" s="84"/>
       <c r="J21" s="84" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="K21" s="84"/>
       <c r="L21" s="84" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>
@@ -17655,46 +17655,46 @@
     </row>
     <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="126" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D6" s="24" t="s">
-        <v>436</v>
-      </c>
-      <c r="E6" s="134" t="s">
+        <v>435</v>
+      </c>
+      <c r="E6" s="135" t="s">
         <v>382</v>
       </c>
-      <c r="F6" s="134"/>
-      <c r="G6" s="134"/>
-      <c r="H6" s="134"/>
-      <c r="I6" s="134"/>
-      <c r="J6" s="134"/>
-      <c r="K6" s="134"/>
-      <c r="L6" s="134"/>
-      <c r="M6" s="134"/>
-      <c r="N6" s="134"/>
-      <c r="O6" s="134"/>
-      <c r="P6" s="134"/>
+      <c r="F6" s="135"/>
+      <c r="G6" s="135"/>
+      <c r="H6" s="135"/>
+      <c r="I6" s="135"/>
+      <c r="J6" s="135"/>
+      <c r="K6" s="135"/>
+      <c r="L6" s="135"/>
+      <c r="M6" s="135"/>
+      <c r="N6" s="135"/>
+      <c r="O6" s="135"/>
+      <c r="P6" s="135"/>
     </row>
     <row r="8" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="24" t="s">
-        <v>437</v>
-      </c>
-      <c r="E8" s="134" t="s">
+        <v>436</v>
+      </c>
+      <c r="E8" s="135" t="s">
         <v>381</v>
       </c>
-      <c r="F8" s="134"/>
-      <c r="G8" s="134"/>
-      <c r="H8" s="134"/>
-      <c r="I8" s="134"/>
-      <c r="J8" s="134"/>
-      <c r="K8" s="134"/>
-      <c r="L8" s="134"/>
-      <c r="M8" s="134"/>
-      <c r="N8" s="134"/>
-      <c r="O8" s="134"/>
-      <c r="P8" s="134"/>
+      <c r="F8" s="135"/>
+      <c r="G8" s="135"/>
+      <c r="H8" s="135"/>
+      <c r="I8" s="135"/>
+      <c r="J8" s="135"/>
+      <c r="K8" s="135"/>
+      <c r="L8" s="135"/>
+      <c r="M8" s="135"/>
+      <c r="N8" s="135"/>
+      <c r="O8" s="135"/>
+      <c r="P8" s="135"/>
     </row>
     <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="127"/>
@@ -17714,39 +17714,51 @@
       <c r="O9" s="124"/>
       <c r="P9" s="124"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D10" s="24" t="s">
-        <v>438</v>
-      </c>
-      <c r="E10" s="23" t="s">
-        <v>383</v>
-      </c>
+        <v>437</v>
+      </c>
+      <c r="E10" s="135" t="s">
+        <v>439</v>
+      </c>
+      <c r="F10" s="135"/>
+      <c r="G10" s="135"/>
+      <c r="H10" s="135"/>
+      <c r="I10" s="135"/>
+      <c r="J10" s="135"/>
+      <c r="K10" s="135"/>
+      <c r="L10" s="135"/>
+      <c r="M10" s="135"/>
+      <c r="N10" s="135"/>
+      <c r="O10" s="135"/>
+      <c r="P10" s="135"/>
     </row>
     <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="131"/>
       <c r="C12" s="131"/>
       <c r="D12" s="24" t="s">
-        <v>439</v>
-      </c>
-      <c r="E12" s="144" t="s">
-        <v>435</v>
-      </c>
-      <c r="F12" s="144"/>
-      <c r="G12" s="144"/>
-      <c r="H12" s="144"/>
-      <c r="I12" s="144"/>
-      <c r="J12" s="144"/>
-      <c r="K12" s="144"/>
-      <c r="L12" s="144"/>
-      <c r="M12" s="144"/>
-      <c r="N12" s="144"/>
-      <c r="O12" s="144"/>
-      <c r="P12" s="144"/>
+        <v>438</v>
+      </c>
+      <c r="E12" s="133" t="s">
+        <v>434</v>
+      </c>
+      <c r="F12" s="133"/>
+      <c r="G12" s="133"/>
+      <c r="H12" s="133"/>
+      <c r="I12" s="133"/>
+      <c r="J12" s="133"/>
+      <c r="K12" s="133"/>
+      <c r="L12" s="133"/>
+      <c r="M12" s="133"/>
+      <c r="N12" s="133"/>
+      <c r="O12" s="133"/>
+      <c r="P12" s="133"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="E6:P6"/>
     <mergeCell ref="E8:P8"/>
+    <mergeCell ref="E10:P10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="68" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -17806,7 +17818,7 @@
       </c>
       <c r="I1" s="114"/>
       <c r="J1" s="114" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="K1" s="114"/>
       <c r="L1" s="114" t="s">
@@ -17818,7 +17830,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="121" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C2" s="121"/>
       <c r="D2" s="121" t="s">
@@ -17838,15 +17850,15 @@
       </c>
       <c r="K2" s="121"/>
       <c r="L2" s="121" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="83" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B3" s="84" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C3" s="84"/>
       <c r="D3" s="84" t="s">
@@ -17866,15 +17878,15 @@
       </c>
       <c r="K3" s="84"/>
       <c r="L3" s="84" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="123" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="83" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B4" s="84" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C4" s="84"/>
       <c r="D4" s="84" t="s">
@@ -17882,19 +17894,19 @@
       </c>
       <c r="E4" s="84"/>
       <c r="F4" s="84" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G4" s="84"/>
       <c r="H4" s="84" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I4" s="84"/>
       <c r="J4" s="84" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="K4" s="84"/>
       <c r="L4" s="84" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="113" customFormat="1" ht="135" x14ac:dyDescent="0.25">
@@ -17902,7 +17914,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="117" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C5" s="117"/>
       <c r="D5" s="117" t="s">
@@ -17922,12 +17934,12 @@
       </c>
       <c r="K5" s="117"/>
       <c r="L5" s="117" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="122" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="118" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B6" s="119" t="s">
         <v>370</v>
@@ -17955,7 +17967,7 @@
     </row>
     <row r="7" spans="1:12" s="122" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="118" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B7" s="119" t="s">
         <v>370</v>
@@ -17983,7 +17995,7 @@
     </row>
     <row r="8" spans="1:12" s="122" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="118" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B8" s="119" t="s">
         <v>370</v>
@@ -18011,7 +18023,7 @@
     </row>
     <row r="9" spans="1:12" s="122" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="118" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B9" s="119" t="s">
         <v>370</v>
@@ -18034,12 +18046,12 @@
       </c>
       <c r="K9" s="119"/>
       <c r="L9" s="119" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="122" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="118" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B10" s="119" t="s">
         <v>370</v>
@@ -18062,12 +18074,12 @@
       </c>
       <c r="K10" s="119"/>
       <c r="L10" s="119" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A11" s="83" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B11" s="84" t="s">
         <v>352</v>
@@ -18095,7 +18107,7 @@
     </row>
     <row r="12" spans="1:12" ht="180" x14ac:dyDescent="0.25">
       <c r="A12" s="83" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B12" s="84" t="s">
         <v>352</v>
@@ -18123,7 +18135,7 @@
     </row>
     <row r="13" spans="1:12" ht="180" x14ac:dyDescent="0.25">
       <c r="A13" s="83" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B13" s="84" t="s">
         <v>352</v>
@@ -18151,7 +18163,7 @@
     </row>
     <row r="14" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="83" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B14" s="84" t="s">
         <v>356</v>
@@ -18179,7 +18191,7 @@
     </row>
     <row r="15" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="83" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B15" s="84" t="s">
         <v>356</v>
@@ -18207,7 +18219,7 @@
     </row>
     <row r="16" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A16" s="116" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B16" s="117" t="s">
         <v>366</v>
@@ -18230,12 +18242,12 @@
       </c>
       <c r="K16" s="117"/>
       <c r="L16" s="117" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="118" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B17" s="119" t="s">
         <v>366</v>
@@ -18246,7 +18258,7 @@
       </c>
       <c r="E17" s="119"/>
       <c r="F17" s="119" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G17" s="119"/>
       <c r="H17" s="119" t="s">
@@ -18254,11 +18266,11 @@
       </c>
       <c r="I17" s="119"/>
       <c r="J17" s="119" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="K17" s="119"/>
       <c r="L17" s="119" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="135" x14ac:dyDescent="0.25">
@@ -18286,7 +18298,7 @@
       </c>
       <c r="K18" s="117"/>
       <c r="L18" s="117" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="90" x14ac:dyDescent="0.25">
@@ -18306,7 +18318,7 @@
       </c>
       <c r="G19" s="84"/>
       <c r="H19" s="84" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I19" s="84"/>
       <c r="J19" s="84" t="s">
@@ -18322,7 +18334,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="84" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C20" s="84"/>
       <c r="D20" s="84" t="s">
@@ -18330,11 +18342,11 @@
       </c>
       <c r="E20" s="84"/>
       <c r="F20" s="84" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G20" s="84"/>
       <c r="H20" s="84" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="I20" s="84"/>
       <c r="J20" s="84" t="s">
@@ -18342,7 +18354,7 @@
       </c>
       <c r="K20" s="84"/>
       <c r="L20" s="84" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="21" spans="1:12" s="128" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -18350,7 +18362,7 @@
         <v>11</v>
       </c>
       <c r="B21" s="84" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C21" s="84"/>
       <c r="D21" s="84" t="s">
@@ -18358,19 +18370,19 @@
       </c>
       <c r="E21" s="84"/>
       <c r="F21" s="84" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G21" s="84"/>
       <c r="H21" s="84" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="I21" s="84"/>
       <c r="J21" s="84" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="K21" s="84"/>
       <c r="L21" s="84" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>
@@ -19204,54 +19216,54 @@
       <c r="H20" s="109"/>
     </row>
     <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="133" t="s">
+      <c r="A21" s="134" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="133"/>
-      <c r="C21" s="133"/>
-      <c r="D21" s="133"/>
-      <c r="E21" s="133"/>
-      <c r="F21" s="133"/>
+      <c r="B21" s="134"/>
+      <c r="C21" s="134"/>
+      <c r="D21" s="134"/>
+      <c r="E21" s="134"/>
+      <c r="F21" s="134"/>
     </row>
     <row r="22" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="134" t="s">
+      <c r="A22" s="135" t="s">
         <v>179</v>
       </c>
-      <c r="B22" s="134"/>
-      <c r="C22" s="134"/>
-      <c r="D22" s="134"/>
-      <c r="E22" s="134"/>
-      <c r="F22" s="134"/>
+      <c r="B22" s="135"/>
+      <c r="C22" s="135"/>
+      <c r="D22" s="135"/>
+      <c r="E22" s="135"/>
+      <c r="F22" s="135"/>
     </row>
     <row r="23" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="133" t="s">
+      <c r="A23" s="134" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="133"/>
-      <c r="C23" s="133"/>
-      <c r="D23" s="133"/>
-      <c r="E23" s="133"/>
-      <c r="F23" s="133"/>
+      <c r="B23" s="134"/>
+      <c r="C23" s="134"/>
+      <c r="D23" s="134"/>
+      <c r="E23" s="134"/>
+      <c r="F23" s="134"/>
     </row>
     <row r="24" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="133" t="s">
+      <c r="A24" s="134" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="133"/>
-      <c r="C24" s="133"/>
-      <c r="D24" s="133"/>
-      <c r="E24" s="133"/>
-      <c r="F24" s="133"/>
+      <c r="B24" s="134"/>
+      <c r="C24" s="134"/>
+      <c r="D24" s="134"/>
+      <c r="E24" s="134"/>
+      <c r="F24" s="134"/>
     </row>
     <row r="25" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="133" t="s">
+      <c r="A25" s="134" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="133"/>
-      <c r="C25" s="133"/>
-      <c r="D25" s="133"/>
-      <c r="E25" s="133"/>
-      <c r="F25" s="133"/>
+      <c r="B25" s="134"/>
+      <c r="C25" s="134"/>
+      <c r="D25" s="134"/>
+      <c r="E25" s="134"/>
+      <c r="F25" s="134"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="30"/>
@@ -19435,38 +19447,38 @@
       <c r="B3" s="69"/>
       <c r="C3" s="70"/>
       <c r="D3" s="71"/>
-      <c r="E3" s="138" t="s">
+      <c r="E3" s="139" t="s">
         <v>276</v>
       </c>
-      <c r="F3" s="139"/>
-      <c r="G3" s="139"/>
-      <c r="H3" s="136"/>
-      <c r="I3" s="135" t="s">
+      <c r="F3" s="140"/>
+      <c r="G3" s="140"/>
+      <c r="H3" s="137"/>
+      <c r="I3" s="136" t="s">
         <v>304</v>
       </c>
-      <c r="J3" s="136"/>
-      <c r="K3" s="135" t="s">
+      <c r="J3" s="137"/>
+      <c r="K3" s="136" t="s">
         <v>305</v>
       </c>
-      <c r="L3" s="137"/>
-      <c r="M3" s="138" t="s">
+      <c r="L3" s="138"/>
+      <c r="M3" s="139" t="s">
         <v>292</v>
       </c>
-      <c r="N3" s="139"/>
-      <c r="O3" s="136"/>
-      <c r="P3" s="140" t="s">
+      <c r="N3" s="140"/>
+      <c r="O3" s="137"/>
+      <c r="P3" s="141" t="s">
         <v>257</v>
       </c>
-      <c r="Q3" s="139"/>
-      <c r="R3" s="139"/>
-      <c r="S3" s="139"/>
-      <c r="T3" s="139"/>
-      <c r="U3" s="139"/>
-      <c r="V3" s="139"/>
-      <c r="W3" s="139"/>
-      <c r="X3" s="139"/>
-      <c r="Y3" s="139"/>
-      <c r="Z3" s="141"/>
+      <c r="Q3" s="140"/>
+      <c r="R3" s="140"/>
+      <c r="S3" s="140"/>
+      <c r="T3" s="140"/>
+      <c r="U3" s="140"/>
+      <c r="V3" s="140"/>
+      <c r="W3" s="140"/>
+      <c r="X3" s="140"/>
+      <c r="Y3" s="140"/>
+      <c r="Z3" s="142"/>
       <c r="AA3" s="90"/>
     </row>
     <row r="4" spans="1:27" ht="170.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -22742,10 +22754,10 @@
       <c r="A3" s="69"/>
       <c r="B3" s="70"/>
       <c r="C3" s="71"/>
-      <c r="D3" s="138" t="s">
+      <c r="D3" s="139" t="s">
         <v>202</v>
       </c>
-      <c r="E3" s="136"/>
+      <c r="E3" s="137"/>
       <c r="F3" s="73"/>
     </row>
     <row r="4" spans="1:6" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -23005,32 +23017,32 @@
       <c r="F23" s="59"/>
     </row>
     <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="133"/>
-      <c r="B24" s="133"/>
-      <c r="C24" s="133"/>
-      <c r="D24" s="133"/>
-      <c r="E24" s="133"/>
+      <c r="A24" s="134"/>
+      <c r="B24" s="134"/>
+      <c r="C24" s="134"/>
+      <c r="D24" s="134"/>
+      <c r="E24" s="134"/>
     </row>
     <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="133"/>
-      <c r="B25" s="133"/>
-      <c r="C25" s="133"/>
-      <c r="D25" s="133"/>
-      <c r="E25" s="133"/>
+      <c r="A25" s="134"/>
+      <c r="B25" s="134"/>
+      <c r="C25" s="134"/>
+      <c r="D25" s="134"/>
+      <c r="E25" s="134"/>
     </row>
     <row r="26" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="133"/>
-      <c r="B26" s="133"/>
-      <c r="C26" s="133"/>
-      <c r="D26" s="133"/>
-      <c r="E26" s="133"/>
+      <c r="A26" s="134"/>
+      <c r="B26" s="134"/>
+      <c r="C26" s="134"/>
+      <c r="D26" s="134"/>
+      <c r="E26" s="134"/>
     </row>
     <row r="27" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="133"/>
-      <c r="B27" s="133"/>
-      <c r="C27" s="133"/>
-      <c r="D27" s="133"/>
-      <c r="E27" s="133"/>
+      <c r="A27" s="134"/>
+      <c r="B27" s="134"/>
+      <c r="C27" s="134"/>
+      <c r="D27" s="134"/>
+      <c r="E27" s="134"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="60"/>
@@ -23832,27 +23844,27 @@
       <c r="H16" s="32"/>
     </row>
     <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="133"/>
-      <c r="B17" s="133"/>
-      <c r="C17" s="133"/>
+      <c r="A17" s="134"/>
+      <c r="B17" s="134"/>
+      <c r="C17" s="134"/>
       <c r="D17" s="32"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="133"/>
-      <c r="B18" s="133"/>
-      <c r="C18" s="133"/>
+      <c r="A18" s="134"/>
+      <c r="B18" s="134"/>
+      <c r="C18" s="134"/>
       <c r="D18" s="32"/>
       <c r="E18" s="32"/>
       <c r="F18" s="32"/>
       <c r="H18" s="32"/>
     </row>
     <row r="19" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="133"/>
-      <c r="B19" s="133"/>
-      <c r="C19" s="133"/>
+      <c r="A19" s="134"/>
+      <c r="B19" s="134"/>
+      <c r="C19" s="134"/>
       <c r="D19" s="32"/>
       <c r="E19" s="32"/>
       <c r="F19" s="32"/>
@@ -24291,30 +24303,30 @@
       <c r="C41" s="52"/>
     </row>
     <row r="42" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="142" t="s">
+      <c r="A42" s="143" t="s">
         <v>174</v>
       </c>
-      <c r="B42" s="142"/>
-      <c r="C42" s="142"/>
+      <c r="B42" s="143"/>
+      <c r="C42" s="143"/>
     </row>
     <row r="43" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="143" t="s">
+      <c r="A43" s="144" t="s">
         <v>175</v>
       </c>
-      <c r="B43" s="143"/>
-      <c r="C43" s="143"/>
+      <c r="B43" s="144"/>
+      <c r="C43" s="144"/>
     </row>
     <row r="44" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="142" t="s">
+      <c r="A44" s="143" t="s">
         <v>176</v>
       </c>
-      <c r="B44" s="142"/>
-      <c r="C44" s="142"/>
+      <c r="B44" s="143"/>
+      <c r="C44" s="143"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="133"/>
-      <c r="B45" s="133"/>
-      <c r="C45" s="133"/>
+      <c r="A45" s="134"/>
+      <c r="B45" s="134"/>
+      <c r="C45" s="134"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="37"/>

</xml_diff>

<commit_message>
Updated table on units of analysis
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="14" activeTab="18"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938"/>
   </bookViews>
   <sheets>
-    <sheet name="Table - Units of Analysis (2)" sheetId="19" r:id="rId1"/>
-    <sheet name="Table - Units of Analysis" sheetId="17" r:id="rId2"/>
+    <sheet name="Table - Units of Analysis" sheetId="19" r:id="rId1"/>
+    <sheet name="Table - Research Questions" sheetId="17" r:id="rId2"/>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId3"/>
     <sheet name="Table - Tech Tran Policies" sheetId="5" r:id="rId4"/>
     <sheet name="Table - Determinants Examined" sheetId="6" r:id="rId5"/>
@@ -34,8 +34,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="4">'Table - Determinants Examined'!$3:$4</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">'Table - Units of Analysis'!$1:$1</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Table - Units of Analysis (2)'!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'Table - Research Questions'!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Table - Units of Analysis'!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="460">
   <si>
     <t>Total</t>
   </si>
@@ -1735,6 +1735,82 @@
   </si>
   <si>
     <t>How does technology maturity level influence the technology transfer priorities and intentions of demand-side private sector organizations?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Example Hypothesis
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>For illustrative purposes only.</t>
+    </r>
+  </si>
+  <si>
+    <t>Subjects will choose to acquire the high maturity level technology more often than the low maturity level technology.</t>
+  </si>
+  <si>
+    <t>Subjects chose to acquire the high maturity level technology twice as often as the low maturity level technology.</t>
+  </si>
+  <si>
+    <t>High maturity level technologies will be pursued more often than low matruity level technologies.</t>
+  </si>
+  <si>
+    <t>High maturity level technologies were pursued twice as often as low matruity level technologies.</t>
+  </si>
+  <si>
+    <t>Subjects will be more likely to acquire a high maturity level technology than a low maturity level.</t>
+  </si>
+  <si>
+    <t>The percent of subjects that choose to pursue the low maturity level technology will be more than the percent of subjects that choose to pursue the high maturity level technology.</t>
+  </si>
+  <si>
+    <t>Subjects will be more likely to acquire the high maturity level technology than the low maturity level technology.</t>
+  </si>
+  <si>
+    <t>Organizations will be more willing to acquire the high maturity level technology than the low maturity level technology.
+Organizations will consistently choose not to acquire the low maturity level technology.</t>
+  </si>
+  <si>
+    <t>Organizations will demonstrated an unwillingness to acquire low maturity level technologies.</t>
+  </si>
+  <si>
+    <t>Organizations will generally choose to pursue the high maturity level technology, all other things being equal.
+Organizations will choose NOT to pursue the low maturity level technology, all other things being equal.</t>
+  </si>
+  <si>
+    <t>Organizations will choose NOT to pursue the low maturity level technology, all other things being equal.</t>
+  </si>
+  <si>
+    <t>Demand-side private sector organizations use a decision premise that a technology has to have attained a minimum maturity level that is higher than the average maturity level of technologies available from universities.</t>
+  </si>
+  <si>
+    <t>Private sector organizations in the life sciences sector will acquired technology at a lower maturity level than private sector organizations in all other sectors.</t>
+  </si>
+  <si>
+    <t>Demand-side private sector organizations use technology maturity level as a proxy for uncertainty.
+Demand-side private sector organizations' perceived uncertainty of a technology will correlate with the maturity level of the technology.</t>
+  </si>
+  <si>
+    <t>Is technology maturity level usedin the sensemaking and sensegiving communications of demand-side private sector organizations?</t>
+  </si>
+  <si>
+    <t>Technology maturity level is regularly incorporated into the sensemaking and sensegiving communications of private sector organizations.</t>
+  </si>
+  <si>
+    <t>Technology transfer decision-makers in demand-side private sector organizations use technology maturity level as a significant component of their sensemaking and sensegiving communications.</t>
+  </si>
+  <si>
+    <t>Documents (organization records)</t>
+  </si>
+  <si>
+    <t>Documents (organization records and allowed patents)</t>
   </si>
 </sst>
 </file>
@@ -1845,7 +1921,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1855,6 +1931,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2098,7 +2180,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -2489,6 +2571,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2517,6 +2602,12 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -15517,9 +15608,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -15538,40 +15629,46 @@
     <col min="8" max="8" width="20.7109375" style="129" customWidth="1"/>
     <col min="9" max="9" width="1.7109375" style="129" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" style="129" customWidth="1"/>
-    <col min="11" max="11" width="1.7109375" style="129" customWidth="1"/>
-    <col min="12" max="12" width="40.7109375" style="129" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="129"/>
-    <col min="14" max="14" width="62" style="129" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="129"/>
+    <col min="11" max="11" width="1.7109375" style="134" customWidth="1"/>
+    <col min="12" max="12" width="40.7109375" style="134" customWidth="1"/>
+    <col min="13" max="13" width="1.7109375" style="129" customWidth="1"/>
+    <col min="14" max="14" width="40.7109375" style="129" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="129"/>
+    <col min="16" max="16" width="62" style="129" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="129"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="115"/>
-      <c r="B1" s="114" t="s">
+    <row r="1" spans="1:16" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="146"/>
+      <c r="B1" s="147" t="s">
         <v>359</v>
       </c>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114" t="s">
+      <c r="C1" s="147"/>
+      <c r="D1" s="147" t="s">
         <v>433</v>
       </c>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114" t="s">
+      <c r="E1" s="147"/>
+      <c r="F1" s="147" t="s">
         <v>358</v>
       </c>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114" t="s">
+      <c r="G1" s="147"/>
+      <c r="H1" s="147" t="s">
         <v>357</v>
       </c>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114" t="s">
+      <c r="I1" s="147"/>
+      <c r="J1" s="147" t="s">
         <v>404</v>
       </c>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114" t="s">
+      <c r="K1" s="147"/>
+      <c r="L1" s="147" t="s">
+        <v>440</v>
+      </c>
+      <c r="M1" s="147"/>
+      <c r="N1" s="147" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="116" t="s">
         <v>423</v>
       </c>
@@ -15596,10 +15693,14 @@
       </c>
       <c r="K2" s="117"/>
       <c r="L2" s="117" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+        <v>441</v>
+      </c>
+      <c r="M2" s="117"/>
+      <c r="N2" s="117" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="118" t="s">
         <v>424</v>
       </c>
@@ -15624,10 +15725,14 @@
       </c>
       <c r="K3" s="119"/>
       <c r="L3" s="119" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+        <v>443</v>
+      </c>
+      <c r="M3" s="119"/>
+      <c r="N3" s="119" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="120">
         <v>2</v>
       </c>
@@ -15652,10 +15757,14 @@
       </c>
       <c r="K4" s="121"/>
       <c r="L4" s="121" t="s">
+        <v>445</v>
+      </c>
+      <c r="M4" s="121"/>
+      <c r="N4" s="121" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="116">
         <v>3</v>
       </c>
@@ -15680,10 +15789,14 @@
       </c>
       <c r="K5" s="117"/>
       <c r="L5" s="117" t="s">
+        <v>446</v>
+      </c>
+      <c r="M5" s="117"/>
+      <c r="N5" s="117" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="116">
         <v>4</v>
       </c>
@@ -15708,10 +15821,14 @@
       </c>
       <c r="K6" s="117"/>
       <c r="L6" s="117" t="s">
+        <v>447</v>
+      </c>
+      <c r="M6" s="117"/>
+      <c r="N6" s="117" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="83">
         <v>5</v>
       </c>
@@ -15736,10 +15853,14 @@
       </c>
       <c r="K7" s="84"/>
       <c r="L7" s="84" t="s">
+        <v>457</v>
+      </c>
+      <c r="M7" s="84"/>
+      <c r="N7" s="84" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="122" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" s="122" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="83" t="s">
         <v>397</v>
       </c>
@@ -15764,12 +15885,16 @@
       </c>
       <c r="K8" s="84"/>
       <c r="L8" s="84" t="s">
+        <v>448</v>
+      </c>
+      <c r="M8" s="84"/>
+      <c r="N8" s="84" t="s">
         <v>383</v>
       </c>
-      <c r="M8" s="129"/>
-      <c r="N8" s="129"/>
-    </row>
-    <row r="9" spans="1:14" s="122" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="O8" s="129"/>
+      <c r="P8" s="129"/>
+    </row>
+    <row r="9" spans="1:16" s="122" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="83" t="s">
         <v>398</v>
       </c>
@@ -15794,12 +15919,16 @@
       </c>
       <c r="K9" s="84"/>
       <c r="L9" s="84" t="s">
+        <v>449</v>
+      </c>
+      <c r="M9" s="84"/>
+      <c r="N9" s="84" t="s">
         <v>405</v>
       </c>
-      <c r="M9" s="129"/>
-      <c r="N9" s="129"/>
-    </row>
-    <row r="10" spans="1:14" s="122" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="O9" s="129"/>
+      <c r="P9" s="129"/>
+    </row>
+    <row r="10" spans="1:16" s="122" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="118" t="s">
         <v>399</v>
       </c>
@@ -15824,10 +15953,14 @@
       </c>
       <c r="K10" s="119"/>
       <c r="L10" s="119" t="s">
+        <v>450</v>
+      </c>
+      <c r="M10" s="119"/>
+      <c r="N10" s="119" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="122" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" s="122" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="118" t="s">
         <v>400</v>
       </c>
@@ -15852,10 +15985,14 @@
       </c>
       <c r="K11" s="119"/>
       <c r="L11" s="119" t="s">
+        <v>450</v>
+      </c>
+      <c r="M11" s="119"/>
+      <c r="N11" s="119" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="122" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="122" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A12" s="118" t="s">
         <v>425</v>
       </c>
@@ -15880,10 +16017,14 @@
       </c>
       <c r="K12" s="119"/>
       <c r="L12" s="119" t="s">
+        <v>451</v>
+      </c>
+      <c r="M12" s="119"/>
+      <c r="N12" s="119" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="118" t="s">
         <v>426</v>
       </c>
@@ -15904,16 +16045,20 @@
       </c>
       <c r="I13" s="119"/>
       <c r="J13" s="119" t="s">
-        <v>348</v>
+        <v>458</v>
       </c>
       <c r="K13" s="119"/>
       <c r="L13" s="119" t="s">
+        <v>451</v>
+      </c>
+      <c r="M13" s="119"/>
+      <c r="N13" s="119" t="s">
         <v>411</v>
       </c>
-      <c r="M13" s="122"/>
-      <c r="N13" s="122"/>
-    </row>
-    <row r="14" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="O13" s="122"/>
+      <c r="P13" s="122"/>
+    </row>
+    <row r="14" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="118" t="s">
         <v>427</v>
       </c>
@@ -15938,12 +16083,16 @@
       </c>
       <c r="K14" s="119"/>
       <c r="L14" s="119" t="s">
+        <v>451</v>
+      </c>
+      <c r="M14" s="119"/>
+      <c r="N14" s="119" t="s">
         <v>410</v>
       </c>
-      <c r="M14" s="122"/>
-      <c r="N14" s="122"/>
-    </row>
-    <row r="15" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+      <c r="O14" s="122"/>
+      <c r="P14" s="122"/>
+    </row>
+    <row r="15" spans="1:16" ht="135" x14ac:dyDescent="0.25">
       <c r="A15" s="83" t="s">
         <v>428</v>
       </c>
@@ -15964,14 +16113,18 @@
       </c>
       <c r="I15" s="84"/>
       <c r="J15" s="84" t="s">
-        <v>348</v>
+        <v>459</v>
       </c>
       <c r="K15" s="84"/>
       <c r="L15" s="84" t="s">
+        <v>452</v>
+      </c>
+      <c r="M15" s="84"/>
+      <c r="N15" s="84" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="180" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="180" x14ac:dyDescent="0.25">
       <c r="A16" s="83" t="s">
         <v>429</v>
       </c>
@@ -15996,10 +16149,14 @@
       </c>
       <c r="K16" s="84"/>
       <c r="L16" s="84" t="s">
+        <v>452</v>
+      </c>
+      <c r="M16" s="84"/>
+      <c r="N16" s="84" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="180" x14ac:dyDescent="0.25">
       <c r="A17" s="83" t="s">
         <v>430</v>
       </c>
@@ -16024,10 +16181,14 @@
       </c>
       <c r="K17" s="84"/>
       <c r="L17" s="84" t="s">
+        <v>452</v>
+      </c>
+      <c r="M17" s="84"/>
+      <c r="N17" s="84" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="83" t="s">
         <v>431</v>
       </c>
@@ -16052,10 +16213,14 @@
       </c>
       <c r="K18" s="84"/>
       <c r="L18" s="84" t="s">
+        <v>453</v>
+      </c>
+      <c r="M18" s="84"/>
+      <c r="N18" s="84" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="83" t="s">
         <v>432</v>
       </c>
@@ -16080,10 +16245,14 @@
       </c>
       <c r="K19" s="84"/>
       <c r="L19" s="84" t="s">
+        <v>453</v>
+      </c>
+      <c r="M19" s="84"/>
+      <c r="N19" s="84" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="83">
         <v>10</v>
       </c>
@@ -16108,10 +16277,14 @@
       </c>
       <c r="K20" s="84"/>
       <c r="L20" s="84" t="s">
+        <v>454</v>
+      </c>
+      <c r="M20" s="84"/>
+      <c r="N20" s="84" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="83">
         <v>11</v>
       </c>
@@ -16120,7 +16293,7 @@
       </c>
       <c r="C21" s="84"/>
       <c r="D21" s="84" t="s">
-        <v>416</v>
+        <v>455</v>
       </c>
       <c r="E21" s="84"/>
       <c r="F21" s="84" t="s">
@@ -16136,6 +16309,10 @@
       </c>
       <c r="K21" s="84"/>
       <c r="L21" s="84" t="s">
+        <v>456</v>
+      </c>
+      <c r="M21" s="84"/>
+      <c r="N21" s="84" t="s">
         <v>418</v>
       </c>
     </row>
@@ -16144,7 +16321,7 @@
     <sortCondition ref="B2:B21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="61" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="50" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;LTable 
 &amp;"-,Italic"Potential research questions by unit of analysis and data collection method</oddHeader>
@@ -17640,7 +17817,7 @@
   </sheetPr>
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17662,39 +17839,39 @@
       <c r="D6" s="24" t="s">
         <v>435</v>
       </c>
-      <c r="E6" s="135" t="s">
+      <c r="E6" s="136" t="s">
         <v>382</v>
       </c>
-      <c r="F6" s="135"/>
-      <c r="G6" s="135"/>
-      <c r="H6" s="135"/>
-      <c r="I6" s="135"/>
-      <c r="J6" s="135"/>
-      <c r="K6" s="135"/>
-      <c r="L6" s="135"/>
-      <c r="M6" s="135"/>
-      <c r="N6" s="135"/>
-      <c r="O6" s="135"/>
-      <c r="P6" s="135"/>
+      <c r="F6" s="136"/>
+      <c r="G6" s="136"/>
+      <c r="H6" s="136"/>
+      <c r="I6" s="136"/>
+      <c r="J6" s="136"/>
+      <c r="K6" s="136"/>
+      <c r="L6" s="136"/>
+      <c r="M6" s="136"/>
+      <c r="N6" s="136"/>
+      <c r="O6" s="136"/>
+      <c r="P6" s="136"/>
     </row>
     <row r="8" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="24" t="s">
         <v>436</v>
       </c>
-      <c r="E8" s="135" t="s">
+      <c r="E8" s="136" t="s">
         <v>381</v>
       </c>
-      <c r="F8" s="135"/>
-      <c r="G8" s="135"/>
-      <c r="H8" s="135"/>
-      <c r="I8" s="135"/>
-      <c r="J8" s="135"/>
-      <c r="K8" s="135"/>
-      <c r="L8" s="135"/>
-      <c r="M8" s="135"/>
-      <c r="N8" s="135"/>
-      <c r="O8" s="135"/>
-      <c r="P8" s="135"/>
+      <c r="F8" s="136"/>
+      <c r="G8" s="136"/>
+      <c r="H8" s="136"/>
+      <c r="I8" s="136"/>
+      <c r="J8" s="136"/>
+      <c r="K8" s="136"/>
+      <c r="L8" s="136"/>
+      <c r="M8" s="136"/>
+      <c r="N8" s="136"/>
+      <c r="O8" s="136"/>
+      <c r="P8" s="136"/>
     </row>
     <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="127"/>
@@ -17718,20 +17895,20 @@
       <c r="D10" s="24" t="s">
         <v>437</v>
       </c>
-      <c r="E10" s="135" t="s">
+      <c r="E10" s="136" t="s">
         <v>439</v>
       </c>
-      <c r="F10" s="135"/>
-      <c r="G10" s="135"/>
-      <c r="H10" s="135"/>
-      <c r="I10" s="135"/>
-      <c r="J10" s="135"/>
-      <c r="K10" s="135"/>
-      <c r="L10" s="135"/>
-      <c r="M10" s="135"/>
-      <c r="N10" s="135"/>
-      <c r="O10" s="135"/>
-      <c r="P10" s="135"/>
+      <c r="F10" s="136"/>
+      <c r="G10" s="136"/>
+      <c r="H10" s="136"/>
+      <c r="I10" s="136"/>
+      <c r="J10" s="136"/>
+      <c r="K10" s="136"/>
+      <c r="L10" s="136"/>
+      <c r="M10" s="136"/>
+      <c r="N10" s="136"/>
+      <c r="O10" s="136"/>
+      <c r="P10" s="136"/>
     </row>
     <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="131"/>
@@ -19216,54 +19393,54 @@
       <c r="H20" s="109"/>
     </row>
     <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="134" t="s">
+      <c r="A21" s="135" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="134"/>
-      <c r="C21" s="134"/>
-      <c r="D21" s="134"/>
-      <c r="E21" s="134"/>
-      <c r="F21" s="134"/>
+      <c r="B21" s="135"/>
+      <c r="C21" s="135"/>
+      <c r="D21" s="135"/>
+      <c r="E21" s="135"/>
+      <c r="F21" s="135"/>
     </row>
     <row r="22" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="135" t="s">
+      <c r="A22" s="136" t="s">
         <v>179</v>
       </c>
-      <c r="B22" s="135"/>
-      <c r="C22" s="135"/>
-      <c r="D22" s="135"/>
-      <c r="E22" s="135"/>
-      <c r="F22" s="135"/>
+      <c r="B22" s="136"/>
+      <c r="C22" s="136"/>
+      <c r="D22" s="136"/>
+      <c r="E22" s="136"/>
+      <c r="F22" s="136"/>
     </row>
     <row r="23" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="134" t="s">
+      <c r="A23" s="135" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="134"/>
-      <c r="C23" s="134"/>
-      <c r="D23" s="134"/>
-      <c r="E23" s="134"/>
-      <c r="F23" s="134"/>
+      <c r="B23" s="135"/>
+      <c r="C23" s="135"/>
+      <c r="D23" s="135"/>
+      <c r="E23" s="135"/>
+      <c r="F23" s="135"/>
     </row>
     <row r="24" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="134" t="s">
+      <c r="A24" s="135" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="134"/>
-      <c r="C24" s="134"/>
-      <c r="D24" s="134"/>
-      <c r="E24" s="134"/>
-      <c r="F24" s="134"/>
+      <c r="B24" s="135"/>
+      <c r="C24" s="135"/>
+      <c r="D24" s="135"/>
+      <c r="E24" s="135"/>
+      <c r="F24" s="135"/>
     </row>
     <row r="25" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="134" t="s">
+      <c r="A25" s="135" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="134"/>
-      <c r="C25" s="134"/>
-      <c r="D25" s="134"/>
-      <c r="E25" s="134"/>
-      <c r="F25" s="134"/>
+      <c r="B25" s="135"/>
+      <c r="C25" s="135"/>
+      <c r="D25" s="135"/>
+      <c r="E25" s="135"/>
+      <c r="F25" s="135"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="30"/>
@@ -19447,38 +19624,38 @@
       <c r="B3" s="69"/>
       <c r="C3" s="70"/>
       <c r="D3" s="71"/>
-      <c r="E3" s="139" t="s">
+      <c r="E3" s="140" t="s">
         <v>276</v>
       </c>
-      <c r="F3" s="140"/>
-      <c r="G3" s="140"/>
-      <c r="H3" s="137"/>
-      <c r="I3" s="136" t="s">
+      <c r="F3" s="141"/>
+      <c r="G3" s="141"/>
+      <c r="H3" s="138"/>
+      <c r="I3" s="137" t="s">
         <v>304</v>
       </c>
-      <c r="J3" s="137"/>
-      <c r="K3" s="136" t="s">
+      <c r="J3" s="138"/>
+      <c r="K3" s="137" t="s">
         <v>305</v>
       </c>
-      <c r="L3" s="138"/>
-      <c r="M3" s="139" t="s">
+      <c r="L3" s="139"/>
+      <c r="M3" s="140" t="s">
         <v>292</v>
       </c>
-      <c r="N3" s="140"/>
-      <c r="O3" s="137"/>
-      <c r="P3" s="141" t="s">
+      <c r="N3" s="141"/>
+      <c r="O3" s="138"/>
+      <c r="P3" s="142" t="s">
         <v>257</v>
       </c>
-      <c r="Q3" s="140"/>
-      <c r="R3" s="140"/>
-      <c r="S3" s="140"/>
-      <c r="T3" s="140"/>
-      <c r="U3" s="140"/>
-      <c r="V3" s="140"/>
-      <c r="W3" s="140"/>
-      <c r="X3" s="140"/>
-      <c r="Y3" s="140"/>
-      <c r="Z3" s="142"/>
+      <c r="Q3" s="141"/>
+      <c r="R3" s="141"/>
+      <c r="S3" s="141"/>
+      <c r="T3" s="141"/>
+      <c r="U3" s="141"/>
+      <c r="V3" s="141"/>
+      <c r="W3" s="141"/>
+      <c r="X3" s="141"/>
+      <c r="Y3" s="141"/>
+      <c r="Z3" s="143"/>
       <c r="AA3" s="90"/>
     </row>
     <row r="4" spans="1:27" ht="170.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -22754,10 +22931,10 @@
       <c r="A3" s="69"/>
       <c r="B3" s="70"/>
       <c r="C3" s="71"/>
-      <c r="D3" s="139" t="s">
+      <c r="D3" s="140" t="s">
         <v>202</v>
       </c>
-      <c r="E3" s="137"/>
+      <c r="E3" s="138"/>
       <c r="F3" s="73"/>
     </row>
     <row r="4" spans="1:6" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -23017,32 +23194,32 @@
       <c r="F23" s="59"/>
     </row>
     <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="134"/>
-      <c r="B24" s="134"/>
-      <c r="C24" s="134"/>
-      <c r="D24" s="134"/>
-      <c r="E24" s="134"/>
+      <c r="A24" s="135"/>
+      <c r="B24" s="135"/>
+      <c r="C24" s="135"/>
+      <c r="D24" s="135"/>
+      <c r="E24" s="135"/>
     </row>
     <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="134"/>
-      <c r="B25" s="134"/>
-      <c r="C25" s="134"/>
-      <c r="D25" s="134"/>
-      <c r="E25" s="134"/>
+      <c r="A25" s="135"/>
+      <c r="B25" s="135"/>
+      <c r="C25" s="135"/>
+      <c r="D25" s="135"/>
+      <c r="E25" s="135"/>
     </row>
     <row r="26" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="134"/>
-      <c r="B26" s="134"/>
-      <c r="C26" s="134"/>
-      <c r="D26" s="134"/>
-      <c r="E26" s="134"/>
+      <c r="A26" s="135"/>
+      <c r="B26" s="135"/>
+      <c r="C26" s="135"/>
+      <c r="D26" s="135"/>
+      <c r="E26" s="135"/>
     </row>
     <row r="27" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="134"/>
-      <c r="B27" s="134"/>
-      <c r="C27" s="134"/>
-      <c r="D27" s="134"/>
-      <c r="E27" s="134"/>
+      <c r="A27" s="135"/>
+      <c r="B27" s="135"/>
+      <c r="C27" s="135"/>
+      <c r="D27" s="135"/>
+      <c r="E27" s="135"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="60"/>
@@ -23844,27 +24021,27 @@
       <c r="H16" s="32"/>
     </row>
     <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="134"/>
-      <c r="B17" s="134"/>
-      <c r="C17" s="134"/>
+      <c r="A17" s="135"/>
+      <c r="B17" s="135"/>
+      <c r="C17" s="135"/>
       <c r="D17" s="32"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="134"/>
-      <c r="B18" s="134"/>
-      <c r="C18" s="134"/>
+      <c r="A18" s="135"/>
+      <c r="B18" s="135"/>
+      <c r="C18" s="135"/>
       <c r="D18" s="32"/>
       <c r="E18" s="32"/>
       <c r="F18" s="32"/>
       <c r="H18" s="32"/>
     </row>
     <row r="19" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="134"/>
-      <c r="B19" s="134"/>
-      <c r="C19" s="134"/>
+      <c r="A19" s="135"/>
+      <c r="B19" s="135"/>
+      <c r="C19" s="135"/>
       <c r="D19" s="32"/>
       <c r="E19" s="32"/>
       <c r="F19" s="32"/>
@@ -24303,30 +24480,30 @@
       <c r="C41" s="52"/>
     </row>
     <row r="42" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="143" t="s">
+      <c r="A42" s="144" t="s">
         <v>174</v>
       </c>
-      <c r="B42" s="143"/>
-      <c r="C42" s="143"/>
+      <c r="B42" s="144"/>
+      <c r="C42" s="144"/>
     </row>
     <row r="43" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="144" t="s">
+      <c r="A43" s="145" t="s">
         <v>175</v>
       </c>
-      <c r="B43" s="144"/>
-      <c r="C43" s="144"/>
+      <c r="B43" s="145"/>
+      <c r="C43" s="145"/>
     </row>
     <row r="44" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="143" t="s">
+      <c r="A44" s="144" t="s">
         <v>176</v>
       </c>
-      <c r="B44" s="143"/>
-      <c r="C44" s="143"/>
+      <c r="B44" s="144"/>
+      <c r="C44" s="144"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="134"/>
-      <c r="B45" s="134"/>
-      <c r="C45" s="134"/>
+      <c r="A45" s="135"/>
+      <c r="B45" s="135"/>
+      <c r="C45" s="135"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="37"/>

</xml_diff>

<commit_message>
Created file for study research questions by units of analysis
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Table - Units of Analysis" sheetId="19" r:id="rId1"/>
@@ -30,14 +30,14 @@
     <sheet name="Figure - Theory the Org" sheetId="15" r:id="rId16"/>
     <sheet name="Figure - Conceptual Framework" sheetId="9" r:id="rId17"/>
     <sheet name="Figure - Literature Landscape" sheetId="14" r:id="rId18"/>
-    <sheet name="Figure - Research Approach" sheetId="18" r:id="rId19"/>
+    <sheet name="Fig - Study Conceptualization" sheetId="18" r:id="rId19"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="4">'Table - Determinants Examined'!$3:$4</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Table - Research Questions'!$1:$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Table - Units of Analysis'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1197" uniqueCount="489">
   <si>
     <t>Total</t>
   </si>
@@ -1406,22 +1406,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Unit of Analysis
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The unit about which one would like to make a generalizing statement.</t>
-    </r>
-  </si>
-  <si>
     <t>Research Question</t>
   </si>
   <si>
@@ -1621,9 +1605,6 @@
     <t>Fifty percent (50%) of technology transfer decision-makers in private sector organizations studied used technology maturity level in their sensemaking and sensegiving communications.</t>
   </si>
   <si>
-    <t>Is technology maturity level used the sensemaking and sensegiving communications of demand-side private sector organizations?</t>
-  </si>
-  <si>
     <t>Individuals (interpersonal interactions)</t>
   </si>
   <si>
@@ -1673,6 +1654,230 @@
   </si>
   <si>
     <t>Potential Research Question</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Policy Problem:  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Policy Question:  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research Focus:  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potential Research Question(s):  </t>
+  </si>
+  <si>
+    <t>How does technology maturity level influence the technology transfer priorities and intentions of demand-side private sector organizations?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Example Hypothesis
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>For illustrative purposes only.</t>
+    </r>
+  </si>
+  <si>
+    <t>Subjects will choose to acquire the high maturity level technology more often than the low maturity level technology.</t>
+  </si>
+  <si>
+    <t>Subjects will be more likely to acquire a high maturity level technology than a low maturity level.</t>
+  </si>
+  <si>
+    <t>The percent of subjects that choose to pursue the low maturity level technology will be more than the percent of subjects that choose to pursue the high maturity level technology.</t>
+  </si>
+  <si>
+    <t>Subjects will be more likely to acquire the high maturity level technology than the low maturity level technology.</t>
+  </si>
+  <si>
+    <t>Organizations will be more willing to acquire the high maturity level technology than the low maturity level technology.
+Organizations will consistently choose not to acquire the low maturity level technology.</t>
+  </si>
+  <si>
+    <t>Organizations will demonstrated an unwillingness to acquire low maturity level technologies.</t>
+  </si>
+  <si>
+    <t>Organizations will generally choose to pursue the high maturity level technology, all other things being equal.
+Organizations will choose NOT to pursue the low maturity level technology, all other things being equal.</t>
+  </si>
+  <si>
+    <t>Organizations will choose NOT to pursue the low maturity level technology, all other things being equal.</t>
+  </si>
+  <si>
+    <t>Demand-side private sector organizations use a decision premise that a technology has to have attained a minimum maturity level that is higher than the average maturity level of technologies available from universities.</t>
+  </si>
+  <si>
+    <t>Private sector organizations in the life sciences sector will acquired technology at a lower maturity level than private sector organizations in all other sectors.</t>
+  </si>
+  <si>
+    <t>Demand-side private sector organizations use technology maturity level as a proxy for uncertainty.
+Demand-side private sector organizations' perceived uncertainty of a technology will correlate with the maturity level of the technology.</t>
+  </si>
+  <si>
+    <t>Technology maturity level is regularly incorporated into the sensemaking and sensegiving communications of private sector organizations.</t>
+  </si>
+  <si>
+    <t>Technology transfer decision-makers in demand-side private sector organizations use technology maturity level as a significant component of their sensemaking and sensegiving communications.</t>
+  </si>
+  <si>
+    <t>Documents (organization records)</t>
+  </si>
+  <si>
+    <t>Is technology maturity level used in the sensemaking and sensegiving communications of demand-side private sector organizations?</t>
+  </si>
+  <si>
+    <t>High maturity level technologies are pursued more often than low matruity level technologies.</t>
+  </si>
+  <si>
+    <t>Entry No.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Unit of Analysis
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The unit about which the study aims to make a generalizing statement.</t>
+    </r>
+  </si>
+  <si>
+    <t>The percent of subjects in the treatment group (high technology maturiy level) that choose to acquire the technology will be higher than the percent of subjects in the comparison group (low technology maturity level) that choose to acquire the technology.</t>
+  </si>
+  <si>
+    <t>Fifty percent (50%) of subjects in the treatment group chose to acquire the technology but only 20 percent of subjects in the comparison group chose to acquire the technology.</t>
+  </si>
+  <si>
+    <t>Documents (news releases and organization records); 
+Individuals (organization members)</t>
+  </si>
+  <si>
+    <t>High maturity level technologies are pursued more often than low maturity level technologies.</t>
+  </si>
+  <si>
+    <t>High maturity level technologies were pursued in 80 percent of the cases.</t>
+  </si>
+  <si>
+    <t>Experiment using demand-side technology transfer decision-makers as subjects.  Random assignment to comparison or treatment group by inidividual. Comparison group presented with case where technology maturity level is low.  Treatment group presented with case where technology maturity level is high.  All other aspects of the case are the same.</t>
+  </si>
+  <si>
+    <t>Experiment using demand-side technology transfer decision-makers as subjects.  Random assignment to comparison or treatment group by organization affiliation.  Comparison group presented with case where technology maturity level is low.  Treatment group presented with case where technology maturity level is high.  All other aspects of the case are the same.</t>
+  </si>
+  <si>
+    <t>The percent of organizations in the treatment group (high technology maturiy level) that have a majority of members choose to acquire the technology will be higher than the percent of organizations in the comparison group (low technology maturity level) that have a majority of members choose to acquire the technology.</t>
+  </si>
+  <si>
+    <t>Fifty percent (50%) of organizations in the treatment group had a majority of members chose to acquire the technology but only 20 percent of organizations in the comparison group had a majority of members chose to acquire the technology.</t>
+  </si>
+  <si>
+    <t>Organizations pursue a high maturity level technologies more often than low maturity level technologies.</t>
+  </si>
+  <si>
+    <t>In 80 percent of the cases the organization acquired a high maturity level technology.</t>
+  </si>
+  <si>
+    <t>Interactions</t>
+  </si>
+  <si>
+    <t>Organizations will generally choose to pursue a high maturity level technology, all other things being equal.
+Organizations will choose NOT to pursue a low maturity level technology, all other things being equal.</t>
+  </si>
+  <si>
+    <t>In 80 percent of the cases the organization acquired or attempted to acquire a high maturity level technology.
+Low technology maturity level was cited as a major reason that an organization chose NOT to purse a technology in 80 percent of the cases.</t>
+  </si>
+  <si>
+    <t>Data about the most recent university technology the organization considered acquiring of which the individual has direct knowledge.</t>
+  </si>
+  <si>
+    <t>Organizations tended to pursue high maturity level technologies.
+Organizations demonstrated a tendency not to pursue low maturity level technologies.</t>
+  </si>
+  <si>
+    <t>Low technology maturity level was cited as a major reason that an organization chose NOT to purse a technology in 80 percent of the cases.</t>
+  </si>
+  <si>
+    <t>Decision premise statements about technology maturity level in company records
+Statements indicating technology maturity level in Univesity-owned patents</t>
+  </si>
+  <si>
+    <t>Documents (organization records and USPTO patent records)</t>
+  </si>
+  <si>
+    <t>In 80 percent of the cases, the private sector organization used a decision premise that a technology had to have attained a minimum maturity level that was higher than the average maturity level of technologies patented by universities.</t>
+  </si>
+  <si>
+    <t>In 80 percent of the cases, the private sector organization used a decision premise that a technology had to have attained a minimum maturity level that was higher than the average maturity level of technologies available from universities.</t>
+  </si>
+  <si>
+    <t>Do certain types of private sector organizations tend to acquire higher maturity level technologies than other types of private sector organizations?</t>
+  </si>
+  <si>
+    <t>Responses about the maturity level of the technologies the organization has acquired.</t>
+  </si>
+  <si>
+    <t>Statements about the maturity level of the technologies the organization has  acquired.</t>
+  </si>
+  <si>
+    <t>Private sector organizations in the life sciences sector acquire technologies at lower maturity levels than private sector organizations in all other sectors.</t>
+  </si>
+  <si>
+    <t>Eighty percent (80%) of private sector organizations in the life sciences sector acquired technology at low maturity levels compared to only 20 percent of organizations in all other sectors.</t>
+  </si>
+  <si>
+    <t>Demand-side private sector organizations use technology maturity level as a proxy for uncertainty.
+Demand-side private sector organizations' perceived uncertainty of a technology correlates with the maturity level of the technology.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">There was a statistically significant association (p </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">≤ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0.05) between the average perceived uncertainty of a technology by demand-side private sector organizations and the maturity level of technologies considered.</t>
+    </r>
+  </si>
+  <si>
+    <t>Technology maturity level was a component of the sensemaking and sensegiving communications of private sector organizations in 80 percent of the observations.</t>
+  </si>
+  <si>
+    <t>Observations; content analysis</t>
+  </si>
+  <si>
+    <t>Individuals (communications); documents (emails, memorandums)</t>
+  </si>
+  <si>
+    <t>Technology maturity level was a component of the sensemaking and sensegiving communications of demand-side technology transfer decision makers in 80 percent of the observations.</t>
   </si>
   <si>
     <r>
@@ -1718,99 +1923,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> (See attached)</t>
+      <t xml:space="preserve"> (See table on units of analysis)</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Policy Problem:  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Policy Question:  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Research Focus:  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Potential Research Question(s):  </t>
-  </si>
-  <si>
-    <t>How does technology maturity level influence the technology transfer priorities and intentions of demand-side private sector organizations?</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Example Hypothesis
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>For illustrative purposes only.</t>
-    </r>
-  </si>
-  <si>
-    <t>Subjects will choose to acquire the high maturity level technology more often than the low maturity level technology.</t>
-  </si>
-  <si>
-    <t>Subjects chose to acquire the high maturity level technology twice as often as the low maturity level technology.</t>
-  </si>
-  <si>
-    <t>High maturity level technologies will be pursued more often than low matruity level technologies.</t>
-  </si>
-  <si>
-    <t>High maturity level technologies were pursued twice as often as low matruity level technologies.</t>
-  </si>
-  <si>
-    <t>Subjects will be more likely to acquire a high maturity level technology than a low maturity level.</t>
-  </si>
-  <si>
-    <t>The percent of subjects that choose to pursue the low maturity level technology will be more than the percent of subjects that choose to pursue the high maturity level technology.</t>
-  </si>
-  <si>
-    <t>Subjects will be more likely to acquire the high maturity level technology than the low maturity level technology.</t>
-  </si>
-  <si>
-    <t>Organizations will be more willing to acquire the high maturity level technology than the low maturity level technology.
-Organizations will consistently choose not to acquire the low maturity level technology.</t>
-  </si>
-  <si>
-    <t>Organizations will demonstrated an unwillingness to acquire low maturity level technologies.</t>
-  </si>
-  <si>
-    <t>Organizations will generally choose to pursue the high maturity level technology, all other things being equal.
-Organizations will choose NOT to pursue the low maturity level technology, all other things being equal.</t>
-  </si>
-  <si>
-    <t>Organizations will choose NOT to pursue the low maturity level technology, all other things being equal.</t>
-  </si>
-  <si>
-    <t>Demand-side private sector organizations use a decision premise that a technology has to have attained a minimum maturity level that is higher than the average maturity level of technologies available from universities.</t>
-  </si>
-  <si>
-    <t>Private sector organizations in the life sciences sector will acquired technology at a lower maturity level than private sector organizations in all other sectors.</t>
-  </si>
-  <si>
-    <t>Demand-side private sector organizations use technology maturity level as a proxy for uncertainty.
-Demand-side private sector organizations' perceived uncertainty of a technology will correlate with the maturity level of the technology.</t>
-  </si>
-  <si>
-    <t>Is technology maturity level usedin the sensemaking and sensegiving communications of demand-side private sector organizations?</t>
-  </si>
-  <si>
-    <t>Technology maturity level is regularly incorporated into the sensemaking and sensegiving communications of private sector organizations.</t>
-  </si>
-  <si>
-    <t>Technology transfer decision-makers in demand-side private sector organizations use technology maturity level as a significant component of their sensemaking and sensegiving communications.</t>
-  </si>
-  <si>
-    <t>Documents (organization records)</t>
-  </si>
-  <si>
-    <t>Documents (organization records and allowed patents)</t>
   </si>
 </sst>
 </file>
@@ -1821,7 +1935,7 @@
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1920,8 +2034,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1937,6 +2057,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2180,7 +2306,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -2502,16 +2628,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2573,6 +2690,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2603,11 +2729,50 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -6917,7 +7082,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:colOff>285750</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
@@ -6929,10 +7094,10 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="34" name="Group 33">
+        <xdr:cNvPr id="2" name="Group 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{445C3D5D-4683-47A0-A2CC-EE65C8C4CC81}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5D9EFC7-1A01-4B49-A26A-97184D35146B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6940,10 +7105,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2705100" y="3371850"/>
-          <a:ext cx="5090160" cy="4175760"/>
-          <a:chOff x="2352675" y="3219450"/>
-          <a:chExt cx="5090160" cy="4175760"/>
+          <a:off x="2724150" y="3371850"/>
+          <a:ext cx="5071110" cy="4175760"/>
+          <a:chOff x="2724150" y="3371850"/>
+          <a:chExt cx="5071110" cy="4175760"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:cxnSp macro="">
@@ -6959,7 +7124,7 @@
         </xdr:nvCxnSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="2695575" y="5048250"/>
+            <a:off x="3048000" y="5200650"/>
             <a:ext cx="1457325" cy="276225"/>
           </a:xfrm>
           <a:prstGeom prst="straightConnector1">
@@ -7000,7 +7165,7 @@
         </xdr:nvCxnSpPr>
         <xdr:spPr>
           <a:xfrm flipH="1" flipV="1">
-            <a:off x="5591176" y="5648325"/>
+            <a:off x="5943601" y="5800725"/>
             <a:ext cx="1523999" cy="361950"/>
           </a:xfrm>
           <a:prstGeom prst="straightConnector1">
@@ -7041,7 +7206,7 @@
         </xdr:nvCxnSpPr>
         <xdr:spPr>
           <a:xfrm flipH="1">
-            <a:off x="5419727" y="4305300"/>
+            <a:off x="5772152" y="4457700"/>
             <a:ext cx="1152523" cy="809625"/>
           </a:xfrm>
           <a:prstGeom prst="straightConnector1">
@@ -7082,7 +7247,7 @@
         </xdr:nvCxnSpPr>
         <xdr:spPr>
           <a:xfrm flipV="1">
-            <a:off x="3038475" y="5972175"/>
+            <a:off x="3390900" y="6124575"/>
             <a:ext cx="1323975" cy="1019176"/>
           </a:xfrm>
           <a:prstGeom prst="straightConnector1">
@@ -7123,7 +7288,7 @@
         </xdr:nvCxnSpPr>
         <xdr:spPr>
           <a:xfrm flipH="1" flipV="1">
-            <a:off x="4905375" y="6153150"/>
+            <a:off x="5257800" y="6305550"/>
             <a:ext cx="9525" cy="847725"/>
           </a:xfrm>
           <a:prstGeom prst="straightConnector1">
@@ -7164,7 +7329,7 @@
         </xdr:nvCxnSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="4838700" y="3562350"/>
+            <a:off x="5191125" y="3714750"/>
             <a:ext cx="9525" cy="1238250"/>
           </a:xfrm>
           <a:prstGeom prst="straightConnector1">
@@ -7205,7 +7370,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="4657725" y="3219450"/>
+            <a:off x="5010150" y="3371850"/>
             <a:ext cx="365760" cy="327660"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -7259,7 +7424,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="2352675" y="4781550"/>
+            <a:off x="6877050" y="4181475"/>
             <a:ext cx="365760" cy="365760"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -7313,7 +7478,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="2705100" y="6905625"/>
+            <a:off x="7429500" y="6000750"/>
             <a:ext cx="365760" cy="365760"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -7367,7 +7532,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="4724400" y="7029450"/>
+            <a:off x="5076825" y="7181850"/>
             <a:ext cx="365760" cy="365760"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -7421,7 +7586,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="7077075" y="5848350"/>
+            <a:off x="3095625" y="7029450"/>
             <a:ext cx="365760" cy="365760"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -7475,7 +7640,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="6562725" y="4067175"/>
+            <a:off x="2724150" y="4924425"/>
             <a:ext cx="365760" cy="365760"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -7542,7 +7707,7 @@
         </xdr:blipFill>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="4324352" y="4943475"/>
+            <a:off x="4676777" y="5095875"/>
             <a:ext cx="1070142" cy="1097280"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -7563,7 +7728,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="4438650" y="5248275"/>
+            <a:off x="4791075" y="5400675"/>
             <a:ext cx="822960" cy="514350"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -15612,268 +15777,289 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="130" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="129" customWidth="1"/>
-    <col min="3" max="3" width="1.7109375" style="129" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" style="129" customWidth="1"/>
-    <col min="5" max="5" width="1.7109375" style="129" customWidth="1"/>
-    <col min="6" max="6" width="40.7109375" style="129" customWidth="1"/>
-    <col min="7" max="7" width="1.7109375" style="129" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" style="129" customWidth="1"/>
-    <col min="9" max="9" width="1.7109375" style="129" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" style="129" customWidth="1"/>
-    <col min="11" max="11" width="1.7109375" style="134" customWidth="1"/>
-    <col min="12" max="12" width="40.7109375" style="134" customWidth="1"/>
-    <col min="13" max="13" width="1.7109375" style="129" customWidth="1"/>
-    <col min="14" max="14" width="40.7109375" style="129" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="129"/>
-    <col min="16" max="16" width="62" style="129" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="129"/>
+    <col min="1" max="1" width="5.7109375" style="127" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="126" customWidth="1"/>
+    <col min="3" max="3" width="1.7109375" style="126" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" style="126" customWidth="1"/>
+    <col min="5" max="5" width="1.7109375" style="126" customWidth="1"/>
+    <col min="6" max="6" width="40.7109375" style="126" customWidth="1"/>
+    <col min="7" max="7" width="1.7109375" style="126" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" style="126" customWidth="1"/>
+    <col min="9" max="9" width="1.7109375" style="126" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" style="126" customWidth="1"/>
+    <col min="11" max="11" width="1.7109375" style="131" customWidth="1"/>
+    <col min="12" max="12" width="40.7109375" style="131" customWidth="1"/>
+    <col min="13" max="13" width="1.7109375" style="126" customWidth="1"/>
+    <col min="14" max="14" width="40.7109375" style="126" customWidth="1"/>
+    <col min="15" max="15" width="5.7109375" style="78" customWidth="1"/>
+    <col min="16" max="16" width="62" style="126" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="126"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="146"/>
-      <c r="B1" s="147" t="s">
-        <v>359</v>
-      </c>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147" t="s">
-        <v>433</v>
-      </c>
-      <c r="E1" s="147"/>
-      <c r="F1" s="147" t="s">
+      <c r="A1" s="133"/>
+      <c r="B1" s="134" t="s">
+        <v>455</v>
+      </c>
+      <c r="C1" s="134"/>
+      <c r="D1" s="134" t="s">
+        <v>431</v>
+      </c>
+      <c r="E1" s="134"/>
+      <c r="F1" s="134" t="s">
         <v>358</v>
       </c>
-      <c r="G1" s="147"/>
-      <c r="H1" s="147" t="s">
+      <c r="G1" s="134"/>
+      <c r="H1" s="134" t="s">
         <v>357</v>
       </c>
-      <c r="I1" s="147"/>
-      <c r="J1" s="147" t="s">
-        <v>404</v>
-      </c>
-      <c r="K1" s="147"/>
-      <c r="L1" s="147" t="s">
-        <v>440</v>
-      </c>
-      <c r="M1" s="147"/>
-      <c r="N1" s="147" t="s">
+      <c r="I1" s="134"/>
+      <c r="J1" s="134" t="s">
+        <v>403</v>
+      </c>
+      <c r="K1" s="134"/>
+      <c r="L1" s="134" t="s">
+        <v>437</v>
+      </c>
+      <c r="M1" s="134"/>
+      <c r="N1" s="134" t="s">
+        <v>362</v>
+      </c>
+      <c r="O1" s="159" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="135" x14ac:dyDescent="0.25">
+      <c r="A2" s="113" t="s">
+        <v>421</v>
+      </c>
+      <c r="B2" s="114" t="s">
+        <v>343</v>
+      </c>
+      <c r="C2" s="114"/>
+      <c r="D2" s="114" t="s">
+        <v>365</v>
+      </c>
+      <c r="E2" s="114"/>
+      <c r="F2" s="114" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="135" x14ac:dyDescent="0.25">
-      <c r="A2" s="116" t="s">
-        <v>423</v>
-      </c>
-      <c r="B2" s="117" t="s">
+      <c r="G2" s="114"/>
+      <c r="H2" s="114" t="s">
+        <v>354</v>
+      </c>
+      <c r="I2" s="114"/>
+      <c r="J2" s="114" t="s">
+        <v>342</v>
+      </c>
+      <c r="K2" s="114"/>
+      <c r="L2" s="114" t="s">
+        <v>456</v>
+      </c>
+      <c r="M2" s="114"/>
+      <c r="N2" s="114" t="s">
+        <v>457</v>
+      </c>
+      <c r="O2" s="149">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="115" t="s">
+        <v>422</v>
+      </c>
+      <c r="B3" s="116" t="s">
         <v>343</v>
       </c>
-      <c r="C2" s="117"/>
-      <c r="D2" s="117" t="s">
-        <v>366</v>
-      </c>
-      <c r="E2" s="117"/>
-      <c r="F2" s="117" t="s">
-        <v>364</v>
-      </c>
-      <c r="G2" s="117"/>
-      <c r="H2" s="117" t="s">
+      <c r="C3" s="116"/>
+      <c r="D3" s="116" t="s">
+        <v>365</v>
+      </c>
+      <c r="E3" s="116"/>
+      <c r="F3" s="116" t="s">
+        <v>406</v>
+      </c>
+      <c r="G3" s="116"/>
+      <c r="H3" s="116" t="s">
+        <v>355</v>
+      </c>
+      <c r="I3" s="116"/>
+      <c r="J3" s="116" t="s">
+        <v>458</v>
+      </c>
+      <c r="K3" s="116"/>
+      <c r="L3" s="116" t="s">
+        <v>459</v>
+      </c>
+      <c r="M3" s="116"/>
+      <c r="N3" s="116" t="s">
+        <v>460</v>
+      </c>
+      <c r="O3" s="151">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="135" x14ac:dyDescent="0.25">
+      <c r="A4" s="113">
+        <v>2</v>
+      </c>
+      <c r="B4" s="114" t="s">
+        <v>342</v>
+      </c>
+      <c r="C4" s="114"/>
+      <c r="D4" s="114" t="s">
+        <v>368</v>
+      </c>
+      <c r="E4" s="114"/>
+      <c r="F4" s="114" t="s">
+        <v>363</v>
+      </c>
+      <c r="G4" s="114"/>
+      <c r="H4" s="114" t="s">
         <v>354</v>
       </c>
-      <c r="I2" s="117"/>
-      <c r="J2" s="117" t="s">
+      <c r="I4" s="114"/>
+      <c r="J4" s="114" t="s">
         <v>342</v>
       </c>
-      <c r="K2" s="117"/>
-      <c r="L2" s="117" t="s">
-        <v>441</v>
-      </c>
-      <c r="M2" s="117"/>
-      <c r="N2" s="117" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="118" t="s">
-        <v>424</v>
-      </c>
-      <c r="B3" s="119" t="s">
-        <v>343</v>
-      </c>
-      <c r="C3" s="119"/>
-      <c r="D3" s="119" t="s">
-        <v>366</v>
-      </c>
-      <c r="E3" s="119"/>
-      <c r="F3" s="119" t="s">
-        <v>407</v>
-      </c>
-      <c r="G3" s="119"/>
-      <c r="H3" s="119" t="s">
-        <v>355</v>
-      </c>
-      <c r="I3" s="119"/>
-      <c r="J3" s="119" t="s">
-        <v>406</v>
-      </c>
-      <c r="K3" s="119"/>
-      <c r="L3" s="119" t="s">
-        <v>443</v>
-      </c>
-      <c r="M3" s="119"/>
-      <c r="N3" s="119" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="135" x14ac:dyDescent="0.25">
-      <c r="A4" s="120">
-        <v>2</v>
-      </c>
-      <c r="B4" s="121" t="s">
+      <c r="K4" s="114"/>
+      <c r="L4" s="114" t="s">
+        <v>456</v>
+      </c>
+      <c r="M4" s="114"/>
+      <c r="N4" s="114" t="s">
+        <v>457</v>
+      </c>
+      <c r="O4" s="149">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="135" x14ac:dyDescent="0.25">
+      <c r="A5" s="113">
+        <v>3</v>
+      </c>
+      <c r="B5" s="114" t="s">
         <v>342</v>
       </c>
-      <c r="C4" s="121"/>
-      <c r="D4" s="121" t="s">
-        <v>403</v>
-      </c>
-      <c r="E4" s="121"/>
-      <c r="F4" s="121" t="s">
-        <v>362</v>
-      </c>
-      <c r="G4" s="121"/>
-      <c r="H4" s="121" t="s">
+      <c r="C5" s="114"/>
+      <c r="D5" s="114" t="s">
+        <v>384</v>
+      </c>
+      <c r="E5" s="114"/>
+      <c r="F5" s="114" t="s">
+        <v>370</v>
+      </c>
+      <c r="G5" s="114"/>
+      <c r="H5" s="114" t="s">
         <v>354</v>
       </c>
-      <c r="I4" s="121"/>
-      <c r="J4" s="121" t="s">
+      <c r="I5" s="114"/>
+      <c r="J5" s="114" t="s">
         <v>342</v>
       </c>
-      <c r="K4" s="121"/>
-      <c r="L4" s="121" t="s">
-        <v>445</v>
-      </c>
-      <c r="M4" s="121"/>
-      <c r="N4" s="121" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="135" x14ac:dyDescent="0.25">
-      <c r="A5" s="116">
-        <v>3</v>
-      </c>
-      <c r="B5" s="117" t="s">
+      <c r="K5" s="114"/>
+      <c r="L5" s="114" t="s">
+        <v>456</v>
+      </c>
+      <c r="M5" s="114"/>
+      <c r="N5" s="114" t="s">
+        <v>457</v>
+      </c>
+      <c r="O5" s="149">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="83">
+        <v>4</v>
+      </c>
+      <c r="B6" s="84" t="s">
         <v>342</v>
       </c>
-      <c r="C5" s="117"/>
-      <c r="D5" s="117" t="s">
-        <v>385</v>
-      </c>
-      <c r="E5" s="117"/>
-      <c r="F5" s="117" t="s">
-        <v>371</v>
-      </c>
-      <c r="G5" s="117"/>
-      <c r="H5" s="117" t="s">
+      <c r="C6" s="84"/>
+      <c r="D6" s="84" t="s">
+        <v>411</v>
+      </c>
+      <c r="E6" s="84"/>
+      <c r="F6" s="84" t="s">
+        <v>485</v>
+      </c>
+      <c r="G6" s="84"/>
+      <c r="H6" s="84" t="s">
+        <v>413</v>
+      </c>
+      <c r="I6" s="84"/>
+      <c r="J6" s="84" t="s">
+        <v>486</v>
+      </c>
+      <c r="K6" s="84"/>
+      <c r="L6" s="84" t="s">
+        <v>450</v>
+      </c>
+      <c r="M6" s="84"/>
+      <c r="N6" s="84" t="s">
+        <v>487</v>
+      </c>
+      <c r="O6" s="150">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="135" x14ac:dyDescent="0.25">
+      <c r="A7" s="117">
+        <v>5</v>
+      </c>
+      <c r="B7" s="118" t="s">
+        <v>342</v>
+      </c>
+      <c r="C7" s="118"/>
+      <c r="D7" s="118" t="s">
+        <v>402</v>
+      </c>
+      <c r="E7" s="118"/>
+      <c r="F7" s="118" t="s">
+        <v>461</v>
+      </c>
+      <c r="G7" s="118"/>
+      <c r="H7" s="118" t="s">
         <v>354</v>
       </c>
-      <c r="I5" s="117"/>
-      <c r="J5" s="117" t="s">
+      <c r="I7" s="118"/>
+      <c r="J7" s="118" t="s">
         <v>342</v>
       </c>
-      <c r="K5" s="117"/>
-      <c r="L5" s="117" t="s">
-        <v>446</v>
-      </c>
-      <c r="M5" s="117"/>
-      <c r="N5" s="117" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="135" x14ac:dyDescent="0.25">
-      <c r="A6" s="116">
-        <v>4</v>
-      </c>
-      <c r="B6" s="117" t="s">
-        <v>342</v>
-      </c>
-      <c r="C6" s="117"/>
-      <c r="D6" s="117" t="s">
-        <v>369</v>
-      </c>
-      <c r="E6" s="117"/>
-      <c r="F6" s="117" t="s">
-        <v>364</v>
-      </c>
-      <c r="G6" s="117"/>
-      <c r="H6" s="117" t="s">
-        <v>354</v>
-      </c>
-      <c r="I6" s="117"/>
-      <c r="J6" s="117" t="s">
-        <v>342</v>
-      </c>
-      <c r="K6" s="117"/>
-      <c r="L6" s="117" t="s">
-        <v>447</v>
-      </c>
-      <c r="M6" s="117"/>
-      <c r="N6" s="117" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="83">
-        <v>5</v>
-      </c>
-      <c r="B7" s="84" t="s">
-        <v>342</v>
-      </c>
-      <c r="C7" s="84"/>
-      <c r="D7" s="84" t="s">
-        <v>412</v>
-      </c>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84" t="s">
-        <v>413</v>
-      </c>
-      <c r="G7" s="84"/>
-      <c r="H7" s="84" t="s">
-        <v>414</v>
-      </c>
-      <c r="I7" s="84"/>
-      <c r="J7" s="84" t="s">
-        <v>342</v>
-      </c>
-      <c r="K7" s="84"/>
-      <c r="L7" s="84" t="s">
+      <c r="K7" s="118"/>
+      <c r="L7" s="118" t="s">
+        <v>456</v>
+      </c>
+      <c r="M7" s="118"/>
+      <c r="N7" s="118" t="s">
         <v>457</v>
       </c>
-      <c r="M7" s="84"/>
-      <c r="N7" s="84" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" s="122" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="O7" s="160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" s="119" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="83" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B8" s="84" t="s">
         <v>341</v>
       </c>
       <c r="C8" s="84"/>
       <c r="D8" s="84" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E8" s="84"/>
       <c r="F8" s="84" t="s">
-        <v>365</v>
+        <v>462</v>
       </c>
       <c r="G8" s="84"/>
       <c r="H8" s="84" t="s">
@@ -15885,216 +16071,233 @@
       </c>
       <c r="K8" s="84"/>
       <c r="L8" s="84" t="s">
-        <v>448</v>
+        <v>463</v>
       </c>
       <c r="M8" s="84"/>
       <c r="N8" s="84" t="s">
-        <v>383</v>
-      </c>
-      <c r="O8" s="129"/>
-      <c r="P8" s="129"/>
-    </row>
-    <row r="9" spans="1:16" s="122" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>464</v>
+      </c>
+      <c r="O8" s="150">
+        <v>2</v>
+      </c>
+      <c r="P8" s="126"/>
+    </row>
+    <row r="9" spans="1:16" s="119" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="83" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B9" s="84" t="s">
         <v>341</v>
       </c>
       <c r="C9" s="84"/>
       <c r="D9" s="84" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E9" s="84"/>
       <c r="F9" s="84" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G9" s="84"/>
       <c r="H9" s="84" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I9" s="84"/>
       <c r="J9" s="84" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="K9" s="84"/>
       <c r="L9" s="84" t="s">
-        <v>449</v>
+        <v>465</v>
       </c>
       <c r="M9" s="84"/>
       <c r="N9" s="84" t="s">
-        <v>405</v>
-      </c>
-      <c r="O9" s="129"/>
-      <c r="P9" s="129"/>
-    </row>
-    <row r="10" spans="1:16" s="122" customFormat="1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A10" s="118" t="s">
+        <v>466</v>
+      </c>
+      <c r="O9" s="150">
+        <v>3</v>
+      </c>
+      <c r="P9" s="126"/>
+    </row>
+    <row r="10" spans="1:16" s="119" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A10" s="115" t="s">
+        <v>398</v>
+      </c>
+      <c r="B10" s="116" t="s">
+        <v>341</v>
+      </c>
+      <c r="C10" s="116"/>
+      <c r="D10" s="116" t="s">
+        <v>369</v>
+      </c>
+      <c r="E10" s="116"/>
+      <c r="F10" s="116" t="s">
+        <v>364</v>
+      </c>
+      <c r="G10" s="116"/>
+      <c r="H10" s="116" t="s">
+        <v>354</v>
+      </c>
+      <c r="I10" s="116"/>
+      <c r="J10" s="116" t="s">
+        <v>344</v>
+      </c>
+      <c r="K10" s="116"/>
+      <c r="L10" s="116" t="s">
+        <v>463</v>
+      </c>
+      <c r="M10" s="116"/>
+      <c r="N10" s="116" t="s">
+        <v>464</v>
+      </c>
+      <c r="O10" s="151">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" s="119" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A11" s="115" t="s">
         <v>399</v>
       </c>
-      <c r="B10" s="119" t="s">
+      <c r="B11" s="116" t="s">
         <v>341</v>
       </c>
-      <c r="C10" s="119"/>
-      <c r="D10" s="119" t="s">
-        <v>370</v>
-      </c>
-      <c r="E10" s="119"/>
-      <c r="F10" s="119" t="s">
-        <v>365</v>
-      </c>
-      <c r="G10" s="119"/>
-      <c r="H10" s="119" t="s">
-        <v>354</v>
-      </c>
-      <c r="I10" s="119"/>
-      <c r="J10" s="119" t="s">
+      <c r="C11" s="116"/>
+      <c r="D11" s="116" t="s">
+        <v>369</v>
+      </c>
+      <c r="E11" s="116"/>
+      <c r="F11" s="116" t="s">
+        <v>346</v>
+      </c>
+      <c r="G11" s="116"/>
+      <c r="H11" s="116" t="s">
+        <v>470</v>
+      </c>
+      <c r="I11" s="116"/>
+      <c r="J11" s="116" t="s">
         <v>344</v>
       </c>
-      <c r="K10" s="119"/>
-      <c r="L10" s="119" t="s">
-        <v>450</v>
-      </c>
-      <c r="M10" s="119"/>
-      <c r="N10" s="119" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" s="122" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A11" s="118" t="s">
-        <v>400</v>
-      </c>
-      <c r="B11" s="119" t="s">
+      <c r="K11" s="116"/>
+      <c r="L11" s="116" t="s">
+        <v>468</v>
+      </c>
+      <c r="M11" s="116"/>
+      <c r="N11" s="116" t="s">
+        <v>469</v>
+      </c>
+      <c r="O11" s="151">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" s="119" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A12" s="115" t="s">
+        <v>423</v>
+      </c>
+      <c r="B12" s="116" t="s">
         <v>341</v>
       </c>
-      <c r="C11" s="119"/>
-      <c r="D11" s="119" t="s">
-        <v>370</v>
-      </c>
-      <c r="E11" s="119"/>
-      <c r="F11" s="119" t="s">
-        <v>346</v>
-      </c>
-      <c r="G11" s="119"/>
-      <c r="H11" s="119" t="s">
-        <v>373</v>
-      </c>
-      <c r="I11" s="119"/>
-      <c r="J11" s="119" t="s">
-        <v>342</v>
-      </c>
-      <c r="K11" s="119"/>
-      <c r="L11" s="119" t="s">
-        <v>450</v>
-      </c>
-      <c r="M11" s="119"/>
-      <c r="N11" s="119" t="s">
+      <c r="C12" s="116"/>
+      <c r="D12" s="116" t="s">
+        <v>369</v>
+      </c>
+      <c r="E12" s="116"/>
+      <c r="F12" s="116" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" s="122" customFormat="1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A12" s="118" t="s">
+      <c r="G12" s="116"/>
+      <c r="H12" s="116" t="s">
+        <v>375</v>
+      </c>
+      <c r="I12" s="116"/>
+      <c r="J12" s="116" t="s">
+        <v>467</v>
+      </c>
+      <c r="K12" s="116"/>
+      <c r="L12" s="116" t="s">
+        <v>468</v>
+      </c>
+      <c r="M12" s="116"/>
+      <c r="N12" s="116" t="s">
+        <v>471</v>
+      </c>
+      <c r="O12" s="151">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="115" t="s">
+        <v>424</v>
+      </c>
+      <c r="B13" s="116" t="s">
+        <v>341</v>
+      </c>
+      <c r="C13" s="116"/>
+      <c r="D13" s="116" t="s">
+        <v>369</v>
+      </c>
+      <c r="E13" s="116"/>
+      <c r="F13" s="116" t="s">
+        <v>347</v>
+      </c>
+      <c r="G13" s="116"/>
+      <c r="H13" s="116" t="s">
+        <v>376</v>
+      </c>
+      <c r="I13" s="116"/>
+      <c r="J13" s="116" t="s">
+        <v>451</v>
+      </c>
+      <c r="K13" s="116"/>
+      <c r="L13" s="116" t="s">
+        <v>445</v>
+      </c>
+      <c r="M13" s="116"/>
+      <c r="N13" s="116" t="s">
+        <v>472</v>
+      </c>
+      <c r="O13" s="151">
+        <v>8</v>
+      </c>
+      <c r="P13" s="119"/>
+    </row>
+    <row r="14" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="115" t="s">
         <v>425</v>
       </c>
-      <c r="B12" s="119" t="s">
+      <c r="B14" s="116" t="s">
         <v>341</v>
       </c>
-      <c r="C12" s="119"/>
-      <c r="D12" s="119" t="s">
-        <v>370</v>
-      </c>
-      <c r="E12" s="119"/>
-      <c r="F12" s="119" t="s">
-        <v>375</v>
-      </c>
-      <c r="G12" s="119"/>
-      <c r="H12" s="119" t="s">
-        <v>376</v>
-      </c>
-      <c r="I12" s="119"/>
-      <c r="J12" s="119" t="s">
-        <v>342</v>
-      </c>
-      <c r="K12" s="119"/>
-      <c r="L12" s="119" t="s">
-        <v>451</v>
-      </c>
-      <c r="M12" s="119"/>
-      <c r="N12" s="119" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="118" t="s">
+      <c r="C14" s="116"/>
+      <c r="D14" s="116" t="s">
+        <v>369</v>
+      </c>
+      <c r="E14" s="116"/>
+      <c r="F14" s="116" t="s">
+        <v>366</v>
+      </c>
+      <c r="G14" s="116"/>
+      <c r="H14" s="116" t="s">
+        <v>377</v>
+      </c>
+      <c r="I14" s="116"/>
+      <c r="J14" s="116" t="s">
+        <v>344</v>
+      </c>
+      <c r="K14" s="116"/>
+      <c r="L14" s="116" t="s">
+        <v>445</v>
+      </c>
+      <c r="M14" s="116"/>
+      <c r="N14" s="116" t="s">
+        <v>472</v>
+      </c>
+      <c r="O14" s="151">
+        <v>9</v>
+      </c>
+      <c r="P14" s="119"/>
+    </row>
+    <row r="15" spans="1:16" ht="150" x14ac:dyDescent="0.25">
+      <c r="A15" s="83" t="s">
         <v>426</v>
-      </c>
-      <c r="B13" s="119" t="s">
-        <v>341</v>
-      </c>
-      <c r="C13" s="119"/>
-      <c r="D13" s="119" t="s">
-        <v>370</v>
-      </c>
-      <c r="E13" s="119"/>
-      <c r="F13" s="119" t="s">
-        <v>347</v>
-      </c>
-      <c r="G13" s="119"/>
-      <c r="H13" s="119" t="s">
-        <v>377</v>
-      </c>
-      <c r="I13" s="119"/>
-      <c r="J13" s="119" t="s">
-        <v>458</v>
-      </c>
-      <c r="K13" s="119"/>
-      <c r="L13" s="119" t="s">
-        <v>451</v>
-      </c>
-      <c r="M13" s="119"/>
-      <c r="N13" s="119" t="s">
-        <v>411</v>
-      </c>
-      <c r="O13" s="122"/>
-      <c r="P13" s="122"/>
-    </row>
-    <row r="14" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="118" t="s">
-        <v>427</v>
-      </c>
-      <c r="B14" s="119" t="s">
-        <v>341</v>
-      </c>
-      <c r="C14" s="119"/>
-      <c r="D14" s="119" t="s">
-        <v>370</v>
-      </c>
-      <c r="E14" s="119"/>
-      <c r="F14" s="119" t="s">
-        <v>367</v>
-      </c>
-      <c r="G14" s="119"/>
-      <c r="H14" s="119" t="s">
-        <v>378</v>
-      </c>
-      <c r="I14" s="119"/>
-      <c r="J14" s="119" t="s">
-        <v>344</v>
-      </c>
-      <c r="K14" s="119"/>
-      <c r="L14" s="119" t="s">
-        <v>451</v>
-      </c>
-      <c r="M14" s="119"/>
-      <c r="N14" s="119" t="s">
-        <v>410</v>
-      </c>
-      <c r="O14" s="122"/>
-      <c r="P14" s="122"/>
-    </row>
-    <row r="15" spans="1:16" ht="135" x14ac:dyDescent="0.25">
-      <c r="A15" s="83" t="s">
-        <v>428</v>
       </c>
       <c r="B15" s="84" t="s">
         <v>341</v>
@@ -16109,24 +16312,27 @@
       </c>
       <c r="G15" s="84"/>
       <c r="H15" s="84" t="s">
-        <v>349</v>
+        <v>473</v>
       </c>
       <c r="I15" s="84"/>
       <c r="J15" s="84" t="s">
-        <v>459</v>
+        <v>474</v>
       </c>
       <c r="K15" s="84"/>
       <c r="L15" s="84" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="M15" s="84"/>
       <c r="N15" s="84" t="s">
-        <v>350</v>
+        <v>475</v>
+      </c>
+      <c r="O15" s="150">
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="180" x14ac:dyDescent="0.25">
       <c r="A16" s="83" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B16" s="84" t="s">
         <v>341</v>
@@ -16149,16 +16355,19 @@
       </c>
       <c r="K16" s="84"/>
       <c r="L16" s="84" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="M16" s="84"/>
       <c r="N16" s="84" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="180" x14ac:dyDescent="0.25">
+        <v>476</v>
+      </c>
+      <c r="O16" s="150">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="180" x14ac:dyDescent="0.25">
       <c r="A17" s="83" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B17" s="84" t="s">
         <v>341</v>
@@ -16169,11 +16378,11 @@
       </c>
       <c r="E17" s="84"/>
       <c r="F17" s="84" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G17" s="84"/>
       <c r="H17" s="84" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="I17" s="84"/>
       <c r="J17" s="84" t="s">
@@ -16181,23 +16390,26 @@
       </c>
       <c r="K17" s="84"/>
       <c r="L17" s="84" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="M17" s="84"/>
       <c r="N17" s="84" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+        <v>476</v>
+      </c>
+      <c r="O17" s="150">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="83" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B18" s="84" t="s">
         <v>341</v>
       </c>
       <c r="C18" s="84"/>
       <c r="D18" s="84" t="s">
-        <v>356</v>
+        <v>477</v>
       </c>
       <c r="E18" s="84"/>
       <c r="F18" s="84" t="s">
@@ -16205,7 +16417,7 @@
       </c>
       <c r="G18" s="84"/>
       <c r="H18" s="84" t="s">
-        <v>361</v>
+        <v>478</v>
       </c>
       <c r="I18" s="84"/>
       <c r="J18" s="84" t="s">
@@ -16213,23 +16425,26 @@
       </c>
       <c r="K18" s="84"/>
       <c r="L18" s="84" t="s">
-        <v>453</v>
+        <v>480</v>
       </c>
       <c r="M18" s="84"/>
       <c r="N18" s="84" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+        <v>481</v>
+      </c>
+      <c r="O18" s="150">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="83" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B19" s="84" t="s">
         <v>341</v>
       </c>
       <c r="C19" s="84"/>
       <c r="D19" s="84" t="s">
-        <v>356</v>
+        <v>477</v>
       </c>
       <c r="E19" s="84"/>
       <c r="F19" s="84" t="s">
@@ -16237,7 +16452,7 @@
       </c>
       <c r="G19" s="84"/>
       <c r="H19" s="84" t="s">
-        <v>355</v>
+        <v>479</v>
       </c>
       <c r="I19" s="84"/>
       <c r="J19" s="84" t="s">
@@ -16245,14 +16460,17 @@
       </c>
       <c r="K19" s="84"/>
       <c r="L19" s="84" t="s">
-        <v>453</v>
+        <v>480</v>
       </c>
       <c r="M19" s="84"/>
       <c r="N19" s="84" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+        <v>481</v>
+      </c>
+      <c r="O19" s="150">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="83">
         <v>10</v>
       </c>
@@ -16261,7 +16479,7 @@
       </c>
       <c r="C20" s="84"/>
       <c r="D20" s="84" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E20" s="84"/>
       <c r="F20" s="84" t="s">
@@ -16269,7 +16487,7 @@
       </c>
       <c r="G20" s="84"/>
       <c r="H20" s="84" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I20" s="84"/>
       <c r="J20" s="84" t="s">
@@ -16277,14 +16495,17 @@
       </c>
       <c r="K20" s="84"/>
       <c r="L20" s="84" t="s">
-        <v>454</v>
+        <v>482</v>
       </c>
       <c r="M20" s="84"/>
       <c r="N20" s="84" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+        <v>483</v>
+      </c>
+      <c r="O20" s="150">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="83">
         <v>11</v>
       </c>
@@ -16293,27 +16514,30 @@
       </c>
       <c r="C21" s="84"/>
       <c r="D21" s="84" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="E21" s="84"/>
       <c r="F21" s="84" t="s">
-        <v>413</v>
+        <v>374</v>
       </c>
       <c r="G21" s="84"/>
       <c r="H21" s="84" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I21" s="84"/>
       <c r="J21" s="84" t="s">
-        <v>417</v>
+        <v>467</v>
       </c>
       <c r="K21" s="84"/>
       <c r="L21" s="84" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="M21" s="84"/>
       <c r="N21" s="84" t="s">
-        <v>418</v>
+        <v>484</v>
+      </c>
+      <c r="O21" s="150">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -17817,7 +18041,7 @@
   </sheetPr>
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17826,21 +18050,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="122" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="126" t="s">
-        <v>402</v>
+      <c r="A3" s="123" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D6" s="24" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="E6" s="136" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F6" s="136"/>
       <c r="G6" s="136"/>
@@ -17856,10 +18080,10 @@
     </row>
     <row r="8" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="24" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="E8" s="136" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F8" s="136"/>
       <c r="G8" s="136"/>
@@ -17874,29 +18098,29 @@
       <c r="P8" s="136"/>
     </row>
     <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="127"/>
-      <c r="B9" s="132"/>
-      <c r="C9" s="132"/>
-      <c r="D9" s="127"/>
-      <c r="E9" s="124"/>
-      <c r="F9" s="124"/>
-      <c r="G9" s="124"/>
-      <c r="H9" s="124"/>
-      <c r="I9" s="124"/>
-      <c r="J9" s="124"/>
-      <c r="K9" s="124"/>
-      <c r="L9" s="124"/>
-      <c r="M9" s="124"/>
-      <c r="N9" s="124"/>
-      <c r="O9" s="124"/>
-      <c r="P9" s="124"/>
+      <c r="A9" s="124"/>
+      <c r="B9" s="129"/>
+      <c r="C9" s="129"/>
+      <c r="D9" s="124"/>
+      <c r="E9" s="121"/>
+      <c r="F9" s="121"/>
+      <c r="G9" s="121"/>
+      <c r="H9" s="121"/>
+      <c r="I9" s="121"/>
+      <c r="J9" s="121"/>
+      <c r="K9" s="121"/>
+      <c r="L9" s="121"/>
+      <c r="M9" s="121"/>
+      <c r="N9" s="121"/>
+      <c r="O9" s="121"/>
+      <c r="P9" s="121"/>
     </row>
     <row r="10" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D10" s="24" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="E10" s="136" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="F10" s="136"/>
       <c r="G10" s="136"/>
@@ -17911,25 +18135,25 @@
       <c r="P10" s="136"/>
     </row>
     <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="131"/>
-      <c r="C12" s="131"/>
+      <c r="B12" s="128"/>
+      <c r="C12" s="128"/>
       <c r="D12" s="24" t="s">
-        <v>438</v>
-      </c>
-      <c r="E12" s="133" t="s">
-        <v>434</v>
-      </c>
-      <c r="F12" s="133"/>
-      <c r="G12" s="133"/>
-      <c r="H12" s="133"/>
-      <c r="I12" s="133"/>
-      <c r="J12" s="133"/>
-      <c r="K12" s="133"/>
-      <c r="L12" s="133"/>
-      <c r="M12" s="133"/>
-      <c r="N12" s="133"/>
-      <c r="O12" s="133"/>
-      <c r="P12" s="133"/>
+        <v>435</v>
+      </c>
+      <c r="E12" s="130" t="s">
+        <v>488</v>
+      </c>
+      <c r="F12" s="130"/>
+      <c r="G12" s="130"/>
+      <c r="H12" s="130"/>
+      <c r="I12" s="130"/>
+      <c r="J12" s="130"/>
+      <c r="K12" s="130"/>
+      <c r="L12" s="130"/>
+      <c r="M12" s="130"/>
+      <c r="N12" s="130"/>
+      <c r="O12" s="130"/>
+      <c r="P12" s="130"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -17948,10 +18172,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight"/>
@@ -17959,7 +18183,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="112" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="158" customWidth="1"/>
     <col min="2" max="2" width="40.7109375" style="111" customWidth="1"/>
     <col min="3" max="3" width="1.7109375" style="111" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" style="111" customWidth="1"/>
@@ -17969,73 +18193,89 @@
     <col min="8" max="8" width="20.7109375" style="111" customWidth="1"/>
     <col min="9" max="9" width="1.7109375" style="111" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" style="111" customWidth="1"/>
-    <col min="11" max="11" width="1.7109375" style="111" customWidth="1"/>
-    <col min="12" max="12" width="40.7109375" style="111" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="111"/>
-    <col min="14" max="14" width="62" style="111" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="111"/>
+    <col min="11" max="11" width="1.7109375" style="132" customWidth="1"/>
+    <col min="12" max="12" width="40.7109375" style="132" customWidth="1"/>
+    <col min="13" max="13" width="1.7109375" style="111" customWidth="1"/>
+    <col min="14" max="14" width="40.7109375" style="111" customWidth="1"/>
+    <col min="15" max="15" width="5.7109375" style="78" customWidth="1"/>
+    <col min="16" max="16" width="62" style="111" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="111"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="115"/>
-      <c r="B1" s="114" t="s">
-        <v>360</v>
-      </c>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114" t="s">
+    <row r="1" spans="1:16" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="153"/>
+      <c r="B1" s="147" t="s">
         <v>359</v>
       </c>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114" t="s">
+      <c r="C1" s="147"/>
+      <c r="D1" s="147" t="s">
+        <v>455</v>
+      </c>
+      <c r="E1" s="147"/>
+      <c r="F1" s="147" t="s">
         <v>358</v>
       </c>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114" t="s">
+      <c r="G1" s="147"/>
+      <c r="H1" s="147" t="s">
         <v>357</v>
       </c>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114" t="s">
-        <v>404</v>
-      </c>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="135" x14ac:dyDescent="0.25">
-      <c r="A2" s="120">
+      <c r="I1" s="147"/>
+      <c r="J1" s="147" t="s">
+        <v>403</v>
+      </c>
+      <c r="K1" s="147"/>
+      <c r="L1" s="147" t="s">
+        <v>437</v>
+      </c>
+      <c r="M1" s="147"/>
+      <c r="N1" s="147" t="s">
+        <v>362</v>
+      </c>
+      <c r="O1" s="152" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="135" x14ac:dyDescent="0.25">
+      <c r="A2" s="154">
         <v>1</v>
       </c>
-      <c r="B2" s="121" t="s">
-        <v>403</v>
-      </c>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121" t="s">
+      <c r="B2" s="146" t="s">
+        <v>402</v>
+      </c>
+      <c r="C2" s="146"/>
+      <c r="D2" s="146" t="s">
         <v>342</v>
       </c>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121" t="s">
-        <v>362</v>
-      </c>
-      <c r="G2" s="121"/>
-      <c r="H2" s="121" t="s">
+      <c r="E2" s="146"/>
+      <c r="F2" s="146" t="s">
+        <v>361</v>
+      </c>
+      <c r="G2" s="146"/>
+      <c r="H2" s="146" t="s">
         <v>354</v>
       </c>
-      <c r="I2" s="121"/>
-      <c r="J2" s="121" t="s">
+      <c r="I2" s="146"/>
+      <c r="J2" s="146" t="s">
         <v>342</v>
       </c>
-      <c r="K2" s="121"/>
-      <c r="L2" s="121" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="135" x14ac:dyDescent="0.25">
-      <c r="A3" s="83" t="s">
-        <v>388</v>
+      <c r="K2" s="146"/>
+      <c r="L2" s="146" t="s">
+        <v>439</v>
+      </c>
+      <c r="M2" s="146"/>
+      <c r="N2" s="146" t="s">
+        <v>417</v>
+      </c>
+      <c r="O2" s="148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="119" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A3" s="155" t="s">
+        <v>387</v>
       </c>
       <c r="B3" s="84" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C3" s="84"/>
       <c r="D3" s="84" t="s">
@@ -18043,7 +18283,7 @@
       </c>
       <c r="E3" s="84"/>
       <c r="F3" s="84" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G3" s="84"/>
       <c r="H3" s="84" t="s">
@@ -18055,15 +18295,23 @@
       </c>
       <c r="K3" s="84"/>
       <c r="L3" s="84" t="s">
+        <v>442</v>
+      </c>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84" t="s">
+        <v>382</v>
+      </c>
+      <c r="O3" s="150">
+        <v>2</v>
+      </c>
+      <c r="P3" s="132"/>
+    </row>
+    <row r="4" spans="1:16" s="119" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="155" t="s">
+        <v>386</v>
+      </c>
+      <c r="B4" s="84" t="s">
         <v>383</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="123" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="83" t="s">
-        <v>387</v>
-      </c>
-      <c r="B4" s="84" t="s">
-        <v>384</v>
       </c>
       <c r="C4" s="84"/>
       <c r="D4" s="84" t="s">
@@ -18071,192 +18319,246 @@
       </c>
       <c r="E4" s="84"/>
       <c r="F4" s="84" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G4" s="84"/>
       <c r="H4" s="84" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I4" s="84"/>
       <c r="J4" s="84" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="K4" s="84"/>
       <c r="L4" s="84" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="113" customFormat="1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A5" s="116">
+        <v>443</v>
+      </c>
+      <c r="M4" s="84"/>
+      <c r="N4" s="84" t="s">
+        <v>404</v>
+      </c>
+      <c r="O4" s="150">
         <v>3</v>
       </c>
-      <c r="B5" s="117" t="s">
-        <v>385</v>
-      </c>
-      <c r="C5" s="117"/>
-      <c r="D5" s="117" t="s">
+      <c r="P4" s="132"/>
+    </row>
+    <row r="5" spans="1:16" ht="135" x14ac:dyDescent="0.25">
+      <c r="A5" s="156">
+        <v>3</v>
+      </c>
+      <c r="B5" s="114" t="s">
+        <v>384</v>
+      </c>
+      <c r="C5" s="114"/>
+      <c r="D5" s="114" t="s">
         <v>342</v>
       </c>
-      <c r="E5" s="117"/>
-      <c r="F5" s="117" t="s">
+      <c r="E5" s="114"/>
+      <c r="F5" s="114" t="s">
+        <v>370</v>
+      </c>
+      <c r="G5" s="114"/>
+      <c r="H5" s="114" t="s">
+        <v>354</v>
+      </c>
+      <c r="I5" s="114"/>
+      <c r="J5" s="114" t="s">
+        <v>342</v>
+      </c>
+      <c r="K5" s="114"/>
+      <c r="L5" s="114" t="s">
+        <v>450</v>
+      </c>
+      <c r="M5" s="114"/>
+      <c r="N5" s="114" t="s">
+        <v>418</v>
+      </c>
+      <c r="O5" s="149">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" s="119" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A6" s="157" t="s">
+        <v>388</v>
+      </c>
+      <c r="B6" s="116" t="s">
+        <v>369</v>
+      </c>
+      <c r="C6" s="116"/>
+      <c r="D6" s="116" t="s">
+        <v>341</v>
+      </c>
+      <c r="E6" s="116"/>
+      <c r="F6" s="116" t="s">
+        <v>364</v>
+      </c>
+      <c r="G6" s="116"/>
+      <c r="H6" s="116" t="s">
+        <v>354</v>
+      </c>
+      <c r="I6" s="116"/>
+      <c r="J6" s="116" t="s">
+        <v>344</v>
+      </c>
+      <c r="K6" s="116"/>
+      <c r="L6" s="116" t="s">
+        <v>444</v>
+      </c>
+      <c r="M6" s="116"/>
+      <c r="N6" s="116" t="s">
         <v>371</v>
       </c>
-      <c r="G5" s="117"/>
-      <c r="H5" s="117" t="s">
-        <v>354</v>
-      </c>
-      <c r="I5" s="117"/>
-      <c r="J5" s="117" t="s">
+      <c r="O6" s="151">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="157" t="s">
+        <v>389</v>
+      </c>
+      <c r="B7" s="116" t="s">
+        <v>369</v>
+      </c>
+      <c r="C7" s="116"/>
+      <c r="D7" s="116" t="s">
+        <v>341</v>
+      </c>
+      <c r="E7" s="116"/>
+      <c r="F7" s="116" t="s">
+        <v>346</v>
+      </c>
+      <c r="G7" s="116"/>
+      <c r="H7" s="116" t="s">
+        <v>372</v>
+      </c>
+      <c r="I7" s="116"/>
+      <c r="J7" s="116" t="s">
         <v>342</v>
       </c>
-      <c r="K5" s="117"/>
-      <c r="L5" s="117" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="122" customFormat="1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A6" s="118" t="s">
-        <v>389</v>
-      </c>
-      <c r="B6" s="119" t="s">
-        <v>370</v>
-      </c>
-      <c r="C6" s="119"/>
-      <c r="D6" s="119" t="s">
+      <c r="K7" s="116"/>
+      <c r="L7" s="116" t="s">
+        <v>444</v>
+      </c>
+      <c r="M7" s="116"/>
+      <c r="N7" s="116" t="s">
+        <v>373</v>
+      </c>
+      <c r="O7" s="151">
+        <v>6</v>
+      </c>
+      <c r="P7" s="119"/>
+    </row>
+    <row r="8" spans="1:16" ht="135" x14ac:dyDescent="0.25">
+      <c r="A8" s="157" t="s">
+        <v>390</v>
+      </c>
+      <c r="B8" s="116" t="s">
+        <v>369</v>
+      </c>
+      <c r="C8" s="116"/>
+      <c r="D8" s="116" t="s">
         <v>341</v>
       </c>
-      <c r="E6" s="119"/>
-      <c r="F6" s="119" t="s">
-        <v>365</v>
-      </c>
-      <c r="G6" s="119"/>
-      <c r="H6" s="119" t="s">
-        <v>354</v>
-      </c>
-      <c r="I6" s="119"/>
-      <c r="J6" s="119" t="s">
+      <c r="E8" s="116"/>
+      <c r="F8" s="116" t="s">
+        <v>374</v>
+      </c>
+      <c r="G8" s="116"/>
+      <c r="H8" s="116" t="s">
+        <v>375</v>
+      </c>
+      <c r="I8" s="116"/>
+      <c r="J8" s="116" t="s">
+        <v>342</v>
+      </c>
+      <c r="K8" s="116"/>
+      <c r="L8" s="116" t="s">
+        <v>445</v>
+      </c>
+      <c r="M8" s="116"/>
+      <c r="N8" s="116" t="s">
+        <v>373</v>
+      </c>
+      <c r="O8" s="151">
+        <v>7</v>
+      </c>
+      <c r="P8" s="119"/>
+    </row>
+    <row r="9" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="157" t="s">
+        <v>391</v>
+      </c>
+      <c r="B9" s="116" t="s">
+        <v>369</v>
+      </c>
+      <c r="C9" s="116"/>
+      <c r="D9" s="116" t="s">
+        <v>341</v>
+      </c>
+      <c r="E9" s="116"/>
+      <c r="F9" s="116" t="s">
+        <v>347</v>
+      </c>
+      <c r="G9" s="116"/>
+      <c r="H9" s="116" t="s">
+        <v>376</v>
+      </c>
+      <c r="I9" s="116"/>
+      <c r="J9" s="116" t="s">
+        <v>348</v>
+      </c>
+      <c r="K9" s="116"/>
+      <c r="L9" s="116" t="s">
+        <v>445</v>
+      </c>
+      <c r="M9" s="116"/>
+      <c r="N9" s="116" t="s">
+        <v>410</v>
+      </c>
+      <c r="O9" s="151">
+        <v>8</v>
+      </c>
+      <c r="P9" s="119"/>
+    </row>
+    <row r="10" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="157" t="s">
+        <v>392</v>
+      </c>
+      <c r="B10" s="116" t="s">
+        <v>369</v>
+      </c>
+      <c r="C10" s="116"/>
+      <c r="D10" s="116" t="s">
+        <v>341</v>
+      </c>
+      <c r="E10" s="116"/>
+      <c r="F10" s="116" t="s">
+        <v>366</v>
+      </c>
+      <c r="G10" s="116"/>
+      <c r="H10" s="116" t="s">
+        <v>377</v>
+      </c>
+      <c r="I10" s="116"/>
+      <c r="J10" s="116" t="s">
         <v>344</v>
       </c>
-      <c r="K6" s="119"/>
-      <c r="L6" s="119" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="122" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="118" t="s">
-        <v>390</v>
-      </c>
-      <c r="B7" s="119" t="s">
-        <v>370</v>
-      </c>
-      <c r="C7" s="119"/>
-      <c r="D7" s="119" t="s">
-        <v>341</v>
-      </c>
-      <c r="E7" s="119"/>
-      <c r="F7" s="119" t="s">
-        <v>346</v>
-      </c>
-      <c r="G7" s="119"/>
-      <c r="H7" s="119" t="s">
-        <v>373</v>
-      </c>
-      <c r="I7" s="119"/>
-      <c r="J7" s="119" t="s">
-        <v>342</v>
-      </c>
-      <c r="K7" s="119"/>
-      <c r="L7" s="119" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="122" customFormat="1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A8" s="118" t="s">
-        <v>391</v>
-      </c>
-      <c r="B8" s="119" t="s">
-        <v>370</v>
-      </c>
-      <c r="C8" s="119"/>
-      <c r="D8" s="119" t="s">
-        <v>341</v>
-      </c>
-      <c r="E8" s="119"/>
-      <c r="F8" s="119" t="s">
-        <v>375</v>
-      </c>
-      <c r="G8" s="119"/>
-      <c r="H8" s="119" t="s">
-        <v>376</v>
-      </c>
-      <c r="I8" s="119"/>
-      <c r="J8" s="119" t="s">
-        <v>342</v>
-      </c>
-      <c r="K8" s="119"/>
-      <c r="L8" s="119" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="122" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="118" t="s">
-        <v>392</v>
-      </c>
-      <c r="B9" s="119" t="s">
-        <v>370</v>
-      </c>
-      <c r="C9" s="119"/>
-      <c r="D9" s="119" t="s">
-        <v>341</v>
-      </c>
-      <c r="E9" s="119"/>
-      <c r="F9" s="119" t="s">
-        <v>347</v>
-      </c>
-      <c r="G9" s="119"/>
-      <c r="H9" s="119" t="s">
-        <v>377</v>
-      </c>
-      <c r="I9" s="119"/>
-      <c r="J9" s="119" t="s">
-        <v>348</v>
-      </c>
-      <c r="K9" s="119"/>
-      <c r="L9" s="119" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="122" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="118" t="s">
+      <c r="K10" s="116"/>
+      <c r="L10" s="116" t="s">
+        <v>445</v>
+      </c>
+      <c r="M10" s="116"/>
+      <c r="N10" s="116" t="s">
+        <v>409</v>
+      </c>
+      <c r="O10" s="151">
+        <v>9</v>
+      </c>
+      <c r="P10" s="119"/>
+    </row>
+    <row r="11" spans="1:16" ht="135" x14ac:dyDescent="0.25">
+      <c r="A11" s="155" t="s">
         <v>393</v>
-      </c>
-      <c r="B10" s="119" t="s">
-        <v>370</v>
-      </c>
-      <c r="C10" s="119"/>
-      <c r="D10" s="119" t="s">
-        <v>341</v>
-      </c>
-      <c r="E10" s="119"/>
-      <c r="F10" s="119" t="s">
-        <v>367</v>
-      </c>
-      <c r="G10" s="119"/>
-      <c r="H10" s="119" t="s">
-        <v>378</v>
-      </c>
-      <c r="I10" s="119"/>
-      <c r="J10" s="119" t="s">
-        <v>342</v>
-      </c>
-      <c r="K10" s="119"/>
-      <c r="L10" s="119" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="135" x14ac:dyDescent="0.25">
-      <c r="A11" s="83" t="s">
-        <v>394</v>
       </c>
       <c r="B11" s="84" t="s">
         <v>352</v>
@@ -18279,12 +18581,19 @@
       </c>
       <c r="K11" s="84"/>
       <c r="L11" s="84" t="s">
+        <v>446</v>
+      </c>
+      <c r="M11" s="84"/>
+      <c r="N11" s="84" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="180" x14ac:dyDescent="0.25">
-      <c r="A12" s="83" t="s">
-        <v>395</v>
+      <c r="O11" s="150">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="180" x14ac:dyDescent="0.25">
+      <c r="A12" s="155" t="s">
+        <v>394</v>
       </c>
       <c r="B12" s="84" t="s">
         <v>352</v>
@@ -18307,12 +18616,19 @@
       </c>
       <c r="K12" s="84"/>
       <c r="L12" s="84" t="s">
+        <v>446</v>
+      </c>
+      <c r="M12" s="84"/>
+      <c r="N12" s="84" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="180" x14ac:dyDescent="0.25">
-      <c r="A13" s="83" t="s">
-        <v>396</v>
+      <c r="O12" s="150">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="180" x14ac:dyDescent="0.25">
+      <c r="A13" s="155" t="s">
+        <v>395</v>
       </c>
       <c r="B13" s="84" t="s">
         <v>352</v>
@@ -18323,11 +18639,11 @@
       </c>
       <c r="E13" s="84"/>
       <c r="F13" s="84" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G13" s="84"/>
       <c r="H13" s="84" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="I13" s="84"/>
       <c r="J13" s="84" t="s">
@@ -18335,12 +18651,19 @@
       </c>
       <c r="K13" s="84"/>
       <c r="L13" s="84" t="s">
+        <v>446</v>
+      </c>
+      <c r="M13" s="84"/>
+      <c r="N13" s="84" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="83" t="s">
-        <v>397</v>
+      <c r="O13" s="150">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="155" t="s">
+        <v>396</v>
       </c>
       <c r="B14" s="84" t="s">
         <v>356</v>
@@ -18355,20 +18678,27 @@
       </c>
       <c r="G14" s="84"/>
       <c r="H14" s="84" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I14" s="84"/>
       <c r="J14" s="84" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="K14" s="84"/>
       <c r="L14" s="84" t="s">
+        <v>447</v>
+      </c>
+      <c r="M14" s="84"/>
+      <c r="N14" s="84" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="83" t="s">
-        <v>398</v>
+      <c r="O14" s="150">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="155" t="s">
+        <v>397</v>
       </c>
       <c r="B15" s="84" t="s">
         <v>356</v>
@@ -18391,99 +18721,127 @@
       </c>
       <c r="K15" s="84"/>
       <c r="L15" s="84" t="s">
+        <v>447</v>
+      </c>
+      <c r="M15" s="84"/>
+      <c r="N15" s="84" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="135" x14ac:dyDescent="0.25">
-      <c r="A16" s="116" t="s">
+      <c r="O15" s="150">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" s="125" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A16" s="156" t="s">
+        <v>398</v>
+      </c>
+      <c r="B16" s="114" t="s">
+        <v>365</v>
+      </c>
+      <c r="C16" s="114"/>
+      <c r="D16" s="114" t="s">
+        <v>343</v>
+      </c>
+      <c r="E16" s="114"/>
+      <c r="F16" s="114" t="s">
+        <v>363</v>
+      </c>
+      <c r="G16" s="114"/>
+      <c r="H16" s="114" t="s">
+        <v>354</v>
+      </c>
+      <c r="I16" s="114"/>
+      <c r="J16" s="114" t="s">
+        <v>342</v>
+      </c>
+      <c r="K16" s="114"/>
+      <c r="L16" s="114" t="s">
+        <v>438</v>
+      </c>
+      <c r="M16" s="114"/>
+      <c r="N16" s="114" t="s">
+        <v>419</v>
+      </c>
+      <c r="O16" s="149">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" s="125" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="157" t="s">
         <v>399</v>
       </c>
-      <c r="B16" s="117" t="s">
-        <v>366</v>
-      </c>
-      <c r="C16" s="117"/>
-      <c r="D16" s="117" t="s">
+      <c r="B17" s="116" t="s">
+        <v>365</v>
+      </c>
+      <c r="C17" s="116"/>
+      <c r="D17" s="116" t="s">
         <v>343</v>
       </c>
-      <c r="E16" s="117"/>
-      <c r="F16" s="117" t="s">
-        <v>364</v>
-      </c>
-      <c r="G16" s="117"/>
-      <c r="H16" s="117" t="s">
+      <c r="E17" s="116"/>
+      <c r="F17" s="116" t="s">
+        <v>406</v>
+      </c>
+      <c r="G17" s="116"/>
+      <c r="H17" s="116" t="s">
+        <v>355</v>
+      </c>
+      <c r="I17" s="116"/>
+      <c r="J17" s="116" t="s">
+        <v>405</v>
+      </c>
+      <c r="K17" s="116"/>
+      <c r="L17" s="116" t="s">
+        <v>453</v>
+      </c>
+      <c r="M17" s="116"/>
+      <c r="N17" s="116" t="s">
+        <v>408</v>
+      </c>
+      <c r="O17" s="151">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" s="120" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A18" s="156">
+        <v>8</v>
+      </c>
+      <c r="B18" s="114" t="s">
+        <v>368</v>
+      </c>
+      <c r="C18" s="114"/>
+      <c r="D18" s="114" t="s">
+        <v>342</v>
+      </c>
+      <c r="E18" s="114"/>
+      <c r="F18" s="114" t="s">
+        <v>363</v>
+      </c>
+      <c r="G18" s="114"/>
+      <c r="H18" s="114" t="s">
         <v>354</v>
       </c>
-      <c r="I16" s="117"/>
-      <c r="J16" s="117" t="s">
+      <c r="I18" s="114"/>
+      <c r="J18" s="114" t="s">
         <v>342</v>
       </c>
-      <c r="K16" s="117"/>
-      <c r="L16" s="117" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="118" t="s">
-        <v>400</v>
-      </c>
-      <c r="B17" s="119" t="s">
-        <v>366</v>
-      </c>
-      <c r="C17" s="119"/>
-      <c r="D17" s="119" t="s">
-        <v>343</v>
-      </c>
-      <c r="E17" s="119"/>
-      <c r="F17" s="119" t="s">
-        <v>407</v>
-      </c>
-      <c r="G17" s="119"/>
-      <c r="H17" s="119" t="s">
-        <v>355</v>
-      </c>
-      <c r="I17" s="119"/>
-      <c r="J17" s="119" t="s">
-        <v>406</v>
-      </c>
-      <c r="K17" s="119"/>
-      <c r="L17" s="119" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="135" x14ac:dyDescent="0.25">
-      <c r="A18" s="116">
-        <v>8</v>
-      </c>
-      <c r="B18" s="117" t="s">
-        <v>369</v>
-      </c>
-      <c r="C18" s="117"/>
-      <c r="D18" s="117" t="s">
-        <v>342</v>
-      </c>
-      <c r="E18" s="117"/>
-      <c r="F18" s="117" t="s">
-        <v>364</v>
-      </c>
-      <c r="G18" s="117"/>
-      <c r="H18" s="117" t="s">
-        <v>354</v>
-      </c>
-      <c r="I18" s="117"/>
-      <c r="J18" s="117" t="s">
-        <v>342</v>
-      </c>
-      <c r="K18" s="117"/>
-      <c r="L18" s="117" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A19" s="83">
+      <c r="K18" s="114"/>
+      <c r="L18" s="114" t="s">
+        <v>441</v>
+      </c>
+      <c r="M18" s="114"/>
+      <c r="N18" s="114" t="s">
+        <v>420</v>
+      </c>
+      <c r="O18" s="149">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" s="112" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A19" s="155">
         <v>9</v>
       </c>
       <c r="B19" s="84" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C19" s="84"/>
       <c r="D19" s="84" t="s">
@@ -18495,7 +18853,7 @@
       </c>
       <c r="G19" s="84"/>
       <c r="H19" s="84" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I19" s="84"/>
       <c r="J19" s="84" t="s">
@@ -18503,15 +18861,22 @@
       </c>
       <c r="K19" s="84"/>
       <c r="L19" s="84" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" s="128" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="83">
+        <v>448</v>
+      </c>
+      <c r="M19" s="84"/>
+      <c r="N19" s="84" t="s">
+        <v>379</v>
+      </c>
+      <c r="O19" s="150">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" s="119" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="155">
         <v>10</v>
       </c>
       <c r="B20" s="84" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C20" s="84"/>
       <c r="D20" s="84" t="s">
@@ -18519,11 +18884,11 @@
       </c>
       <c r="E20" s="84"/>
       <c r="F20" s="84" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G20" s="84"/>
       <c r="H20" s="84" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I20" s="84"/>
       <c r="J20" s="84" t="s">
@@ -18531,15 +18896,23 @@
       </c>
       <c r="K20" s="84"/>
       <c r="L20" s="84" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" s="128" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="83">
+        <v>440</v>
+      </c>
+      <c r="M20" s="84"/>
+      <c r="N20" s="84" t="s">
+        <v>414</v>
+      </c>
+      <c r="O20" s="150">
+        <v>19</v>
+      </c>
+      <c r="P20" s="132"/>
+    </row>
+    <row r="21" spans="1:16" s="119" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="155">
         <v>11</v>
       </c>
       <c r="B21" s="84" t="s">
-        <v>416</v>
+        <v>452</v>
       </c>
       <c r="C21" s="84"/>
       <c r="D21" s="84" t="s">
@@ -18547,22 +18920,33 @@
       </c>
       <c r="E21" s="84"/>
       <c r="F21" s="84" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G21" s="84"/>
       <c r="H21" s="84" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I21" s="84"/>
       <c r="J21" s="84" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="K21" s="84"/>
       <c r="L21" s="84" t="s">
-        <v>418</v>
-      </c>
+        <v>449</v>
+      </c>
+      <c r="M21" s="84"/>
+      <c r="N21" s="84" t="s">
+        <v>416</v>
+      </c>
+      <c r="O21" s="150">
+        <v>20</v>
+      </c>
+      <c r="P21" s="132"/>
     </row>
   </sheetData>
+  <sortState ref="A2:P21">
+    <sortCondition ref="A2:A21"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="61" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>

</xml_diff>

<commit_message>
Completed restructuring introduction of paper and modified figure on technological advancement
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="11" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="11" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId1"/>
@@ -7235,16 +7235,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>126207</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>64294</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>81915</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -7256,14 +7256,14 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="34" idx="3"/>
-          <a:endCxn id="6" idx="2"/>
+          <a:stCxn id="44" idx="0"/>
+          <a:endCxn id="12" idx="3"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="9270207" y="5231130"/>
-          <a:ext cx="547687" cy="737235"/>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="6813233" y="3469957"/>
+          <a:ext cx="708660" cy="1533525"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -7294,14 +7294,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>597694</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>207169</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>140494</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>359569</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>106680</xdr:rowOff>
     </xdr:to>
@@ -7318,7 +7318,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9132094" y="4591050"/>
+          <a:off x="11179969" y="4591050"/>
           <a:ext cx="1371600" cy="640080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7373,8 +7373,8 @@
       <xdr:rowOff>167640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>597694</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
@@ -7389,13 +7389,13 @@
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="8" idx="3"/>
-          <a:endCxn id="6" idx="1"/>
+          <a:endCxn id="44" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4276725" y="4911090"/>
-          <a:ext cx="4855369" cy="0"/>
+          <a:ext cx="2971800" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -7727,14 +7727,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
@@ -7751,7 +7751,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5991225" y="3562350"/>
+          <a:off x="5029200" y="3562350"/>
           <a:ext cx="1371600" cy="640080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7800,14 +7800,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -7826,7 +7826,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6677025" y="4202430"/>
+          <a:off x="5715000" y="4202430"/>
           <a:ext cx="0" cy="731520"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -7920,13 +7920,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>118111</xdr:colOff>
+      <xdr:colOff>118110</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>91439</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>504826</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>161924</xdr:rowOff>
     </xdr:to>
@@ -7946,8 +7946,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000" flipV="1">
-          <a:off x="2556511" y="3882389"/>
-          <a:ext cx="3434715" cy="1022985"/>
+          <a:off x="2556510" y="3882389"/>
+          <a:ext cx="2472690" cy="1022985"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -7978,14 +7978,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>340519</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>83344</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>154305</xdr:rowOff>
     </xdr:to>
@@ -8002,7 +8002,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1504950" y="1304925"/>
+          <a:off x="2466975" y="1304925"/>
           <a:ext cx="7979569" cy="640080"/>
           <a:chOff x="1257300" y="1304925"/>
           <a:chExt cx="7979569" cy="640080"/>
@@ -8404,151 +8404,6 @@
         </xdr:style>
       </xdr:cxnSp>
     </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>583407</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>126207</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>20955</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="34" name="Rectangle 33">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30064B99-B5E4-4FA7-9153-392CB43A5AA4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7898607" y="5648325"/>
-          <a:ext cx="1371600" cy="640080"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Production</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> and Operations</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1200">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>102394</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>81915</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>583407</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>81915</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="35" name="Straight Arrow Connector 34">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA8634AC-5478-4559-AF72-46C5FB8803D7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="33" idx="3"/>
-          <a:endCxn id="34" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7417594" y="5968365"/>
-          <a:ext cx="481013" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -9034,46 +8889,467 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>391160</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>14606</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>56357</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>27306</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>70247</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="50" name="Connector: Elbow 49">
+        <xdr:cNvPr id="41" name="Straight Arrow Connector 40">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B88F430-BF77-48B6-8F32-92CF55A91BBB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F30CCE68-0B67-4615-B8EC-48FF2C9AFD7C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="34" idx="2"/>
-          <a:endCxn id="46" idx="2"/>
+          <a:stCxn id="44" idx="3"/>
+          <a:endCxn id="52" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="7837409" y="5541407"/>
-          <a:ext cx="12700" cy="1493997"/>
+        <a:xfrm>
+          <a:off x="8620125" y="4911090"/>
+          <a:ext cx="594122" cy="0"/>
         </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 1800000"/>
-          </a:avLst>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
         </a:prstGeom>
         <a:ln w="25400">
           <a:solidFill>
             <a:schemeClr val="tx1"/>
           </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="med"/>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="42" name="Group 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A89986A6-2211-4D1C-A134-3FB702EA0CB1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="7248525" y="4591050"/>
+          <a:ext cx="1371600" cy="640080"/>
+          <a:chOff x="6131719" y="5648325"/>
+          <a:chExt cx="1371600" cy="640080"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="44" name="Rectangle 43">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECCED5CC-C24A-450F-A1A4-02BD9E6B8FCD}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6131719" y="5648325"/>
+            <a:ext cx="1371600" cy="640080"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Technology</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="47" name="Rectangle 46">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5502011-ECC5-4A5D-92AB-DD6EBDFA4C3B}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7038975" y="5648325"/>
+            <a:ext cx="274320" cy="640080"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="19050">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US" sz="1200" baseline="-25000">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>222647</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>207169</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="48" name="Straight Arrow Connector 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{509DE82A-65AB-4313-93E0-A1961A31BC6E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="52" idx="3"/>
+          <a:endCxn id="6" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10585847" y="4911090"/>
+          <a:ext cx="594122" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>70247</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>222647</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="51" name="Group 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99000497-BB36-4E3E-A2A1-351F107E1B6D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="9214247" y="4591050"/>
+          <a:ext cx="1371600" cy="640080"/>
+          <a:chOff x="6131719" y="5648325"/>
+          <a:chExt cx="1371600" cy="640080"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="52" name="Rectangle 51">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDA5E272-8BA6-4FC6-8F84-29EA3F8303B8}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6131719" y="5648325"/>
+            <a:ext cx="1371600" cy="640080"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Production</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> and Operations</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="53" name="Rectangle 52">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0BC34A3-F78A-44A9-B3D7-E7211C26673D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7038975" y="5648325"/>
+            <a:ext cx="274320" cy="640080"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="19050">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US" sz="1200" baseline="-25000">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>102394</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>81915</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="54" name="Connector: Elbow 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09123B16-A685-4F72-ADA6-1EC8B210F3C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="33" idx="3"/>
+          <a:endCxn id="44" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7417594" y="5231130"/>
+          <a:ext cx="516731" cy="737235"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -16676,62 +16952,62 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="108" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="110"/>
     </row>
-    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="110"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="110"/>
     </row>
-    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="110"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="110"/>
     </row>
-    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="110"/>
     </row>
-    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="110"/>
     </row>
-    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="110"/>
     </row>
-    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="110"/>
-      <c r="J12" s="79" t="s">
+      <c r="K12" s="79" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="110"/>
     </row>
-    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="110"/>
     </row>
-    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="110"/>
     </row>
-    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="110"/>
     </row>
     <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
@@ -16743,8 +17019,8 @@
     <row r="19" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="110"/>
     </row>
-    <row r="36" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J36" s="79" t="s">
+    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K36" s="79" t="s">
         <v>341</v>
       </c>
     </row>
@@ -16815,7 +17091,7 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Added technology maturity level to Chapter 1 Introduction
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="11" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId1"/>
@@ -316,25 +316,10 @@
     <t>Basic principles observed and reported.  Scientific research begins to be translated into applied research and development.</t>
   </si>
   <si>
-    <t>Following the observation of high critical temperature (Htc) superconductivity, potential applications of the new material for thin film devices (e.g., SIS mixers) and in instrument systems (e.g., telescope sensors) can be defined.</t>
-  </si>
-  <si>
     <t>Very Low</t>
   </si>
   <si>
     <t>Technology concept and/or application formulated. Once basic physical principles are observed, practical applications of those characteristics can be ‘invented’ or identified.  The application is still speculative; there is not experimental proof or detailed analysis to support the conjecture.</t>
-  </si>
-  <si>
-    <t>Analytical and experimental critical function and/or characteristic proof-of-concept.  Active research and development (R&amp;D) is initiated.  This must include both analytical studies to set the technology into an appropriate context and laboratory-based studies to physically validate that the analytical predictions are correct.  These studies and experiments should constitute “proof-of-concept” validation of the applications/concepts formulated at TRL-2.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Component and/or breadboard validation in laboratory environment.  Basic technological elements must be integrated to establish that the “pieces” will work together to achieve concept-enabling levels of performance for a component and/or breadboard.  This validation must [be] devised to support the concept that was formulated earlier and should also be consistent with the requirements of potential system applications.  The validation is relatively “low-fidelity” compared to the eventual system.  It could be composed of ad hoc discrete components in a laboratory. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Component and/or breadboard validation in relevant environment.  The basic technological elements must be integrated with reasonably realistic supporting elements so that the total applications (component-level, sub-system level, or system-level) can be tested in a ‘simulated’ or somewhat realistic environment. From one-to-several new technologies might be involved in the demonstration. </t>
-  </si>
-  <si>
-    <t>A new type of solar photovoltaic material promising higher efficiencies would be used in an actual fabricated solar array ‘blanket’ that would be integrated with power supplies, supporting structure, etc., and tested in a thermal vacuum chamber with solar simulation capability.</t>
   </si>
   <si>
     <t>Moderate;
@@ -348,22 +333,13 @@
     <t>System/subsystem model or prototype demonstration in a relevant environment (ground or space).  A representative model or prototype system or system — which would go well beyond ad hoc, ‘patch-cord’ or discrete component level breadboarding — would be tested in a relevant environment.  The demonstration might represent an actual system application or it might only be similar to the planned application but using the same technologies.  Several-to-many new technologies might be integrated into the demonstration.  The demonstration should be successful to represent a true TRL-6.  At this point, the maturation step is driven more by assuring management confidence than by R&amp;D requirements.</t>
   </si>
   <si>
-    <t>An innovative approach to high temperature / low mass radiators, involving liquid droplets and composite materials, would be demonstrated to TRL 6 by actually flying a working, sub-scale (but scaleable) model of the system on a Space Shuttle or International Space Station ‘pallet’.  In this example, the ‘relevant’ environment is the microgravity plus vacuum plus thermal environment effects which will dictate the success or failure of the system — and the only way to validate the technology is in space.</t>
-  </si>
-  <si>
     <t>A fraction of TRL-7 if on ground but nearly the same if validation in space is required</t>
   </si>
   <si>
-    <t>System prototype demonstration in a space environment.  An actual system prototype demonstration in a space environment.  The prototype should be near or at the scale of the planned operational system and the demonstration must take place in space.  The driving purposes for achieving this level of maturity are to assure system engineering and development and management confidence (more than for purposes of technology R&amp;D). The demonstration must be of a prototype of that application.  Normally only performed in cases where the technology and/or subsystem application is mission critical and relatively high risk.</t>
-  </si>
-  <si>
     <t>The Mars Pathfinder Rover is a TRL 7 technology demonstration for future Mars micro-rovers based on that system design.</t>
   </si>
   <si>
     <t>Significant fraction of the cost of TRL-8</t>
-  </si>
-  <si>
-    <t>Actual system completed and “flight qualified” through test and demonstration (ground or space).  By definition, all technologies being applied in actual systems go through TRL-8.  In almost all cases, this level is the end of true ‘system development’ for most technology elements.</t>
   </si>
   <si>
     <t>Loading and successfully testing  a new control algorithm into the onboard computer on the Hubble Space Telescope while in orbit.</t>
@@ -1095,9 +1071,6 @@
     <t>Factors</t>
   </si>
   <si>
-    <t>Factors of Technology Transfer Outcomes Examined in the Literature</t>
-  </si>
-  <si>
     <t>Type of Analysis</t>
   </si>
   <si>
@@ -1323,6 +1296,41 @@
   </si>
   <si>
     <t>a) Linear model of technological advancement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual system completed and “flight qualified” through test and demonstration (ground or space).  By definition, all technologies being applied in actual systems go through TRL-8.  In almost all cases, this level is the end of true ‘system development’ for most technology elements.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Component and/or breadboard validation in relevant environment.  The basic technological elements must be integrated with reasonably realistic supporting elements so that the total applications (component-level, sub-system level, or system-level) can be tested in a ‘simulated’ or somewhat realistic environment. From one-to-several new technologies might be involved in the demonstration. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Component and/or breadboard validation in laboratory environment.  Basic technological elements must be integrated to establish that the “pieces” will work together to achieve concept-enabling levels of performance for a component and/or breadboard.  This validation must [be] devised to support the concept that was formulated earlier and should also be consistent with the requirements of potential system applications.  The validation is relatively “low-fidelity” compared to the eventual system.  It could be composed of ad hoc discrete components in a laboratory. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System prototype demonstration in a space environment.  An actual system prototype demonstration in a space environment.  The prototype should be near or at the scale of the planned operational system and the demonstration must take place in space.  The driving purposes for achieving this level of maturity are to assure system engineering and development and management confidence (more than for purposes of technology R&amp;D). The demonstration must be of a prototype of that application.  Normally only performed in cases where the technology and/or subsystem application is mission critical and relatively high risk.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analytical and experimental critical function and/or characteristic proof-of-concept.  Active research and development (R&amp;D) is initiated.  This must include both analytical studies to set the technology into an appropriate context and laboratory-based studies to physically validate that the analytical predictions are correct.  These studies and experiments should constitute “proof-of-concept” validation of the applications/concepts formulated at TRL-2.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Following the observation of high critical temperature (Htc) superconductivity, potential applications of the new material for thin film devices (e.g., SIS mixers) and in instrument systems (e.g., telescope sensors) can be defined.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A new type of solar photovoltaic material promising higher efficiencies would be used in an actual fabricated solar array ‘blanket’ that would be integrated with power supplies, supporting structure, etc., and tested in a thermal vacuum chamber with solar simulation capability.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An innovative approach to high temperature / low mass radiators, involving liquid droplets and composite materials, would be demonstrated to TRL 6 by actually flying a working, sub-scale (but scaleable) model of the system on a Space Shuttle or International Space Station ‘pallet’.  In this example, the ‘relevant’ environment is the microgravity plus vacuum plus thermal environment effects which will dictate the success or failure of the system — and the only way to validate the technology is in space.
+</t>
+  </si>
+  <si>
+    <t>Determinants of Technology Transfer Outcomes Examined in the Technology Transfer Literature</t>
   </si>
 </sst>
 </file>
@@ -15636,7 +15644,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="E1" s="22"/>
       <c r="H1" s="24"/>
@@ -16929,7 +16937,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="108" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
@@ -16937,7 +16945,7 @@
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -16954,18 +16962,18 @@
   </sheetPr>
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="108" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -16995,7 +17003,7 @@
     <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="110"/>
       <c r="K12" s="79" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -17021,7 +17029,7 @@
     </row>
     <row r="36" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K36" s="79" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -17044,12 +17052,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="108" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -17069,12 +17077,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="108" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -17097,12 +17105,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="108" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -17132,7 +17140,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -17157,7 +17165,7 @@
       </c>
       <c r="G3" s="34"/>
       <c r="H3" s="34" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -17177,7 +17185,7 @@
       </c>
       <c r="G4" s="109"/>
       <c r="H4" s="109" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17197,7 +17205,7 @@
       </c>
       <c r="G5" s="109"/>
       <c r="H5" s="109" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
@@ -17217,7 +17225,7 @@
       </c>
       <c r="G6" s="109"/>
       <c r="H6" s="109" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -17237,7 +17245,7 @@
       </c>
       <c r="G7" s="109"/>
       <c r="H7" s="109" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17257,7 +17265,7 @@
       </c>
       <c r="G8" s="109"/>
       <c r="H8" s="109" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -17277,7 +17285,7 @@
       </c>
       <c r="G9" s="109"/>
       <c r="H9" s="109" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -17297,7 +17305,7 @@
       </c>
       <c r="G10" s="109"/>
       <c r="H10" s="109" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17317,7 +17325,7 @@
       </c>
       <c r="G11" s="109"/>
       <c r="H11" s="109" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17337,7 +17345,7 @@
       </c>
       <c r="G12" s="109"/>
       <c r="H12" s="109" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -17357,7 +17365,7 @@
       </c>
       <c r="G13" s="109"/>
       <c r="H13" s="109" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17377,7 +17385,7 @@
       </c>
       <c r="G14" s="109"/>
       <c r="H14" s="109" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17397,7 +17405,7 @@
       </c>
       <c r="G15" s="109"/>
       <c r="H15" s="109" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="72" customHeight="1" x14ac:dyDescent="0.25">
@@ -17417,7 +17425,7 @@
       </c>
       <c r="G16" s="38"/>
       <c r="H16" s="38" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -17425,19 +17433,19 @@
         <v>2011</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="C17" s="38"/>
       <c r="D17" s="38" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="E17" s="38"/>
       <c r="F17" s="38" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="G17" s="38"/>
       <c r="H17" s="38" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -17486,7 +17494,7 @@
     </row>
     <row r="22" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="112" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="B22" s="112"/>
       <c r="C22" s="112"/>
@@ -17627,8 +17635,8 @@
   </sheetPr>
   <dimension ref="A1:AA78"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="4" ySplit="4" topLeftCell="E15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight"/>
@@ -17647,7 +17655,7 @@
   <sheetData>
     <row r="1" spans="1:27" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="E1" s="61"/>
       <c r="F1" s="61"/>
@@ -17675,7 +17683,7 @@
     </row>
     <row r="2" spans="1:27" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>291</v>
+        <v>342</v>
       </c>
       <c r="E2" s="61"/>
       <c r="F2" s="61"/>
@@ -17707,26 +17715,26 @@
       <c r="C3" s="70"/>
       <c r="D3" s="71"/>
       <c r="E3" s="116" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="F3" s="117"/>
       <c r="G3" s="117"/>
       <c r="H3" s="114"/>
       <c r="I3" s="113" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="J3" s="114"/>
       <c r="K3" s="113" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="L3" s="115"/>
       <c r="M3" s="116" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="N3" s="117"/>
       <c r="O3" s="114"/>
       <c r="P3" s="118" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="Q3" s="117"/>
       <c r="R3" s="117"/>
@@ -17743,84 +17751,84 @@
     <row r="4" spans="1:27" ht="170.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="67"/>
       <c r="B4" s="104" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="C4" s="68"/>
       <c r="D4" s="68"/>
       <c r="E4" s="105" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="F4" s="107" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="G4" s="62" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="H4" s="106" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="I4" s="65" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="J4" s="66" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="K4" s="65" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="L4" s="66" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="M4" s="105" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="N4" s="62" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="O4" s="106" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="P4" s="62" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="Q4" s="62" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="R4" s="62" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="S4" s="62" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="T4" s="62" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="U4" s="62" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="V4" s="62" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="W4" s="62" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="X4" s="62" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="Y4" s="62" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="Z4" s="62" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="AA4" s="72" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="49"/>
       <c r="B5" s="49" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="C5" s="93"/>
       <c r="D5" s="93"/>
@@ -17852,25 +17860,25 @@
       <c r="A6" s="94"/>
       <c r="B6" s="82"/>
       <c r="C6" s="81" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="D6" s="81"/>
       <c r="E6" s="74"/>
       <c r="F6" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G6" s="92"/>
       <c r="H6" s="75"/>
       <c r="I6" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J6" s="75"/>
       <c r="K6" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="L6" s="75"/>
       <c r="M6" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N6" s="92"/>
       <c r="O6" s="75"/>
@@ -17879,7 +17887,7 @@
       <c r="R6" s="92"/>
       <c r="S6" s="78"/>
       <c r="T6" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="U6" s="78"/>
       <c r="V6" s="78"/>
@@ -17888,32 +17896,32 @@
       <c r="Y6" s="78"/>
       <c r="Z6" s="78"/>
       <c r="AA6" s="63" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="94"/>
       <c r="B7" s="82"/>
       <c r="C7" s="93" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="D7" s="81"/>
       <c r="E7" s="74"/>
       <c r="F7" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G7" s="92"/>
       <c r="H7" s="75"/>
       <c r="I7" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J7" s="75"/>
       <c r="K7" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="L7" s="75"/>
       <c r="M7" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N7" s="92"/>
       <c r="O7" s="75"/>
@@ -17922,7 +17930,7 @@
       <c r="R7" s="92"/>
       <c r="S7" s="78"/>
       <c r="T7" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="U7" s="78"/>
       <c r="V7" s="78"/>
@@ -17931,32 +17939,32 @@
       <c r="Y7" s="78"/>
       <c r="Z7" s="78"/>
       <c r="AA7" s="63" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="94"/>
       <c r="B8" s="82"/>
       <c r="C8" s="81" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="D8" s="81"/>
       <c r="E8" s="74"/>
       <c r="F8" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G8" s="92"/>
       <c r="H8" s="75"/>
       <c r="I8" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J8" s="75"/>
       <c r="K8" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="L8" s="75"/>
       <c r="M8" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N8" s="92"/>
       <c r="O8" s="75"/>
@@ -17965,7 +17973,7 @@
       <c r="R8" s="92"/>
       <c r="S8" s="78"/>
       <c r="T8" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="U8" s="78"/>
       <c r="V8" s="78"/>
@@ -17974,47 +17982,47 @@
       <c r="Y8" s="78"/>
       <c r="Z8" s="78"/>
       <c r="AA8" s="63" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="94"/>
       <c r="B9" s="82"/>
       <c r="C9" s="93" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="D9" s="81"/>
       <c r="E9" s="74"/>
       <c r="F9" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G9" s="92"/>
       <c r="H9" s="75"/>
       <c r="I9" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J9" s="75"/>
       <c r="K9" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="L9" s="75"/>
       <c r="M9" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N9" s="92"/>
       <c r="O9" s="75"/>
       <c r="P9" s="92"/>
       <c r="Q9" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="R9" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="S9" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T9" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="U9" s="78"/>
       <c r="V9" s="78"/>
@@ -18023,104 +18031,104 @@
       <c r="Y9" s="78"/>
       <c r="Z9" s="78"/>
       <c r="AA9" s="63" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="94"/>
       <c r="B10" s="30"/>
       <c r="C10" s="32" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="74"/>
       <c r="F10" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G10" s="92"/>
       <c r="H10" s="75"/>
       <c r="I10" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J10" s="75"/>
       <c r="K10" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="L10" s="75"/>
       <c r="M10" s="74"/>
       <c r="N10" s="92"/>
       <c r="O10" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="P10" s="92"/>
       <c r="Q10" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="R10" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="S10" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T10" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="U10" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="V10" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="W10" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="X10" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="Y10" s="78"/>
       <c r="Z10" s="78"/>
       <c r="AA10" s="63" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="94"/>
       <c r="B11" s="82"/>
       <c r="C11" s="95" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="D11" s="81"/>
       <c r="E11" s="96"/>
       <c r="F11" s="102" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G11" s="98"/>
       <c r="H11" s="97"/>
       <c r="I11" s="96" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J11" s="97"/>
       <c r="K11" s="96" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="L11" s="97"/>
       <c r="M11" s="96" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N11" s="98"/>
       <c r="O11" s="97"/>
       <c r="P11" s="98"/>
       <c r="Q11" s="98" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="R11" s="98" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="S11" s="99" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T11" s="99" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="U11" s="99"/>
       <c r="V11" s="99"/>
@@ -18129,7 +18137,7 @@
       <c r="Y11" s="99"/>
       <c r="Z11" s="99"/>
       <c r="AA11" s="100" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -18164,7 +18172,7 @@
     <row r="13" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="49"/>
       <c r="B13" s="49" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="C13" s="93"/>
       <c r="D13" s="93"/>
@@ -18196,241 +18204,241 @@
       <c r="A14" s="94"/>
       <c r="B14" s="30"/>
       <c r="C14" s="32" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="D14" s="32"/>
       <c r="E14" s="74"/>
       <c r="F14" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G14" s="92"/>
       <c r="H14" s="75"/>
       <c r="I14" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J14" s="75"/>
       <c r="K14" s="74"/>
       <c r="L14" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M14" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N14" s="92"/>
       <c r="O14" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="P14" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="Q14" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="R14" s="92"/>
       <c r="S14" s="78"/>
       <c r="T14" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="U14" s="78"/>
       <c r="V14" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="W14" s="78"/>
       <c r="X14" s="78"/>
       <c r="Y14" s="78"/>
       <c r="Z14" s="78"/>
       <c r="AA14" s="63" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="94"/>
       <c r="B15" s="30"/>
       <c r="C15" s="32" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="D15" s="32"/>
       <c r="E15" s="74"/>
       <c r="F15" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G15" s="92"/>
       <c r="H15" s="75"/>
       <c r="I15" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J15" s="75"/>
       <c r="K15" s="74"/>
       <c r="L15" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M15" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N15" s="92"/>
       <c r="O15" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="P15" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="Q15" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="R15" s="92"/>
       <c r="S15" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T15" s="78"/>
       <c r="U15" s="78"/>
       <c r="V15" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="W15" s="78"/>
       <c r="X15" s="78"/>
       <c r="Y15" s="78"/>
       <c r="Z15" s="78"/>
       <c r="AA15" s="63" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="94"/>
       <c r="B16" s="82"/>
       <c r="C16" s="81" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="D16" s="81"/>
       <c r="E16" s="74"/>
       <c r="F16" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G16" s="92"/>
       <c r="H16" s="75"/>
       <c r="I16" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J16" s="75"/>
       <c r="K16" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="L16" s="75"/>
       <c r="M16" s="74"/>
       <c r="N16" s="92"/>
       <c r="O16" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="P16" s="92"/>
       <c r="Q16" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="R16" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="S16" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T16" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="U16" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="V16" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="W16" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="X16" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="Y16" s="78"/>
       <c r="Z16" s="78"/>
       <c r="AA16" s="63" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="17" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="94"/>
       <c r="B17" s="82"/>
       <c r="C17" s="81" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="D17" s="81"/>
       <c r="E17" s="74"/>
       <c r="F17" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G17" s="92"/>
       <c r="H17" s="75"/>
       <c r="I17" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J17" s="75"/>
       <c r="K17" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="L17" s="75"/>
       <c r="M17" s="74"/>
       <c r="N17" s="92"/>
       <c r="O17" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="P17" s="92"/>
       <c r="Q17" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="R17" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="S17" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T17" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="U17" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="V17" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="W17" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="X17" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="Y17" s="78"/>
       <c r="Z17" s="78"/>
       <c r="AA17" s="63" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="18" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="94"/>
       <c r="B18" s="60"/>
       <c r="C18" s="59" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="D18" s="59"/>
       <c r="E18" s="74"/>
       <c r="F18" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G18" s="92"/>
       <c r="H18" s="75"/>
       <c r="I18" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J18" s="75"/>
       <c r="K18" s="74"/>
       <c r="L18" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M18" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N18" s="92"/>
       <c r="O18" s="75"/>
@@ -18441,39 +18449,39 @@
       <c r="T18" s="78"/>
       <c r="U18" s="78"/>
       <c r="V18" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="W18" s="78"/>
       <c r="X18" s="78"/>
       <c r="Y18" s="78"/>
       <c r="Z18" s="78"/>
       <c r="AA18" s="63" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="94"/>
       <c r="B19" s="30"/>
       <c r="C19" s="32" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="D19" s="32"/>
       <c r="E19" s="74"/>
       <c r="F19" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G19" s="92"/>
       <c r="H19" s="75"/>
       <c r="I19" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J19" s="75"/>
       <c r="K19" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="L19" s="75"/>
       <c r="M19" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N19" s="92"/>
       <c r="O19" s="75"/>
@@ -18481,7 +18489,7 @@
       <c r="Q19" s="92"/>
       <c r="R19" s="92"/>
       <c r="S19" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T19" s="78"/>
       <c r="U19" s="78"/>
@@ -18491,32 +18499,32 @@
       <c r="Y19" s="78"/>
       <c r="Z19" s="78"/>
       <c r="AA19" s="63" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="94"/>
       <c r="B20" s="30"/>
       <c r="C20" s="32" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="D20" s="32"/>
       <c r="E20" s="74"/>
       <c r="F20" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G20" s="92"/>
       <c r="H20" s="75"/>
       <c r="I20" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J20" s="75"/>
       <c r="K20" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="L20" s="75"/>
       <c r="M20" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N20" s="92"/>
       <c r="O20" s="75"/>
@@ -18524,7 +18532,7 @@
       <c r="Q20" s="92"/>
       <c r="R20" s="92"/>
       <c r="S20" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T20" s="78"/>
       <c r="U20" s="78"/>
@@ -18534,32 +18542,32 @@
       <c r="Y20" s="78"/>
       <c r="Z20" s="78"/>
       <c r="AA20" s="63" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="94"/>
       <c r="B21" s="30"/>
       <c r="C21" s="32" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="D21" s="32"/>
       <c r="E21" s="74"/>
       <c r="F21" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G21" s="92"/>
       <c r="H21" s="75"/>
       <c r="I21" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J21" s="75"/>
       <c r="K21" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="L21" s="75"/>
       <c r="M21" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N21" s="92"/>
       <c r="O21" s="75"/>
@@ -18567,7 +18575,7 @@
       <c r="Q21" s="92"/>
       <c r="R21" s="92"/>
       <c r="S21" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T21" s="78"/>
       <c r="U21" s="78"/>
@@ -18577,349 +18585,349 @@
       <c r="Y21" s="78"/>
       <c r="Z21" s="78"/>
       <c r="AA21" s="63" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="22" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="94"/>
       <c r="B22" s="82"/>
       <c r="C22" s="81" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="D22" s="81"/>
       <c r="E22" s="74"/>
       <c r="F22" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G22" s="92"/>
       <c r="H22" s="75"/>
       <c r="I22" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J22" s="75"/>
       <c r="K22" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="L22" s="75"/>
       <c r="M22" s="74"/>
       <c r="N22" s="92"/>
       <c r="O22" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="P22" s="92"/>
       <c r="Q22" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="R22" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="S22" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T22" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="U22" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="V22" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="W22" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="X22" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="Y22" s="78"/>
       <c r="Z22" s="78"/>
       <c r="AA22" s="63" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="23" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="94"/>
       <c r="B23" s="82"/>
       <c r="C23" s="81" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="D23" s="81"/>
       <c r="E23" s="74"/>
       <c r="F23" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G23" s="92"/>
       <c r="H23" s="75"/>
       <c r="I23" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J23" s="75"/>
       <c r="K23" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="L23" s="75"/>
       <c r="M23" s="74"/>
       <c r="N23" s="92"/>
       <c r="O23" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="P23" s="92"/>
       <c r="Q23" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="R23" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="S23" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T23" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="U23" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="V23" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="W23" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="X23" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="Y23" s="78"/>
       <c r="Z23" s="78"/>
       <c r="AA23" s="63" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="24" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="94"/>
       <c r="B24" s="30"/>
       <c r="C24" s="32" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D24" s="32"/>
       <c r="E24" s="74"/>
       <c r="F24" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G24" s="92"/>
       <c r="H24" s="75"/>
       <c r="I24" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J24" s="75"/>
       <c r="K24" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="L24" s="75"/>
       <c r="M24" s="74"/>
       <c r="N24" s="92"/>
       <c r="O24" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="P24" s="92"/>
       <c r="Q24" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="R24" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="S24" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T24" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="U24" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="V24" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="W24" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="X24" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="Y24" s="78"/>
       <c r="Z24" s="78"/>
       <c r="AA24" s="63" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="25" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="94"/>
       <c r="B25" s="30"/>
       <c r="C25" s="32" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="D25" s="32"/>
       <c r="E25" s="74"/>
       <c r="F25" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G25" s="92"/>
       <c r="H25" s="75"/>
       <c r="I25" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J25" s="75"/>
       <c r="K25" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="L25" s="75"/>
       <c r="M25" s="74"/>
       <c r="N25" s="92"/>
       <c r="O25" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="P25" s="92"/>
       <c r="Q25" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="R25" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="S25" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T25" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="U25" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="V25" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="W25" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="X25" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="Y25" s="78"/>
       <c r="Z25" s="78"/>
       <c r="AA25" s="63" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="26" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="94"/>
       <c r="B26" s="82"/>
       <c r="C26" s="81" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="D26" s="81"/>
       <c r="E26" s="74"/>
       <c r="F26" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G26" s="92"/>
       <c r="H26" s="75"/>
       <c r="I26" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J26" s="75"/>
       <c r="K26" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="L26" s="75"/>
       <c r="M26" s="74"/>
       <c r="N26" s="92"/>
       <c r="O26" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="P26" s="92"/>
       <c r="Q26" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="R26" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="S26" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T26" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="U26" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="V26" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="W26" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="X26" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="Y26" s="78"/>
       <c r="Z26" s="78"/>
       <c r="AA26" s="63" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="94"/>
       <c r="B27" s="82"/>
       <c r="C27" s="81" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="D27" s="81"/>
       <c r="E27" s="74"/>
       <c r="F27" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G27" s="92"/>
       <c r="H27" s="75"/>
       <c r="I27" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J27" s="75"/>
       <c r="K27" s="74"/>
       <c r="L27" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M27" s="74"/>
       <c r="N27" s="92"/>
       <c r="O27" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="P27" s="92"/>
       <c r="Q27" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="R27" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="S27" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T27" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="U27" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="V27" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="W27" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="X27" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="Y27" s="78"/>
       <c r="Z27" s="78"/>
       <c r="AA27" s="63" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="28" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -18954,7 +18962,7 @@
     <row r="29" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="94"/>
       <c r="B29" s="31" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="C29" s="93"/>
       <c r="D29" s="93"/>
@@ -18986,40 +18994,40 @@
       <c r="A30" s="94"/>
       <c r="B30" s="82"/>
       <c r="C30" s="81" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="D30" s="81"/>
       <c r="E30" s="74"/>
       <c r="F30" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G30" s="92"/>
       <c r="H30" s="75"/>
       <c r="I30" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J30" s="75"/>
       <c r="K30" s="74"/>
       <c r="L30" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M30" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N30" s="92"/>
       <c r="O30" s="75"/>
       <c r="P30" s="92"/>
       <c r="Q30" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="R30" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="S30" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T30" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="U30" s="78"/>
       <c r="V30" s="78"/>
@@ -19028,32 +19036,32 @@
       <c r="Y30" s="78"/>
       <c r="Z30" s="78"/>
       <c r="AA30" s="63" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
     </row>
     <row r="31" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="94"/>
       <c r="B31" s="94"/>
       <c r="C31" s="93" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="D31" s="93"/>
       <c r="E31" s="74"/>
       <c r="F31" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G31" s="92"/>
       <c r="H31" s="75"/>
       <c r="I31" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J31" s="75"/>
       <c r="K31" s="74"/>
       <c r="L31" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M31" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N31" s="92"/>
       <c r="O31" s="75"/>
@@ -19062,7 +19070,7 @@
       <c r="R31" s="92"/>
       <c r="S31" s="78"/>
       <c r="T31" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="U31" s="78"/>
       <c r="V31" s="78"/>
@@ -19071,32 +19079,32 @@
       <c r="Y31" s="78"/>
       <c r="Z31" s="78"/>
       <c r="AA31" s="63" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="32" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="94"/>
       <c r="B32" s="94"/>
       <c r="C32" s="93" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="D32" s="93"/>
       <c r="E32" s="74"/>
       <c r="F32" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G32" s="92"/>
       <c r="H32" s="75"/>
       <c r="I32" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J32" s="75"/>
       <c r="K32" s="74"/>
       <c r="L32" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M32" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N32" s="92"/>
       <c r="O32" s="75"/>
@@ -19105,7 +19113,7 @@
       <c r="R32" s="92"/>
       <c r="S32" s="78"/>
       <c r="T32" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="U32" s="78"/>
       <c r="V32" s="78"/>
@@ -19114,38 +19122,38 @@
       <c r="Y32" s="78"/>
       <c r="Z32" s="78"/>
       <c r="AA32" s="63" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="33" spans="1:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="94"/>
       <c r="B33" s="94"/>
       <c r="C33" s="93" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="D33" s="93"/>
       <c r="E33" s="74"/>
       <c r="F33" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G33" s="92"/>
       <c r="H33" s="75"/>
       <c r="I33" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J33" s="75"/>
       <c r="K33" s="74"/>
       <c r="L33" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M33" s="74"/>
       <c r="N33" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="O33" s="75"/>
       <c r="P33" s="92"/>
       <c r="Q33" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="R33" s="92"/>
       <c r="S33" s="78"/>
@@ -19157,7 +19165,7 @@
       <c r="Y33" s="78"/>
       <c r="Z33" s="78"/>
       <c r="AA33" s="63" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="34" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -19192,7 +19200,7 @@
     <row r="35" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="49"/>
       <c r="B35" s="49" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="C35" s="93"/>
       <c r="D35" s="93"/>
@@ -19224,25 +19232,25 @@
       <c r="A36" s="94"/>
       <c r="B36" s="30"/>
       <c r="C36" s="32" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="D36" s="32"/>
       <c r="E36" s="74"/>
       <c r="F36" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G36" s="92"/>
       <c r="H36" s="75"/>
       <c r="I36" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J36" s="75"/>
       <c r="K36" s="74"/>
       <c r="L36" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M36" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N36" s="92"/>
       <c r="O36" s="75"/>
@@ -19250,7 +19258,7 @@
       <c r="Q36" s="92"/>
       <c r="R36" s="92"/>
       <c r="S36" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T36" s="78"/>
       <c r="U36" s="78"/>
@@ -19260,32 +19268,32 @@
       <c r="Y36" s="78"/>
       <c r="Z36" s="78"/>
       <c r="AA36" s="63" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="37" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="94"/>
       <c r="B37" s="30"/>
       <c r="C37" s="32" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="D37" s="32"/>
       <c r="E37" s="74"/>
       <c r="F37" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G37" s="92"/>
       <c r="H37" s="75"/>
       <c r="I37" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J37" s="75"/>
       <c r="K37" s="74"/>
       <c r="L37" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M37" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N37" s="92"/>
       <c r="O37" s="75"/>
@@ -19296,39 +19304,39 @@
       <c r="T37" s="78"/>
       <c r="U37" s="78"/>
       <c r="V37" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="W37" s="78"/>
       <c r="X37" s="78"/>
       <c r="Y37" s="78"/>
       <c r="Z37" s="78"/>
       <c r="AA37" s="63" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="38" spans="1:27" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="94"/>
       <c r="B38" s="94"/>
       <c r="C38" s="93" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="D38" s="93"/>
       <c r="E38" s="74"/>
       <c r="F38" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G38" s="92"/>
       <c r="H38" s="75"/>
       <c r="I38" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J38" s="75"/>
       <c r="K38" s="74"/>
       <c r="L38" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M38" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N38" s="92"/>
       <c r="O38" s="75"/>
@@ -19336,7 +19344,7 @@
       <c r="Q38" s="92"/>
       <c r="R38" s="92"/>
       <c r="S38" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T38" s="78"/>
       <c r="U38" s="78"/>
@@ -19346,32 +19354,32 @@
       <c r="Y38" s="78"/>
       <c r="Z38" s="78"/>
       <c r="AA38" s="63" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="39" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="94"/>
       <c r="B39" s="94"/>
       <c r="C39" s="93" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="D39" s="93"/>
       <c r="E39" s="74"/>
       <c r="F39" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G39" s="92"/>
       <c r="H39" s="75"/>
       <c r="I39" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J39" s="75"/>
       <c r="K39" s="74"/>
       <c r="L39" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M39" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N39" s="92"/>
       <c r="O39" s="75"/>
@@ -19379,44 +19387,44 @@
       <c r="Q39" s="92"/>
       <c r="R39" s="92"/>
       <c r="S39" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T39" s="78"/>
       <c r="U39" s="78"/>
       <c r="V39" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="W39" s="78"/>
       <c r="X39" s="78"/>
       <c r="Y39" s="78"/>
       <c r="Z39" s="78"/>
       <c r="AA39" s="63" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="40" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="94"/>
       <c r="B40" s="94"/>
       <c r="C40" s="93" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="D40" s="93"/>
       <c r="E40" s="74"/>
       <c r="F40" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G40" s="92"/>
       <c r="H40" s="75"/>
       <c r="I40" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J40" s="75"/>
       <c r="K40" s="74"/>
       <c r="L40" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M40" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N40" s="92"/>
       <c r="O40" s="75"/>
@@ -19424,93 +19432,93 @@
       <c r="Q40" s="92"/>
       <c r="R40" s="92"/>
       <c r="S40" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T40" s="78"/>
       <c r="U40" s="78"/>
       <c r="V40" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="W40" s="78"/>
       <c r="X40" s="78"/>
       <c r="Y40" s="78"/>
       <c r="Z40" s="78"/>
       <c r="AA40" s="63" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="41" spans="1:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="94"/>
       <c r="B41" s="94"/>
       <c r="C41" s="93" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="D41" s="93"/>
       <c r="E41" s="74"/>
       <c r="F41" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G41" s="92"/>
       <c r="H41" s="75"/>
       <c r="I41" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J41" s="75"/>
       <c r="K41" s="74"/>
       <c r="L41" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M41" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N41" s="92"/>
       <c r="O41" s="75"/>
       <c r="P41" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="Q41" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="R41" s="92"/>
       <c r="S41" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T41" s="78"/>
       <c r="U41" s="78"/>
       <c r="V41" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="W41" s="78"/>
       <c r="X41" s="78"/>
       <c r="Y41" s="78"/>
       <c r="Z41" s="78"/>
       <c r="AA41" s="63" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
     </row>
     <row r="42" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="94"/>
       <c r="B42" s="94"/>
       <c r="C42" s="93" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="D42" s="93"/>
       <c r="E42" s="74"/>
       <c r="F42" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G42" s="92"/>
       <c r="H42" s="75"/>
       <c r="I42" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J42" s="75"/>
       <c r="K42" s="74"/>
       <c r="L42" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M42" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N42" s="92"/>
       <c r="O42" s="75"/>
@@ -19519,7 +19527,7 @@
       <c r="R42" s="92"/>
       <c r="S42" s="78"/>
       <c r="T42" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="U42" s="78"/>
       <c r="V42" s="78"/>
@@ -19528,32 +19536,32 @@
       <c r="Y42" s="78"/>
       <c r="Z42" s="78"/>
       <c r="AA42" s="63" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="43" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="94"/>
       <c r="B43" s="94"/>
       <c r="C43" s="93" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="D43" s="93"/>
       <c r="E43" s="74"/>
       <c r="F43" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G43" s="92"/>
       <c r="H43" s="75"/>
       <c r="I43" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J43" s="75"/>
       <c r="K43" s="74"/>
       <c r="L43" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M43" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N43" s="92"/>
       <c r="O43" s="75"/>
@@ -19561,44 +19569,44 @@
       <c r="Q43" s="92"/>
       <c r="R43" s="92"/>
       <c r="S43" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T43" s="78"/>
       <c r="U43" s="78"/>
       <c r="V43" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="W43" s="78"/>
       <c r="X43" s="78"/>
       <c r="Y43" s="78"/>
       <c r="Z43" s="78"/>
       <c r="AA43" s="63" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="44" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="94"/>
       <c r="B44" s="94"/>
       <c r="C44" s="93" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="D44" s="93"/>
       <c r="E44" s="74"/>
       <c r="F44" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G44" s="92"/>
       <c r="H44" s="75"/>
       <c r="I44" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J44" s="75"/>
       <c r="K44" s="74"/>
       <c r="L44" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M44" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N44" s="92"/>
       <c r="O44" s="75"/>
@@ -19606,101 +19614,101 @@
       <c r="Q44" s="92"/>
       <c r="R44" s="92"/>
       <c r="S44" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T44" s="78"/>
       <c r="U44" s="78"/>
       <c r="V44" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="W44" s="78"/>
       <c r="X44" s="78"/>
       <c r="Y44" s="78"/>
       <c r="Z44" s="78"/>
       <c r="AA44" s="63" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="45" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="94"/>
       <c r="B45" s="82"/>
       <c r="C45" s="81" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="D45" s="81"/>
       <c r="E45" s="74"/>
       <c r="F45" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G45" s="92"/>
       <c r="H45" s="75"/>
       <c r="I45" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J45" s="75"/>
       <c r="K45" s="74"/>
       <c r="L45" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M45" s="74"/>
       <c r="N45" s="92"/>
       <c r="O45" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="P45" s="92"/>
       <c r="Q45" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="R45" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="S45" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T45" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="U45" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="V45" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="W45" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="X45" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="Y45" s="78"/>
       <c r="Z45" s="78"/>
       <c r="AA45" s="63" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="46" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="94"/>
       <c r="B46" s="60"/>
       <c r="C46" s="59" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="D46" s="59"/>
       <c r="E46" s="74"/>
       <c r="F46" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G46" s="92"/>
       <c r="H46" s="75"/>
       <c r="I46" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J46" s="75"/>
       <c r="K46" s="74"/>
       <c r="L46" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M46" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N46" s="92"/>
       <c r="O46" s="75"/>
@@ -19708,44 +19716,44 @@
       <c r="Q46" s="92"/>
       <c r="R46" s="92"/>
       <c r="S46" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T46" s="78"/>
       <c r="U46" s="78"/>
       <c r="V46" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="W46" s="78"/>
       <c r="X46" s="78"/>
       <c r="Y46" s="78"/>
       <c r="Z46" s="78"/>
       <c r="AA46" s="63" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="94"/>
       <c r="B47" s="60"/>
       <c r="C47" s="59" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="D47" s="59"/>
       <c r="E47" s="74"/>
       <c r="F47" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G47" s="92"/>
       <c r="H47" s="75"/>
       <c r="I47" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J47" s="75"/>
       <c r="K47" s="74"/>
       <c r="L47" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M47" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N47" s="92"/>
       <c r="O47" s="75"/>
@@ -19753,7 +19761,7 @@
       <c r="Q47" s="92"/>
       <c r="R47" s="92"/>
       <c r="S47" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T47" s="78"/>
       <c r="U47" s="78"/>
@@ -19763,32 +19771,32 @@
       <c r="Y47" s="78"/>
       <c r="Z47" s="78"/>
       <c r="AA47" s="63" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="48" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="94"/>
       <c r="B48" s="82"/>
       <c r="C48" s="81" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="D48" s="81"/>
       <c r="E48" s="74"/>
       <c r="F48" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G48" s="92"/>
       <c r="H48" s="75"/>
       <c r="I48" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J48" s="75"/>
       <c r="K48" s="74"/>
       <c r="L48" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M48" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N48" s="92"/>
       <c r="O48" s="75"/>
@@ -19797,7 +19805,7 @@
       <c r="R48" s="92"/>
       <c r="S48" s="78"/>
       <c r="T48" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="U48" s="78"/>
       <c r="V48" s="78"/>
@@ -19806,32 +19814,32 @@
       <c r="Y48" s="78"/>
       <c r="Z48" s="78"/>
       <c r="AA48" s="63" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="49" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="94"/>
       <c r="B49" s="94"/>
       <c r="C49" s="93" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="D49" s="93"/>
       <c r="E49" s="74"/>
       <c r="F49" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G49" s="92"/>
       <c r="H49" s="75"/>
       <c r="I49" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J49" s="75"/>
       <c r="K49" s="74"/>
       <c r="L49" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M49" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N49" s="92"/>
       <c r="O49" s="75"/>
@@ -19840,7 +19848,7 @@
       <c r="R49" s="92"/>
       <c r="S49" s="78"/>
       <c r="T49" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="U49" s="78"/>
       <c r="V49" s="78"/>
@@ -19849,32 +19857,32 @@
       <c r="Y49" s="78"/>
       <c r="Z49" s="78"/>
       <c r="AA49" s="63" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="50" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="94"/>
       <c r="B50" s="82"/>
       <c r="C50" s="81" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="D50" s="81"/>
       <c r="E50" s="74"/>
       <c r="F50" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G50" s="92"/>
       <c r="H50" s="75"/>
       <c r="I50" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J50" s="75"/>
       <c r="K50" s="74"/>
       <c r="L50" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M50" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N50" s="92"/>
       <c r="O50" s="75"/>
@@ -19883,7 +19891,7 @@
       <c r="R50" s="92"/>
       <c r="S50" s="78"/>
       <c r="T50" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="U50" s="78"/>
       <c r="V50" s="78"/>
@@ -19892,32 +19900,32 @@
       <c r="Y50" s="78"/>
       <c r="Z50" s="78"/>
       <c r="AA50" s="63" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="51" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="94"/>
       <c r="B51" s="82"/>
       <c r="C51" s="81" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="D51" s="81"/>
       <c r="E51" s="74"/>
       <c r="F51" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G51" s="92"/>
       <c r="H51" s="75"/>
       <c r="I51" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J51" s="75"/>
       <c r="K51" s="74"/>
       <c r="L51" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M51" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N51" s="92"/>
       <c r="O51" s="75"/>
@@ -19926,7 +19934,7 @@
       <c r="R51" s="92"/>
       <c r="S51" s="78"/>
       <c r="T51" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="U51" s="78"/>
       <c r="V51" s="78"/>
@@ -19935,32 +19943,32 @@
       <c r="Y51" s="78"/>
       <c r="Z51" s="78"/>
       <c r="AA51" s="63" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="52" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="94"/>
       <c r="B52" s="89"/>
       <c r="C52" s="88" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="D52" s="88"/>
       <c r="E52" s="74"/>
       <c r="F52" s="101"/>
       <c r="G52" s="92"/>
       <c r="H52" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="I52" s="74"/>
       <c r="J52" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="K52" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="L52" s="75"/>
       <c r="M52" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N52" s="92"/>
       <c r="O52" s="75"/>
@@ -19975,35 +19983,35 @@
       <c r="X52" s="78"/>
       <c r="Y52" s="78"/>
       <c r="Z52" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="AA52" s="63" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="53" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="94"/>
       <c r="B53" s="89"/>
       <c r="C53" s="88" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="D53" s="88"/>
       <c r="E53" s="74"/>
       <c r="F53" s="101"/>
       <c r="G53" s="92"/>
       <c r="H53" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="I53" s="74"/>
       <c r="J53" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="K53" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="L53" s="75"/>
       <c r="M53" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N53" s="92"/>
       <c r="O53" s="75"/>
@@ -20018,10 +20026,10 @@
       <c r="X53" s="78"/>
       <c r="Y53" s="78"/>
       <c r="Z53" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="AA53" s="63" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="54" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -20056,7 +20064,7 @@
     <row r="55" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="49"/>
       <c r="B55" s="49" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="C55" s="93"/>
       <c r="D55" s="93"/>
@@ -20088,29 +20096,29 @@
       <c r="A56" s="94"/>
       <c r="B56" s="89"/>
       <c r="C56" s="88" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="D56" s="88"/>
       <c r="E56" s="74"/>
       <c r="F56" s="101"/>
       <c r="G56" s="92"/>
       <c r="H56" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="I56" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J56" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="K56" s="74"/>
       <c r="L56" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M56" s="74"/>
       <c r="N56" s="92"/>
       <c r="O56" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="P56" s="92"/>
       <c r="Q56" s="92"/>
@@ -20123,39 +20131,39 @@
       <c r="X56" s="78"/>
       <c r="Y56" s="78"/>
       <c r="Z56" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="AA56" s="63" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="57" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="94"/>
       <c r="B57" s="89"/>
       <c r="C57" s="88" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="D57" s="88"/>
       <c r="E57" s="74"/>
       <c r="F57" s="101"/>
       <c r="G57" s="92"/>
       <c r="H57" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="I57" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J57" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="K57" s="74"/>
       <c r="L57" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M57" s="74"/>
       <c r="N57" s="92"/>
       <c r="O57" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="P57" s="92"/>
       <c r="Q57" s="92"/>
@@ -20168,39 +20176,39 @@
       <c r="X57" s="78"/>
       <c r="Y57" s="78"/>
       <c r="Z57" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="AA57" s="63" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="58" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="94"/>
       <c r="B58" s="89"/>
       <c r="C58" s="88" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="D58" s="88"/>
       <c r="E58" s="74"/>
       <c r="F58" s="101"/>
       <c r="G58" s="92"/>
       <c r="H58" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="I58" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J58" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="K58" s="74"/>
       <c r="L58" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M58" s="74"/>
       <c r="N58" s="92"/>
       <c r="O58" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="P58" s="92"/>
       <c r="Q58" s="92"/>
@@ -20213,39 +20221,39 @@
       <c r="X58" s="78"/>
       <c r="Y58" s="78"/>
       <c r="Z58" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="AA58" s="63" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="59" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="94"/>
       <c r="B59" s="89"/>
       <c r="C59" s="88" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="D59" s="88"/>
       <c r="E59" s="74"/>
       <c r="F59" s="101"/>
       <c r="G59" s="92"/>
       <c r="H59" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="I59" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J59" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="K59" s="74"/>
       <c r="L59" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M59" s="74"/>
       <c r="N59" s="92"/>
       <c r="O59" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="P59" s="92"/>
       <c r="Q59" s="92"/>
@@ -20258,39 +20266,39 @@
       <c r="X59" s="78"/>
       <c r="Y59" s="78"/>
       <c r="Z59" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="AA59" s="63" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="60" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="94"/>
       <c r="B60" s="89"/>
       <c r="C60" s="88" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="D60" s="88"/>
       <c r="E60" s="74"/>
       <c r="F60" s="101"/>
       <c r="G60" s="92"/>
       <c r="H60" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="I60" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J60" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="K60" s="74"/>
       <c r="L60" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M60" s="74"/>
       <c r="N60" s="92"/>
       <c r="O60" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="P60" s="92"/>
       <c r="Q60" s="92"/>
@@ -20303,39 +20311,39 @@
       <c r="X60" s="78"/>
       <c r="Y60" s="78"/>
       <c r="Z60" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="AA60" s="63" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="61" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="94"/>
       <c r="B61" s="89"/>
       <c r="C61" s="88" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="D61" s="88"/>
       <c r="E61" s="74"/>
       <c r="F61" s="101"/>
       <c r="G61" s="92"/>
       <c r="H61" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="I61" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J61" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="K61" s="74"/>
       <c r="L61" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M61" s="74"/>
       <c r="N61" s="92"/>
       <c r="O61" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="P61" s="92"/>
       <c r="Q61" s="92"/>
@@ -20348,39 +20356,39 @@
       <c r="X61" s="78"/>
       <c r="Y61" s="78"/>
       <c r="Z61" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="AA61" s="63" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="62" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="94"/>
       <c r="B62" s="89"/>
       <c r="C62" s="88" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="D62" s="88"/>
       <c r="E62" s="74"/>
       <c r="F62" s="101"/>
       <c r="G62" s="92"/>
       <c r="H62" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="I62" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J62" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="K62" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="L62" s="75"/>
       <c r="M62" s="74"/>
       <c r="N62" s="92"/>
       <c r="O62" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="P62" s="92"/>
       <c r="Q62" s="92"/>
@@ -20393,39 +20401,39 @@
       <c r="X62" s="78"/>
       <c r="Y62" s="78"/>
       <c r="Z62" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="AA62" s="63" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="63" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="94"/>
       <c r="B63" s="89"/>
       <c r="C63" s="88" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="D63" s="88"/>
       <c r="E63" s="74"/>
       <c r="F63" s="101"/>
       <c r="G63" s="92"/>
       <c r="H63" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="I63" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J63" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="K63" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="L63" s="75"/>
       <c r="M63" s="74"/>
       <c r="N63" s="92"/>
       <c r="O63" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="P63" s="92"/>
       <c r="Q63" s="92"/>
@@ -20438,35 +20446,35 @@
       <c r="X63" s="78"/>
       <c r="Y63" s="78"/>
       <c r="Z63" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="AA63" s="63" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="64" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="94"/>
       <c r="B64" s="94"/>
       <c r="C64" s="93" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="D64" s="93"/>
       <c r="E64" s="74"/>
       <c r="F64" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G64" s="92"/>
       <c r="H64" s="75"/>
       <c r="I64" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J64" s="75"/>
       <c r="K64" s="74"/>
       <c r="L64" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M64" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N64" s="92"/>
       <c r="O64" s="75"/>
@@ -20474,44 +20482,44 @@
       <c r="Q64" s="92"/>
       <c r="R64" s="92"/>
       <c r="S64" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T64" s="78"/>
       <c r="U64" s="78"/>
       <c r="V64" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="W64" s="78"/>
       <c r="X64" s="78"/>
       <c r="Y64" s="78"/>
       <c r="Z64" s="78"/>
       <c r="AA64" s="63" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="65" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="94"/>
       <c r="B65" s="94"/>
       <c r="C65" s="93" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="D65" s="93"/>
       <c r="E65" s="74"/>
       <c r="F65" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G65" s="92"/>
       <c r="H65" s="75"/>
       <c r="I65" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J65" s="75"/>
       <c r="K65" s="74"/>
       <c r="L65" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M65" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N65" s="92"/>
       <c r="O65" s="75"/>
@@ -20519,44 +20527,44 @@
       <c r="Q65" s="92"/>
       <c r="R65" s="92"/>
       <c r="S65" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T65" s="78"/>
       <c r="U65" s="78"/>
       <c r="V65" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="W65" s="78"/>
       <c r="X65" s="78"/>
       <c r="Y65" s="78"/>
       <c r="Z65" s="78"/>
       <c r="AA65" s="63" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="66" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="94"/>
       <c r="B66" s="94"/>
       <c r="C66" s="93" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="D66" s="93"/>
       <c r="E66" s="74"/>
       <c r="F66" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G66" s="92"/>
       <c r="H66" s="75"/>
       <c r="I66" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J66" s="75"/>
       <c r="K66" s="74"/>
       <c r="L66" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M66" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N66" s="92"/>
       <c r="O66" s="75"/>
@@ -20564,44 +20572,44 @@
       <c r="Q66" s="92"/>
       <c r="R66" s="92"/>
       <c r="S66" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T66" s="78"/>
       <c r="U66" s="78"/>
       <c r="V66" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="W66" s="78"/>
       <c r="X66" s="78"/>
       <c r="Y66" s="78"/>
       <c r="Z66" s="78"/>
       <c r="AA66" s="63" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="67" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="94"/>
       <c r="B67" s="94"/>
       <c r="C67" s="93" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="D67" s="93"/>
       <c r="E67" s="74"/>
       <c r="F67" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G67" s="92"/>
       <c r="H67" s="75"/>
       <c r="I67" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J67" s="75"/>
       <c r="K67" s="74"/>
       <c r="L67" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M67" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N67" s="92"/>
       <c r="O67" s="75"/>
@@ -20609,44 +20617,44 @@
       <c r="Q67" s="92"/>
       <c r="R67" s="92"/>
       <c r="S67" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T67" s="78"/>
       <c r="U67" s="78"/>
       <c r="V67" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="W67" s="78"/>
       <c r="X67" s="78"/>
       <c r="Y67" s="78"/>
       <c r="Z67" s="78"/>
       <c r="AA67" s="63" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="68" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="94"/>
       <c r="B68" s="94"/>
       <c r="C68" s="93" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="D68" s="93"/>
       <c r="E68" s="74"/>
       <c r="F68" s="101" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G68" s="92"/>
       <c r="H68" s="75"/>
       <c r="I68" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J68" s="75"/>
       <c r="K68" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="L68" s="75"/>
       <c r="M68" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="N68" s="92"/>
       <c r="O68" s="75"/>
@@ -20654,19 +20662,19 @@
       <c r="Q68" s="92"/>
       <c r="R68" s="92"/>
       <c r="S68" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="T68" s="78"/>
       <c r="U68" s="78"/>
       <c r="V68" s="78" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="W68" s="78"/>
       <c r="X68" s="78"/>
       <c r="Y68" s="78"/>
       <c r="Z68" s="78"/>
       <c r="AA68" s="63" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="69" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -20997,14 +21005,14 @@
   <sheetData>
     <row r="1" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="D1" s="61"/>
       <c r="E1" s="61"/>
     </row>
     <row r="2" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="D2" s="61"/>
       <c r="E2" s="61"/>
@@ -21014,7 +21022,7 @@
       <c r="B3" s="70"/>
       <c r="C3" s="71"/>
       <c r="D3" s="116" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="E3" s="114"/>
       <c r="F3" s="73"/>
@@ -21022,213 +21030,213 @@
     <row r="4" spans="1:6" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="67"/>
       <c r="B4" s="68" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C4" s="68"/>
       <c r="D4" s="65" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="E4" s="66" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="F4" s="72" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="60"/>
       <c r="B5" s="59" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="C5" s="59"/>
       <c r="D5" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="E5" s="75"/>
       <c r="F5" s="63" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="60"/>
       <c r="B6" s="59" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="C6" s="59"/>
       <c r="D6" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="E6" s="75"/>
       <c r="F6" s="63" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="60"/>
       <c r="B7" s="59" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="C7" s="59"/>
       <c r="D7" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="E7" s="75"/>
       <c r="F7" s="63" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="60"/>
       <c r="B8" s="59" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="C8" s="59"/>
       <c r="D8" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="E8" s="75"/>
       <c r="F8" s="63" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="60"/>
       <c r="B9" s="59" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="C9" s="59"/>
       <c r="D9" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="E9" s="75"/>
       <c r="F9" s="63" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="60"/>
       <c r="B10" s="59" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="C10" s="59"/>
       <c r="D10" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="E10" s="75"/>
       <c r="F10" s="63" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="60"/>
       <c r="B11" s="59" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="C11" s="59"/>
       <c r="D11" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="E11" s="75"/>
       <c r="F11" s="63" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="60"/>
       <c r="B12" s="59" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="C12" s="59"/>
       <c r="D12" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="E12" s="75"/>
       <c r="F12" s="63" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="60"/>
       <c r="B13" s="59" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="C13" s="59"/>
       <c r="D13" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="E13" s="75"/>
       <c r="F13" s="63" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="60"/>
       <c r="B14" s="59" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="C14" s="59"/>
       <c r="D14" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="E14" s="75"/>
       <c r="F14" s="63" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="60"/>
       <c r="B15" s="81" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="C15" s="59"/>
       <c r="D15" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="E15" s="75"/>
       <c r="F15" s="63" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="60"/>
       <c r="B16" s="81" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="C16" s="59"/>
       <c r="D16" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="E16" s="75"/>
       <c r="F16" s="63" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="60"/>
       <c r="B17" s="59" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="C17" s="59"/>
       <c r="D17" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="E17" s="75"/>
       <c r="F17" s="63" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="60"/>
       <c r="B18" s="59" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C18" s="59"/>
       <c r="D18" s="74" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="E18" s="75"/>
       <c r="F18" s="63" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -21414,162 +21422,162 @@
   <sheetData>
     <row r="1" spans="1:14" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="85" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="86" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="87"/>
       <c r="B3" s="39" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="39" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="E3" s="39"/>
       <c r="F3" s="39" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="G3" s="39"/>
       <c r="H3" s="39" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="I3" s="39"/>
       <c r="J3" s="39" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="K3" s="39"/>
       <c r="L3" s="39" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="M3" s="39"/>
       <c r="N3" s="39" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="57"/>
       <c r="B4" s="56" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="C4" s="56"/>
       <c r="D4" s="56" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="E4" s="58"/>
       <c r="F4" s="58" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="G4" s="58"/>
       <c r="H4" s="58" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="I4" s="58"/>
       <c r="J4" s="56" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K4" s="56"/>
       <c r="L4" s="56" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="M4" s="56"/>
       <c r="N4" s="56" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="195" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="83"/>
       <c r="B5" s="84" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="C5" s="84"/>
       <c r="D5" s="84" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="E5" s="84"/>
       <c r="F5" s="84" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="G5" s="84"/>
       <c r="H5" s="84" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="I5" s="84"/>
       <c r="J5" s="84" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="K5" s="84"/>
       <c r="L5" s="84" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="M5" s="84"/>
       <c r="N5" s="84" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="83"/>
       <c r="B6" s="84" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="C6" s="84"/>
       <c r="D6" s="84" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="E6" s="84"/>
       <c r="F6" s="84" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="G6" s="84"/>
       <c r="H6" s="84" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="I6" s="84"/>
       <c r="J6" s="84" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="K6" s="84"/>
       <c r="L6" s="84" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="M6" s="84"/>
       <c r="N6" s="84" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="83"/>
       <c r="B7" s="84" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="C7" s="84"/>
       <c r="D7" s="84" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="E7" s="84"/>
       <c r="F7" s="84" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="G7" s="84"/>
       <c r="H7" s="84" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="I7" s="84"/>
       <c r="J7" s="84" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="K7" s="84"/>
       <c r="L7" s="84" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="M7" s="84"/>
       <c r="N7" s="84" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -21626,7 +21634,7 @@
     </row>
     <row r="11" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="B11" s="23"/>
       <c r="C11" s="23"/>
@@ -21636,7 +21644,7 @@
     </row>
     <row r="12" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="B12" s="23"/>
       <c r="C12" s="23"/>
@@ -21646,7 +21654,7 @@
     </row>
     <row r="13" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="B13" s="23"/>
       <c r="C13" s="23"/>
@@ -21656,7 +21664,7 @@
     </row>
     <row r="14" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B14" s="56"/>
       <c r="C14" s="56"/>
@@ -21819,7 +21827,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight"/>
@@ -21831,11 +21839,11 @@
     <col min="2" max="2" width="2.7109375" customWidth="1"/>
     <col min="3" max="3" width="80.7109375" customWidth="1"/>
     <col min="4" max="4" width="2.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="5" max="5" width="50.7109375" customWidth="1"/>
     <col min="6" max="6" width="2.7109375" customWidth="1"/>
     <col min="7" max="7" width="20.7109375" customWidth="1"/>
-    <col min="8" max="8" width="2.7109375" customWidth="1"/>
-    <col min="9" max="9" width="25.7109375" customWidth="1"/>
+    <col min="8" max="8" width="2.7109375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -21845,7 +21853,7 @@
     </row>
     <row r="2" spans="1:9" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="27" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -21866,7 +21874,7 @@
       </c>
       <c r="H3" s="39"/>
       <c r="I3" s="40" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="23" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -21890,38 +21898,38 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="23" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="23" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
         <v>68</v>
       </c>
       <c r="B5" s="32"/>
       <c r="C5" s="32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D5" s="32"/>
       <c r="E5" s="32" t="s">
-        <v>83</v>
+        <v>339</v>
       </c>
       <c r="F5" s="32"/>
       <c r="G5" s="32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H5" s="32"/>
       <c r="I5" s="32" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="23" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="23" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
         <v>69</v>
       </c>
       <c r="B6" s="32"/>
       <c r="C6" s="32" t="s">
-        <v>86</v>
+        <v>338</v>
       </c>
       <c r="D6" s="32"/>
       <c r="E6" s="32" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="F6" s="32"/>
       <c r="G6" s="32" t="s">
@@ -21929,133 +21937,133 @@
       </c>
       <c r="H6" s="32"/>
       <c r="I6" s="32" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="23" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="23" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
         <v>70</v>
       </c>
       <c r="B7" s="32"/>
       <c r="C7" s="32" t="s">
-        <v>87</v>
+        <v>336</v>
       </c>
       <c r="D7" s="32"/>
       <c r="E7" s="32" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="F7" s="32"/>
       <c r="G7" s="32" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="H7" s="32"/>
       <c r="I7" s="32" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" s="23" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="23" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
         <v>71</v>
       </c>
       <c r="B8" s="32"/>
       <c r="C8" s="32" t="s">
-        <v>88</v>
+        <v>335</v>
       </c>
       <c r="D8" s="32"/>
       <c r="E8" s="32" t="s">
-        <v>89</v>
+        <v>340</v>
       </c>
       <c r="F8" s="32"/>
       <c r="G8" s="32" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H8" s="32"/>
       <c r="I8" s="32" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="23" customFormat="1" ht="210" customHeight="1" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="23" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
         <v>72</v>
       </c>
       <c r="B9" s="32"/>
       <c r="C9" s="32" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D9" s="32"/>
       <c r="E9" s="32" t="s">
-        <v>93</v>
+        <v>341</v>
       </c>
       <c r="F9" s="32"/>
       <c r="G9" s="32" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H9" s="32"/>
       <c r="I9" s="32" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="23" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="23" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
         <v>73</v>
       </c>
       <c r="B10" s="32"/>
       <c r="C10" s="32" t="s">
-        <v>95</v>
+        <v>337</v>
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="32" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="F10" s="32"/>
       <c r="G10" s="32" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="H10" s="32"/>
       <c r="I10" s="32" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" s="23" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="23" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
         <v>74</v>
       </c>
       <c r="B11" s="32"/>
       <c r="C11" s="32" t="s">
-        <v>98</v>
+        <v>334</v>
       </c>
       <c r="D11" s="32"/>
       <c r="E11" s="32" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="F11" s="32"/>
       <c r="G11" s="32" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="H11" s="32"/>
       <c r="I11" s="32" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" s="23" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="23" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
         <v>75</v>
       </c>
       <c r="B12" s="36"/>
       <c r="C12" s="36" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D12" s="36"/>
       <c r="E12" s="38" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="F12" s="36"/>
       <c r="G12" s="32" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="H12" s="36"/>
       <c r="I12" s="32" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -22092,15 +22100,17 @@
       <c r="H15" s="32"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="H16" s="32"/>
+      <c r="A16" s="112" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16" s="112"/>
+      <c r="C16" s="112"/>
+      <c r="D16" s="112"/>
+      <c r="E16" s="112"/>
+      <c r="F16" s="112"/>
+      <c r="G16" s="112"/>
+      <c r="H16" s="112"/>
+      <c r="I16" s="112"/>
     </row>
     <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="111"/>
@@ -22202,10 +22212,11 @@
       <c r="H27" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A16:I16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -22230,12 +22241,12 @@
   <sheetData>
     <row r="1" spans="1:3" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="B2" s="45"/>
       <c r="C2" s="45"/>
@@ -22247,272 +22258,272 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B4" s="44"/>
       <c r="C4" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B5" s="44"/>
       <c r="C5" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B6" s="44"/>
       <c r="C6" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B7" s="44"/>
       <c r="C7" s="23" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B8" s="44"/>
       <c r="C8" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B9" s="44"/>
       <c r="C9" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B10" s="44"/>
       <c r="C10" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B11" s="44"/>
       <c r="C11" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B12" s="44"/>
       <c r="C12" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B13" s="44"/>
       <c r="C13" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B14" s="44"/>
       <c r="C14" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B15" s="44"/>
       <c r="C15" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B16" s="44"/>
       <c r="C16" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B17" s="44"/>
       <c r="C17" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B18" s="44"/>
       <c r="C18" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B19" s="44"/>
       <c r="C19" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B20" s="44"/>
       <c r="C20" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B21" s="37"/>
       <c r="C21" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B22" s="37"/>
       <c r="C22" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B23" s="37"/>
       <c r="C23" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B24" s="37"/>
       <c r="C24" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B25" s="37"/>
       <c r="C25" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B26" s="37"/>
       <c r="C26" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B27" s="37"/>
       <c r="C27" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B28" s="37"/>
       <c r="C28" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B29" s="37"/>
       <c r="C29" s="23" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B30" s="37"/>
       <c r="C30" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B31" s="37"/>
       <c r="C31" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="B32" s="43"/>
       <c r="C32" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="B33" s="37"/>
       <c r="C33" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -22527,7 +22538,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="51" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B36" s="52"/>
       <c r="C36" s="52"/>
@@ -22563,21 +22574,21 @@
     </row>
     <row r="42" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="120" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="B42" s="120"/>
       <c r="C42" s="120"/>
     </row>
     <row r="43" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="121" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="B43" s="121"/>
       <c r="C43" s="121"/>
     </row>
     <row r="44" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="120" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B44" s="120"/>
       <c r="C44" s="120"/>
@@ -22657,12 +22668,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="108" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added content and edited Chapter 2 Literature Review
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="11" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId1"/>
@@ -23,11 +23,12 @@
     <sheet name="Figure - R&amp;D Funding 1967-2019" sheetId="3" r:id="rId9"/>
     <sheet name="Figure - R&amp;D Funding 1990-2015" sheetId="1" r:id="rId10"/>
     <sheet name="Figure - R&amp;D Funding 1951-2019" sheetId="2" r:id="rId11"/>
-    <sheet name="Figure - Research Cycle" sheetId="13" r:id="rId12"/>
-    <sheet name="Figure - Research Model" sheetId="16" r:id="rId13"/>
-    <sheet name="Figure - Theory the Org" sheetId="15" r:id="rId14"/>
-    <sheet name="Figure - Conceptual Framework" sheetId="9" r:id="rId15"/>
-    <sheet name="Figure - Literature Landscape" sheetId="14" r:id="rId16"/>
+    <sheet name="Figure - Stokes Model" sheetId="17" r:id="rId12"/>
+    <sheet name="Figure - Research Cycle" sheetId="13" r:id="rId13"/>
+    <sheet name="Figure - Research Model" sheetId="16" r:id="rId14"/>
+    <sheet name="Figure - Theory the Org" sheetId="15" r:id="rId15"/>
+    <sheet name="Figure - Conceptual Framework" sheetId="9" r:id="rId16"/>
+    <sheet name="Figure - Literature Landscape" sheetId="14" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Table - Determinants Examined'!$3:$4</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="344">
   <si>
     <t>Total</t>
   </si>
@@ -1331,6 +1332,9 @@
   </si>
   <si>
     <t>Determinants of Technology Transfer Outcomes Examined in the Technology Transfer Literature</t>
+  </si>
+  <si>
+    <t>Four-Quandrant Model of Scientific Research</t>
   </si>
 </sst>
 </file>
@@ -6323,6 +6327,618 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>555625</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>565150</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="TextBox 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22E619F1-71AD-4CC5-9132-621D821EE49E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2365375" y="7480300"/>
+          <a:ext cx="1819275" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Supply-Side</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="TextBox 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17F6B6C1-9C8C-4C36-8602-B1402047338C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5610225" y="7486650"/>
+          <a:ext cx="1838325" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Demand-Side</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>166688</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>176213</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="TextBox 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FD3130E-F110-467E-827C-B7BBA17952B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="166688" y="5305425"/>
+          <a:ext cx="1838325" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Economic</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Theory</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>185738</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>195263</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="TextBox 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1276320-DCDF-453E-8D71-B1F49995CD3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="185738" y="2276475"/>
+          <a:ext cx="1838325" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Organization</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Theory</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>217487</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>260350</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="13" name="Group 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C8E447B-EC35-45FE-B02D-B1754FAF62D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="217487" y="823912"/>
+          <a:ext cx="7967663" cy="7240588"/>
+          <a:chOff x="138112" y="836612"/>
+          <a:chExt cx="7885113" cy="7240588"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="14" name="TextBox 13">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17CB8D6C-AA5E-4022-9F24-C42E3BAD2D8F}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3948113" y="7810500"/>
+            <a:ext cx="1819275" cy="266700"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1"/>
+              <a:t>Study</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
+              <a:t> Perspective</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400" b="1"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="15" name="TextBox 14">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D91C2FB0-30B3-47C7-B9E3-B25BB2E8E3F8}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000">
+            <a:off x="-871538" y="3903662"/>
+            <a:ext cx="2286000" cy="266700"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1"/>
+              <a:t>Theorectical Framework</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="9" name="Group 8">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B95D76F0-DF02-4C8B-A70B-710F15E84147}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="1692275" y="836612"/>
+            <a:ext cx="6330950" cy="6400800"/>
+            <a:chOff x="2038350" y="1309687"/>
+            <a:chExt cx="6400800" cy="6400800"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="3" name="Straight Connector 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D052D879-FECA-4ED7-8CEE-F3EAA04FB3AD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr/>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5133975" y="1309687"/>
+              <a:ext cx="0" cy="6400800"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="4" name="Straight Connector 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4150CF5C-937B-4CE7-9150-CE8938AF1378}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr/>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm rot="16200000">
+              <a:off x="5238750" y="1309688"/>
+              <a:ext cx="0" cy="6400800"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="Freeform: Shape 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EA5A996-1E33-41F8-AA5F-AF4891FB8A2B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2038350" y="1309687"/>
+              <a:ext cx="6400800" cy="6400800"/>
+            </a:xfrm>
+            <a:custGeom>
+              <a:avLst/>
+              <a:gdLst>
+                <a:gd name="connsiteX0" fmla="*/ 0 w 4819650"/>
+                <a:gd name="connsiteY0" fmla="*/ 0 h 3143250"/>
+                <a:gd name="connsiteX1" fmla="*/ 0 w 4819650"/>
+                <a:gd name="connsiteY1" fmla="*/ 3143250 h 3143250"/>
+                <a:gd name="connsiteX2" fmla="*/ 4819650 w 4819650"/>
+                <a:gd name="connsiteY2" fmla="*/ 3143250 h 3143250"/>
+              </a:gdLst>
+              <a:ahLst/>
+              <a:cxnLst>
+                <a:cxn ang="0">
+                  <a:pos x="connsiteX0" y="connsiteY0"/>
+                </a:cxn>
+                <a:cxn ang="0">
+                  <a:pos x="connsiteX1" y="connsiteY1"/>
+                </a:cxn>
+                <a:cxn ang="0">
+                  <a:pos x="connsiteX2" y="connsiteY2"/>
+                </a:cxn>
+              </a:cxnLst>
+              <a:rect l="l" t="t" r="r" b="b"/>
+              <a:pathLst>
+                <a:path w="4819650" h="3143250">
+                  <a:moveTo>
+                    <a:pt x="0" y="0"/>
+                  </a:moveTo>
+                  <a:lnTo>
+                    <a:pt x="0" y="3143250"/>
+                  </a:lnTo>
+                  <a:lnTo>
+                    <a:pt x="4819650" y="3143250"/>
+                  </a:lnTo>
+                </a:path>
+              </a:pathLst>
+            </a:custGeom>
+            <a:noFill/>
+            <a:ln w="31750">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -6447,6 +7063,768 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>309564</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>1588</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="31" name="Group 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61C069D6-13D9-469D-8D79-2418E7167566}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="714375" y="790575"/>
+          <a:ext cx="7519989" cy="7240588"/>
+          <a:chOff x="714375" y="790575"/>
+          <a:chExt cx="7519989" cy="7240588"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="13" name="TextBox 12">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F0EEB92-5EE7-4F29-AFCE-572CEF049BDC}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4116588" y="7764463"/>
+            <a:ext cx="1838321" cy="266700"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1"/>
+              <a:t>Consideration</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
+              <a:t> of Use</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400" b="1"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="14" name="TextBox 13">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B40ACD5-7D84-40DA-B594-67082104E501}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000">
+            <a:off x="-751079" y="3865754"/>
+            <a:ext cx="3200400" cy="269492"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1"/>
+              <a:t>Desire for Fundamental</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
+              <a:t> Understanding</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400" b="1"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="22" name="Group 21">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF3C186B-6F01-4870-AE99-982AC91FF1B7}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="1837134" y="790575"/>
+            <a:ext cx="6397230" cy="6400800"/>
+            <a:chOff x="1837134" y="790575"/>
+            <a:chExt cx="6397230" cy="6400800"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="16" name="Straight Connector 15">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95E17D05-D89E-4EB3-BEB7-CF77D4167B9E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr/>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5035749" y="790575"/>
+              <a:ext cx="0" cy="6400800"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="17" name="Straight Connector 16">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBAC8ED7-A572-4653-A44D-A6E29A6FB15D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr/>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm rot="16200000">
+              <a:off x="5035749" y="792361"/>
+              <a:ext cx="0" cy="6397229"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="18" name="Freeform: Shape 17">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13A6DE05-2738-4DB6-9617-0A83D46AF2BA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1837135" y="790575"/>
+              <a:ext cx="6397229" cy="6400800"/>
+            </a:xfrm>
+            <a:custGeom>
+              <a:avLst/>
+              <a:gdLst>
+                <a:gd name="connsiteX0" fmla="*/ 0 w 4819650"/>
+                <a:gd name="connsiteY0" fmla="*/ 0 h 3143250"/>
+                <a:gd name="connsiteX1" fmla="*/ 0 w 4819650"/>
+                <a:gd name="connsiteY1" fmla="*/ 3143250 h 3143250"/>
+                <a:gd name="connsiteX2" fmla="*/ 4819650 w 4819650"/>
+                <a:gd name="connsiteY2" fmla="*/ 3143250 h 3143250"/>
+              </a:gdLst>
+              <a:ahLst/>
+              <a:cxnLst>
+                <a:cxn ang="0">
+                  <a:pos x="connsiteX0" y="connsiteY0"/>
+                </a:cxn>
+                <a:cxn ang="0">
+                  <a:pos x="connsiteX1" y="connsiteY1"/>
+                </a:cxn>
+                <a:cxn ang="0">
+                  <a:pos x="connsiteX2" y="connsiteY2"/>
+                </a:cxn>
+              </a:cxnLst>
+              <a:rect l="l" t="t" r="r" b="b"/>
+              <a:pathLst>
+                <a:path w="4819650" h="3143250">
+                  <a:moveTo>
+                    <a:pt x="0" y="0"/>
+                  </a:moveTo>
+                  <a:lnTo>
+                    <a:pt x="0" y="3143250"/>
+                  </a:lnTo>
+                  <a:lnTo>
+                    <a:pt x="4819650" y="3143250"/>
+                  </a:lnTo>
+                </a:path>
+              </a:pathLst>
+            </a:custGeom>
+            <a:noFill/>
+            <a:ln w="31750">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="19" name="TextBox 18">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89631154-EB6D-4659-86BA-C92F444A22B0}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2419350" y="7315200"/>
+            <a:ext cx="1838321" cy="266700"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0"/>
+              <a:t>No Consideration</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="21" name="TextBox 20">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5851F50-D8A6-4F20-BCB8-3C4A18967CBF}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5772150" y="7315200"/>
+            <a:ext cx="1838321" cy="266700"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0"/>
+              <a:t>Use-Driven</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="24" name="TextBox 23">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A578927F-5E98-4D5A-836A-4128F11AC49D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000">
+            <a:off x="588170" y="5276850"/>
+            <a:ext cx="1838321" cy="266700"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0"/>
+              <a:t>Low</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="25" name="TextBox 24">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72D5008F-F891-4D3B-A0BE-A8E8AE033DF1}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000">
+            <a:off x="588170" y="2205039"/>
+            <a:ext cx="1838321" cy="266700"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0"/>
+              <a:t>High</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="26" name="TextBox 25">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1FD4576-C432-4E39-8214-7794F4BFA230}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2338387" y="1743075"/>
+            <a:ext cx="2247900" cy="1190625"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1"/>
+              <a:t>Pure Basic Research</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="27" name="TextBox 26">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F293771-E21A-4EC2-8612-C3CF5D862E44}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5562600" y="1743075"/>
+            <a:ext cx="2247900" cy="1190625"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1"/>
+              <a:t>Use-Inspired</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" baseline="0"/>
+              <a:t>Basic </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1"/>
+              <a:t>Research</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="28" name="TextBox 27">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57DA036B-9CB8-4C65-BBB3-2B78226D65D1}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2338387" y="4800600"/>
+            <a:ext cx="2247900" cy="1190625"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1"/>
+              <a:t>Descriptive Research</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="30" name="TextBox 29">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9B95D51-CAA0-431E-AF0B-1E0442026B35}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5562600" y="4781550"/>
+            <a:ext cx="2247900" cy="1190625"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1"/>
+              <a:t>Applied Research</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -7094,7 +8472,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -9380,7 +10758,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -13174,7 +14552,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -14718,618 +16096,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>555625</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>565150</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="TextBox 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22E619F1-71AD-4CC5-9132-621D821EE49E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2365375" y="7480300"/>
-          <a:ext cx="1819275" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Supply-Side</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="TextBox 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17F6B6C1-9C8C-4C36-8602-B1402047338C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5610225" y="7486650"/>
-          <a:ext cx="1838325" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Demand-Side</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>166688</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>176213</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="TextBox 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FD3130E-F110-467E-827C-B7BBA17952B1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="166688" y="5305425"/>
-          <a:ext cx="1838325" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Economic</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> Theory</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>185738</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>195263</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="TextBox 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1276320-DCDF-453E-8D71-B1F49995CD3F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="185738" y="2276475"/>
-          <a:ext cx="1838325" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Organization</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> Theory</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>217487</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>260350</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="13" name="Group 12">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C8E447B-EC35-45FE-B02D-B1754FAF62D6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="217487" y="823912"/>
-          <a:ext cx="7967663" cy="7240588"/>
-          <a:chOff x="138112" y="836612"/>
-          <a:chExt cx="7885113" cy="7240588"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="14" name="TextBox 13">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17CB8D6C-AA5E-4022-9F24-C42E3BAD2D8F}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="3948113" y="7810500"/>
-            <a:ext cx="1819275" cy="266700"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="lt1"/>
-          </a:solidFill>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400" b="1"/>
-              <a:t>Study</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
-              <a:t> Perspective</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1400" b="1"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="15" name="TextBox 14">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D91C2FB0-30B3-47C7-B9E3-B25BB2E8E3F8}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm rot="16200000">
-            <a:off x="-871538" y="3903662"/>
-            <a:ext cx="2286000" cy="266700"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="lt1"/>
-          </a:solidFill>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400" b="1"/>
-              <a:t>Theorectical Framework</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="9" name="Group 8">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B95D76F0-DF02-4C8B-A70B-710F15E84147}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="1692275" y="836612"/>
-            <a:ext cx="6330950" cy="6400800"/>
-            <a:chOff x="2038350" y="1309687"/>
-            <a:chExt cx="6400800" cy="6400800"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:cxnSp macro="">
-          <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="3" name="Straight Connector 2">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D052D879-FECA-4ED7-8CEE-F3EAA04FB3AD}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvCxnSpPr/>
-          </xdr:nvCxnSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="5133975" y="1309687"/>
-              <a:ext cx="0" cy="6400800"/>
-            </a:xfrm>
-            <a:prstGeom prst="line">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln w="19050">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-        </xdr:cxnSp>
-        <xdr:cxnSp macro="">
-          <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="4" name="Straight Connector 3">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4150CF5C-937B-4CE7-9150-CE8938AF1378}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvCxnSpPr/>
-          </xdr:nvCxnSpPr>
-          <xdr:spPr>
-            <a:xfrm rot="16200000">
-              <a:off x="5238750" y="1309688"/>
-              <a:ext cx="0" cy="6400800"/>
-            </a:xfrm>
-            <a:prstGeom prst="line">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:ln w="19050">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-        </xdr:cxnSp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="5" name="Freeform: Shape 4">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EA5A996-1E33-41F8-AA5F-AF4891FB8A2B}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2038350" y="1309687"/>
-              <a:ext cx="6400800" cy="6400800"/>
-            </a:xfrm>
-            <a:custGeom>
-              <a:avLst/>
-              <a:gdLst>
-                <a:gd name="connsiteX0" fmla="*/ 0 w 4819650"/>
-                <a:gd name="connsiteY0" fmla="*/ 0 h 3143250"/>
-                <a:gd name="connsiteX1" fmla="*/ 0 w 4819650"/>
-                <a:gd name="connsiteY1" fmla="*/ 3143250 h 3143250"/>
-                <a:gd name="connsiteX2" fmla="*/ 4819650 w 4819650"/>
-                <a:gd name="connsiteY2" fmla="*/ 3143250 h 3143250"/>
-              </a:gdLst>
-              <a:ahLst/>
-              <a:cxnLst>
-                <a:cxn ang="0">
-                  <a:pos x="connsiteX0" y="connsiteY0"/>
-                </a:cxn>
-                <a:cxn ang="0">
-                  <a:pos x="connsiteX1" y="connsiteY1"/>
-                </a:cxn>
-                <a:cxn ang="0">
-                  <a:pos x="connsiteX2" y="connsiteY2"/>
-                </a:cxn>
-              </a:cxnLst>
-              <a:rect l="l" t="t" r="r" b="b"/>
-              <a:pathLst>
-                <a:path w="4819650" h="3143250">
-                  <a:moveTo>
-                    <a:pt x="0" y="0"/>
-                  </a:moveTo>
-                  <a:lnTo>
-                    <a:pt x="0" y="3143250"/>
-                  </a:lnTo>
-                  <a:lnTo>
-                    <a:pt x="4819650" y="3143250"/>
-                  </a:lnTo>
-                </a:path>
-              </a:pathLst>
-            </a:custGeom>
-            <a:noFill/>
-            <a:ln w="31750">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -16931,7 +17697,9 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="O40" sqref="O40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -16945,7 +17713,7 @@
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
-        <v>331</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -16960,9 +17728,40 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="108" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="108"/>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="110" t="s">
+        <v>331</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="70" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -17039,7 +17838,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -17067,7 +17866,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -17092,7 +17891,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -17124,7 +17923,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17635,8 +18436,8 @@
   </sheetPr>
   <dimension ref="A1:AA78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E15" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="4" ySplit="4" topLeftCell="E58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight"/>
@@ -17825,7 +18626,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="49"/>
       <c r="B5" s="49" t="s">
         <v>294</v>
@@ -17856,7 +18657,7 @@
       <c r="Z5" s="78"/>
       <c r="AA5" s="63"/>
     </row>
-    <row r="6" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="94"/>
       <c r="B6" s="82"/>
       <c r="C6" s="81" t="s">
@@ -17899,7 +18700,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="94"/>
       <c r="B7" s="82"/>
       <c r="C7" s="93" t="s">
@@ -17942,7 +18743,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="94"/>
       <c r="B8" s="82"/>
       <c r="C8" s="81" t="s">
@@ -17985,7 +18786,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="94"/>
       <c r="B9" s="82"/>
       <c r="C9" s="93" t="s">
@@ -18034,7 +18835,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="94"/>
       <c r="B10" s="30"/>
       <c r="C10" s="32" t="s">
@@ -18091,7 +18892,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="94"/>
       <c r="B11" s="82"/>
       <c r="C11" s="95" t="s">
@@ -18140,7 +18941,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="94"/>
       <c r="B12" s="94"/>
       <c r="C12" s="95"/>
@@ -18169,7 +18970,7 @@
       <c r="Z12" s="99"/>
       <c r="AA12" s="100"/>
     </row>
-    <row r="13" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="49"/>
       <c r="B13" s="49" t="s">
         <v>271</v>
@@ -18200,7 +19001,7 @@
       <c r="Z13" s="78"/>
       <c r="AA13" s="63"/>
     </row>
-    <row r="14" spans="1:27" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="94"/>
       <c r="B14" s="30"/>
       <c r="C14" s="32" t="s">
@@ -18251,7 +19052,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" ht="49.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="94"/>
       <c r="B15" s="30"/>
       <c r="C15" s="32" t="s">
@@ -18302,7 +19103,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="94"/>
       <c r="B16" s="82"/>
       <c r="C16" s="81" t="s">
@@ -18359,7 +19160,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="94"/>
       <c r="B17" s="82"/>
       <c r="C17" s="81" t="s">
@@ -18416,7 +19217,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="18" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="94"/>
       <c r="B18" s="60"/>
       <c r="C18" s="59" t="s">
@@ -18459,7 +19260,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="94"/>
       <c r="B19" s="30"/>
       <c r="C19" s="32" t="s">
@@ -18502,7 +19303,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="94"/>
       <c r="B20" s="30"/>
       <c r="C20" s="32" t="s">
@@ -18545,7 +19346,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="94"/>
       <c r="B21" s="30"/>
       <c r="C21" s="32" t="s">
@@ -18588,7 +19389,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="94"/>
       <c r="B22" s="82"/>
       <c r="C22" s="81" t="s">
@@ -18645,7 +19446,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="23" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="94"/>
       <c r="B23" s="82"/>
       <c r="C23" s="81" t="s">
@@ -18702,7 +19503,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="24" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="94"/>
       <c r="B24" s="30"/>
       <c r="C24" s="32" t="s">
@@ -18759,7 +19560,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="25" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="94"/>
       <c r="B25" s="30"/>
       <c r="C25" s="32" t="s">
@@ -18816,7 +19617,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="26" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="94"/>
       <c r="B26" s="82"/>
       <c r="C26" s="81" t="s">
@@ -18873,7 +19674,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="27" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="94"/>
       <c r="B27" s="82"/>
       <c r="C27" s="81" t="s">
@@ -18930,7 +19731,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="28" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="94"/>
       <c r="B28" s="94"/>
       <c r="C28" s="93"/>
@@ -18959,7 +19760,7 @@
       <c r="Z28" s="78"/>
       <c r="AA28" s="63"/>
     </row>
-    <row r="29" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="94"/>
       <c r="B29" s="31" t="s">
         <v>287</v>
@@ -18990,7 +19791,7 @@
       <c r="Z29" s="78"/>
       <c r="AA29" s="63"/>
     </row>
-    <row r="30" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="94"/>
       <c r="B30" s="82"/>
       <c r="C30" s="81" t="s">
@@ -19039,7 +19840,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="31" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="94"/>
       <c r="B31" s="94"/>
       <c r="C31" s="93" t="s">
@@ -19082,7 +19883,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="32" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="94"/>
       <c r="B32" s="94"/>
       <c r="C32" s="93" t="s">
@@ -19125,7 +19926,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="33" spans="1:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="94"/>
       <c r="B33" s="94"/>
       <c r="C33" s="93" t="s">
@@ -19168,7 +19969,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="34" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="94"/>
       <c r="B34" s="94"/>
       <c r="C34" s="93"/>
@@ -19197,7 +19998,7 @@
       <c r="Z34" s="78"/>
       <c r="AA34" s="63"/>
     </row>
-    <row r="35" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="49"/>
       <c r="B35" s="49" t="s">
         <v>293</v>
@@ -19228,7 +20029,7 @@
       <c r="Z35" s="78"/>
       <c r="AA35" s="63"/>
     </row>
-    <row r="36" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="94"/>
       <c r="B36" s="30"/>
       <c r="C36" s="32" t="s">
@@ -19271,7 +20072,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="37" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="94"/>
       <c r="B37" s="30"/>
       <c r="C37" s="32" t="s">
@@ -19314,7 +20115,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:27" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="94"/>
       <c r="B38" s="94"/>
       <c r="C38" s="93" t="s">
@@ -19357,7 +20158,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="39" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="94"/>
       <c r="B39" s="94"/>
       <c r="C39" s="93" t="s">
@@ -19402,7 +20203,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="40" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="94"/>
       <c r="B40" s="94"/>
       <c r="C40" s="93" t="s">
@@ -19447,7 +20248,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="41" spans="1:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="94"/>
       <c r="B41" s="94"/>
       <c r="C41" s="93" t="s">
@@ -19496,7 +20297,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="42" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="94"/>
       <c r="B42" s="94"/>
       <c r="C42" s="93" t="s">
@@ -19539,7 +20340,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="43" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="94"/>
       <c r="B43" s="94"/>
       <c r="C43" s="93" t="s">
@@ -19584,7 +20385,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="44" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="94"/>
       <c r="B44" s="94"/>
       <c r="C44" s="93" t="s">
@@ -19629,7 +20430,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="45" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="94"/>
       <c r="B45" s="82"/>
       <c r="C45" s="81" t="s">
@@ -19686,7 +20487,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="46" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="94"/>
       <c r="B46" s="60"/>
       <c r="C46" s="59" t="s">
@@ -19731,7 +20532,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="47" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="94"/>
       <c r="B47" s="60"/>
       <c r="C47" s="59" t="s">
@@ -19774,7 +20575,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="48" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="94"/>
       <c r="B48" s="82"/>
       <c r="C48" s="81" t="s">
@@ -19817,7 +20618,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="49" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="94"/>
       <c r="B49" s="94"/>
       <c r="C49" s="93" t="s">
@@ -19860,7 +20661,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="50" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="94"/>
       <c r="B50" s="82"/>
       <c r="C50" s="81" t="s">
@@ -19903,7 +20704,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="51" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="94"/>
       <c r="B51" s="82"/>
       <c r="C51" s="81" t="s">
@@ -19946,7 +20747,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="52" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="94"/>
       <c r="B52" s="89"/>
       <c r="C52" s="88" t="s">
@@ -19989,7 +20790,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="53" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="94"/>
       <c r="B53" s="89"/>
       <c r="C53" s="88" t="s">
@@ -20032,7 +20833,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="54" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="94"/>
       <c r="B54" s="94"/>
       <c r="C54" s="93"/>

</xml_diff>

<commit_message>
Added citations for low tech transfer pct and figure of the valley of death
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="11" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="11" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId1"/>
@@ -26,9 +26,10 @@
     <sheet name="Figure - Stokes Model" sheetId="17" r:id="rId12"/>
     <sheet name="Figure - Research Cycle" sheetId="13" r:id="rId13"/>
     <sheet name="Figure - Research Model" sheetId="16" r:id="rId14"/>
-    <sheet name="Figure - Theory the Org" sheetId="15" r:id="rId15"/>
-    <sheet name="Figure - Conceptual Framework" sheetId="9" r:id="rId16"/>
-    <sheet name="Figure - Literature Landscape" sheetId="14" r:id="rId17"/>
+    <sheet name="Figure - Valley of Death" sheetId="18" r:id="rId15"/>
+    <sheet name="Figure - Theory the Org" sheetId="15" r:id="rId16"/>
+    <sheet name="Figure - Conceptual Framework" sheetId="9" r:id="rId17"/>
+    <sheet name="Figure - Literature Landscape" sheetId="14" r:id="rId18"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Table - Determinants Examined'!$3:$4</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="346">
   <si>
     <t>Total</t>
   </si>
@@ -1335,6 +1336,35 @@
   </si>
   <si>
     <t>Four-Quandrant Model of Scientific Research</t>
+  </si>
+  <si>
+    <t>The Valley of Death</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dacey, J. (2014). Navigating the valley of death. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Physics World, 27</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(11), 29. </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1673,7 +1703,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -2023,6 +2053,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -6328,6 +6361,1550 @@
 </file>
 
 <file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>604837</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>604837</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EDF8CFA-62CE-4CD9-A1E4-E2051F7B335E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3043237" y="4857750"/>
+          <a:ext cx="1828800" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>DP</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="-25000">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>1</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> : Technology maturity level must be at least M.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" baseline="-25000">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>604837</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>604837</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B0DC8DD-F6A6-40DC-831A-338DFA26E651}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3043237" y="5976937"/>
+          <a:ext cx="1828800" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>DP</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="-25000">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>2</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>604837</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>604837</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CB89335-6580-458F-8E57-39173AA7E02B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3043237" y="7496175"/>
+          <a:ext cx="1828800" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>DP</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="-25000">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>n</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA9B58F4-BE0E-4B02-98BA-EB1FC72D1482}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="3"/>
+          <a:endCxn id="8" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2314575" y="3681412"/>
+          <a:ext cx="3248025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>525779</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>604836</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Connector: Elbow 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3BFF46A-19D4-4457-9D4F-D6C6E98861B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="32" idx="2"/>
+          <a:endCxn id="9" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="1803558" y="4075271"/>
+          <a:ext cx="1181100" cy="1298257"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>119061</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>604838</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>128586</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Connector: Elbow 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52FF6E3E-4187-43E2-8A05-5FF131F06074}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="2"/>
+          <a:endCxn id="10" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="1073944" y="4464843"/>
+          <a:ext cx="2295525" cy="1643062"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>468630</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>604837</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Connector: Elbow 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BB21842-A987-4D88-A9C0-33EB2875A2D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="35" idx="2"/>
+          <a:endCxn id="11" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="150971" y="5061108"/>
+          <a:ext cx="3819525" cy="1965007"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>604837</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>11430</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Connector: Elbow 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1206A40E-C509-4A7E-8F73-FB30DDBCCC48}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="9" idx="3"/>
+          <a:endCxn id="37" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4872037" y="4133850"/>
+          <a:ext cx="1235393" cy="1181100"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>604837</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Connector: Elbow 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CB449B0-6103-42E2-BE6D-DE4E2DD869CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="10" idx="3"/>
+          <a:endCxn id="8" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4872037" y="4138612"/>
+          <a:ext cx="1604963" cy="2295525"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>604837</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Connector: Elbow 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{703ADAEA-785F-4395-B619-4D90E53856D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="11" idx="3"/>
+          <a:endCxn id="38" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4872037" y="4124325"/>
+          <a:ext cx="1978343" cy="3829050"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>123824</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>80964</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>157164</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11B7D077-5FD9-4402-9CB4-F8AAA2C8A7B5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="3729037" y="7010401"/>
+          <a:ext cx="457200" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>. . .</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Rectangle 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{607722A7-0A06-44C0-835D-2088A6A4A6C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="2409825" y="1171575"/>
+          <a:ext cx="1828800" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Asborptive capacity</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Rectangle 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC4F0E75-89CB-4D8A-8F57-C110832D2580}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="3514725" y="1171575"/>
+          <a:ext cx="1828800" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Organizational slack</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>278130</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8CC71DE-30FA-4561-98F8-E7B24F9EBA13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="16" idx="1"/>
+          <a:endCxn id="48" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3324225" y="2562225"/>
+          <a:ext cx="1905" cy="1123950"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>173355</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{927C467B-1531-4473-9834-ECF608E77259}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="18" idx="1"/>
+          <a:endCxn id="50" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4429125" y="2562225"/>
+          <a:ext cx="11430" cy="1123950"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="46" name="Group 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8AB265B-49A2-437B-828B-4AD1C1E7D9E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="485775" y="3219450"/>
+          <a:ext cx="1828800" cy="919162"/>
+          <a:chOff x="485775" y="3219450"/>
+          <a:chExt cx="1828800" cy="919162"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="2" name="Rectangle 1">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7FBD581-9132-4175-AC34-BD98A9A52BD0}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="485775" y="3224212"/>
+            <a:ext cx="1828800" cy="914400"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Options</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> of technologies available for assimilation</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="32" name="Rectangle 31">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DC3709F-D574-4E57-89EC-0CDECD34117B}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1562100" y="3219450"/>
+            <a:ext cx="365760" cy="914400"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="6350">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="35" name="Rectangle 34">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FDD3252-11D9-4AEB-B425-CC96512F2D88}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="895350" y="3219450"/>
+            <a:ext cx="365760" cy="914400"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="6350">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="47" name="Group 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7ADE4B7-8C02-4E8B-ACFE-60C896C73203}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="5562600" y="3209925"/>
+          <a:ext cx="1828800" cy="928687"/>
+          <a:chOff x="5562600" y="3209925"/>
+          <a:chExt cx="1828800" cy="928687"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="Rectangle 7">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78775CEB-9626-4660-A44C-8F70D0A13B5B}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5562600" y="3224212"/>
+            <a:ext cx="1828800" cy="914400"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Add the technology to the decision agenda</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="37" name="Rectangle 36">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{114C3F18-C8CE-46E0-B7B4-16DED6DD6983}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5924550" y="3219450"/>
+            <a:ext cx="365760" cy="914400"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="6350">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="38" name="Rectangle 37">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A64F5185-592A-40E2-9337-78D549A3B3AB}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6667500" y="3209925"/>
+            <a:ext cx="365760" cy="914400"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="6350">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>461010</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>40005</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="Rectangle 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C3D8628-D7D9-4F45-8B23-01A54DB84423}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3143250" y="3686175"/>
+          <a:ext cx="365760" cy="182880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>356235</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>40005</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="Rectangle 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3342E0FA-E413-4BF7-A9D0-695F0D0764AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4257675" y="3686175"/>
+          <a:ext cx="365760" cy="182880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -10760,6 +12337,116 @@
 
 <file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>78275</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="http://live.iop-pp01.agh.sleek.net/wp-content/uploads/2014/10/PWNov14DACEY-fig1-full.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E1C6410-71A1-42F0-8C78-6D5A348D191D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="76200" y="657226"/>
+          <a:ext cx="5943600" cy="3821599"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>9530</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>74848</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20C8BA26-C7F2-484F-A99A-CCEBC4C385C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="76200" y="4600580"/>
+          <a:ext cx="5943600" cy="4637318"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
@@ -14552,1550 +16239,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>604837</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>604837</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Rectangle 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EDF8CFA-62CE-4CD9-A1E4-E2051F7B335E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3043237" y="4857750"/>
-          <a:ext cx="1828800" cy="914400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>DP</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" baseline="-25000">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>1</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> : Technology maturity level must be at least M.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1200" baseline="-25000">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>604837</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>604837</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Rectangle 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B0DC8DD-F6A6-40DC-831A-338DFA26E651}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3043237" y="5976937"/>
-          <a:ext cx="1828800" cy="914400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>DP</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" baseline="-25000">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>2</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>604837</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>604837</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="Rectangle 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CB89335-6580-458F-8E57-39173AA7E02B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3043237" y="7496175"/>
-          <a:ext cx="1828800" cy="914400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>DP</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" baseline="-25000">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>n</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA9B58F4-BE0E-4B02-98BA-EB1FC72D1482}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="2" idx="3"/>
-          <a:endCxn id="8" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2314575" y="3681412"/>
-          <a:ext cx="3248025" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>525779</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>604836</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="15" name="Connector: Elbow 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3BFF46A-19D4-4457-9D4F-D6C6E98861B2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="32" idx="2"/>
-          <a:endCxn id="9" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000" flipH="1">
-          <a:off x="1803558" y="4075271"/>
-          <a:ext cx="1181100" cy="1298257"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>180976</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>119061</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>604838</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>128586</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="17" name="Connector: Elbow 16">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52FF6E3E-4187-43E2-8A05-5FF131F06074}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="2" idx="2"/>
-          <a:endCxn id="10" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000" flipH="1">
-          <a:off x="1073944" y="4464843"/>
-          <a:ext cx="2295525" cy="1643062"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>468630</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>604837</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="19" name="Connector: Elbow 18">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BB21842-A987-4D88-A9C0-33EB2875A2D0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="35" idx="2"/>
-          <a:endCxn id="11" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000" flipH="1">
-          <a:off x="150971" y="5061108"/>
-          <a:ext cx="3819525" cy="1965007"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>604837</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>11430</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="21" name="Connector: Elbow 20">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1206A40E-C509-4A7E-8F73-FB30DDBCCC48}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="9" idx="3"/>
-          <a:endCxn id="37" idx="2"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="4872037" y="4133850"/>
-          <a:ext cx="1235393" cy="1181100"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>604837</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="23" name="Connector: Elbow 22">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CB449B0-6103-42E2-BE6D-DE4E2DD869CE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="10" idx="3"/>
-          <a:endCxn id="8" idx="2"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="4872037" y="4138612"/>
-          <a:ext cx="1604963" cy="2295525"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>604837</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>144780</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="25" name="Connector: Elbow 24">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{703ADAEA-785F-4395-B619-4D90E53856D5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="11" idx="3"/>
-          <a:endCxn id="38" idx="2"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="4872037" y="4124325"/>
-          <a:ext cx="1978343" cy="3829050"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>123824</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>80964</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>476249</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>157164</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11B7D077-5FD9-4402-9CB4-F8AAA2C8A7B5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="3729037" y="7010401"/>
-          <a:ext cx="457200" cy="352425"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>. . .</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="Rectangle 15">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{607722A7-0A06-44C0-835D-2088A6A4A6C3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000">
-          <a:off x="2409825" y="1171575"/>
-          <a:ext cx="1828800" cy="914400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Asborptive capacity</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="Rectangle 17">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC4F0E75-89CB-4D8A-8F57-C110832D2580}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000">
-          <a:off x="3514725" y="1171575"/>
-          <a:ext cx="1828800" cy="914400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Organizational slack</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>278130</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8CC71DE-30FA-4561-98F8-E7B24F9EBA13}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="16" idx="1"/>
-          <a:endCxn id="48" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3324225" y="2562225"/>
-          <a:ext cx="1905" cy="1123950"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>173355</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{927C467B-1531-4473-9834-ECF608E77259}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="18" idx="1"/>
-          <a:endCxn id="50" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4429125" y="2562225"/>
-          <a:ext cx="11430" cy="1123950"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="46" name="Group 45">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8AB265B-49A2-437B-828B-4AD1C1E7D9E9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="485775" y="3219450"/>
-          <a:ext cx="1828800" cy="919162"/>
-          <a:chOff x="485775" y="3219450"/>
-          <a:chExt cx="1828800" cy="919162"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="2" name="Rectangle 1">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7FBD581-9132-4175-AC34-BD98A9A52BD0}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="485775" y="3224212"/>
-            <a:ext cx="1828800" cy="914400"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="19050">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-US" sz="1200">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Options</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1200" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t> of technologies available for assimilation</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="32" name="Rectangle 31">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DC3709F-D574-4E57-89EC-0CDECD34117B}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1562100" y="3219450"/>
-            <a:ext cx="365760" cy="914400"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="6350">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-US" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="35" name="Rectangle 34">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FDD3252-11D9-4AEB-B425-CC96512F2D88}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="895350" y="3219450"/>
-            <a:ext cx="365760" cy="914400"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="6350">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-US" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="47" name="Group 46">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7ADE4B7-8C02-4E8B-ACFE-60C896C73203}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="5562600" y="3209925"/>
-          <a:ext cx="1828800" cy="928687"/>
-          <a:chOff x="5562600" y="3209925"/>
-          <a:chExt cx="1828800" cy="928687"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="8" name="Rectangle 7">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78775CEB-9626-4660-A44C-8F70D0A13B5B}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5562600" y="3224212"/>
-            <a:ext cx="1828800" cy="914400"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="19050">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-US" sz="1200" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Add the technology to the decision agenda</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1200">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="37" name="Rectangle 36">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{114C3F18-C8CE-46E0-B7B4-16DED6DD6983}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5924550" y="3219450"/>
-            <a:ext cx="365760" cy="914400"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="6350">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-US" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="38" name="Rectangle 37">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A64F5185-592A-40E2-9337-78D549A3B3AB}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="6667500" y="3209925"/>
-            <a:ext cx="365760" cy="914400"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="6350">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-US" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>461010</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>40005</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="48" name="Rectangle 47">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C3D8628-D7D9-4F45-8B23-01A54DB84423}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3143250" y="3686175"/>
-          <a:ext cx="365760" cy="182880"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>356235</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>40005</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="50" name="Rectangle 49">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3342E0FA-E413-4BF7-A9D0-695F0D0764AC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4257675" y="3686175"/>
-          <a:ext cx="365760" cy="182880"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -17761,7 +17904,9 @@
   </sheetPr>
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -17839,6 +17984,48 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J50"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="108" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="110" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="122" t="s">
+        <v>345</v>
+      </c>
+      <c r="B50" s="122"/>
+      <c r="C50" s="122"/>
+      <c r="D50" s="122"/>
+      <c r="E50" s="122"/>
+      <c r="F50" s="122"/>
+      <c r="G50" s="122"/>
+      <c r="H50" s="122"/>
+      <c r="I50" s="122"/>
+      <c r="J50" s="122"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A50:J50"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -17866,7 +18053,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -17891,7 +18078,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>

</xml_diff>

<commit_message>
Additions to section on uncertainty avoidance
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="11" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId1"/>
@@ -980,9 +980,6 @@
     <t>Exogenous</t>
   </si>
   <si>
-    <t>Development stage of technology</t>
-  </si>
-  <si>
     <t>Munteanu (2012)</t>
   </si>
   <si>
@@ -1365,6 +1362,9 @@
       </rPr>
       <t xml:space="preserve">(11), 29. </t>
     </r>
+  </si>
+  <si>
+    <t>Technology maturity level</t>
   </si>
 </sst>
 </file>
@@ -1467,12 +1467,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="19">
@@ -1703,7 +1709,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -2056,6 +2062,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -17848,7 +17878,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="108" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
@@ -17856,7 +17886,7 @@
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -17879,7 +17909,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="108" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
@@ -17887,7 +17917,7 @@
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -17912,12 +17942,12 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="108" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -17947,7 +17977,7 @@
     <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="110"/>
       <c r="K12" s="79" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -17973,7 +18003,7 @@
     </row>
     <row r="36" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K36" s="79" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -17987,23 +18017,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="108" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="122" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B50" s="122"/>
       <c r="C50" s="122"/>
@@ -18038,12 +18068,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="108" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -18063,12 +18093,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="108" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -18091,12 +18121,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="108" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -18153,7 +18183,7 @@
       </c>
       <c r="G3" s="34"/>
       <c r="H3" s="34" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -18173,7 +18203,7 @@
       </c>
       <c r="G4" s="109"/>
       <c r="H4" s="109" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -18193,7 +18223,7 @@
       </c>
       <c r="G5" s="109"/>
       <c r="H5" s="109" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
@@ -18213,7 +18243,7 @@
       </c>
       <c r="G6" s="109"/>
       <c r="H6" s="109" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -18233,7 +18263,7 @@
       </c>
       <c r="G7" s="109"/>
       <c r="H7" s="109" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -18253,7 +18283,7 @@
       </c>
       <c r="G8" s="109"/>
       <c r="H8" s="109" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -18273,7 +18303,7 @@
       </c>
       <c r="G9" s="109"/>
       <c r="H9" s="109" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -18293,7 +18323,7 @@
       </c>
       <c r="G10" s="109"/>
       <c r="H10" s="109" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -18313,7 +18343,7 @@
       </c>
       <c r="G11" s="109"/>
       <c r="H11" s="109" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -18333,7 +18363,7 @@
       </c>
       <c r="G12" s="109"/>
       <c r="H12" s="109" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
@@ -18353,7 +18383,7 @@
       </c>
       <c r="G13" s="109"/>
       <c r="H13" s="109" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -18373,7 +18403,7 @@
       </c>
       <c r="G14" s="109"/>
       <c r="H14" s="109" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -18393,7 +18423,7 @@
       </c>
       <c r="G15" s="109"/>
       <c r="H15" s="109" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="72" customHeight="1" x14ac:dyDescent="0.25">
@@ -18413,7 +18443,7 @@
       </c>
       <c r="G16" s="38"/>
       <c r="H16" s="38" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -18433,7 +18463,7 @@
       </c>
       <c r="G17" s="38"/>
       <c r="H17" s="38" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -18623,11 +18653,11 @@
   </sheetPr>
   <dimension ref="A1:AA78"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E58" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="4" ySplit="4" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18671,7 +18701,7 @@
     </row>
     <row r="2" spans="1:27" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E2" s="61"/>
       <c r="F2" s="61"/>
@@ -18703,21 +18733,21 @@
       <c r="C3" s="70"/>
       <c r="D3" s="71"/>
       <c r="E3" s="116" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F3" s="117"/>
       <c r="G3" s="117"/>
       <c r="H3" s="114"/>
       <c r="I3" s="113" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J3" s="114"/>
       <c r="K3" s="113" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L3" s="115"/>
       <c r="M3" s="116" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="N3" s="117"/>
       <c r="O3" s="114"/>
@@ -18739,21 +18769,21 @@
     <row r="4" spans="1:27" ht="170.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="67"/>
       <c r="B4" s="104" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C4" s="68"/>
       <c r="D4" s="68"/>
       <c r="E4" s="105" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F4" s="107" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G4" s="62" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H4" s="106" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I4" s="65" t="s">
         <v>192</v>
@@ -18768,16 +18798,16 @@
         <v>251</v>
       </c>
       <c r="M4" s="105" t="s">
+        <v>284</v>
+      </c>
+      <c r="N4" s="62" t="s">
         <v>285</v>
       </c>
-      <c r="N4" s="62" t="s">
-        <v>286</v>
-      </c>
       <c r="O4" s="106" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="P4" s="62" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="Q4" s="62" t="s">
         <v>229</v>
@@ -18804,19 +18834,19 @@
         <v>228</v>
       </c>
       <c r="Y4" s="62" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Z4" s="62" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AA4" s="72" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="49"/>
       <c r="B5" s="49" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C5" s="93"/>
       <c r="D5" s="93"/>
@@ -18844,7 +18874,7 @@
       <c r="Z5" s="78"/>
       <c r="AA5" s="63"/>
     </row>
-    <row r="6" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="94"/>
       <c r="B6" s="82"/>
       <c r="C6" s="81" t="s">
@@ -18887,7 +18917,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="94"/>
       <c r="B7" s="82"/>
       <c r="C7" s="93" t="s">
@@ -18930,7 +18960,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="94"/>
       <c r="B8" s="82"/>
       <c r="C8" s="81" t="s">
@@ -18973,11 +19003,11 @@
         <v>243</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="94"/>
       <c r="B9" s="82"/>
       <c r="C9" s="93" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D9" s="81"/>
       <c r="E9" s="74"/>
@@ -19019,10 +19049,10 @@
       <c r="Y9" s="78"/>
       <c r="Z9" s="78"/>
       <c r="AA9" s="63" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="94"/>
       <c r="B10" s="30"/>
       <c r="C10" s="32" t="s">
@@ -19079,56 +19109,56 @@
         <v>226</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="94"/>
-      <c r="B11" s="82"/>
-      <c r="C11" s="95" t="s">
+    <row r="11" spans="1:27" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="123"/>
+      <c r="B11" s="123"/>
+      <c r="C11" s="124" t="s">
+        <v>345</v>
+      </c>
+      <c r="D11" s="124"/>
+      <c r="E11" s="125"/>
+      <c r="F11" s="126" t="s">
+        <v>201</v>
+      </c>
+      <c r="G11" s="127"/>
+      <c r="H11" s="128"/>
+      <c r="I11" s="125" t="s">
+        <v>201</v>
+      </c>
+      <c r="J11" s="128"/>
+      <c r="K11" s="125" t="s">
+        <v>201</v>
+      </c>
+      <c r="L11" s="128"/>
+      <c r="M11" s="125" t="s">
+        <v>201</v>
+      </c>
+      <c r="N11" s="127"/>
+      <c r="O11" s="128"/>
+      <c r="P11" s="127"/>
+      <c r="Q11" s="127" t="s">
+        <v>201</v>
+      </c>
+      <c r="R11" s="127" t="s">
+        <v>201</v>
+      </c>
+      <c r="S11" s="129" t="s">
+        <v>201</v>
+      </c>
+      <c r="T11" s="129" t="s">
+        <v>201</v>
+      </c>
+      <c r="U11" s="129"/>
+      <c r="V11" s="129"/>
+      <c r="W11" s="129"/>
+      <c r="X11" s="129"/>
+      <c r="Y11" s="129"/>
+      <c r="Z11" s="129"/>
+      <c r="AA11" s="130" t="s">
         <v>252</v>
       </c>
-      <c r="D11" s="81"/>
-      <c r="E11" s="96"/>
-      <c r="F11" s="102" t="s">
-        <v>201</v>
-      </c>
-      <c r="G11" s="98"/>
-      <c r="H11" s="97"/>
-      <c r="I11" s="96" t="s">
-        <v>201</v>
-      </c>
-      <c r="J11" s="97"/>
-      <c r="K11" s="96" t="s">
-        <v>201</v>
-      </c>
-      <c r="L11" s="97"/>
-      <c r="M11" s="96" t="s">
-        <v>201</v>
-      </c>
-      <c r="N11" s="98"/>
-      <c r="O11" s="97"/>
-      <c r="P11" s="98"/>
-      <c r="Q11" s="98" t="s">
-        <v>201</v>
-      </c>
-      <c r="R11" s="98" t="s">
-        <v>201</v>
-      </c>
-      <c r="S11" s="99" t="s">
-        <v>201</v>
-      </c>
-      <c r="T11" s="99" t="s">
-        <v>201</v>
-      </c>
-      <c r="U11" s="99"/>
-      <c r="V11" s="99"/>
-      <c r="W11" s="99"/>
-      <c r="X11" s="99"/>
-      <c r="Y11" s="99"/>
-      <c r="Z11" s="99"/>
-      <c r="AA11" s="100" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="94"/>
       <c r="B12" s="94"/>
       <c r="C12" s="95"/>
@@ -19157,10 +19187,10 @@
       <c r="Z12" s="99"/>
       <c r="AA12" s="100"/>
     </row>
-    <row r="13" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="49"/>
       <c r="B13" s="49" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C13" s="93"/>
       <c r="D13" s="93"/>
@@ -19188,7 +19218,7 @@
       <c r="Z13" s="78"/>
       <c r="AA13" s="63"/>
     </row>
-    <row r="14" spans="1:27" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="94"/>
       <c r="B14" s="30"/>
       <c r="C14" s="32" t="s">
@@ -19236,10 +19266,10 @@
       <c r="Y14" s="78"/>
       <c r="Z14" s="78"/>
       <c r="AA14" s="63" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" ht="49.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="94"/>
       <c r="B15" s="30"/>
       <c r="C15" s="32" t="s">
@@ -19287,10 +19317,10 @@
       <c r="Y15" s="78"/>
       <c r="Z15" s="78"/>
       <c r="AA15" s="63" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="94"/>
       <c r="B16" s="82"/>
       <c r="C16" s="81" t="s">
@@ -19347,7 +19377,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="94"/>
       <c r="B17" s="82"/>
       <c r="C17" s="81" t="s">
@@ -19404,7 +19434,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="18" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="94"/>
       <c r="B18" s="60"/>
       <c r="C18" s="59" t="s">
@@ -19447,11 +19477,11 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="94"/>
       <c r="B19" s="30"/>
       <c r="C19" s="32" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D19" s="32"/>
       <c r="E19" s="74"/>
@@ -19490,11 +19520,11 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="94"/>
       <c r="B20" s="30"/>
       <c r="C20" s="32" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D20" s="32"/>
       <c r="E20" s="74"/>
@@ -19533,11 +19563,11 @@
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="94"/>
       <c r="B21" s="30"/>
       <c r="C21" s="32" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D21" s="32"/>
       <c r="E21" s="74"/>
@@ -19576,7 +19606,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="94"/>
       <c r="B22" s="82"/>
       <c r="C22" s="81" t="s">
@@ -19633,7 +19663,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="23" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="94"/>
       <c r="B23" s="82"/>
       <c r="C23" s="81" t="s">
@@ -19690,7 +19720,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="24" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="94"/>
       <c r="B24" s="30"/>
       <c r="C24" s="32" t="s">
@@ -19747,7 +19777,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="25" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="94"/>
       <c r="B25" s="30"/>
       <c r="C25" s="32" t="s">
@@ -19804,7 +19834,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="26" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="94"/>
       <c r="B26" s="82"/>
       <c r="C26" s="81" t="s">
@@ -19861,7 +19891,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="27" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="94"/>
       <c r="B27" s="82"/>
       <c r="C27" s="81" t="s">
@@ -19918,7 +19948,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="28" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="94"/>
       <c r="B28" s="94"/>
       <c r="C28" s="93"/>
@@ -19947,10 +19977,10 @@
       <c r="Z28" s="78"/>
       <c r="AA28" s="63"/>
     </row>
-    <row r="29" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="94"/>
       <c r="B29" s="31" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C29" s="93"/>
       <c r="D29" s="93"/>
@@ -19978,7 +20008,7 @@
       <c r="Z29" s="78"/>
       <c r="AA29" s="63"/>
     </row>
-    <row r="30" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="94"/>
       <c r="B30" s="82"/>
       <c r="C30" s="81" t="s">
@@ -20024,10 +20054,10 @@
       <c r="Y30" s="78"/>
       <c r="Z30" s="78"/>
       <c r="AA30" s="63" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="31" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="94"/>
       <c r="B31" s="94"/>
       <c r="C31" s="93" t="s">
@@ -20070,7 +20100,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="32" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="94"/>
       <c r="B32" s="94"/>
       <c r="C32" s="93" t="s">
@@ -20113,11 +20143,11 @@
         <v>243</v>
       </c>
     </row>
-    <row r="33" spans="1:27" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="94"/>
       <c r="B33" s="94"/>
       <c r="C33" s="93" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D33" s="93"/>
       <c r="E33" s="74"/>
@@ -20153,10 +20183,10 @@
       <c r="Y33" s="78"/>
       <c r="Z33" s="78"/>
       <c r="AA33" s="63" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="34" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="94"/>
       <c r="B34" s="94"/>
       <c r="C34" s="93"/>
@@ -20185,10 +20215,10 @@
       <c r="Z34" s="78"/>
       <c r="AA34" s="63"/>
     </row>
-    <row r="35" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="49"/>
       <c r="B35" s="49" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C35" s="93"/>
       <c r="D35" s="93"/>
@@ -20216,7 +20246,7 @@
       <c r="Z35" s="78"/>
       <c r="AA35" s="63"/>
     </row>
-    <row r="36" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="94"/>
       <c r="B36" s="30"/>
       <c r="C36" s="32" t="s">
@@ -20259,7 +20289,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="37" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="94"/>
       <c r="B37" s="30"/>
       <c r="C37" s="32" t="s">
@@ -20302,11 +20332,11 @@
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:27" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="94"/>
       <c r="B38" s="94"/>
       <c r="C38" s="93" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D38" s="93"/>
       <c r="E38" s="74"/>
@@ -20342,10 +20372,10 @@
       <c r="Y38" s="78"/>
       <c r="Z38" s="78"/>
       <c r="AA38" s="63" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="39" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="94"/>
       <c r="B39" s="94"/>
       <c r="C39" s="93" t="s">
@@ -20390,7 +20420,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="40" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="94"/>
       <c r="B40" s="94"/>
       <c r="C40" s="93" t="s">
@@ -20435,11 +20465,11 @@
         <v>200</v>
       </c>
     </row>
-    <row r="41" spans="1:27" ht="35.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="94"/>
       <c r="B41" s="94"/>
       <c r="C41" s="93" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D41" s="93"/>
       <c r="E41" s="74"/>
@@ -20481,10 +20511,10 @@
       <c r="Y41" s="78"/>
       <c r="Z41" s="78"/>
       <c r="AA41" s="63" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="42" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="94"/>
       <c r="B42" s="94"/>
       <c r="C42" s="93" t="s">
@@ -20527,7 +20557,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="43" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="94"/>
       <c r="B43" s="94"/>
       <c r="C43" s="93" t="s">
@@ -20572,7 +20602,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="44" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="94"/>
       <c r="B44" s="94"/>
       <c r="C44" s="93" t="s">
@@ -20617,7 +20647,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="45" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="94"/>
       <c r="B45" s="82"/>
       <c r="C45" s="81" t="s">
@@ -20674,7 +20704,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="46" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="94"/>
       <c r="B46" s="60"/>
       <c r="C46" s="59" t="s">
@@ -20719,7 +20749,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="47" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="94"/>
       <c r="B47" s="60"/>
       <c r="C47" s="59" t="s">
@@ -20762,11 +20792,11 @@
         <v>200</v>
       </c>
     </row>
-    <row r="48" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="94"/>
       <c r="B48" s="82"/>
       <c r="C48" s="81" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D48" s="81"/>
       <c r="E48" s="74"/>
@@ -20805,11 +20835,11 @@
         <v>243</v>
       </c>
     </row>
-    <row r="49" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="94"/>
       <c r="B49" s="94"/>
       <c r="C49" s="93" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D49" s="93"/>
       <c r="E49" s="74"/>
@@ -20848,11 +20878,11 @@
         <v>243</v>
       </c>
     </row>
-    <row r="50" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="94"/>
       <c r="B50" s="82"/>
       <c r="C50" s="81" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D50" s="81"/>
       <c r="E50" s="74"/>
@@ -20891,11 +20921,11 @@
         <v>243</v>
       </c>
     </row>
-    <row r="51" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="94"/>
       <c r="B51" s="82"/>
       <c r="C51" s="81" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D51" s="81"/>
       <c r="E51" s="74"/>
@@ -20934,11 +20964,11 @@
         <v>243</v>
       </c>
     </row>
-    <row r="52" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="94"/>
       <c r="B52" s="89"/>
       <c r="C52" s="88" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D52" s="88"/>
       <c r="E52" s="74"/>
@@ -20974,14 +21004,14 @@
         <v>201</v>
       </c>
       <c r="AA52" s="63" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="53" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="53" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="94"/>
       <c r="B53" s="89"/>
       <c r="C53" s="88" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D53" s="88"/>
       <c r="E53" s="74"/>
@@ -21017,10 +21047,10 @@
         <v>201</v>
       </c>
       <c r="AA53" s="63" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="54" spans="1:27" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="54" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="94"/>
       <c r="B54" s="94"/>
       <c r="C54" s="93"/>
@@ -21052,7 +21082,7 @@
     <row r="55" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="49"/>
       <c r="B55" s="49" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C55" s="93"/>
       <c r="D55" s="93"/>
@@ -21084,7 +21114,7 @@
       <c r="A56" s="94"/>
       <c r="B56" s="89"/>
       <c r="C56" s="88" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D56" s="88"/>
       <c r="E56" s="74"/>
@@ -21122,14 +21152,14 @@
         <v>201</v>
       </c>
       <c r="AA56" s="63" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="57" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="94"/>
       <c r="B57" s="89"/>
       <c r="C57" s="88" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D57" s="88"/>
       <c r="E57" s="74"/>
@@ -21167,14 +21197,14 @@
         <v>201</v>
       </c>
       <c r="AA57" s="63" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="58" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="94"/>
       <c r="B58" s="89"/>
       <c r="C58" s="88" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D58" s="88"/>
       <c r="E58" s="74"/>
@@ -21212,14 +21242,14 @@
         <v>201</v>
       </c>
       <c r="AA58" s="63" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="59" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="94"/>
       <c r="B59" s="89"/>
       <c r="C59" s="88" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D59" s="88"/>
       <c r="E59" s="74"/>
@@ -21257,14 +21287,14 @@
         <v>201</v>
       </c>
       <c r="AA59" s="63" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="60" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="94"/>
       <c r="B60" s="89"/>
       <c r="C60" s="88" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D60" s="88"/>
       <c r="E60" s="74"/>
@@ -21302,14 +21332,14 @@
         <v>201</v>
       </c>
       <c r="AA60" s="63" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="61" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="94"/>
       <c r="B61" s="89"/>
       <c r="C61" s="88" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D61" s="88"/>
       <c r="E61" s="74"/>
@@ -21347,14 +21377,14 @@
         <v>201</v>
       </c>
       <c r="AA61" s="63" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="62" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="94"/>
       <c r="B62" s="89"/>
       <c r="C62" s="88" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D62" s="88"/>
       <c r="E62" s="74"/>
@@ -21392,14 +21422,14 @@
         <v>201</v>
       </c>
       <c r="AA62" s="63" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="63" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="94"/>
       <c r="B63" s="89"/>
       <c r="C63" s="88" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D63" s="88"/>
       <c r="E63" s="74"/>
@@ -21437,7 +21467,7 @@
         <v>201</v>
       </c>
       <c r="AA63" s="63" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="64" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -21534,7 +21564,7 @@
       <c r="A66" s="94"/>
       <c r="B66" s="94"/>
       <c r="C66" s="93" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D66" s="93"/>
       <c r="E66" s="74"/>
@@ -22415,7 +22445,7 @@
     </row>
     <row r="2" spans="1:14" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="86" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -22429,7 +22459,7 @@
       </c>
       <c r="E3" s="39"/>
       <c r="F3" s="39" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G3" s="39"/>
       <c r="H3" s="39" t="s">
@@ -22445,7 +22475,7 @@
       </c>
       <c r="M3" s="39"/>
       <c r="N3" s="39" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.25">
@@ -22459,7 +22489,7 @@
       </c>
       <c r="E4" s="58"/>
       <c r="F4" s="58" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G4" s="58"/>
       <c r="H4" s="58" t="s">
@@ -22475,7 +22505,7 @@
       </c>
       <c r="M4" s="56"/>
       <c r="N4" s="56" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="195" customHeight="1" x14ac:dyDescent="0.25">
@@ -22493,7 +22523,7 @@
       </c>
       <c r="G5" s="84"/>
       <c r="H5" s="84" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I5" s="84"/>
       <c r="J5" s="84" t="s">
@@ -22505,7 +22535,7 @@
       </c>
       <c r="M5" s="84"/>
       <c r="N5" s="84" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="105" customHeight="1" x14ac:dyDescent="0.25">
@@ -22515,19 +22545,19 @@
       </c>
       <c r="C6" s="84"/>
       <c r="D6" s="84" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E6" s="84"/>
       <c r="F6" s="84" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G6" s="84"/>
       <c r="H6" s="84" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I6" s="84"/>
       <c r="J6" s="84" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="K6" s="84"/>
       <c r="L6" s="84" t="s">
@@ -22535,7 +22565,7 @@
       </c>
       <c r="M6" s="84"/>
       <c r="N6" s="84" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="135" customHeight="1" x14ac:dyDescent="0.25">
@@ -22545,15 +22575,15 @@
       </c>
       <c r="C7" s="84"/>
       <c r="D7" s="84" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E7" s="84"/>
       <c r="F7" s="84" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G7" s="84"/>
       <c r="H7" s="84" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I7" s="84"/>
       <c r="J7" s="84" t="s">
@@ -22565,7 +22595,7 @@
       </c>
       <c r="M7" s="84"/>
       <c r="N7" s="84" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -22622,7 +22652,7 @@
     </row>
     <row r="11" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B11" s="23"/>
       <c r="C11" s="23"/>
@@ -22632,7 +22662,7 @@
     </row>
     <row r="12" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B12" s="23"/>
       <c r="C12" s="23"/>
@@ -22896,7 +22926,7 @@
       </c>
       <c r="D5" s="32"/>
       <c r="E5" s="32" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F5" s="32"/>
       <c r="G5" s="32" t="s">
@@ -22913,7 +22943,7 @@
       </c>
       <c r="B6" s="32"/>
       <c r="C6" s="32" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D6" s="32"/>
       <c r="E6" s="32" t="s">
@@ -22934,7 +22964,7 @@
       </c>
       <c r="B7" s="32"/>
       <c r="C7" s="32" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D7" s="32"/>
       <c r="E7" s="32" t="s">
@@ -22955,11 +22985,11 @@
       </c>
       <c r="B8" s="32"/>
       <c r="C8" s="32" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D8" s="32"/>
       <c r="E8" s="32" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F8" s="32"/>
       <c r="G8" s="32" t="s">
@@ -22980,7 +23010,7 @@
       </c>
       <c r="D9" s="32"/>
       <c r="E9" s="32" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F9" s="32"/>
       <c r="G9" s="32" t="s">
@@ -22997,7 +23027,7 @@
       </c>
       <c r="B10" s="32"/>
       <c r="C10" s="32" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="32" t="s">
@@ -23018,7 +23048,7 @@
       </c>
       <c r="B11" s="32"/>
       <c r="C11" s="32" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D11" s="32"/>
       <c r="E11" s="32" t="s">
@@ -23656,12 +23686,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="108" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Began section on demand-side model of technology transfer
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="345">
   <si>
     <t>Total</t>
   </si>
@@ -1273,10 +1273,6 @@
   </si>
   <si>
     <t>Demand-side</t>
-  </si>
-  <si>
-    <t>Demand-side
-Supply-side</t>
   </si>
   <si>
     <t>Conceptual Framework</t>
@@ -2027,6 +2023,30 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2062,30 +2082,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -6394,1023 +6390,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>604837</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>604837</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Rectangle 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EDF8CFA-62CE-4CD9-A1E4-E2051F7B335E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3043237" y="4857750"/>
-          <a:ext cx="1828800" cy="914400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>DP</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" baseline="-25000">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>1</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> : Technology maturity level must be at least M.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1200" baseline="-25000">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>604837</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>604837</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Rectangle 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B0DC8DD-F6A6-40DC-831A-338DFA26E651}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3043237" y="5976937"/>
-          <a:ext cx="1828800" cy="914400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>DP</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" baseline="-25000">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>2</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>604837</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>604837</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="Rectangle 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CB89335-6580-458F-8E57-39173AA7E02B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3043237" y="7496175"/>
-          <a:ext cx="1828800" cy="914400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>DP</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" baseline="-25000">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>n</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA9B58F4-BE0E-4B02-98BA-EB1FC72D1482}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="2" idx="3"/>
-          <a:endCxn id="8" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2314575" y="3681412"/>
-          <a:ext cx="3248025" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>525779</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>604836</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="15" name="Connector: Elbow 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3BFF46A-19D4-4457-9D4F-D6C6E98861B2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="32" idx="2"/>
-          <a:endCxn id="9" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000" flipH="1">
-          <a:off x="1803558" y="4075271"/>
-          <a:ext cx="1181100" cy="1298257"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>180976</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>119061</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>604838</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>128586</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="17" name="Connector: Elbow 16">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52FF6E3E-4187-43E2-8A05-5FF131F06074}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="2" idx="2"/>
-          <a:endCxn id="10" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000" flipH="1">
-          <a:off x="1073944" y="4464843"/>
-          <a:ext cx="2295525" cy="1643062"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>468630</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>604837</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="19" name="Connector: Elbow 18">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BB21842-A987-4D88-A9C0-33EB2875A2D0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="35" idx="2"/>
-          <a:endCxn id="11" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000" flipH="1">
-          <a:off x="150971" y="5061108"/>
-          <a:ext cx="3819525" cy="1965007"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>604837</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>11430</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="21" name="Connector: Elbow 20">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1206A40E-C509-4A7E-8F73-FB30DDBCCC48}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="9" idx="3"/>
-          <a:endCxn id="37" idx="2"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="4872037" y="4133850"/>
-          <a:ext cx="1235393" cy="1181100"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>604837</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="23" name="Connector: Elbow 22">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CB449B0-6103-42E2-BE6D-DE4E2DD869CE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="10" idx="3"/>
-          <a:endCxn id="8" idx="2"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="4872037" y="4138612"/>
-          <a:ext cx="1604963" cy="2295525"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>604837</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>144780</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="25" name="Connector: Elbow 24">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{703ADAEA-785F-4395-B619-4D90E53856D5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="11" idx="3"/>
-          <a:endCxn id="38" idx="2"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="4872037" y="4124325"/>
-          <a:ext cx="1978343" cy="3829050"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>123824</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>80964</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>476249</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>157164</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11B7D077-5FD9-4402-9CB4-F8AAA2C8A7B5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="3729037" y="7010401"/>
-          <a:ext cx="457200" cy="352425"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>. . .</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="Rectangle 15">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{607722A7-0A06-44C0-835D-2088A6A4A6C3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000">
-          <a:off x="2409825" y="1171575"/>
-          <a:ext cx="1828800" cy="914400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Asborptive capacity</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="Rectangle 17">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC4F0E75-89CB-4D8A-8F57-C110832D2580}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000">
-          <a:off x="3514725" y="1171575"/>
-          <a:ext cx="1828800" cy="914400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Organizational slack</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>278130</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8CC71DE-30FA-4561-98F8-E7B24F9EBA13}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="16" idx="1"/>
-          <a:endCxn id="48" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3324225" y="2562225"/>
-          <a:ext cx="1905" cy="1123950"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>173355</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{927C467B-1531-4473-9834-ECF608E77259}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="18" idx="1"/>
-          <a:endCxn id="50" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4429125" y="2562225"/>
-          <a:ext cx="11430" cy="1123950"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="46" name="Group 45">
+        <xdr:cNvPr id="24" name="Group 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8AB265B-49A2-437B-828B-4AD1C1E7D9E9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{755933F2-C06E-41F4-B6D9-B82DA65DB791}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7418,18 +6414,18 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="485775" y="3219450"/>
-          <a:ext cx="1828800" cy="919162"/>
-          <a:chOff x="485775" y="3219450"/>
-          <a:chExt cx="1828800" cy="919162"/>
+          <a:off x="209550" y="733425"/>
+          <a:ext cx="9953625" cy="8924925"/>
+          <a:chOff x="209550" y="733425"/>
+          <a:chExt cx="9953625" cy="8924925"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="2" name="Rectangle 1">
+          <xdr:cNvPr id="9" name="Rectangle 8">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7FBD581-9132-4175-AC34-BD98A9A52BD0}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EDF8CFA-62CE-4CD9-A1E4-E2051F7B335E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -7437,7 +6433,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="485775" y="3224212"/>
+            <a:off x="2767012" y="6105525"/>
             <a:ext cx="1828800" cy="914400"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -7477,7 +6473,15 @@
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>Options</a:t>
+              <a:t>Decision Premise (DP</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="-25000">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>1</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1200" baseline="0">
@@ -7485,7 +6489,790 @@
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t> of technologies available for assimilation</a:t>
+              <a:t>): </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Technology maturity level must be at least L.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1200" baseline="-25000">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="Rectangle 9">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B0DC8DD-F6A6-40DC-831A-338DFA26E651}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2767012" y="7224712"/>
+            <a:ext cx="1828800" cy="914400"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>DP</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="-25000">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>2</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="11" name="Rectangle 10">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CB89335-6580-458F-8E57-39173AA7E02B}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2767012" y="8743950"/>
+            <a:ext cx="1828800" cy="914400"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>DP</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="-25000">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>n</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA9B58F4-BE0E-4B02-98BA-EB1FC72D1482}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="2" idx="3"/>
+            <a:endCxn id="8" idx="1"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2038350" y="3681412"/>
+            <a:ext cx="3248025" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="lg" len="lg"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="15" name="Connector: Elbow 14">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3BFF46A-19D4-4457-9D4F-D6C6E98861B2}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="32" idx="2"/>
+            <a:endCxn id="9" idx="1"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="851059" y="4646771"/>
+            <a:ext cx="2428875" cy="1403032"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector2">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="lg" len="lg"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="17" name="Connector: Elbow 16">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52FF6E3E-4187-43E2-8A05-5FF131F06074}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="40" idx="2"/>
+            <a:endCxn id="10" idx="1"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="53340" y="4968240"/>
+            <a:ext cx="3548062" cy="1879282"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector2">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="lg" len="lg"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="19" name="Connector: Elbow 18">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BB21842-A987-4D88-A9C0-33EB2875A2D0}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="35" idx="2"/>
+            <a:endCxn id="11" idx="1"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="-944404" y="5489734"/>
+            <a:ext cx="5067300" cy="2355532"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector2">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="lg" len="lg"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="21" name="Connector: Elbow 20">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1206A40E-C509-4A7E-8F73-FB30DDBCCC48}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="9" idx="3"/>
+            <a:endCxn id="37" idx="2"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="4595812" y="4133850"/>
+            <a:ext cx="1365568" cy="2428875"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector2">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="lg" len="lg"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="23" name="Connector: Elbow 22">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CB449B0-6103-42E2-BE6D-DE4E2DD869CE}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="10" idx="3"/>
+            <a:endCxn id="41" idx="2"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="4595812" y="4133850"/>
+            <a:ext cx="1848168" cy="3548062"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector2">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="lg" len="lg"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="25" name="Connector: Elbow 24">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{703ADAEA-785F-4395-B619-4D90E53856D5}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="11" idx="3"/>
+            <a:endCxn id="38" idx="2"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="4595812" y="4124325"/>
+            <a:ext cx="2330768" cy="5076825"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector2">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="lg" len="lg"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="TextBox 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11B7D077-5FD9-4402-9CB4-F8AAA2C8A7B5}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="5400000">
+            <a:off x="3452812" y="8258176"/>
+            <a:ext cx="457200" cy="352425"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>. . .</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="16" name="Rectangle 15">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{607722A7-0A06-44C0-835D-2088A6A4A6C3}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000">
+            <a:off x="2133600" y="1190625"/>
+            <a:ext cx="1828800" cy="914400"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Uncertainty</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> avoidance</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="18" name="Rectangle 17">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC4F0E75-89CB-4D8A-8F57-C110832D2580}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000">
+            <a:off x="3238500" y="1190625"/>
+            <a:ext cx="1828800" cy="914400"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Absorptive capacity</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8CC71DE-30FA-4561-98F8-E7B24F9EBA13}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="16" idx="1"/>
+            <a:endCxn id="48" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3048000" y="2562225"/>
+            <a:ext cx="1905" cy="1123950"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="lg" len="lg"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{927C467B-1531-4473-9834-ECF608E77259}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="18" idx="1"/>
+            <a:endCxn id="50" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4152900" y="2562225"/>
+            <a:ext cx="11430" cy="1123950"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="lg" len="lg"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="2" name="Rectangle 1">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7FBD581-9132-4175-AC34-BD98A9A52BD0}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="209550" y="3224212"/>
+            <a:ext cx="1828800" cy="914400"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Technology available for assimilation</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -7503,7 +7290,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="1562100" y="3219450"/>
+            <a:off x="1181100" y="3219450"/>
             <a:ext cx="365760" cy="914400"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -7556,7 +7343,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="895350" y="3219450"/>
+            <a:off x="228600" y="3219450"/>
             <a:ext cx="365760" cy="914400"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -7596,41 +7383,6 @@
           </a:p>
         </xdr:txBody>
       </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="47" name="Group 46">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7ADE4B7-8C02-4E8B-ACFE-60C896C73203}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="5562600" y="3209925"/>
-          <a:ext cx="1828800" cy="928687"/>
-          <a:chOff x="5562600" y="3209925"/>
-          <a:chExt cx="1828800" cy="928687"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
           <xdr:cNvPr id="8" name="Rectangle 7">
@@ -7644,7 +7396,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="5562600" y="3224212"/>
+            <a:off x="5286375" y="3224212"/>
             <a:ext cx="1828800" cy="914400"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -7684,7 +7436,7 @@
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>Add the technology to the decision agenda</a:t>
+              <a:t>Decision of whether to assimilate the technology</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="1200">
               <a:solidFill>
@@ -7707,7 +7459,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="5924550" y="3219450"/>
+            <a:off x="5778500" y="3219450"/>
             <a:ext cx="365760" cy="914400"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -7760,7 +7512,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="6667500" y="3209925"/>
+            <a:off x="6743700" y="3209925"/>
             <a:ext cx="365760" cy="914400"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -7800,135 +7552,575 @@
           </a:p>
         </xdr:txBody>
       </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="48" name="Rectangle 47">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C3D8628-D7D9-4F45-8B23-01A54DB84423}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2867025" y="3686175"/>
+            <a:ext cx="365760" cy="182880"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="50" name="Rectangle 49">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3342E0FA-E413-4BF7-A9D0-695F0D0764AC}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3981450" y="3686175"/>
+            <a:ext cx="365760" cy="182880"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="31" name="Rectangle 30">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{597FD77F-84EB-43A0-9CE6-3C8DED2BE1F4}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2765108" y="4610100"/>
+            <a:ext cx="1828800" cy="914400"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Communication</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1200" baseline="-25000">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="33" name="Connector: Elbow 32">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95FF0E0F-F33C-42A2-AC74-3F51A65B2B95}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="36" idx="2"/>
+            <a:endCxn id="31" idx="1"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="1835944" y="4138136"/>
+            <a:ext cx="933450" cy="924878"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector2">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="lg" len="lg"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="34" name="Connector: Elbow 33">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C37640CA-1A85-474A-B4BB-2176EF4682EA}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="31" idx="3"/>
+            <a:endCxn id="39" idx="2"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="4593908" y="4133850"/>
+            <a:ext cx="884872" cy="933450"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector2">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="lg" len="lg"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="36" name="Rectangle 35">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF57490B-5492-4EE6-87DD-05E4B8B99F52}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1657350" y="3219450"/>
+            <a:ext cx="365760" cy="914400"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="6350">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="39" name="Rectangle 38">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0A1E29A-7304-413D-A2E7-71D244BF9E02}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5295900" y="3219450"/>
+            <a:ext cx="365760" cy="914400"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="6350">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="40" name="Rectangle 39">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13BA36FD-E0ED-484F-98D9-44CC7BCD0DAB}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="704850" y="3219450"/>
+            <a:ext cx="365760" cy="914400"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="6350">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="41" name="Rectangle 40">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E98D282F-8894-4BB5-9C97-14272DCB7D6B}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6261100" y="3219450"/>
+            <a:ext cx="365760" cy="914400"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="6350">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="44" name="Straight Arrow Connector 43">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26DB750F-87E5-4885-AD94-C90A4F06D302}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="8" idx="3"/>
+            <a:endCxn id="45" idx="1"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="7115175" y="3676650"/>
+            <a:ext cx="1219200" cy="4762"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="lg" len="lg"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="45" name="Rectangle 44">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6343A56F-410C-4D52-A3E6-E84569A3DCB7}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8334375" y="3219450"/>
+            <a:ext cx="1828800" cy="914400"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Action necessitated by decision</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
     </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>461010</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>40005</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="48" name="Rectangle 47">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C3D8628-D7D9-4F45-8B23-01A54DB84423}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3143250" y="3686175"/>
-          <a:ext cx="365760" cy="182880"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>356235</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>40005</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="50" name="Rectangle 49">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3342E0FA-E413-4BF7-A9D0-695F0D0764AC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4257675" y="3686175"/>
-          <a:ext cx="365760" cy="182880"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -17886,7 +18078,7 @@
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -17917,7 +18109,7 @@
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -17947,7 +18139,7 @@
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -17977,7 +18169,7 @@
     <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="110"/>
       <c r="K12" s="79" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -18003,7 +18195,7 @@
     </row>
     <row r="36" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K36" s="79" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -18028,22 +18220,22 @@
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="130" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="122" t="s">
-        <v>344</v>
-      </c>
-      <c r="B50" s="122"/>
-      <c r="C50" s="122"/>
-      <c r="D50" s="122"/>
-      <c r="E50" s="122"/>
-      <c r="F50" s="122"/>
-      <c r="G50" s="122"/>
-      <c r="H50" s="122"/>
-      <c r="I50" s="122"/>
-      <c r="J50" s="122"/>
+      <c r="B50" s="130"/>
+      <c r="C50" s="130"/>
+      <c r="D50" s="130"/>
+      <c r="E50" s="130"/>
+      <c r="F50" s="130"/>
+      <c r="G50" s="130"/>
+      <c r="H50" s="130"/>
+      <c r="I50" s="130"/>
+      <c r="J50" s="130"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -18062,7 +18254,9 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -18073,7 +18267,7 @@
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -18098,7 +18292,7 @@
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -18138,11 +18332,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18186,7 +18381,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="90" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30">
         <v>1980</v>
       </c>
@@ -18206,7 +18401,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="72.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30">
         <v>1980</v>
       </c>
@@ -18226,7 +18421,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="105" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30">
         <v>1982</v>
       </c>
@@ -18246,7 +18441,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="90" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="30">
         <v>1984</v>
       </c>
@@ -18266,7 +18461,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="120.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="30">
         <v>1986</v>
       </c>
@@ -18283,10 +18478,10 @@
       </c>
       <c r="G8" s="109"/>
       <c r="H8" s="109" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="30">
         <v>1987</v>
       </c>
@@ -18303,10 +18498,10 @@
       </c>
       <c r="G9" s="109"/>
       <c r="H9" s="109" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30">
         <v>1987</v>
       </c>
@@ -18323,10 +18518,10 @@
       </c>
       <c r="G10" s="109"/>
       <c r="H10" s="109" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="75.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="30">
         <v>1988</v>
       </c>
@@ -18346,7 +18541,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="77.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="30">
         <v>1989</v>
       </c>
@@ -18363,10 +18558,10 @@
       </c>
       <c r="G12" s="109"/>
       <c r="H12" s="109" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="90" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="30">
         <v>1991</v>
       </c>
@@ -18501,54 +18696,54 @@
       <c r="H20" s="109"/>
     </row>
     <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="111" t="s">
+      <c r="A21" s="119" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="111"/>
-      <c r="C21" s="111"/>
-      <c r="D21" s="111"/>
-      <c r="E21" s="111"/>
-      <c r="F21" s="111"/>
+      <c r="B21" s="119"/>
+      <c r="C21" s="119"/>
+      <c r="D21" s="119"/>
+      <c r="E21" s="119"/>
+      <c r="F21" s="119"/>
     </row>
     <row r="22" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="112" t="s">
+      <c r="A22" s="120" t="s">
         <v>171</v>
       </c>
-      <c r="B22" s="112"/>
-      <c r="C22" s="112"/>
-      <c r="D22" s="112"/>
-      <c r="E22" s="112"/>
-      <c r="F22" s="112"/>
+      <c r="B22" s="120"/>
+      <c r="C22" s="120"/>
+      <c r="D22" s="120"/>
+      <c r="E22" s="120"/>
+      <c r="F22" s="120"/>
     </row>
     <row r="23" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="111" t="s">
+      <c r="A23" s="119" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="111"/>
-      <c r="C23" s="111"/>
-      <c r="D23" s="111"/>
-      <c r="E23" s="111"/>
-      <c r="F23" s="111"/>
+      <c r="B23" s="119"/>
+      <c r="C23" s="119"/>
+      <c r="D23" s="119"/>
+      <c r="E23" s="119"/>
+      <c r="F23" s="119"/>
     </row>
     <row r="24" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="111" t="s">
+      <c r="A24" s="119" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="111"/>
-      <c r="C24" s="111"/>
-      <c r="D24" s="111"/>
-      <c r="E24" s="111"/>
-      <c r="F24" s="111"/>
+      <c r="B24" s="119"/>
+      <c r="C24" s="119"/>
+      <c r="D24" s="119"/>
+      <c r="E24" s="119"/>
+      <c r="F24" s="119"/>
     </row>
     <row r="25" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="111" t="s">
+      <c r="A25" s="119" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="111"/>
-      <c r="C25" s="111"/>
-      <c r="D25" s="111"/>
-      <c r="E25" s="111"/>
-      <c r="F25" s="111"/>
+      <c r="B25" s="119"/>
+      <c r="C25" s="119"/>
+      <c r="D25" s="119"/>
+      <c r="E25" s="119"/>
+      <c r="F25" s="119"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="30"/>
@@ -18642,7 +18837,7 @@
     <mergeCell ref="A22:F22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="69" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -18653,7 +18848,7 @@
   </sheetPr>
   <dimension ref="A1:AA78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="4" ySplit="4" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -18701,7 +18896,7 @@
     </row>
     <row r="2" spans="1:27" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E2" s="61"/>
       <c r="F2" s="61"/>
@@ -18732,38 +18927,38 @@
       <c r="B3" s="69"/>
       <c r="C3" s="70"/>
       <c r="D3" s="71"/>
-      <c r="E3" s="116" t="s">
+      <c r="E3" s="124" t="s">
         <v>267</v>
       </c>
-      <c r="F3" s="117"/>
-      <c r="G3" s="117"/>
-      <c r="H3" s="114"/>
-      <c r="I3" s="113" t="s">
+      <c r="F3" s="125"/>
+      <c r="G3" s="125"/>
+      <c r="H3" s="122"/>
+      <c r="I3" s="121" t="s">
         <v>294</v>
       </c>
-      <c r="J3" s="114"/>
-      <c r="K3" s="113" t="s">
+      <c r="J3" s="122"/>
+      <c r="K3" s="121" t="s">
         <v>295</v>
       </c>
-      <c r="L3" s="115"/>
-      <c r="M3" s="116" t="s">
+      <c r="L3" s="123"/>
+      <c r="M3" s="124" t="s">
         <v>282</v>
       </c>
-      <c r="N3" s="117"/>
-      <c r="O3" s="114"/>
-      <c r="P3" s="118" t="s">
+      <c r="N3" s="125"/>
+      <c r="O3" s="122"/>
+      <c r="P3" s="126" t="s">
         <v>249</v>
       </c>
-      <c r="Q3" s="117"/>
-      <c r="R3" s="117"/>
-      <c r="S3" s="117"/>
-      <c r="T3" s="117"/>
-      <c r="U3" s="117"/>
-      <c r="V3" s="117"/>
-      <c r="W3" s="117"/>
-      <c r="X3" s="117"/>
-      <c r="Y3" s="117"/>
-      <c r="Z3" s="119"/>
+      <c r="Q3" s="125"/>
+      <c r="R3" s="125"/>
+      <c r="S3" s="125"/>
+      <c r="T3" s="125"/>
+      <c r="U3" s="125"/>
+      <c r="V3" s="125"/>
+      <c r="W3" s="125"/>
+      <c r="X3" s="125"/>
+      <c r="Y3" s="125"/>
+      <c r="Z3" s="127"/>
       <c r="AA3" s="90"/>
     </row>
     <row r="4" spans="1:27" ht="170.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -19110,51 +19305,51 @@
       </c>
     </row>
     <row r="11" spans="1:27" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="123"/>
-      <c r="B11" s="123"/>
-      <c r="C11" s="124" t="s">
-        <v>345</v>
-      </c>
-      <c r="D11" s="124"/>
-      <c r="E11" s="125"/>
-      <c r="F11" s="126" t="s">
-        <v>201</v>
-      </c>
-      <c r="G11" s="127"/>
-      <c r="H11" s="128"/>
-      <c r="I11" s="125" t="s">
-        <v>201</v>
-      </c>
-      <c r="J11" s="128"/>
-      <c r="K11" s="125" t="s">
-        <v>201</v>
-      </c>
-      <c r="L11" s="128"/>
-      <c r="M11" s="125" t="s">
-        <v>201</v>
-      </c>
-      <c r="N11" s="127"/>
-      <c r="O11" s="128"/>
-      <c r="P11" s="127"/>
-      <c r="Q11" s="127" t="s">
-        <v>201</v>
-      </c>
-      <c r="R11" s="127" t="s">
-        <v>201</v>
-      </c>
-      <c r="S11" s="129" t="s">
-        <v>201</v>
-      </c>
-      <c r="T11" s="129" t="s">
-        <v>201</v>
-      </c>
-      <c r="U11" s="129"/>
-      <c r="V11" s="129"/>
-      <c r="W11" s="129"/>
-      <c r="X11" s="129"/>
-      <c r="Y11" s="129"/>
-      <c r="Z11" s="129"/>
-      <c r="AA11" s="130" t="s">
+      <c r="A11" s="111"/>
+      <c r="B11" s="111"/>
+      <c r="C11" s="112" t="s">
+        <v>344</v>
+      </c>
+      <c r="D11" s="112"/>
+      <c r="E11" s="113"/>
+      <c r="F11" s="114" t="s">
+        <v>201</v>
+      </c>
+      <c r="G11" s="115"/>
+      <c r="H11" s="116"/>
+      <c r="I11" s="113" t="s">
+        <v>201</v>
+      </c>
+      <c r="J11" s="116"/>
+      <c r="K11" s="113" t="s">
+        <v>201</v>
+      </c>
+      <c r="L11" s="116"/>
+      <c r="M11" s="113" t="s">
+        <v>201</v>
+      </c>
+      <c r="N11" s="115"/>
+      <c r="O11" s="116"/>
+      <c r="P11" s="115"/>
+      <c r="Q11" s="115" t="s">
+        <v>201</v>
+      </c>
+      <c r="R11" s="115" t="s">
+        <v>201</v>
+      </c>
+      <c r="S11" s="117" t="s">
+        <v>201</v>
+      </c>
+      <c r="T11" s="117" t="s">
+        <v>201</v>
+      </c>
+      <c r="U11" s="117"/>
+      <c r="V11" s="117"/>
+      <c r="W11" s="117"/>
+      <c r="X11" s="117"/>
+      <c r="Y11" s="117"/>
+      <c r="Z11" s="117"/>
+      <c r="AA11" s="118" t="s">
         <v>252</v>
       </c>
     </row>
@@ -22039,10 +22234,10 @@
       <c r="A3" s="69"/>
       <c r="B3" s="70"/>
       <c r="C3" s="71"/>
-      <c r="D3" s="116" t="s">
+      <c r="D3" s="124" t="s">
         <v>194</v>
       </c>
-      <c r="E3" s="114"/>
+      <c r="E3" s="122"/>
       <c r="F3" s="73"/>
     </row>
     <row r="4" spans="1:6" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -22302,32 +22497,32 @@
       <c r="F23" s="59"/>
     </row>
     <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="111"/>
-      <c r="B24" s="111"/>
-      <c r="C24" s="111"/>
-      <c r="D24" s="111"/>
-      <c r="E24" s="111"/>
+      <c r="A24" s="119"/>
+      <c r="B24" s="119"/>
+      <c r="C24" s="119"/>
+      <c r="D24" s="119"/>
+      <c r="E24" s="119"/>
     </row>
     <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="111"/>
-      <c r="B25" s="111"/>
-      <c r="C25" s="111"/>
-      <c r="D25" s="111"/>
-      <c r="E25" s="111"/>
+      <c r="A25" s="119"/>
+      <c r="B25" s="119"/>
+      <c r="C25" s="119"/>
+      <c r="D25" s="119"/>
+      <c r="E25" s="119"/>
     </row>
     <row r="26" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="111"/>
-      <c r="B26" s="111"/>
-      <c r="C26" s="111"/>
-      <c r="D26" s="111"/>
-      <c r="E26" s="111"/>
+      <c r="A26" s="119"/>
+      <c r="B26" s="119"/>
+      <c r="C26" s="119"/>
+      <c r="D26" s="119"/>
+      <c r="E26" s="119"/>
     </row>
     <row r="27" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="111"/>
-      <c r="B27" s="111"/>
-      <c r="C27" s="111"/>
-      <c r="D27" s="111"/>
-      <c r="E27" s="111"/>
+      <c r="A27" s="119"/>
+      <c r="B27" s="119"/>
+      <c r="C27" s="119"/>
+      <c r="D27" s="119"/>
+      <c r="E27" s="119"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="60"/>
@@ -22926,7 +23121,7 @@
       </c>
       <c r="D5" s="32"/>
       <c r="E5" s="32" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F5" s="32"/>
       <c r="G5" s="32" t="s">
@@ -22943,7 +23138,7 @@
       </c>
       <c r="B6" s="32"/>
       <c r="C6" s="32" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D6" s="32"/>
       <c r="E6" s="32" t="s">
@@ -22964,7 +23159,7 @@
       </c>
       <c r="B7" s="32"/>
       <c r="C7" s="32" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D7" s="32"/>
       <c r="E7" s="32" t="s">
@@ -22985,11 +23180,11 @@
       </c>
       <c r="B8" s="32"/>
       <c r="C8" s="32" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D8" s="32"/>
       <c r="E8" s="32" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F8" s="32"/>
       <c r="G8" s="32" t="s">
@@ -23010,7 +23205,7 @@
       </c>
       <c r="D9" s="32"/>
       <c r="E9" s="32" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F9" s="32"/>
       <c r="G9" s="32" t="s">
@@ -23027,7 +23222,7 @@
       </c>
       <c r="B10" s="32"/>
       <c r="C10" s="32" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="32" t="s">
@@ -23048,7 +23243,7 @@
       </c>
       <c r="B11" s="32"/>
       <c r="C11" s="32" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D11" s="32"/>
       <c r="E11" s="32" t="s">
@@ -23118,40 +23313,40 @@
       <c r="H15" s="32"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="112" t="s">
+      <c r="A16" s="120" t="s">
         <v>99</v>
       </c>
-      <c r="B16" s="112"/>
-      <c r="C16" s="112"/>
-      <c r="D16" s="112"/>
-      <c r="E16" s="112"/>
-      <c r="F16" s="112"/>
-      <c r="G16" s="112"/>
-      <c r="H16" s="112"/>
-      <c r="I16" s="112"/>
+      <c r="B16" s="120"/>
+      <c r="C16" s="120"/>
+      <c r="D16" s="120"/>
+      <c r="E16" s="120"/>
+      <c r="F16" s="120"/>
+      <c r="G16" s="120"/>
+      <c r="H16" s="120"/>
+      <c r="I16" s="120"/>
     </row>
     <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="111"/>
-      <c r="B17" s="111"/>
-      <c r="C17" s="111"/>
+      <c r="A17" s="119"/>
+      <c r="B17" s="119"/>
+      <c r="C17" s="119"/>
       <c r="D17" s="32"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="111"/>
-      <c r="B18" s="111"/>
-      <c r="C18" s="111"/>
+      <c r="A18" s="119"/>
+      <c r="B18" s="119"/>
+      <c r="C18" s="119"/>
       <c r="D18" s="32"/>
       <c r="E18" s="32"/>
       <c r="F18" s="32"/>
       <c r="H18" s="32"/>
     </row>
     <row r="19" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="111"/>
-      <c r="B19" s="111"/>
-      <c r="C19" s="111"/>
+      <c r="A19" s="119"/>
+      <c r="B19" s="119"/>
+      <c r="C19" s="119"/>
       <c r="D19" s="32"/>
       <c r="E19" s="32"/>
       <c r="F19" s="32"/>
@@ -23591,30 +23786,30 @@
       <c r="C41" s="52"/>
     </row>
     <row r="42" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="120" t="s">
+      <c r="A42" s="128" t="s">
         <v>166</v>
       </c>
-      <c r="B42" s="120"/>
-      <c r="C42" s="120"/>
+      <c r="B42" s="128"/>
+      <c r="C42" s="128"/>
     </row>
     <row r="43" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="121" t="s">
+      <c r="A43" s="129" t="s">
         <v>167</v>
       </c>
-      <c r="B43" s="121"/>
-      <c r="C43" s="121"/>
+      <c r="B43" s="129"/>
+      <c r="C43" s="129"/>
     </row>
     <row r="44" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="120" t="s">
+      <c r="A44" s="128" t="s">
         <v>168</v>
       </c>
-      <c r="B44" s="120"/>
-      <c r="C44" s="120"/>
+      <c r="B44" s="128"/>
+      <c r="C44" s="128"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="111"/>
-      <c r="B45" s="111"/>
-      <c r="C45" s="111"/>
+      <c r="A45" s="119"/>
+      <c r="B45" s="119"/>
+      <c r="C45" s="119"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="37"/>

</xml_diff>

<commit_message>
Updated table for figure on technology utilization
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="359">
   <si>
     <t>Total</t>
   </si>
@@ -1373,12 +1373,6 @@
     <t>Non-Exclusive License</t>
   </si>
   <si>
-    <t>Estimated Number of Technologies Licensed Non-Exclusively</t>
-  </si>
-  <si>
-    <t>Patent Applications</t>
-  </si>
-  <si>
     <t>Estimated Number of Technologies Transferred</t>
   </si>
   <si>
@@ -1413,6 +1407,93 @@
       <t>. Oakbrook Terrace, IL: Association of University Technology Managers. Available from http://www.autm.net</t>
     </r>
   </si>
+  <si>
+    <t>Worldwide Patent Applications</t>
+  </si>
+  <si>
+    <t>U.S. Utility Patent Applications</t>
+  </si>
+  <si>
+    <t>U.S. Provisional Patent Applications</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Estimated Number of Technologies Licensed Non-Exclusively </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Estimated Number of Technologies Transferred </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>b</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Assumes one unique technology per three non-exclusive license</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> The sum of exclusive licenses, options, and the estimated number of unique technologies licensed non-exclusively.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -1424,7 +1505,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1510,6 +1591,14 @@
     <font>
       <i/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1760,7 +1849,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -2164,6 +2253,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -2211,7 +2309,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Figure - Tech Utilization'!$B$13</c:f>
+              <c:f>'Figure - Tech Utilization'!$B$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2292,7 +2390,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'Figure - Tech Utilization'!$A$14:$A$18</c:f>
+              <c:f>'Figure - Tech Utilization'!$A$18:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2316,7 +2414,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Figure - Tech Utilization'!$B$14:$B$18</c:f>
+              <c:f>'Figure - Tech Utilization'!$B$18:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2349,7 +2447,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Figure - Tech Utilization'!$C$13</c:f>
+              <c:f>'Figure - Tech Utilization'!$C$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2428,7 +2526,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'Figure - Tech Utilization'!$A$14:$A$18</c:f>
+              <c:f>'Figure - Tech Utilization'!$A$18:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2452,7 +2550,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Figure - Tech Utilization'!$C$14:$C$18</c:f>
+              <c:f>'Figure - Tech Utilization'!$C$18:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2504,7 +2602,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Figure - Tech Utilization'!$A$13</c15:sqref>
+                          <c15:sqref>'Figure - Tech Utilization'!$A$17</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2589,7 +2687,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Figure - Tech Utilization'!$A$14:$A$18</c15:sqref>
+                          <c15:sqref>'Figure - Tech Utilization'!$A$18:$A$22</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2619,7 +2717,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Figure - Tech Utilization'!$A$14:$A$18</c15:sqref>
+                          <c15:sqref>'Figure - Tech Utilization'!$A$18:$A$22</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -6545,13 +6643,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1028700</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -18074,7 +18172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -25641,26 +25739,27 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="10" width="15.7109375" style="91" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="108" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A5" s="122" t="s">
         <v>1</v>
       </c>
@@ -25668,29 +25767,35 @@
         <v>275</v>
       </c>
       <c r="C5" s="123" t="s">
+        <v>352</v>
+      </c>
+      <c r="D5" s="123" t="s">
+        <v>354</v>
+      </c>
+      <c r="E5" s="123" t="s">
+        <v>353</v>
+      </c>
+      <c r="F5" s="123" t="s">
+        <v>345</v>
+      </c>
+      <c r="G5" s="123" t="s">
+        <v>346</v>
+      </c>
+      <c r="H5" s="123" t="s">
+        <v>347</v>
+      </c>
+      <c r="I5" s="123" t="s">
+        <v>355</v>
+      </c>
+      <c r="J5" s="123" t="s">
+        <v>356</v>
+      </c>
+      <c r="K5" s="123" t="s">
         <v>349</v>
       </c>
-      <c r="D5" s="123" t="s">
-        <v>345</v>
-      </c>
-      <c r="E5" s="123" t="s">
-        <v>346</v>
-      </c>
-      <c r="F5" s="123" t="s">
-        <v>347</v>
-      </c>
-      <c r="G5" s="123" t="s">
-        <v>348</v>
-      </c>
-      <c r="H5" s="123" t="s">
-        <v>350</v>
-      </c>
-      <c r="I5" s="123" t="s">
-        <v>351</v>
-      </c>
-      <c r="J5" s="120"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L5" s="120"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>2013</v>
       </c>
@@ -25701,29 +25806,35 @@
         <v>14987</v>
       </c>
       <c r="D6" s="119">
+        <v>11626</v>
+      </c>
+      <c r="E6" s="119">
+        <v>1531</v>
+      </c>
+      <c r="F6" s="119">
         <v>1764</v>
       </c>
-      <c r="E6" s="119">
+      <c r="G6" s="119">
         <v>1356</v>
       </c>
-      <c r="F6" s="119">
+      <c r="H6" s="119">
         <v>3410</v>
       </c>
-      <c r="G6" s="119">
-        <f>F6/3</f>
+      <c r="I6" s="119">
+        <f>H6/3</f>
         <v>1136.6666666666667</v>
       </c>
-      <c r="H6" s="119">
-        <f>SUM(D6,E6,G6)</f>
+      <c r="J6" s="119">
+        <f>SUM(F6,G6,I6)</f>
         <v>4256.666666666667</v>
       </c>
-      <c r="I6" s="121">
-        <f t="shared" ref="I6:I11" si="0">H6/B6</f>
+      <c r="K6" s="121">
+        <f>J6/B6</f>
         <v>0.17700709691727656</v>
       </c>
-      <c r="J6" s="119"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L6" s="119"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>2014</v>
       </c>
@@ -25734,29 +25845,35 @@
         <v>13907</v>
       </c>
       <c r="D7" s="119">
+        <v>10715</v>
+      </c>
+      <c r="E7" s="119">
+        <v>1504</v>
+      </c>
+      <c r="F7" s="119">
         <v>2029</v>
       </c>
-      <c r="E7" s="119">
+      <c r="G7" s="119">
         <v>1461</v>
       </c>
-      <c r="F7" s="119">
+      <c r="H7" s="119">
         <v>3398</v>
       </c>
-      <c r="G7" s="119">
-        <f>F7/3</f>
+      <c r="I7" s="119">
+        <f>H7/3</f>
         <v>1132.6666666666667</v>
       </c>
-      <c r="H7" s="119">
-        <f t="shared" ref="H7:H10" si="1">SUM(D7,E7,G7)</f>
+      <c r="J7" s="119">
+        <f t="shared" ref="J7:J10" si="0">SUM(F7,G7,I7)</f>
         <v>4622.666666666667</v>
       </c>
-      <c r="I7" s="121">
-        <f t="shared" si="0"/>
+      <c r="K7" s="121">
+        <f>J7/B7</f>
         <v>0.19167668726071513</v>
       </c>
-      <c r="J7" s="119"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L7" s="119"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>2015</v>
       </c>
@@ -25767,29 +25884,35 @@
         <v>15953</v>
       </c>
       <c r="D8" s="119">
+        <v>11516</v>
+      </c>
+      <c r="E8" s="119">
+        <v>1672</v>
+      </c>
+      <c r="F8" s="119">
         <v>2107</v>
       </c>
-      <c r="E8" s="119">
+      <c r="G8" s="119">
         <v>1547</v>
       </c>
-      <c r="F8" s="119">
+      <c r="H8" s="119">
         <v>4115</v>
       </c>
-      <c r="G8" s="119">
-        <f>F8/3</f>
+      <c r="I8" s="119">
+        <f>H8/3</f>
         <v>1371.6666666666667</v>
       </c>
-      <c r="H8" s="119">
-        <f t="shared" si="1"/>
+      <c r="J8" s="119">
+        <f t="shared" si="0"/>
         <v>5025.666666666667</v>
       </c>
-      <c r="I8" s="121">
-        <f t="shared" si="0"/>
+      <c r="K8" s="121">
+        <f>J8/B8</f>
         <v>0.19854093417084767</v>
       </c>
-      <c r="J8" s="119"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L8" s="119"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>2016</v>
       </c>
@@ -25800,29 +25923,35 @@
         <v>16487</v>
       </c>
       <c r="D9" s="119">
+        <v>12114</v>
+      </c>
+      <c r="E9" s="119">
+        <v>1391</v>
+      </c>
+      <c r="F9" s="119">
         <v>2063</v>
       </c>
-      <c r="E9" s="119">
+      <c r="G9" s="119">
         <v>1438</v>
       </c>
-      <c r="F9" s="119">
+      <c r="H9" s="119">
         <v>4201</v>
       </c>
-      <c r="G9" s="119">
-        <f>F9/3</f>
+      <c r="I9" s="119">
+        <f>H9/3</f>
         <v>1400.3333333333333</v>
       </c>
-      <c r="H9" s="119">
-        <f t="shared" si="1"/>
+      <c r="J9" s="119">
+        <f t="shared" si="0"/>
         <v>4901.333333333333</v>
       </c>
-      <c r="I9" s="121">
-        <f t="shared" si="0"/>
+      <c r="K9" s="121">
+        <f>J9/B9</f>
         <v>0.18979025492094223</v>
       </c>
-      <c r="J9" s="119"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L9" s="119"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>2017</v>
       </c>
@@ -25833,147 +25962,149 @@
         <v>15335</v>
       </c>
       <c r="D10" s="119">
+        <v>11418</v>
+      </c>
+      <c r="E10" s="119">
+        <v>1381</v>
+      </c>
+      <c r="F10" s="119">
         <v>2037</v>
       </c>
-      <c r="E10" s="119">
+      <c r="G10" s="119">
         <v>1566</v>
       </c>
-      <c r="F10" s="119">
+      <c r="H10" s="119">
         <v>4195</v>
       </c>
-      <c r="G10" s="119">
-        <f>F10/3</f>
+      <c r="I10" s="119">
+        <f>H10/3</f>
         <v>1398.3333333333333</v>
       </c>
-      <c r="H10" s="119">
-        <f t="shared" si="1"/>
+      <c r="J10" s="119">
+        <f t="shared" si="0"/>
         <v>5001.333333333333</v>
       </c>
-      <c r="I10" s="121">
-        <f t="shared" si="0"/>
+      <c r="K10" s="121">
+        <f>J10/B10</f>
         <v>0.20006933888044376</v>
       </c>
-      <c r="J10" s="119"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L10" s="119"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="124">
-        <f t="shared" ref="B11:H11" si="2">SUM(B6:B10)</f>
+        <f t="shared" ref="B11:J11" si="1">SUM(B6:B10)</f>
         <v>124301</v>
       </c>
       <c r="C11" s="124">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>76669</v>
       </c>
       <c r="D11" s="124">
-        <f t="shared" si="2"/>
-        <v>10000</v>
+        <f t="shared" ref="D11:E11" si="2">SUM(D6:D10)</f>
+        <v>57389</v>
       </c>
       <c r="E11" s="124">
         <f t="shared" si="2"/>
+        <v>7479</v>
+      </c>
+      <c r="F11" s="124">
+        <f t="shared" si="1"/>
+        <v>10000</v>
+      </c>
+      <c r="G11" s="124">
+        <f t="shared" si="1"/>
         <v>7368</v>
       </c>
-      <c r="F11" s="124">
-        <f t="shared" si="2"/>
+      <c r="H11" s="124">
+        <f t="shared" si="1"/>
         <v>19319</v>
       </c>
-      <c r="G11" s="124">
-        <f t="shared" si="2"/>
+      <c r="I11" s="124">
+        <f t="shared" si="1"/>
         <v>6439.6666666666661</v>
       </c>
-      <c r="H11" s="124">
-        <f t="shared" si="2"/>
+      <c r="J11" s="124">
+        <f t="shared" si="1"/>
         <v>23807.666666666664</v>
       </c>
-      <c r="I11" s="125">
-        <f t="shared" si="0"/>
+      <c r="K11" s="125">
+        <f>J11/B11</f>
         <v>0.19153238241580248</v>
       </c>
-      <c r="J11" s="119"/>
-    </row>
-    <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="122" t="s">
+      <c r="L11" s="119"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="141"/>
+      <c r="B12" s="142"/>
+      <c r="C12" s="142"/>
+      <c r="D12" s="142"/>
+      <c r="E12" s="142"/>
+      <c r="F12" s="142"/>
+      <c r="G12" s="142"/>
+      <c r="H12" s="142"/>
+      <c r="I12" s="142"/>
+      <c r="J12" s="142"/>
+      <c r="K12" s="143"/>
+      <c r="L12" s="119"/>
+    </row>
+    <row r="13" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="141" t="s">
+        <v>357</v>
+      </c>
+      <c r="B13" s="142"/>
+      <c r="C13" s="142"/>
+      <c r="D13" s="142"/>
+      <c r="E13" s="142"/>
+      <c r="F13" s="142"/>
+      <c r="G13" s="142"/>
+      <c r="H13" s="142"/>
+      <c r="I13" s="142"/>
+      <c r="J13" s="142"/>
+      <c r="K13" s="143"/>
+      <c r="L13" s="119"/>
+    </row>
+    <row r="14" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="141" t="s">
+        <v>358</v>
+      </c>
+      <c r="B14" s="142"/>
+      <c r="C14" s="142"/>
+      <c r="D14" s="142"/>
+      <c r="E14" s="142"/>
+      <c r="F14" s="142"/>
+      <c r="G14" s="142"/>
+      <c r="H14" s="142"/>
+      <c r="I14" s="142"/>
+      <c r="J14" s="142"/>
+      <c r="K14" s="143"/>
+      <c r="L14" s="119"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="141"/>
+      <c r="B15" s="142"/>
+      <c r="C15" s="142"/>
+      <c r="D15" s="142"/>
+      <c r="E15" s="142"/>
+      <c r="F15" s="142"/>
+      <c r="G15" s="142"/>
+      <c r="H15" s="142"/>
+      <c r="I15" s="142"/>
+      <c r="J15" s="142"/>
+      <c r="K15" s="143"/>
+      <c r="L15" s="119"/>
+    </row>
+    <row r="17" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="123" t="s">
+      <c r="B17" s="123" t="s">
         <v>275</v>
       </c>
-      <c r="C13" s="123" t="s">
-        <v>350</v>
-      </c>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
-      <c r="G13"/>
-      <c r="H13"/>
-      <c r="I13"/>
-      <c r="J13"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
-        <v>2013</v>
-      </c>
-      <c r="B14" s="119">
-        <v>24048</v>
-      </c>
-      <c r="C14" s="119">
-        <v>4256.666666666667</v>
-      </c>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14"/>
-      <c r="G14"/>
-      <c r="H14"/>
-      <c r="I14"/>
-      <c r="J14"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
-        <v>2014</v>
-      </c>
-      <c r="B15" s="119">
-        <v>24117</v>
-      </c>
-      <c r="C15" s="119">
-        <v>4622.666666666667</v>
-      </c>
-      <c r="D15"/>
-      <c r="E15"/>
-      <c r="F15"/>
-      <c r="G15"/>
-      <c r="H15"/>
-      <c r="I15"/>
-      <c r="J15"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
-        <v>2015</v>
-      </c>
-      <c r="B16" s="119">
-        <v>25313</v>
-      </c>
-      <c r="C16" s="119">
-        <v>5025.666666666667</v>
-      </c>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16"/>
-      <c r="G16"/>
-      <c r="H16"/>
-      <c r="I16"/>
-      <c r="J16"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
-        <v>2016</v>
-      </c>
-      <c r="B17" s="119">
-        <v>25825</v>
-      </c>
-      <c r="C17" s="119">
-        <v>4901.333333333333</v>
+      <c r="C17" s="123" t="s">
+        <v>348</v>
       </c>
       <c r="D17"/>
       <c r="E17"/>
@@ -25985,13 +26116,13 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
-        <v>2017</v>
+        <v>2013</v>
       </c>
       <c r="B18" s="119">
-        <v>24998</v>
+        <v>24048</v>
       </c>
       <c r="C18" s="119">
-        <v>5001.333333333333</v>
+        <v>4256.666666666667</v>
       </c>
       <c r="D18"/>
       <c r="E18"/>
@@ -26002,42 +26133,114 @@
       <c r="J18"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="122" t="s">
+      <c r="A19" s="10">
+        <v>2014</v>
+      </c>
+      <c r="B19" s="119">
+        <v>24117</v>
+      </c>
+      <c r="C19" s="119">
+        <v>4622.666666666667</v>
+      </c>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>2015</v>
+      </c>
+      <c r="B20" s="119">
+        <v>25313</v>
+      </c>
+      <c r="C20" s="119">
+        <v>5025.666666666667</v>
+      </c>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>2016</v>
+      </c>
+      <c r="B21" s="119">
+        <v>25825</v>
+      </c>
+      <c r="C21" s="119">
+        <v>4901.333333333333</v>
+      </c>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <v>2017</v>
+      </c>
+      <c r="B22" s="119">
+        <v>24998</v>
+      </c>
+      <c r="C22" s="119">
+        <v>5001.333333333333</v>
+      </c>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="122" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="126">
-        <f>SUM(B14:B18)</f>
+      <c r="B23" s="126">
+        <f>SUM(B18:B22)</f>
         <v>124301</v>
       </c>
-      <c r="C19" s="126">
-        <f>SUM(C14:C18)</f>
+      <c r="C23" s="126">
+        <f>SUM(C18:C22)</f>
         <v>23807.666666666664</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="127"/>
-      <c r="B20" s="128"/>
-      <c r="C20" s="128"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="127"/>
+      <c r="B24" s="128"/>
+      <c r="C24" s="128"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="140" t="s">
-        <v>353</v>
-      </c>
-      <c r="B46" s="140"/>
-      <c r="C46" s="140"/>
-      <c r="D46" s="140"/>
-      <c r="E46" s="140"/>
-      <c r="F46" s="140"/>
-      <c r="G46" s="140"/>
+    <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="140" t="s">
+        <v>351</v>
+      </c>
+      <c r="B50" s="140"/>
+      <c r="C50" s="140"/>
+      <c r="D50" s="140"/>
+      <c r="E50" s="140"/>
+      <c r="F50" s="140"/>
+      <c r="G50" s="140"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A46:G46"/>
+    <mergeCell ref="A50:G50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Completed draft of paper for 10/21/2020 discussion
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="6" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="360">
   <si>
     <t>Total</t>
   </si>
@@ -1493,6 +1493,9 @@
       </rPr>
       <t xml:space="preserve"> The sum of exclusive licenses, options, and the estimated number of unique technologies licensed non-exclusively.</t>
     </r>
+  </si>
+  <si>
+    <t>Baek, Hwang, &amp; Park (2018); Munteanu (2012); Song, Park, &amp; Park (2017)</t>
   </si>
 </sst>
 </file>
@@ -2217,6 +2220,15 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2252,15 +2264,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -20095,18 +20098,18 @@
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="140" t="s">
+      <c r="A50" s="143" t="s">
         <v>343</v>
       </c>
-      <c r="B50" s="140"/>
-      <c r="C50" s="140"/>
-      <c r="D50" s="140"/>
-      <c r="E50" s="140"/>
-      <c r="F50" s="140"/>
-      <c r="G50" s="140"/>
-      <c r="H50" s="140"/>
-      <c r="I50" s="140"/>
-      <c r="J50" s="140"/>
+      <c r="B50" s="143"/>
+      <c r="C50" s="143"/>
+      <c r="D50" s="143"/>
+      <c r="E50" s="143"/>
+      <c r="F50" s="143"/>
+      <c r="G50" s="143"/>
+      <c r="H50" s="143"/>
+      <c r="I50" s="143"/>
+      <c r="J50" s="143"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -20567,54 +20570,54 @@
       <c r="H20" s="109"/>
     </row>
     <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="129" t="s">
+      <c r="A21" s="132" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="129"/>
-      <c r="C21" s="129"/>
-      <c r="D21" s="129"/>
-      <c r="E21" s="129"/>
-      <c r="F21" s="129"/>
+      <c r="B21" s="132"/>
+      <c r="C21" s="132"/>
+      <c r="D21" s="132"/>
+      <c r="E21" s="132"/>
+      <c r="F21" s="132"/>
     </row>
     <row r="22" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="130" t="s">
+      <c r="A22" s="133" t="s">
         <v>171</v>
       </c>
-      <c r="B22" s="130"/>
-      <c r="C22" s="130"/>
-      <c r="D22" s="130"/>
-      <c r="E22" s="130"/>
-      <c r="F22" s="130"/>
+      <c r="B22" s="133"/>
+      <c r="C22" s="133"/>
+      <c r="D22" s="133"/>
+      <c r="E22" s="133"/>
+      <c r="F22" s="133"/>
     </row>
     <row r="23" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="129" t="s">
+      <c r="A23" s="132" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="129"/>
-      <c r="C23" s="129"/>
-      <c r="D23" s="129"/>
-      <c r="E23" s="129"/>
-      <c r="F23" s="129"/>
+      <c r="B23" s="132"/>
+      <c r="C23" s="132"/>
+      <c r="D23" s="132"/>
+      <c r="E23" s="132"/>
+      <c r="F23" s="132"/>
     </row>
     <row r="24" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="129" t="s">
+      <c r="A24" s="132" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="129"/>
-      <c r="C24" s="129"/>
-      <c r="D24" s="129"/>
-      <c r="E24" s="129"/>
-      <c r="F24" s="129"/>
+      <c r="B24" s="132"/>
+      <c r="C24" s="132"/>
+      <c r="D24" s="132"/>
+      <c r="E24" s="132"/>
+      <c r="F24" s="132"/>
     </row>
     <row r="25" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="129" t="s">
+      <c r="A25" s="132" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="129"/>
-      <c r="C25" s="129"/>
-      <c r="D25" s="129"/>
-      <c r="E25" s="129"/>
-      <c r="F25" s="129"/>
+      <c r="B25" s="132"/>
+      <c r="C25" s="132"/>
+      <c r="D25" s="132"/>
+      <c r="E25" s="132"/>
+      <c r="F25" s="132"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="30"/>
@@ -20719,11 +20722,11 @@
   </sheetPr>
   <dimension ref="A1:AA78"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="4" ySplit="4" topLeftCell="E15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20798,38 +20801,38 @@
       <c r="B3" s="69"/>
       <c r="C3" s="70"/>
       <c r="D3" s="71"/>
-      <c r="E3" s="134" t="s">
+      <c r="E3" s="137" t="s">
         <v>267</v>
       </c>
-      <c r="F3" s="135"/>
-      <c r="G3" s="135"/>
-      <c r="H3" s="132"/>
-      <c r="I3" s="131" t="s">
+      <c r="F3" s="138"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="135"/>
+      <c r="I3" s="134" t="s">
         <v>294</v>
       </c>
-      <c r="J3" s="132"/>
-      <c r="K3" s="131" t="s">
+      <c r="J3" s="135"/>
+      <c r="K3" s="134" t="s">
         <v>295</v>
       </c>
-      <c r="L3" s="133"/>
-      <c r="M3" s="134" t="s">
+      <c r="L3" s="136"/>
+      <c r="M3" s="137" t="s">
         <v>282</v>
       </c>
-      <c r="N3" s="135"/>
-      <c r="O3" s="132"/>
-      <c r="P3" s="136" t="s">
+      <c r="N3" s="138"/>
+      <c r="O3" s="135"/>
+      <c r="P3" s="139" t="s">
         <v>249</v>
       </c>
-      <c r="Q3" s="135"/>
-      <c r="R3" s="135"/>
-      <c r="S3" s="135"/>
-      <c r="T3" s="135"/>
-      <c r="U3" s="135"/>
-      <c r="V3" s="135"/>
-      <c r="W3" s="135"/>
-      <c r="X3" s="135"/>
-      <c r="Y3" s="135"/>
-      <c r="Z3" s="137"/>
+      <c r="Q3" s="138"/>
+      <c r="R3" s="138"/>
+      <c r="S3" s="138"/>
+      <c r="T3" s="138"/>
+      <c r="U3" s="138"/>
+      <c r="V3" s="138"/>
+      <c r="W3" s="138"/>
+      <c r="X3" s="138"/>
+      <c r="Y3" s="138"/>
+      <c r="Z3" s="140"/>
       <c r="AA3" s="90"/>
     </row>
     <row r="4" spans="1:27" ht="170.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -21175,7 +21178,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="11" spans="1:27" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" s="11" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="111"/>
       <c r="B11" s="111"/>
       <c r="C11" s="112" t="s">
@@ -21221,7 +21224,7 @@
       <c r="Y11" s="117"/>
       <c r="Z11" s="117"/>
       <c r="AA11" s="118" t="s">
-        <v>252</v>
+        <v>359</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -24105,10 +24108,10 @@
       <c r="A3" s="69"/>
       <c r="B3" s="70"/>
       <c r="C3" s="71"/>
-      <c r="D3" s="134" t="s">
+      <c r="D3" s="137" t="s">
         <v>194</v>
       </c>
-      <c r="E3" s="132"/>
+      <c r="E3" s="135"/>
       <c r="F3" s="73"/>
     </row>
     <row r="4" spans="1:6" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -24368,32 +24371,32 @@
       <c r="F23" s="59"/>
     </row>
     <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="129"/>
-      <c r="B24" s="129"/>
-      <c r="C24" s="129"/>
-      <c r="D24" s="129"/>
-      <c r="E24" s="129"/>
+      <c r="A24" s="132"/>
+      <c r="B24" s="132"/>
+      <c r="C24" s="132"/>
+      <c r="D24" s="132"/>
+      <c r="E24" s="132"/>
     </row>
     <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="129"/>
-      <c r="B25" s="129"/>
-      <c r="C25" s="129"/>
-      <c r="D25" s="129"/>
-      <c r="E25" s="129"/>
+      <c r="A25" s="132"/>
+      <c r="B25" s="132"/>
+      <c r="C25" s="132"/>
+      <c r="D25" s="132"/>
+      <c r="E25" s="132"/>
     </row>
     <row r="26" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="129"/>
-      <c r="B26" s="129"/>
-      <c r="C26" s="129"/>
-      <c r="D26" s="129"/>
-      <c r="E26" s="129"/>
+      <c r="A26" s="132"/>
+      <c r="B26" s="132"/>
+      <c r="C26" s="132"/>
+      <c r="D26" s="132"/>
+      <c r="E26" s="132"/>
     </row>
     <row r="27" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="129"/>
-      <c r="B27" s="129"/>
-      <c r="C27" s="129"/>
-      <c r="D27" s="129"/>
-      <c r="E27" s="129"/>
+      <c r="A27" s="132"/>
+      <c r="B27" s="132"/>
+      <c r="C27" s="132"/>
+      <c r="D27" s="132"/>
+      <c r="E27" s="132"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="60"/>
@@ -25184,40 +25187,40 @@
       <c r="H15" s="32"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="130" t="s">
+      <c r="A16" s="133" t="s">
         <v>99</v>
       </c>
-      <c r="B16" s="130"/>
-      <c r="C16" s="130"/>
-      <c r="D16" s="130"/>
-      <c r="E16" s="130"/>
-      <c r="F16" s="130"/>
-      <c r="G16" s="130"/>
-      <c r="H16" s="130"/>
-      <c r="I16" s="130"/>
+      <c r="B16" s="133"/>
+      <c r="C16" s="133"/>
+      <c r="D16" s="133"/>
+      <c r="E16" s="133"/>
+      <c r="F16" s="133"/>
+      <c r="G16" s="133"/>
+      <c r="H16" s="133"/>
+      <c r="I16" s="133"/>
     </row>
     <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="129"/>
-      <c r="B17" s="129"/>
-      <c r="C17" s="129"/>
+      <c r="A17" s="132"/>
+      <c r="B17" s="132"/>
+      <c r="C17" s="132"/>
       <c r="D17" s="32"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="129"/>
-      <c r="B18" s="129"/>
-      <c r="C18" s="129"/>
+      <c r="A18" s="132"/>
+      <c r="B18" s="132"/>
+      <c r="C18" s="132"/>
       <c r="D18" s="32"/>
       <c r="E18" s="32"/>
       <c r="F18" s="32"/>
       <c r="H18" s="32"/>
     </row>
     <row r="19" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="129"/>
-      <c r="B19" s="129"/>
-      <c r="C19" s="129"/>
+      <c r="A19" s="132"/>
+      <c r="B19" s="132"/>
+      <c r="C19" s="132"/>
       <c r="D19" s="32"/>
       <c r="E19" s="32"/>
       <c r="F19" s="32"/>
@@ -25657,30 +25660,30 @@
       <c r="C41" s="52"/>
     </row>
     <row r="42" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="138" t="s">
+      <c r="A42" s="141" t="s">
         <v>166</v>
       </c>
-      <c r="B42" s="138"/>
-      <c r="C42" s="138"/>
+      <c r="B42" s="141"/>
+      <c r="C42" s="141"/>
     </row>
     <row r="43" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="139" t="s">
+      <c r="A43" s="142" t="s">
         <v>167</v>
       </c>
-      <c r="B43" s="139"/>
-      <c r="C43" s="139"/>
+      <c r="B43" s="142"/>
+      <c r="C43" s="142"/>
     </row>
     <row r="44" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="138" t="s">
+      <c r="A44" s="141" t="s">
         <v>168</v>
       </c>
-      <c r="B44" s="138"/>
-      <c r="C44" s="138"/>
+      <c r="B44" s="141"/>
+      <c r="C44" s="141"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="129"/>
-      <c r="B45" s="129"/>
-      <c r="C45" s="129"/>
+      <c r="A45" s="132"/>
+      <c r="B45" s="132"/>
+      <c r="C45" s="132"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="37"/>
@@ -25741,7 +25744,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -25829,7 +25832,7 @@
         <v>4256.666666666667</v>
       </c>
       <c r="K6" s="121">
-        <f>J6/B6</f>
+        <f t="shared" ref="K6:K11" si="0">J6/B6</f>
         <v>0.17700709691727656</v>
       </c>
       <c r="L6" s="119"/>
@@ -25864,11 +25867,11 @@
         <v>1132.6666666666667</v>
       </c>
       <c r="J7" s="119">
-        <f t="shared" ref="J7:J10" si="0">SUM(F7,G7,I7)</f>
+        <f t="shared" ref="J7:J10" si="1">SUM(F7,G7,I7)</f>
         <v>4622.666666666667</v>
       </c>
       <c r="K7" s="121">
-        <f>J7/B7</f>
+        <f t="shared" si="0"/>
         <v>0.19167668726071513</v>
       </c>
       <c r="L7" s="119"/>
@@ -25903,11 +25906,11 @@
         <v>1371.6666666666667</v>
       </c>
       <c r="J8" s="119">
+        <f t="shared" si="1"/>
+        <v>5025.666666666667</v>
+      </c>
+      <c r="K8" s="121">
         <f t="shared" si="0"/>
-        <v>5025.666666666667</v>
-      </c>
-      <c r="K8" s="121">
-        <f>J8/B8</f>
         <v>0.19854093417084767</v>
       </c>
       <c r="L8" s="119"/>
@@ -25942,11 +25945,11 @@
         <v>1400.3333333333333</v>
       </c>
       <c r="J9" s="119">
+        <f t="shared" si="1"/>
+        <v>4901.333333333333</v>
+      </c>
+      <c r="K9" s="121">
         <f t="shared" si="0"/>
-        <v>4901.333333333333</v>
-      </c>
-      <c r="K9" s="121">
-        <f>J9/B9</f>
         <v>0.18979025492094223</v>
       </c>
       <c r="L9" s="119"/>
@@ -25981,11 +25984,11 @@
         <v>1398.3333333333333</v>
       </c>
       <c r="J10" s="119">
+        <f t="shared" si="1"/>
+        <v>5001.333333333333</v>
+      </c>
+      <c r="K10" s="121">
         <f t="shared" si="0"/>
-        <v>5001.333333333333</v>
-      </c>
-      <c r="K10" s="121">
-        <f>J10/B10</f>
         <v>0.20006933888044376</v>
       </c>
       <c r="L10" s="119"/>
@@ -25995,105 +25998,105 @@
         <v>0</v>
       </c>
       <c r="B11" s="124">
-        <f t="shared" ref="B11:J11" si="1">SUM(B6:B10)</f>
+        <f t="shared" ref="B11:J11" si="2">SUM(B6:B10)</f>
         <v>124301</v>
       </c>
       <c r="C11" s="124">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>76669</v>
       </c>
       <c r="D11" s="124">
-        <f t="shared" ref="D11:E11" si="2">SUM(D6:D10)</f>
+        <f t="shared" ref="D11:E11" si="3">SUM(D6:D10)</f>
         <v>57389</v>
       </c>
       <c r="E11" s="124">
+        <f t="shared" si="3"/>
+        <v>7479</v>
+      </c>
+      <c r="F11" s="124">
         <f t="shared" si="2"/>
-        <v>7479</v>
-      </c>
-      <c r="F11" s="124">
-        <f t="shared" si="1"/>
         <v>10000</v>
       </c>
       <c r="G11" s="124">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7368</v>
       </c>
       <c r="H11" s="124">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19319</v>
       </c>
       <c r="I11" s="124">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6439.6666666666661</v>
       </c>
       <c r="J11" s="124">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23807.666666666664</v>
       </c>
       <c r="K11" s="125">
-        <f>J11/B11</f>
+        <f t="shared" si="0"/>
         <v>0.19153238241580248</v>
       </c>
       <c r="L11" s="119"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="141"/>
-      <c r="B12" s="142"/>
-      <c r="C12" s="142"/>
-      <c r="D12" s="142"/>
-      <c r="E12" s="142"/>
-      <c r="F12" s="142"/>
-      <c r="G12" s="142"/>
-      <c r="H12" s="142"/>
-      <c r="I12" s="142"/>
-      <c r="J12" s="142"/>
-      <c r="K12" s="143"/>
+      <c r="A12" s="129"/>
+      <c r="B12" s="130"/>
+      <c r="C12" s="130"/>
+      <c r="D12" s="130"/>
+      <c r="E12" s="130"/>
+      <c r="F12" s="130"/>
+      <c r="G12" s="130"/>
+      <c r="H12" s="130"/>
+      <c r="I12" s="130"/>
+      <c r="J12" s="130"/>
+      <c r="K12" s="131"/>
       <c r="L12" s="119"/>
     </row>
     <row r="13" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="141" t="s">
+      <c r="A13" s="129" t="s">
         <v>357</v>
       </c>
-      <c r="B13" s="142"/>
-      <c r="C13" s="142"/>
-      <c r="D13" s="142"/>
-      <c r="E13" s="142"/>
-      <c r="F13" s="142"/>
-      <c r="G13" s="142"/>
-      <c r="H13" s="142"/>
-      <c r="I13" s="142"/>
-      <c r="J13" s="142"/>
-      <c r="K13" s="143"/>
+      <c r="B13" s="130"/>
+      <c r="C13" s="130"/>
+      <c r="D13" s="130"/>
+      <c r="E13" s="130"/>
+      <c r="F13" s="130"/>
+      <c r="G13" s="130"/>
+      <c r="H13" s="130"/>
+      <c r="I13" s="130"/>
+      <c r="J13" s="130"/>
+      <c r="K13" s="131"/>
       <c r="L13" s="119"/>
     </row>
     <row r="14" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="141" t="s">
+      <c r="A14" s="129" t="s">
         <v>358</v>
       </c>
-      <c r="B14" s="142"/>
-      <c r="C14" s="142"/>
-      <c r="D14" s="142"/>
-      <c r="E14" s="142"/>
-      <c r="F14" s="142"/>
-      <c r="G14" s="142"/>
-      <c r="H14" s="142"/>
-      <c r="I14" s="142"/>
-      <c r="J14" s="142"/>
-      <c r="K14" s="143"/>
+      <c r="B14" s="130"/>
+      <c r="C14" s="130"/>
+      <c r="D14" s="130"/>
+      <c r="E14" s="130"/>
+      <c r="F14" s="130"/>
+      <c r="G14" s="130"/>
+      <c r="H14" s="130"/>
+      <c r="I14" s="130"/>
+      <c r="J14" s="130"/>
+      <c r="K14" s="131"/>
       <c r="L14" s="119"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="141"/>
-      <c r="B15" s="142"/>
-      <c r="C15" s="142"/>
-      <c r="D15" s="142"/>
-      <c r="E15" s="142"/>
-      <c r="F15" s="142"/>
-      <c r="G15" s="142"/>
-      <c r="H15" s="142"/>
-      <c r="I15" s="142"/>
-      <c r="J15" s="142"/>
-      <c r="K15" s="143"/>
+      <c r="A15" s="129"/>
+      <c r="B15" s="130"/>
+      <c r="C15" s="130"/>
+      <c r="D15" s="130"/>
+      <c r="E15" s="130"/>
+      <c r="F15" s="130"/>
+      <c r="G15" s="130"/>
+      <c r="H15" s="130"/>
+      <c r="I15" s="130"/>
+      <c r="J15" s="130"/>
+      <c r="K15" s="131"/>
       <c r="L15" s="119"/>
     </row>
     <row r="17" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -26228,15 +26231,15 @@
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="140" t="s">
+      <c r="A50" s="143" t="s">
         <v>351</v>
       </c>
-      <c r="B50" s="140"/>
-      <c r="C50" s="140"/>
-      <c r="D50" s="140"/>
-      <c r="E50" s="140"/>
-      <c r="F50" s="140"/>
-      <c r="G50" s="140"/>
+      <c r="B50" s="143"/>
+      <c r="C50" s="143"/>
+      <c r="D50" s="143"/>
+      <c r="E50" s="143"/>
+      <c r="F50" s="143"/>
+      <c r="G50" s="143"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Added content about occupational culture and edited figure on federal obligations to universities
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="5" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="363">
   <si>
     <t>Total</t>
   </si>
@@ -1496,6 +1496,38 @@
   </si>
   <si>
     <t>Baek, Hwang, &amp; Park (2018); Munteanu (2012); Song, Park, &amp; Park (2017)</t>
+  </si>
+  <si>
+    <t>Federal Obligations to Universities for Research and Development, 2000-2019</t>
+  </si>
+  <si>
+    <t>Figure created by author.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">National Science Foundation, National Center for Science and Engineering Statistics [NCSES]. (2020). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Survey of Federal Funds for Research and Development, Fiscal Years 2018-19</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Retrieved May 7, 2020 from http://www.nsf.gov/statistics/fedfunds/</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2945,67 +2977,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Federal Obligations to Universities</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> for Research and Development</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -3017,7 +2989,7 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -13951,16 +13923,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>14286</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>33336</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -18630,9 +18602,9 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:W54"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18640,7 +18612,7 @@
     <col min="2" max="2" width="23.42578125" style="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
@@ -18650,8 +18622,11 @@
       <c r="D1" s="18" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="M1" s="108" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>1967</v>
       </c>
@@ -18662,15 +18637,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>1968</v>
       </c>
       <c r="B3" s="19">
         <v>1487.4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="M3" s="110" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>1969</v>
       </c>
@@ -18681,7 +18659,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>1970</v>
       </c>
@@ -18689,7 +18667,7 @@
         <v>1475.6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>1971</v>
       </c>
@@ -18697,7 +18675,7 @@
         <v>1644.6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>1972</v>
       </c>
@@ -18705,7 +18683,7 @@
         <v>1903.5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>1973</v>
       </c>
@@ -18713,7 +18691,7 @@
         <v>1916.6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>1974</v>
       </c>
@@ -18721,7 +18699,7 @@
         <v>2214</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>1975</v>
       </c>
@@ -18729,7 +18707,7 @@
         <v>2411.4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>1976</v>
       </c>
@@ -18737,7 +18715,7 @@
         <v>2551.8000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>1977</v>
       </c>
@@ -18745,7 +18723,7 @@
         <v>2905.5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>1978</v>
       </c>
@@ -18753,7 +18731,7 @@
         <v>3374.6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>1979</v>
       </c>
@@ -18761,7 +18739,7 @@
         <v>3888.8</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>1980</v>
       </c>
@@ -18769,7 +18747,7 @@
         <v>4263.3999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>1981</v>
       </c>
@@ -18777,7 +18755,7 @@
         <v>4465.8</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>1982</v>
       </c>
@@ -18785,7 +18763,7 @@
         <v>4605.5</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>1983</v>
       </c>
@@ -18793,7 +18771,7 @@
         <v>4966.3999999999996</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>1984</v>
       </c>
@@ -18801,7 +18779,7 @@
         <v>5546.9</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>1985</v>
       </c>
@@ -18809,7 +18787,7 @@
         <v>6339.7</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>1986</v>
       </c>
@@ -18817,7 +18795,7 @@
         <v>6558.8</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>1987</v>
       </c>
@@ -18825,7 +18803,7 @@
         <v>7337.3</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>1988</v>
       </c>
@@ -18833,7 +18811,7 @@
         <v>7827.7</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>1989</v>
       </c>
@@ -18841,7 +18819,7 @@
         <v>8672</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>1990</v>
       </c>
@@ -18849,7 +18827,7 @@
         <v>9137.5</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>1991</v>
       </c>
@@ -18857,7 +18835,7 @@
         <v>10168.5</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>1992</v>
       </c>
@@ -18865,7 +18843,7 @@
         <v>10271.200000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>1993</v>
       </c>
@@ -18873,15 +18851,18 @@
         <v>11208.4</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>1994</v>
       </c>
       <c r="B29" s="19">
         <v>11796.9</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="M29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>1995</v>
       </c>
@@ -18889,15 +18870,18 @@
         <v>11927.5</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>1996</v>
       </c>
       <c r="B31" s="19">
         <v>11977.8</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="M31" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>1997</v>
       </c>
@@ -18905,39 +18889,77 @@
         <v>12559</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>1998</v>
       </c>
       <c r="B33" s="19">
         <v>13380.7</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="M33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>1999</v>
       </c>
       <c r="B34" s="19">
         <v>14959.1</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="M34" s="133" t="s">
+        <v>362</v>
+      </c>
+      <c r="N34" s="133"/>
+      <c r="O34" s="133"/>
+      <c r="P34" s="133"/>
+      <c r="Q34" s="133"/>
+      <c r="R34" s="133"/>
+      <c r="S34" s="133"/>
+      <c r="T34" s="133"/>
+      <c r="U34" s="133"/>
+      <c r="V34" s="133"/>
+      <c r="W34" s="133"/>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>2000</v>
       </c>
       <c r="B35" s="19">
         <v>16890.7</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="M35" s="133"/>
+      <c r="N35" s="133"/>
+      <c r="O35" s="133"/>
+      <c r="P35" s="133"/>
+      <c r="Q35" s="133"/>
+      <c r="R35" s="133"/>
+      <c r="S35" s="133"/>
+      <c r="T35" s="133"/>
+      <c r="U35" s="133"/>
+      <c r="V35" s="133"/>
+      <c r="W35" s="133"/>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <v>2001</v>
       </c>
       <c r="B36" s="19">
         <v>20065.099999999999</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="M36" s="133"/>
+      <c r="N36" s="133"/>
+      <c r="O36" s="133"/>
+      <c r="P36" s="133"/>
+      <c r="Q36" s="133"/>
+      <c r="R36" s="133"/>
+      <c r="S36" s="133"/>
+      <c r="T36" s="133"/>
+      <c r="U36" s="133"/>
+      <c r="V36" s="133"/>
+      <c r="W36" s="133"/>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
         <v>2002</v>
       </c>
@@ -18945,7 +18967,7 @@
         <v>21620</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>2003</v>
       </c>
@@ -18953,7 +18975,7 @@
         <v>23005.8</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
         <v>2004</v>
       </c>
@@ -18961,7 +18983,7 @@
         <v>24947</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
         <v>2005</v>
       </c>
@@ -18969,7 +18991,7 @@
         <v>25687.5</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" s="10">
         <v>2006</v>
       </c>
@@ -18977,7 +18999,7 @@
         <v>24669.7</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" s="10">
         <v>2007</v>
       </c>
@@ -18985,7 +19007,7 @@
         <v>25547.8</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" s="10">
         <v>2008</v>
       </c>
@@ -18993,7 +19015,7 @@
         <v>26026.5</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" s="10">
         <v>2009</v>
       </c>
@@ -19001,7 +19023,7 @@
         <v>31557.8</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45" s="10">
         <v>2010</v>
       </c>
@@ -19009,7 +19031,7 @@
         <v>31192.3</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" s="10">
         <v>2011</v>
       </c>
@@ -19017,7 +19039,7 @@
         <v>27680.3</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" s="10">
         <v>2012</v>
       </c>
@@ -19025,7 +19047,7 @@
         <v>27509.5</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48" s="10">
         <v>2013</v>
       </c>
@@ -19082,8 +19104,12 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="M34:W36"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -20722,7 +20748,7 @@
   </sheetPr>
   <dimension ref="A1:AA78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="4" ySplit="4" topLeftCell="E15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>

</xml_diff>

<commit_message>
Rename prompt as motivation in figure on theory of organization
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="5" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="11" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId1"/>
@@ -6875,13 +6875,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>514349</xdr:colOff>
+      <xdr:colOff>333375</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>314324</xdr:colOff>
+      <xdr:colOff>314325</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
@@ -6901,72 +6901,11 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="909637" y="3881437"/>
-          <a:ext cx="838200" cy="409575"/>
+          <a:off x="819150" y="3790950"/>
+          <a:ext cx="838200" cy="590550"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>19051</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>42863</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="9" name="Connector: Elbow 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F35639BC-17AA-4A20-B1FE-C31691DD264E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="96" idx="2"/>
-          <a:endCxn id="2" idx="2"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="9098757" y="-4688681"/>
-          <a:ext cx="23812" cy="16716375"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 9260192"/>
-          </a:avLst>
         </a:prstGeom>
         <a:ln w="25400">
           <a:solidFill>
@@ -8075,13 +8014,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
+      <xdr:colOff>142876</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:rowOff>42861</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>314323</xdr:colOff>
+      <xdr:colOff>314324</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>119062</xdr:rowOff>
     </xdr:to>
@@ -8095,14 +8034,14 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="71" idx="2"/>
+          <a:stCxn id="2" idx="2"/>
           <a:endCxn id="42" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="545305" y="4102894"/>
-          <a:ext cx="1414463" cy="561973"/>
+          <a:off x="438149" y="3995738"/>
+          <a:ext cx="1409701" cy="781048"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -8388,8 +8327,8 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
@@ -8399,52 +8338,118 @@
       <xdr:row>19</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="49" name="Connector: Elbow 48">
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="21" name="Group 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAB35973-1A11-4FB9-BAFA-554FA922B9C9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8282F3FE-F038-40E7-87C4-96C2CA5AB907}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="96" idx="2"/>
-          <a:endCxn id="118" idx="2"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="10591800" y="-3200400"/>
-          <a:ext cx="19050" cy="13735050"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="552450" y="3657600"/>
+          <a:ext cx="16916400" cy="19050"/>
+          <a:chOff x="552450" y="3657600"/>
+          <a:chExt cx="16916400" cy="19050"/>
         </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 11600000"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="9" name="Connector: Elbow 8">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F35639BC-17AA-4A20-B1FE-C31691DD264E}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="96" idx="2"/>
+            <a:endCxn id="71" idx="2"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="5400000">
+            <a:off x="9001125" y="-4791075"/>
+            <a:ext cx="19050" cy="16916400"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 11600000"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="lg" len="lg"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
             <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="49" name="Connector: Elbow 48">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAB35973-1A11-4FB9-BAFA-554FA922B9C9}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="96" idx="2"/>
+            <a:endCxn id="118" idx="2"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="5400000">
+            <a:off x="10591800" y="-3200400"/>
+            <a:ext cx="19050" cy="13735050"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 11600000"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle" w="lg" len="lg"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -8970,7 +8975,7 @@
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>Prompts</a:t>
+              <a:t>Motivation</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -8988,7 +8993,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="742950" y="3219450"/>
+            <a:off x="323850" y="3219450"/>
             <a:ext cx="457200" cy="457200"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -9041,7 +9046,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="895350" y="3209925"/>
+            <a:off x="714375" y="3209925"/>
             <a:ext cx="457200" cy="457200"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -9169,7 +9174,7 @@
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>Options</a:t>
+              <a:t>Options for Action</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -18604,7 +18609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -20154,9 +20159,7 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Minor update to conceptual framework
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="11" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="12" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId1"/>
@@ -11340,7 +11340,7 @@
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>Technology available for assimilation</a:t>
+              <a:t>Option for Action: Assimilate a given available technology</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -20159,7 +20159,7 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -20184,7 +20184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Created figure on narrowing conception of technology
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="12" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="7" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId1"/>
@@ -21,16 +21,17 @@
     <sheet name="Table - Alt Readiness Scales" sheetId="8" r:id="rId7"/>
     <sheet name="Figure - Tech Utilization" sheetId="19" r:id="rId8"/>
     <sheet name="Figure - Defining Technology" sheetId="12" r:id="rId9"/>
-    <sheet name="Figure - R&amp;D Funding 1967-2019" sheetId="3" r:id="rId10"/>
-    <sheet name="Figure - R&amp;D Funding 1990-2015" sheetId="1" r:id="rId11"/>
-    <sheet name="Figure - R&amp;D Funding 1951-2019" sheetId="2" r:id="rId12"/>
-    <sheet name="Figure - Stokes Model" sheetId="17" r:id="rId13"/>
-    <sheet name="Figure - Research Cycle" sheetId="13" r:id="rId14"/>
-    <sheet name="Figure - Research Model" sheetId="16" r:id="rId15"/>
-    <sheet name="Figure - Valley of Death" sheetId="18" r:id="rId16"/>
-    <sheet name="Figure - Theory the Org" sheetId="15" r:id="rId17"/>
-    <sheet name="Figure - Conceptual Framework" sheetId="9" r:id="rId18"/>
-    <sheet name="Figure - Literature Landscape" sheetId="14" r:id="rId19"/>
+    <sheet name="Figure - Conception of Techn" sheetId="20" r:id="rId10"/>
+    <sheet name="Figure - R&amp;D Funding 1967-2019" sheetId="3" r:id="rId11"/>
+    <sheet name="Figure - R&amp;D Funding 1990-2015" sheetId="1" r:id="rId12"/>
+    <sheet name="Figure - R&amp;D Funding 1951-2019" sheetId="2" r:id="rId13"/>
+    <sheet name="Figure - Stokes Model" sheetId="17" r:id="rId14"/>
+    <sheet name="Figure - Research Cycle" sheetId="13" r:id="rId15"/>
+    <sheet name="Figure - Research Model" sheetId="16" r:id="rId16"/>
+    <sheet name="Figure - Valley of Death" sheetId="18" r:id="rId17"/>
+    <sheet name="Figure - Theory the Org" sheetId="15" r:id="rId18"/>
+    <sheet name="Figure - Conceptual Framework" sheetId="9" r:id="rId19"/>
+    <sheet name="Figure - Literature Landscape" sheetId="14" r:id="rId20"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Table - Determinants Examined'!$3:$4</definedName>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="364">
   <si>
     <t>Total</t>
   </si>
@@ -1528,6 +1529,9 @@
       </rPr>
       <t>. Retrieved May 7, 2020 from http://www.nsf.gov/statistics/fedfunds/</t>
     </r>
+  </si>
+  <si>
+    <t>The Narrowing Conception of Technology</t>
   </si>
 </sst>
 </file>
@@ -6657,6 +6661,116 @@
 
 <file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>78275</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="http://live.iop-pp01.agh.sleek.net/wp-content/uploads/2014/10/PWNov14DACEY-fig1-full.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E1C6410-71A1-42F0-8C78-6D5A348D191D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="76200" y="657226"/>
+          <a:ext cx="5943600" cy="3821599"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>9530</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>74848</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20C8BA26-C7F2-484F-A99A-CCEBC4C385C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="76200" y="4600580"/>
+          <a:ext cx="5943600" cy="4637318"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
@@ -10454,7 +10568,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -12194,7 +12308,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -13928,6 +14042,1098 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>533399</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Oval 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF779A5F-111F-4F3A-AFD5-4AC1205F7B1F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="76199" y="742950"/>
+          <a:ext cx="5943600" cy="5943600"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="31750">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100" i="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>457199</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Oval 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B7320A3-467E-4BE5-80B1-A207CC74E379}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="761999" y="2114550"/>
+          <a:ext cx="4572000" cy="4572000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="31750">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>533399</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABEE8726-4A04-4F17-9D34-57F7325C5D5E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1904999" y="1000125"/>
+          <a:ext cx="2286000" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Ancient Greek concept of </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" i="1"/>
+            <a:t>techne</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>396239</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>213359</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A1C3625-672B-429F-9593-18F4006D0A70}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2225039" y="2305049"/>
+          <a:ext cx="1645920" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Modern</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> English </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>concept of</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> technology</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" i="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Oval 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6626ECF1-A32E-4DB1-A201-4876D683903F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219199" y="3028950"/>
+          <a:ext cx="3657600" cy="3657600"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="31750">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>304799</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304799</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>112395</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="TextBox 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7FB99FD-F281-4494-8249-6C5F9EE8C5CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2133599" y="3286125"/>
+          <a:ext cx="1828800" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Patentable subject matter</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" i="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>533399</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="TextBox 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{467692E7-3CF3-4060-B6AB-645E4BC31D83}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2362199" y="3752850"/>
+          <a:ext cx="1371600" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Patent applications</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" i="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>320039</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>289559</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Oval 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D008CCB-821B-480A-A1C9-15C5148E7A1F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1539239" y="3669030"/>
+          <a:ext cx="3017520" cy="3017520"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="31750">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>304799</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304799</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Oval 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{643BDBF7-4880-49FB-8064-179CC59E31C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2133599" y="4857750"/>
+          <a:ext cx="1828800" cy="1828800"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="31750">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>533399</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>150495</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="TextBox 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{044C68DF-13C7-4B82-A0E4-5BB1B343455B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2362199" y="5038725"/>
+          <a:ext cx="1371600" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Allowed patents</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" i="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Oval 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DAA0048-0705-497B-9E2B-D869F4BFE041}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2333625" y="2105025"/>
+          <a:ext cx="3657600" cy="3657600"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="31750">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>17145</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Oval 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8667881C-AD2A-4426-B7FF-74BF708F46F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3400425" y="3619500"/>
+          <a:ext cx="2103120" cy="2103120"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="31750">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="TextBox 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{648F2381-9932-4042-B406-88FFCB646914}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6076950" y="2124074"/>
+          <a:ext cx="1828800" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" i="0"/>
+            <a:t>Manuscript s</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" i="0" baseline="0"/>
+            <a:t>ubmissions to scientific journals</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" i="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>255270</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>316230</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="TextBox 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE9696B6-BC73-4796-8FDC-4D3798CA9244}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6351270" y="3095624"/>
+          <a:ext cx="1280160" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" i="0"/>
+            <a:t>Published scientific journal</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" i="0" baseline="0"/>
+            <a:t> articles</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" i="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>318750</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>255270</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>98445</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Straight Arrow Connector 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5ACBB61-1A5F-4403-B6C9-0889FED8D2B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="19" idx="1"/>
+          <a:endCxn id="16" idx="7"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5195550" y="3324224"/>
+          <a:ext cx="1155720" cy="603271"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>578782</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>145118</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Straight Arrow Connector 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DCFA087-14F4-4929-B34F-A43404EEF255}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="18" idx="1"/>
+          <a:endCxn id="15" idx="7"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5455582" y="2352674"/>
+          <a:ext cx="621368" cy="287994"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>33336</xdr:colOff>
       <xdr:row>4</xdr:row>
@@ -13965,7 +15171,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -14006,7 +15212,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -14047,7 +15253,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -14809,7 +16015,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -15457,7 +16663,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -17743,116 +18949,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>66676</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>78275</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="http://live.iop-pp01.agh.sleek.net/wp-content/uploads/2014/10/PWNov14DACEY-fig1-full.jpg">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E1C6410-71A1-42F0-8C78-6D5A348D191D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="76200" y="657226"/>
-          <a:ext cx="5943600" cy="3821599"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>9530</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>74848</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20C8BA26-C7F2-484F-A99A-CCEBC4C385C0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="76200" y="4600580"/>
-          <a:ext cx="5943600" cy="4637318"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -18607,6 +19703,34 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="108" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="110" t="s">
+        <v>363</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="76" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W54"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -19118,7 +20242,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
@@ -19375,7 +20499,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D70"/>
   <sheetViews>
@@ -19960,7 +21084,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -19993,7 +21117,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -20024,7 +21148,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -20110,7 +21234,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
@@ -20152,7 +21276,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -20180,11 +21304,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -20201,34 +21325,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="108" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="110" t="s">
-        <v>322</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="82" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -20741,6 +21837,34 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="69" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="108" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="110" t="s">
+        <v>322</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="82" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Minor edit to figure on conception of technology
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="365">
   <si>
     <t>Total</t>
   </si>
@@ -1532,6 +1532,9 @@
   </si>
   <si>
     <t>The Narrowing Conception of Technology</t>
+  </si>
+  <si>
+    <t>What civilization considers to be technology has narrowed considerably over time.</t>
   </si>
 </sst>
 </file>
@@ -1888,7 +1891,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -2300,6 +2303,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -14249,84 +14255,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>396239</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>213359</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A1C3625-672B-429F-9593-18F4006D0A70}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2225039" y="2305049"/>
-          <a:ext cx="1645920" cy="457200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Modern</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> English </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>concept of</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> technology</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" i="1"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>609599</xdr:colOff>
       <xdr:row>15</xdr:row>
@@ -14388,72 +14316,6 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>304799</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>304799</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>112395</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="TextBox 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7FB99FD-F281-4494-8249-6C5F9EE8C5CC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2133599" y="3286125"/>
-          <a:ext cx="1828800" cy="274320"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Patentable subject matter</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" i="1"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -14766,7 +14628,7 @@
           <a:solidFill>
             <a:schemeClr val="tx1"/>
           </a:solidFill>
-          <a:prstDash val="dash"/>
+          <a:prstDash val="sysDot"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -15125,6 +14987,150 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>396239</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>213359</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A1C3625-672B-429F-9593-18F4006D0A70}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2225039" y="2305049"/>
+          <a:ext cx="1645920" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Modern</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> English </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>concept of</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> technology</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" i="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>304799</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304799</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>112395</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="TextBox 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7FB99FD-F281-4494-8249-6C5F9EE8C5CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2133599" y="3286125"/>
+          <a:ext cx="1828800" cy="274320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Patentable subject matter</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" i="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -19706,7 +19712,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -19722,7 +19728,27 @@
         <v>363</v>
       </c>
     </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="144" t="s">
+        <v>364</v>
+      </c>
+      <c r="B37" s="144"/>
+      <c r="C37" s="144"/>
+      <c r="D37" s="144"/>
+      <c r="E37" s="144"/>
+      <c r="F37" s="144"/>
+      <c r="G37" s="144"/>
+      <c r="H37" s="144"/>
+      <c r="I37" s="144"/>
+      <c r="J37" s="144"/>
+      <c r="K37" s="144"/>
+      <c r="L37" s="144"/>
+      <c r="M37" s="144"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A37:M37"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="76" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Updated page breaks and Figure 1
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="7" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="7" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="366">
   <si>
     <t>Total</t>
   </si>
@@ -1374,9 +1374,6 @@
     <t>Non-Exclusive License</t>
   </si>
   <si>
-    <t>Estimated Number of Technologies Transferred</t>
-  </si>
-  <si>
     <t>Estimated Pct of Technologies Transferred</t>
   </si>
   <si>
@@ -1535,6 +1532,12 @@
   </si>
   <si>
     <t>What civilization considers to be technology has narrowed considerably over time.</t>
+  </si>
+  <si>
+    <t>Estimated Number of Disclosures</t>
+  </si>
+  <si>
+    <t>Est. No. of Inventions Optioned, Licensed Exclusively, and Licensed Non-exclusively</t>
   </si>
 </sst>
 </file>
@@ -2358,7 +2361,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Disclosures</c:v>
+                  <c:v>Estimated Number of Disclosures</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2496,7 +2499,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Estimated Number of Technologies Transferred</c:v>
+                  <c:v>Est. No. of Inventions Optioned, Licensed Exclusively, and Licensed Non-exclusively</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -19714,7 +19717,7 @@
   </sheetPr>
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -19725,12 +19728,12 @@
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="144" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B37" s="144"/>
       <c r="C37" s="144"/>
@@ -19800,7 +19803,7 @@
         <v>1487.4</v>
       </c>
       <c r="M3" s="110" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -20033,7 +20036,7 @@
         <v>11977.8</v>
       </c>
       <c r="M31" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -20063,7 +20066,7 @@
         <v>14959.1</v>
       </c>
       <c r="M34" s="133" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="N34" s="133"/>
       <c r="O34" s="133"/>
@@ -22403,7 +22406,7 @@
       <c r="Y11" s="117"/>
       <c r="Z11" s="117"/>
       <c r="AA11" s="118" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -26923,7 +26926,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -26938,7 +26941,7 @@
     </row>
     <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="110" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="77.25" x14ac:dyDescent="0.25">
@@ -26949,13 +26952,13 @@
         <v>275</v>
       </c>
       <c r="C5" s="123" t="s">
+        <v>351</v>
+      </c>
+      <c r="D5" s="123" t="s">
+        <v>353</v>
+      </c>
+      <c r="E5" s="123" t="s">
         <v>352</v>
-      </c>
-      <c r="D5" s="123" t="s">
-        <v>354</v>
-      </c>
-      <c r="E5" s="123" t="s">
-        <v>353</v>
       </c>
       <c r="F5" s="123" t="s">
         <v>345</v>
@@ -26967,13 +26970,13 @@
         <v>347</v>
       </c>
       <c r="I5" s="123" t="s">
+        <v>354</v>
+      </c>
+      <c r="J5" s="123" t="s">
         <v>355</v>
       </c>
-      <c r="J5" s="123" t="s">
-        <v>356</v>
-      </c>
       <c r="K5" s="123" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="L5" s="120"/>
     </row>
@@ -27234,7 +27237,7 @@
     </row>
     <row r="13" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A13" s="129" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B13" s="130"/>
       <c r="C13" s="130"/>
@@ -27250,7 +27253,7 @@
     </row>
     <row r="14" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A14" s="129" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B14" s="130"/>
       <c r="C14" s="130"/>
@@ -27278,15 +27281,15 @@
       <c r="K15" s="131"/>
       <c r="L15" s="119"/>
     </row>
-    <row r="17" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="122" t="s">
         <v>1</v>
       </c>
       <c r="B17" s="123" t="s">
-        <v>275</v>
+        <v>364</v>
       </c>
       <c r="C17" s="123" t="s">
-        <v>348</v>
+        <v>365</v>
       </c>
       <c r="D17"/>
       <c r="E17"/>
@@ -27411,7 +27414,7 @@
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="143" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B50" s="143"/>
       <c r="C50" s="143"/>

</xml_diff>

<commit_message>
Minor edits to paper and added tables for knowledge premises and variables
</commit_message>
<xml_diff>
--- a/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
+++ b/Docs/PSP6980_2020_Fall_Townes_Paper_Tables-and-Figures_v00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="7" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="938" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Table - R&amp;D Funding 1967-2019" sheetId="4" r:id="rId1"/>
@@ -19,19 +19,21 @@
     <sheet name="Table - Org Studies" sheetId="10" r:id="rId5"/>
     <sheet name="Table - NASA TRL Scale" sheetId="7" r:id="rId6"/>
     <sheet name="Table - Alt Readiness Scales" sheetId="8" r:id="rId7"/>
-    <sheet name="Figure - Tech Utilization" sheetId="19" r:id="rId8"/>
-    <sheet name="Figure - Defining Technology" sheetId="12" r:id="rId9"/>
-    <sheet name="Figure - Conception of Techn" sheetId="20" r:id="rId10"/>
-    <sheet name="Figure - R&amp;D Funding 1967-2019" sheetId="3" r:id="rId11"/>
-    <sheet name="Figure - R&amp;D Funding 1990-2015" sheetId="1" r:id="rId12"/>
-    <sheet name="Figure - R&amp;D Funding 1951-2019" sheetId="2" r:id="rId13"/>
-    <sheet name="Figure - Stokes Model" sheetId="17" r:id="rId14"/>
-    <sheet name="Figure - Research Cycle" sheetId="13" r:id="rId15"/>
-    <sheet name="Figure - Research Model" sheetId="16" r:id="rId16"/>
-    <sheet name="Figure - Valley of Death" sheetId="18" r:id="rId17"/>
-    <sheet name="Figure - Theory the Org" sheetId="15" r:id="rId18"/>
-    <sheet name="Figure - Conceptual Framework" sheetId="9" r:id="rId19"/>
-    <sheet name="Figure - Literature Landscape" sheetId="14" r:id="rId20"/>
+    <sheet name="Table - Premise Hypotheses" sheetId="21" r:id="rId8"/>
+    <sheet name="Table - Control Variables" sheetId="22" r:id="rId9"/>
+    <sheet name="Figure - Tech Utilization" sheetId="19" r:id="rId10"/>
+    <sheet name="Figure - Defining Technology" sheetId="12" r:id="rId11"/>
+    <sheet name="Figure - Conception of Techn" sheetId="20" r:id="rId12"/>
+    <sheet name="Figure - R&amp;D Funding 1967-2019" sheetId="3" r:id="rId13"/>
+    <sheet name="Figure - R&amp;D Funding 1990-2015" sheetId="1" r:id="rId14"/>
+    <sheet name="Figure - R&amp;D Funding 1951-2019" sheetId="2" r:id="rId15"/>
+    <sheet name="Figure - Stokes Model" sheetId="17" r:id="rId16"/>
+    <sheet name="Figure - Research Cycle" sheetId="13" r:id="rId17"/>
+    <sheet name="Figure - Research Model" sheetId="16" r:id="rId18"/>
+    <sheet name="Figure - Valley of Death" sheetId="18" r:id="rId19"/>
+    <sheet name="Figure - Theory the Org" sheetId="15" r:id="rId20"/>
+    <sheet name="Figure - Conceptual Framework" sheetId="9" r:id="rId21"/>
+    <sheet name="Figure - Literature Landscape" sheetId="14" r:id="rId22"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Table - Determinants Examined'!$3:$4</definedName>
@@ -46,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="381">
   <si>
     <t>Total</t>
   </si>
@@ -1538,6 +1540,53 @@
   </si>
   <si>
     <t>Est. No. of Inventions Optioned, Licensed Exclusively, and Licensed Non-exclusively</t>
+  </si>
+  <si>
+    <t>Hypothesized Knowledge Decision Premises</t>
+  </si>
+  <si>
+    <t>KP1</t>
+  </si>
+  <si>
+    <t>KP2</t>
+  </si>
+  <si>
+    <t>KP3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only technologies that have reached a technology maturity level of at least X as measured by the validated technology maturity level measurement instrument can be successfully commercialized by the organization. 
+</t>
+  </si>
+  <si>
+    <t>Organizational superiors will only approve obtaining and assimilating technologies that have reached a technology maturity level of at least X as measured by the validated technology maturity level measurement instrument.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recommending obtaining and assimilating a technology that is less than X as measured by the validated technology maturity level measurementn instrument will reflect negatively on the individual making the recommendation.
+</t>
+  </si>
+  <si>
+    <t>CV1</t>
+  </si>
+  <si>
+    <t>CV2</t>
+  </si>
+  <si>
+    <t>CV3</t>
+  </si>
+  <si>
+    <t>Commit</t>
+  </si>
+  <si>
+    <t>Maturity</t>
+  </si>
+  <si>
+    <t>Whether the subject recommends committing organization resources to obtain and assimilate the technology. Takes on dichotomous values  1 - Yes, 0 - No.</t>
+  </si>
+  <si>
+    <t>The maturity level of the technology as measured by the validated measurement instrument.</t>
+  </si>
+  <si>
+    <t>List of Variables</t>
   </si>
 </sst>
 </file>
@@ -1894,7 +1943,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -2275,6 +2324,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2309,6 +2361,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -9098,7 +9153,7 @@
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>Motivation</a:t>
+              <a:t>Motivations</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -9712,7 +9767,7 @@
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>Assessment</a:t>
+              <a:t>Assessments</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -10691,7 +10746,23 @@
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>Technology maturity level must be at least L.</a:t>
+              <a:t>Technology maturity level must be at least L, where L &gt; L</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="-25000">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>low</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>.</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="1200" baseline="-25000">
               <a:solidFill>
@@ -11463,7 +11534,22 @@
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>Option for Action: Assimilate a given available technology</a:t>
+              <a:t>Option for Action: </a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-US" sz="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Obtain and assimilate a given available technology</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -19712,6 +19798,547 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L50"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="10" width="15.7109375" style="91" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="108" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="110" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="77.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="122" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="123" t="s">
+        <v>275</v>
+      </c>
+      <c r="C5" s="123" t="s">
+        <v>351</v>
+      </c>
+      <c r="D5" s="123" t="s">
+        <v>353</v>
+      </c>
+      <c r="E5" s="123" t="s">
+        <v>352</v>
+      </c>
+      <c r="F5" s="123" t="s">
+        <v>345</v>
+      </c>
+      <c r="G5" s="123" t="s">
+        <v>346</v>
+      </c>
+      <c r="H5" s="123" t="s">
+        <v>347</v>
+      </c>
+      <c r="I5" s="123" t="s">
+        <v>354</v>
+      </c>
+      <c r="J5" s="123" t="s">
+        <v>355</v>
+      </c>
+      <c r="K5" s="123" t="s">
+        <v>348</v>
+      </c>
+      <c r="L5" s="120"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>2013</v>
+      </c>
+      <c r="B6" s="119">
+        <v>24048</v>
+      </c>
+      <c r="C6" s="119">
+        <v>14987</v>
+      </c>
+      <c r="D6" s="119">
+        <v>11626</v>
+      </c>
+      <c r="E6" s="119">
+        <v>1531</v>
+      </c>
+      <c r="F6" s="119">
+        <v>1764</v>
+      </c>
+      <c r="G6" s="119">
+        <v>1356</v>
+      </c>
+      <c r="H6" s="119">
+        <v>3410</v>
+      </c>
+      <c r="I6" s="119">
+        <f>H6/3</f>
+        <v>1136.6666666666667</v>
+      </c>
+      <c r="J6" s="119">
+        <f>SUM(F6,G6,I6)</f>
+        <v>4256.666666666667</v>
+      </c>
+      <c r="K6" s="121">
+        <f t="shared" ref="K6:K11" si="0">J6/B6</f>
+        <v>0.17700709691727656</v>
+      </c>
+      <c r="L6" s="119"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>2014</v>
+      </c>
+      <c r="B7" s="119">
+        <v>24117</v>
+      </c>
+      <c r="C7" s="119">
+        <v>13907</v>
+      </c>
+      <c r="D7" s="119">
+        <v>10715</v>
+      </c>
+      <c r="E7" s="119">
+        <v>1504</v>
+      </c>
+      <c r="F7" s="119">
+        <v>2029</v>
+      </c>
+      <c r="G7" s="119">
+        <v>1461</v>
+      </c>
+      <c r="H7" s="119">
+        <v>3398</v>
+      </c>
+      <c r="I7" s="119">
+        <f>H7/3</f>
+        <v>1132.6666666666667</v>
+      </c>
+      <c r="J7" s="119">
+        <f t="shared" ref="J7:J10" si="1">SUM(F7,G7,I7)</f>
+        <v>4622.666666666667</v>
+      </c>
+      <c r="K7" s="121">
+        <f t="shared" si="0"/>
+        <v>0.19167668726071513</v>
+      </c>
+      <c r="L7" s="119"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>2015</v>
+      </c>
+      <c r="B8" s="119">
+        <v>25313</v>
+      </c>
+      <c r="C8" s="119">
+        <v>15953</v>
+      </c>
+      <c r="D8" s="119">
+        <v>11516</v>
+      </c>
+      <c r="E8" s="119">
+        <v>1672</v>
+      </c>
+      <c r="F8" s="119">
+        <v>2107</v>
+      </c>
+      <c r="G8" s="119">
+        <v>1547</v>
+      </c>
+      <c r="H8" s="119">
+        <v>4115</v>
+      </c>
+      <c r="I8" s="119">
+        <f>H8/3</f>
+        <v>1371.6666666666667</v>
+      </c>
+      <c r="J8" s="119">
+        <f t="shared" si="1"/>
+        <v>5025.666666666667</v>
+      </c>
+      <c r="K8" s="121">
+        <f t="shared" si="0"/>
+        <v>0.19854093417084767</v>
+      </c>
+      <c r="L8" s="119"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>2016</v>
+      </c>
+      <c r="B9" s="119">
+        <v>25825</v>
+      </c>
+      <c r="C9" s="119">
+        <v>16487</v>
+      </c>
+      <c r="D9" s="119">
+        <v>12114</v>
+      </c>
+      <c r="E9" s="119">
+        <v>1391</v>
+      </c>
+      <c r="F9" s="119">
+        <v>2063</v>
+      </c>
+      <c r="G9" s="119">
+        <v>1438</v>
+      </c>
+      <c r="H9" s="119">
+        <v>4201</v>
+      </c>
+      <c r="I9" s="119">
+        <f>H9/3</f>
+        <v>1400.3333333333333</v>
+      </c>
+      <c r="J9" s="119">
+        <f t="shared" si="1"/>
+        <v>4901.333333333333</v>
+      </c>
+      <c r="K9" s="121">
+        <f t="shared" si="0"/>
+        <v>0.18979025492094223</v>
+      </c>
+      <c r="L9" s="119"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>2017</v>
+      </c>
+      <c r="B10" s="119">
+        <v>24998</v>
+      </c>
+      <c r="C10" s="119">
+        <v>15335</v>
+      </c>
+      <c r="D10" s="119">
+        <v>11418</v>
+      </c>
+      <c r="E10" s="119">
+        <v>1381</v>
+      </c>
+      <c r="F10" s="119">
+        <v>2037</v>
+      </c>
+      <c r="G10" s="119">
+        <v>1566</v>
+      </c>
+      <c r="H10" s="119">
+        <v>4195</v>
+      </c>
+      <c r="I10" s="119">
+        <f>H10/3</f>
+        <v>1398.3333333333333</v>
+      </c>
+      <c r="J10" s="119">
+        <f t="shared" si="1"/>
+        <v>5001.333333333333</v>
+      </c>
+      <c r="K10" s="121">
+        <f t="shared" si="0"/>
+        <v>0.20006933888044376</v>
+      </c>
+      <c r="L10" s="119"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="124">
+        <f t="shared" ref="B11:J11" si="2">SUM(B6:B10)</f>
+        <v>124301</v>
+      </c>
+      <c r="C11" s="124">
+        <f t="shared" si="2"/>
+        <v>76669</v>
+      </c>
+      <c r="D11" s="124">
+        <f t="shared" ref="D11:E11" si="3">SUM(D6:D10)</f>
+        <v>57389</v>
+      </c>
+      <c r="E11" s="124">
+        <f t="shared" si="3"/>
+        <v>7479</v>
+      </c>
+      <c r="F11" s="124">
+        <f t="shared" si="2"/>
+        <v>10000</v>
+      </c>
+      <c r="G11" s="124">
+        <f t="shared" si="2"/>
+        <v>7368</v>
+      </c>
+      <c r="H11" s="124">
+        <f t="shared" si="2"/>
+        <v>19319</v>
+      </c>
+      <c r="I11" s="124">
+        <f t="shared" si="2"/>
+        <v>6439.6666666666661</v>
+      </c>
+      <c r="J11" s="124">
+        <f t="shared" si="2"/>
+        <v>23807.666666666664</v>
+      </c>
+      <c r="K11" s="125">
+        <f t="shared" si="0"/>
+        <v>0.19153238241580248</v>
+      </c>
+      <c r="L11" s="119"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="129"/>
+      <c r="B12" s="130"/>
+      <c r="C12" s="130"/>
+      <c r="D12" s="130"/>
+      <c r="E12" s="130"/>
+      <c r="F12" s="130"/>
+      <c r="G12" s="130"/>
+      <c r="H12" s="130"/>
+      <c r="I12" s="130"/>
+      <c r="J12" s="130"/>
+      <c r="K12" s="131"/>
+      <c r="L12" s="119"/>
+    </row>
+    <row r="13" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="129" t="s">
+        <v>356</v>
+      </c>
+      <c r="B13" s="130"/>
+      <c r="C13" s="130"/>
+      <c r="D13" s="130"/>
+      <c r="E13" s="130"/>
+      <c r="F13" s="130"/>
+      <c r="G13" s="130"/>
+      <c r="H13" s="130"/>
+      <c r="I13" s="130"/>
+      <c r="J13" s="130"/>
+      <c r="K13" s="131"/>
+      <c r="L13" s="119"/>
+    </row>
+    <row r="14" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="129" t="s">
+        <v>357</v>
+      </c>
+      <c r="B14" s="130"/>
+      <c r="C14" s="130"/>
+      <c r="D14" s="130"/>
+      <c r="E14" s="130"/>
+      <c r="F14" s="130"/>
+      <c r="G14" s="130"/>
+      <c r="H14" s="130"/>
+      <c r="I14" s="130"/>
+      <c r="J14" s="130"/>
+      <c r="K14" s="131"/>
+      <c r="L14" s="119"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="129"/>
+      <c r="B15" s="130"/>
+      <c r="C15" s="130"/>
+      <c r="D15" s="130"/>
+      <c r="E15" s="130"/>
+      <c r="F15" s="130"/>
+      <c r="G15" s="130"/>
+      <c r="H15" s="130"/>
+      <c r="I15" s="130"/>
+      <c r="J15" s="130"/>
+      <c r="K15" s="131"/>
+      <c r="L15" s="119"/>
+    </row>
+    <row r="17" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A17" s="122" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="123" t="s">
+        <v>364</v>
+      </c>
+      <c r="C17" s="123" t="s">
+        <v>365</v>
+      </c>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>2013</v>
+      </c>
+      <c r="B18" s="119">
+        <v>24048</v>
+      </c>
+      <c r="C18" s="119">
+        <v>4256.666666666667</v>
+      </c>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
+        <v>2014</v>
+      </c>
+      <c r="B19" s="119">
+        <v>24117</v>
+      </c>
+      <c r="C19" s="119">
+        <v>4622.666666666667</v>
+      </c>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>2015</v>
+      </c>
+      <c r="B20" s="119">
+        <v>25313</v>
+      </c>
+      <c r="C20" s="119">
+        <v>5025.666666666667</v>
+      </c>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>2016</v>
+      </c>
+      <c r="B21" s="119">
+        <v>25825</v>
+      </c>
+      <c r="C21" s="119">
+        <v>4901.333333333333</v>
+      </c>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <v>2017</v>
+      </c>
+      <c r="B22" s="119">
+        <v>24998</v>
+      </c>
+      <c r="C22" s="119">
+        <v>5001.333333333333</v>
+      </c>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="122" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="126">
+        <f>SUM(B18:B22)</f>
+        <v>124301</v>
+      </c>
+      <c r="C23" s="126">
+        <f>SUM(C18:C22)</f>
+        <v>23807.666666666664</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="127"/>
+      <c r="B24" s="128"/>
+      <c r="C24" s="128"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="144" t="s">
+        <v>350</v>
+      </c>
+      <c r="B50" s="144"/>
+      <c r="C50" s="144"/>
+      <c r="D50" s="144"/>
+      <c r="E50" s="144"/>
+      <c r="F50" s="144"/>
+      <c r="G50" s="144"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A50:G50"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="108" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="110" t="s">
+        <v>321</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="54" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -19732,21 +20359,21 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="144" t="s">
+      <c r="A37" s="145" t="s">
         <v>363</v>
       </c>
-      <c r="B37" s="144"/>
-      <c r="C37" s="144"/>
-      <c r="D37" s="144"/>
-      <c r="E37" s="144"/>
-      <c r="F37" s="144"/>
-      <c r="G37" s="144"/>
-      <c r="H37" s="144"/>
-      <c r="I37" s="144"/>
-      <c r="J37" s="144"/>
-      <c r="K37" s="144"/>
-      <c r="L37" s="144"/>
-      <c r="M37" s="144"/>
+      <c r="B37" s="145"/>
+      <c r="C37" s="145"/>
+      <c r="D37" s="145"/>
+      <c r="E37" s="145"/>
+      <c r="F37" s="145"/>
+      <c r="G37" s="145"/>
+      <c r="H37" s="145"/>
+      <c r="I37" s="145"/>
+      <c r="J37" s="145"/>
+      <c r="K37" s="145"/>
+      <c r="L37" s="145"/>
+      <c r="M37" s="145"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -19758,7 +20385,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W54"/>
   <sheetViews>
@@ -20065,19 +20692,19 @@
       <c r="B34" s="19">
         <v>14959.1</v>
       </c>
-      <c r="M34" s="133" t="s">
+      <c r="M34" s="134" t="s">
         <v>361</v>
       </c>
-      <c r="N34" s="133"/>
-      <c r="O34" s="133"/>
-      <c r="P34" s="133"/>
-      <c r="Q34" s="133"/>
-      <c r="R34" s="133"/>
-      <c r="S34" s="133"/>
-      <c r="T34" s="133"/>
-      <c r="U34" s="133"/>
-      <c r="V34" s="133"/>
-      <c r="W34" s="133"/>
+      <c r="N34" s="134"/>
+      <c r="O34" s="134"/>
+      <c r="P34" s="134"/>
+      <c r="Q34" s="134"/>
+      <c r="R34" s="134"/>
+      <c r="S34" s="134"/>
+      <c r="T34" s="134"/>
+      <c r="U34" s="134"/>
+      <c r="V34" s="134"/>
+      <c r="W34" s="134"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
@@ -20086,17 +20713,17 @@
       <c r="B35" s="19">
         <v>16890.7</v>
       </c>
-      <c r="M35" s="133"/>
-      <c r="N35" s="133"/>
-      <c r="O35" s="133"/>
-      <c r="P35" s="133"/>
-      <c r="Q35" s="133"/>
-      <c r="R35" s="133"/>
-      <c r="S35" s="133"/>
-      <c r="T35" s="133"/>
-      <c r="U35" s="133"/>
-      <c r="V35" s="133"/>
-      <c r="W35" s="133"/>
+      <c r="M35" s="134"/>
+      <c r="N35" s="134"/>
+      <c r="O35" s="134"/>
+      <c r="P35" s="134"/>
+      <c r="Q35" s="134"/>
+      <c r="R35" s="134"/>
+      <c r="S35" s="134"/>
+      <c r="T35" s="134"/>
+      <c r="U35" s="134"/>
+      <c r="V35" s="134"/>
+      <c r="W35" s="134"/>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
@@ -20105,17 +20732,17 @@
       <c r="B36" s="19">
         <v>20065.099999999999</v>
       </c>
-      <c r="M36" s="133"/>
-      <c r="N36" s="133"/>
-      <c r="O36" s="133"/>
-      <c r="P36" s="133"/>
-      <c r="Q36" s="133"/>
-      <c r="R36" s="133"/>
-      <c r="S36" s="133"/>
-      <c r="T36" s="133"/>
-      <c r="U36" s="133"/>
-      <c r="V36" s="133"/>
-      <c r="W36" s="133"/>
+      <c r="M36" s="134"/>
+      <c r="N36" s="134"/>
+      <c r="O36" s="134"/>
+      <c r="P36" s="134"/>
+      <c r="Q36" s="134"/>
+      <c r="R36" s="134"/>
+      <c r="S36" s="134"/>
+      <c r="T36" s="134"/>
+      <c r="U36" s="134"/>
+      <c r="V36" s="134"/>
+      <c r="W36" s="134"/>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
@@ -20271,7 +20898,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
@@ -20528,7 +21155,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D70"/>
   <sheetViews>
@@ -21113,7 +21740,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -21146,7 +21773,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -21177,7 +21804,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -21263,7 +21890,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
@@ -21282,76 +21909,23 @@
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="143" t="s">
+      <c r="A50" s="144" t="s">
         <v>343</v>
       </c>
-      <c r="B50" s="143"/>
-      <c r="C50" s="143"/>
-      <c r="D50" s="143"/>
-      <c r="E50" s="143"/>
-      <c r="F50" s="143"/>
-      <c r="G50" s="143"/>
-      <c r="H50" s="143"/>
-      <c r="I50" s="143"/>
-      <c r="J50" s="143"/>
+      <c r="B50" s="144"/>
+      <c r="C50" s="144"/>
+      <c r="D50" s="144"/>
+      <c r="E50" s="144"/>
+      <c r="F50" s="144"/>
+      <c r="G50" s="144"/>
+      <c r="H50" s="144"/>
+      <c r="I50" s="144"/>
+      <c r="J50" s="144"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A50:J50"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="108" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="110" t="s">
-        <v>328</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="44" fitToHeight="0" orientation="landscape" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="108" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="110" t="s">
-        <v>326</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -21724,54 +22298,54 @@
       <c r="H20" s="109"/>
     </row>
     <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="132" t="s">
+      <c r="A21" s="133" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="132"/>
-      <c r="C21" s="132"/>
-      <c r="D21" s="132"/>
-      <c r="E21" s="132"/>
-      <c r="F21" s="132"/>
+      <c r="B21" s="133"/>
+      <c r="C21" s="133"/>
+      <c r="D21" s="133"/>
+      <c r="E21" s="133"/>
+      <c r="F21" s="133"/>
     </row>
     <row r="22" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="133" t="s">
+      <c r="A22" s="134" t="s">
         <v>171</v>
       </c>
-      <c r="B22" s="133"/>
-      <c r="C22" s="133"/>
-      <c r="D22" s="133"/>
-      <c r="E22" s="133"/>
-      <c r="F22" s="133"/>
+      <c r="B22" s="134"/>
+      <c r="C22" s="134"/>
+      <c r="D22" s="134"/>
+      <c r="E22" s="134"/>
+      <c r="F22" s="134"/>
     </row>
     <row r="23" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="132" t="s">
+      <c r="A23" s="133" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="132"/>
-      <c r="C23" s="132"/>
-      <c r="D23" s="132"/>
-      <c r="E23" s="132"/>
-      <c r="F23" s="132"/>
+      <c r="B23" s="133"/>
+      <c r="C23" s="133"/>
+      <c r="D23" s="133"/>
+      <c r="E23" s="133"/>
+      <c r="F23" s="133"/>
     </row>
     <row r="24" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="132" t="s">
+      <c r="A24" s="133" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="132"/>
-      <c r="C24" s="132"/>
-      <c r="D24" s="132"/>
-      <c r="E24" s="132"/>
-      <c r="F24" s="132"/>
+      <c r="B24" s="133"/>
+      <c r="C24" s="133"/>
+      <c r="D24" s="133"/>
+      <c r="E24" s="133"/>
+      <c r="F24" s="133"/>
     </row>
     <row r="25" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="132" t="s">
+      <c r="A25" s="133" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="132"/>
-      <c r="C25" s="132"/>
-      <c r="D25" s="132"/>
-      <c r="E25" s="132"/>
-      <c r="F25" s="132"/>
+      <c r="B25" s="133"/>
+      <c r="C25" s="133"/>
+      <c r="D25" s="133"/>
+      <c r="E25" s="133"/>
+      <c r="F25" s="133"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="30"/>
@@ -21870,6 +22444,61 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="108" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="110" t="s">
+        <v>328</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="44" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="108" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="110" t="s">
+        <v>326</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -21983,38 +22612,38 @@
       <c r="B3" s="69"/>
       <c r="C3" s="70"/>
       <c r="D3" s="71"/>
-      <c r="E3" s="137" t="s">
+      <c r="E3" s="138" t="s">
         <v>267</v>
       </c>
-      <c r="F3" s="138"/>
-      <c r="G3" s="138"/>
-      <c r="H3" s="135"/>
-      <c r="I3" s="134" t="s">
+      <c r="F3" s="139"/>
+      <c r="G3" s="139"/>
+      <c r="H3" s="136"/>
+      <c r="I3" s="135" t="s">
         <v>294</v>
       </c>
-      <c r="J3" s="135"/>
-      <c r="K3" s="134" t="s">
+      <c r="J3" s="136"/>
+      <c r="K3" s="135" t="s">
         <v>295</v>
       </c>
-      <c r="L3" s="136"/>
-      <c r="M3" s="137" t="s">
+      <c r="L3" s="137"/>
+      <c r="M3" s="138" t="s">
         <v>282</v>
       </c>
-      <c r="N3" s="138"/>
-      <c r="O3" s="135"/>
-      <c r="P3" s="139" t="s">
+      <c r="N3" s="139"/>
+      <c r="O3" s="136"/>
+      <c r="P3" s="140" t="s">
         <v>249</v>
       </c>
-      <c r="Q3" s="138"/>
-      <c r="R3" s="138"/>
-      <c r="S3" s="138"/>
-      <c r="T3" s="138"/>
-      <c r="U3" s="138"/>
-      <c r="V3" s="138"/>
-      <c r="W3" s="138"/>
-      <c r="X3" s="138"/>
-      <c r="Y3" s="138"/>
-      <c r="Z3" s="140"/>
+      <c r="Q3" s="139"/>
+      <c r="R3" s="139"/>
+      <c r="S3" s="139"/>
+      <c r="T3" s="139"/>
+      <c r="U3" s="139"/>
+      <c r="V3" s="139"/>
+      <c r="W3" s="139"/>
+      <c r="X3" s="139"/>
+      <c r="Y3" s="139"/>
+      <c r="Z3" s="141"/>
       <c r="AA3" s="90"/>
     </row>
     <row r="4" spans="1:27" ht="170.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -25290,10 +25919,10 @@
       <c r="A3" s="69"/>
       <c r="B3" s="70"/>
       <c r="C3" s="71"/>
-      <c r="D3" s="137" t="s">
+      <c r="D3" s="138" t="s">
         <v>194</v>
       </c>
-      <c r="E3" s="135"/>
+      <c r="E3" s="136"/>
       <c r="F3" s="73"/>
     </row>
     <row r="4" spans="1:6" ht="125.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -25553,32 +26182,32 @@
       <c r="F23" s="59"/>
     </row>
     <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="132"/>
-      <c r="B24" s="132"/>
-      <c r="C24" s="132"/>
-      <c r="D24" s="132"/>
-      <c r="E24" s="132"/>
+      <c r="A24" s="133"/>
+      <c r="B24" s="133"/>
+      <c r="C24" s="133"/>
+      <c r="D24" s="133"/>
+      <c r="E24" s="133"/>
     </row>
     <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="132"/>
-      <c r="B25" s="132"/>
-      <c r="C25" s="132"/>
-      <c r="D25" s="132"/>
-      <c r="E25" s="132"/>
+      <c r="A25" s="133"/>
+      <c r="B25" s="133"/>
+      <c r="C25" s="133"/>
+      <c r="D25" s="133"/>
+      <c r="E25" s="133"/>
     </row>
     <row r="26" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="132"/>
-      <c r="B26" s="132"/>
-      <c r="C26" s="132"/>
-      <c r="D26" s="132"/>
-      <c r="E26" s="132"/>
+      <c r="A26" s="133"/>
+      <c r="B26" s="133"/>
+      <c r="C26" s="133"/>
+      <c r="D26" s="133"/>
+      <c r="E26" s="133"/>
     </row>
     <row r="27" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="132"/>
-      <c r="B27" s="132"/>
-      <c r="C27" s="132"/>
-      <c r="D27" s="132"/>
-      <c r="E27" s="132"/>
+      <c r="A27" s="133"/>
+      <c r="B27" s="133"/>
+      <c r="C27" s="133"/>
+      <c r="D27" s="133"/>
+      <c r="E27" s="133"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="60"/>
@@ -26369,40 +26998,40 @@
       <c r="H15" s="32"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="133" t="s">
+      <c r="A16" s="134" t="s">
         <v>99</v>
       </c>
-      <c r="B16" s="133"/>
-      <c r="C16" s="133"/>
-      <c r="D16" s="133"/>
-      <c r="E16" s="133"/>
-      <c r="F16" s="133"/>
-      <c r="G16" s="133"/>
-      <c r="H16" s="133"/>
-      <c r="I16" s="133"/>
+      <c r="B16" s="134"/>
+      <c r="C16" s="134"/>
+      <c r="D16" s="134"/>
+      <c r="E16" s="134"/>
+      <c r="F16" s="134"/>
+      <c r="G16" s="134"/>
+      <c r="H16" s="134"/>
+      <c r="I16" s="134"/>
     </row>
     <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="132"/>
-      <c r="B17" s="132"/>
-      <c r="C17" s="132"/>
+      <c r="A17" s="133"/>
+      <c r="B17" s="133"/>
+      <c r="C17" s="133"/>
       <c r="D17" s="32"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="132"/>
-      <c r="B18" s="132"/>
-      <c r="C18" s="132"/>
+      <c r="A18" s="133"/>
+      <c r="B18" s="133"/>
+      <c r="C18" s="133"/>
       <c r="D18" s="32"/>
       <c r="E18" s="32"/>
       <c r="F18" s="32"/>
       <c r="H18" s="32"/>
     </row>
     <row r="19" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="132"/>
-      <c r="B19" s="132"/>
-      <c r="C19" s="132"/>
+      <c r="A19" s="133"/>
+      <c r="B19" s="133"/>
+      <c r="C19" s="133"/>
       <c r="D19" s="32"/>
       <c r="E19" s="32"/>
       <c r="F19" s="32"/>
@@ -26498,7 +27127,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26842,30 +27471,30 @@
       <c r="C41" s="52"/>
     </row>
     <row r="42" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="141" t="s">
+      <c r="A42" s="142" t="s">
         <v>166</v>
       </c>
-      <c r="B42" s="141"/>
-      <c r="C42" s="141"/>
+      <c r="B42" s="142"/>
+      <c r="C42" s="142"/>
     </row>
     <row r="43" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="142" t="s">
+      <c r="A43" s="143" t="s">
         <v>167</v>
       </c>
-      <c r="B43" s="142"/>
-      <c r="C43" s="142"/>
+      <c r="B43" s="143"/>
+      <c r="C43" s="143"/>
     </row>
     <row r="44" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="141" t="s">
+      <c r="A44" s="142" t="s">
         <v>168</v>
       </c>
-      <c r="B44" s="141"/>
-      <c r="C44" s="141"/>
+      <c r="B44" s="142"/>
+      <c r="C44" s="142"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="132"/>
-      <c r="B45" s="132"/>
-      <c r="C45" s="132"/>
+      <c r="A45" s="133"/>
+      <c r="B45" s="133"/>
+      <c r="C45" s="133"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="37"/>
@@ -26924,541 +27553,252 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L50"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="10" width="15.7109375" style="91" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="1" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="108" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="110" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="77.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="122" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="123" t="s">
-        <v>275</v>
-      </c>
-      <c r="C5" s="123" t="s">
-        <v>351</v>
-      </c>
-      <c r="D5" s="123" t="s">
-        <v>353</v>
-      </c>
-      <c r="E5" s="123" t="s">
-        <v>352</v>
-      </c>
-      <c r="F5" s="123" t="s">
-        <v>345</v>
-      </c>
-      <c r="G5" s="123" t="s">
-        <v>346</v>
-      </c>
-      <c r="H5" s="123" t="s">
-        <v>347</v>
-      </c>
-      <c r="I5" s="123" t="s">
-        <v>354</v>
-      </c>
-      <c r="J5" s="123" t="s">
-        <v>355</v>
-      </c>
-      <c r="K5" s="123" t="s">
-        <v>348</v>
-      </c>
-      <c r="L5" s="120"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
-        <v>2013</v>
-      </c>
-      <c r="B6" s="119">
-        <v>24048</v>
-      </c>
-      <c r="C6" s="119">
-        <v>14987</v>
-      </c>
-      <c r="D6" s="119">
-        <v>11626</v>
-      </c>
-      <c r="E6" s="119">
-        <v>1531</v>
-      </c>
-      <c r="F6" s="119">
-        <v>1764</v>
-      </c>
-      <c r="G6" s="119">
-        <v>1356</v>
-      </c>
-      <c r="H6" s="119">
-        <v>3410</v>
-      </c>
-      <c r="I6" s="119">
-        <f>H6/3</f>
-        <v>1136.6666666666667</v>
-      </c>
-      <c r="J6" s="119">
-        <f>SUM(F6,G6,I6)</f>
-        <v>4256.666666666667</v>
-      </c>
-      <c r="K6" s="121">
-        <f t="shared" ref="K6:K11" si="0">J6/B6</f>
-        <v>0.17700709691727656</v>
-      </c>
-      <c r="L6" s="119"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
-        <v>2014</v>
-      </c>
-      <c r="B7" s="119">
-        <v>24117</v>
-      </c>
-      <c r="C7" s="119">
-        <v>13907</v>
-      </c>
-      <c r="D7" s="119">
-        <v>10715</v>
-      </c>
-      <c r="E7" s="119">
-        <v>1504</v>
-      </c>
-      <c r="F7" s="119">
-        <v>2029</v>
-      </c>
-      <c r="G7" s="119">
-        <v>1461</v>
-      </c>
-      <c r="H7" s="119">
-        <v>3398</v>
-      </c>
-      <c r="I7" s="119">
-        <f>H7/3</f>
-        <v>1132.6666666666667</v>
-      </c>
-      <c r="J7" s="119">
-        <f t="shared" ref="J7:J10" si="1">SUM(F7,G7,I7)</f>
-        <v>4622.666666666667</v>
-      </c>
-      <c r="K7" s="121">
-        <f t="shared" si="0"/>
-        <v>0.19167668726071513</v>
-      </c>
-      <c r="L7" s="119"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
-        <v>2015</v>
-      </c>
-      <c r="B8" s="119">
-        <v>25313</v>
-      </c>
-      <c r="C8" s="119">
-        <v>15953</v>
-      </c>
-      <c r="D8" s="119">
-        <v>11516</v>
-      </c>
-      <c r="E8" s="119">
-        <v>1672</v>
-      </c>
-      <c r="F8" s="119">
-        <v>2107</v>
-      </c>
-      <c r="G8" s="119">
-        <v>1547</v>
-      </c>
-      <c r="H8" s="119">
-        <v>4115</v>
-      </c>
-      <c r="I8" s="119">
-        <f>H8/3</f>
-        <v>1371.6666666666667</v>
-      </c>
-      <c r="J8" s="119">
-        <f t="shared" si="1"/>
-        <v>5025.666666666667</v>
-      </c>
-      <c r="K8" s="121">
-        <f t="shared" si="0"/>
-        <v>0.19854093417084767</v>
-      </c>
-      <c r="L8" s="119"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
-        <v>2016</v>
-      </c>
-      <c r="B9" s="119">
-        <v>25825</v>
-      </c>
-      <c r="C9" s="119">
-        <v>16487</v>
-      </c>
-      <c r="D9" s="119">
-        <v>12114</v>
-      </c>
-      <c r="E9" s="119">
-        <v>1391</v>
-      </c>
-      <c r="F9" s="119">
-        <v>2063</v>
-      </c>
-      <c r="G9" s="119">
-        <v>1438</v>
-      </c>
-      <c r="H9" s="119">
-        <v>4201</v>
-      </c>
-      <c r="I9" s="119">
-        <f>H9/3</f>
-        <v>1400.3333333333333</v>
-      </c>
-      <c r="J9" s="119">
-        <f t="shared" si="1"/>
-        <v>4901.333333333333</v>
-      </c>
-      <c r="K9" s="121">
-        <f t="shared" si="0"/>
-        <v>0.18979025492094223</v>
-      </c>
-      <c r="L9" s="119"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
-        <v>2017</v>
-      </c>
-      <c r="B10" s="119">
-        <v>24998</v>
-      </c>
-      <c r="C10" s="119">
-        <v>15335</v>
-      </c>
-      <c r="D10" s="119">
-        <v>11418</v>
-      </c>
-      <c r="E10" s="119">
-        <v>1381</v>
-      </c>
-      <c r="F10" s="119">
-        <v>2037</v>
-      </c>
-      <c r="G10" s="119">
-        <v>1566</v>
-      </c>
-      <c r="H10" s="119">
-        <v>4195</v>
-      </c>
-      <c r="I10" s="119">
-        <f>H10/3</f>
-        <v>1398.3333333333333</v>
-      </c>
-      <c r="J10" s="119">
-        <f t="shared" si="1"/>
-        <v>5001.333333333333</v>
-      </c>
-      <c r="K10" s="121">
-        <f t="shared" si="0"/>
-        <v>0.20006933888044376</v>
-      </c>
-      <c r="L10" s="119"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="124">
-        <f t="shared" ref="B11:J11" si="2">SUM(B6:B10)</f>
-        <v>124301</v>
-      </c>
-      <c r="C11" s="124">
-        <f t="shared" si="2"/>
-        <v>76669</v>
-      </c>
-      <c r="D11" s="124">
-        <f t="shared" ref="D11:E11" si="3">SUM(D6:D10)</f>
-        <v>57389</v>
-      </c>
-      <c r="E11" s="124">
-        <f t="shared" si="3"/>
-        <v>7479</v>
-      </c>
-      <c r="F11" s="124">
-        <f t="shared" si="2"/>
-        <v>10000</v>
-      </c>
-      <c r="G11" s="124">
-        <f t="shared" si="2"/>
-        <v>7368</v>
-      </c>
-      <c r="H11" s="124">
-        <f t="shared" si="2"/>
-        <v>19319</v>
-      </c>
-      <c r="I11" s="124">
-        <f t="shared" si="2"/>
-        <v>6439.6666666666661</v>
-      </c>
-      <c r="J11" s="124">
-        <f t="shared" si="2"/>
-        <v>23807.666666666664</v>
-      </c>
-      <c r="K11" s="125">
-        <f t="shared" si="0"/>
-        <v>0.19153238241580248</v>
-      </c>
-      <c r="L11" s="119"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="129"/>
-      <c r="B12" s="130"/>
-      <c r="C12" s="130"/>
-      <c r="D12" s="130"/>
-      <c r="E12" s="130"/>
-      <c r="F12" s="130"/>
-      <c r="G12" s="130"/>
-      <c r="H12" s="130"/>
-      <c r="I12" s="130"/>
-      <c r="J12" s="130"/>
-      <c r="K12" s="131"/>
-      <c r="L12" s="119"/>
-    </row>
-    <row r="13" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="129" t="s">
-        <v>356</v>
-      </c>
-      <c r="B13" s="130"/>
-      <c r="C13" s="130"/>
-      <c r="D13" s="130"/>
-      <c r="E13" s="130"/>
-      <c r="F13" s="130"/>
-      <c r="G13" s="130"/>
-      <c r="H13" s="130"/>
-      <c r="I13" s="130"/>
-      <c r="J13" s="130"/>
-      <c r="K13" s="131"/>
-      <c r="L13" s="119"/>
-    </row>
-    <row r="14" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="129" t="s">
-        <v>357</v>
-      </c>
-      <c r="B14" s="130"/>
-      <c r="C14" s="130"/>
-      <c r="D14" s="130"/>
-      <c r="E14" s="130"/>
-      <c r="F14" s="130"/>
-      <c r="G14" s="130"/>
-      <c r="H14" s="130"/>
-      <c r="I14" s="130"/>
-      <c r="J14" s="130"/>
-      <c r="K14" s="131"/>
-      <c r="L14" s="119"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="129"/>
-      <c r="B15" s="130"/>
-      <c r="C15" s="130"/>
-      <c r="D15" s="130"/>
-      <c r="E15" s="130"/>
-      <c r="F15" s="130"/>
-      <c r="G15" s="130"/>
-      <c r="H15" s="130"/>
-      <c r="I15" s="130"/>
-      <c r="J15" s="130"/>
-      <c r="K15" s="131"/>
-      <c r="L15" s="119"/>
-    </row>
-    <row r="17" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A17" s="122" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="123" t="s">
-        <v>364</v>
-      </c>
-      <c r="C17" s="123" t="s">
-        <v>365</v>
-      </c>
-      <c r="D17"/>
-      <c r="E17"/>
-      <c r="F17"/>
-      <c r="G17"/>
-      <c r="H17"/>
-      <c r="I17"/>
-      <c r="J17"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
-        <v>2013</v>
-      </c>
-      <c r="B18" s="119">
-        <v>24048</v>
-      </c>
-      <c r="C18" s="119">
-        <v>4256.666666666667</v>
-      </c>
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18"/>
-      <c r="G18"/>
-      <c r="H18"/>
-      <c r="I18"/>
-      <c r="J18"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
-        <v>2014</v>
-      </c>
-      <c r="B19" s="119">
-        <v>24117</v>
-      </c>
-      <c r="C19" s="119">
-        <v>4622.666666666667</v>
-      </c>
-      <c r="D19"/>
-      <c r="E19"/>
-      <c r="F19"/>
-      <c r="G19"/>
-      <c r="H19"/>
-      <c r="I19"/>
-      <c r="J19"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
-        <v>2015</v>
-      </c>
-      <c r="B20" s="119">
-        <v>25313</v>
-      </c>
-      <c r="C20" s="119">
-        <v>5025.666666666667</v>
-      </c>
-      <c r="D20"/>
-      <c r="E20"/>
-      <c r="F20"/>
-      <c r="G20"/>
-      <c r="H20"/>
-      <c r="I20"/>
-      <c r="J20"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="10">
-        <v>2016</v>
-      </c>
-      <c r="B21" s="119">
-        <v>25825</v>
-      </c>
-      <c r="C21" s="119">
-        <v>4901.333333333333</v>
-      </c>
-      <c r="D21"/>
-      <c r="E21"/>
-      <c r="F21"/>
-      <c r="G21"/>
-      <c r="H21"/>
-      <c r="I21"/>
-      <c r="J21"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="10">
-        <v>2017</v>
-      </c>
-      <c r="B22" s="119">
-        <v>24998</v>
-      </c>
-      <c r="C22" s="119">
-        <v>5001.333333333333</v>
-      </c>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22"/>
-      <c r="G22"/>
-      <c r="H22"/>
-      <c r="I22"/>
-      <c r="J22"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="122" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="126">
-        <f>SUM(B18:B22)</f>
-        <v>124301</v>
-      </c>
-      <c r="C23" s="126">
-        <f>SUM(C18:C22)</f>
-        <v>23807.666666666664</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="127"/>
-      <c r="B24" s="128"/>
-      <c r="C24" s="128"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="143" t="s">
-        <v>350</v>
-      </c>
-      <c r="B50" s="143"/>
-      <c r="C50" s="143"/>
-      <c r="D50" s="143"/>
-      <c r="E50" s="143"/>
-      <c r="F50" s="143"/>
-      <c r="G50" s="143"/>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="146" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
+        <v>367</v>
+      </c>
+      <c r="B5" s="134" t="s">
+        <v>370</v>
+      </c>
+      <c r="C5" s="134"/>
+      <c r="D5" s="134"/>
+      <c r="E5" s="134"/>
+      <c r="F5" s="134"/>
+      <c r="G5" s="134"/>
+      <c r="H5" s="134"/>
+      <c r="I5" s="134"/>
+      <c r="J5" s="134"/>
+      <c r="K5" s="134"/>
+    </row>
+    <row r="6" spans="1:11" s="132" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="132" t="s">
+        <v>368</v>
+      </c>
+      <c r="B6" s="134" t="s">
+        <v>371</v>
+      </c>
+      <c r="C6" s="134"/>
+      <c r="D6" s="134"/>
+      <c r="E6" s="134"/>
+      <c r="F6" s="134"/>
+      <c r="G6" s="134"/>
+      <c r="H6" s="134"/>
+      <c r="I6" s="134"/>
+      <c r="J6" s="134"/>
+      <c r="K6" s="134"/>
+    </row>
+    <row r="7" spans="1:11" s="132" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="132" t="s">
+        <v>369</v>
+      </c>
+      <c r="B7" s="134" t="s">
+        <v>372</v>
+      </c>
+      <c r="C7" s="134"/>
+      <c r="D7" s="134"/>
+      <c r="E7" s="134"/>
+      <c r="F7" s="134"/>
+      <c r="G7" s="134"/>
+      <c r="H7" s="134"/>
+      <c r="I7" s="134"/>
+      <c r="J7" s="134"/>
+      <c r="K7" s="134"/>
+    </row>
+    <row r="8" spans="1:11" s="132" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="134"/>
+      <c r="C8" s="134"/>
+      <c r="D8" s="134"/>
+      <c r="E8" s="134"/>
+      <c r="F8" s="134"/>
+      <c r="G8" s="134"/>
+      <c r="H8" s="134"/>
+      <c r="I8" s="134"/>
+      <c r="J8" s="134"/>
+      <c r="K8" s="134"/>
+    </row>
+    <row r="9" spans="1:11" s="132" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="134"/>
+      <c r="C9" s="134"/>
+      <c r="D9" s="134"/>
+      <c r="E9" s="134"/>
+      <c r="F9" s="134"/>
+      <c r="G9" s="134"/>
+      <c r="H9" s="134"/>
+      <c r="I9" s="134"/>
+      <c r="J9" s="134"/>
+      <c r="K9" s="134"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A50:G50"/>
+  <mergeCells count="5">
+    <mergeCell ref="B5:K5"/>
+    <mergeCell ref="B6:K6"/>
+    <mergeCell ref="B7:K7"/>
+    <mergeCell ref="B8:K8"/>
+    <mergeCell ref="B9:K9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:A3"/>
+      <selection activeCell="B7" sqref="B7:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="23"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="108" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="110" t="s">
-        <v>321</v>
-      </c>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="146" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
+        <v>376</v>
+      </c>
+      <c r="B5" s="134" t="s">
+        <v>378</v>
+      </c>
+      <c r="C5" s="134"/>
+      <c r="D5" s="134"/>
+      <c r="E5" s="134"/>
+      <c r="F5" s="134"/>
+      <c r="G5" s="134"/>
+      <c r="H5" s="134"/>
+      <c r="I5" s="134"/>
+      <c r="J5" s="134"/>
+      <c r="K5" s="134"/>
+    </row>
+    <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
+        <v>377</v>
+      </c>
+      <c r="B6" s="134" t="s">
+        <v>379</v>
+      </c>
+      <c r="C6" s="134"/>
+      <c r="D6" s="134"/>
+      <c r="E6" s="134"/>
+      <c r="F6" s="134"/>
+      <c r="G6" s="134"/>
+      <c r="H6" s="134"/>
+      <c r="I6" s="134"/>
+      <c r="J6" s="134"/>
+      <c r="K6" s="134"/>
+    </row>
+    <row r="7" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
+        <v>373</v>
+      </c>
+      <c r="B7" s="134"/>
+      <c r="C7" s="134"/>
+      <c r="D7" s="134"/>
+      <c r="E7" s="134"/>
+      <c r="F7" s="134"/>
+      <c r="G7" s="134"/>
+      <c r="H7" s="134"/>
+      <c r="I7" s="134"/>
+      <c r="J7" s="134"/>
+      <c r="K7" s="134"/>
+    </row>
+    <row r="8" spans="1:11" s="132" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="132" t="s">
+        <v>374</v>
+      </c>
+      <c r="B8" s="134"/>
+      <c r="C8" s="134"/>
+      <c r="D8" s="134"/>
+      <c r="E8" s="134"/>
+      <c r="F8" s="134"/>
+      <c r="G8" s="134"/>
+      <c r="H8" s="134"/>
+      <c r="I8" s="134"/>
+      <c r="J8" s="134"/>
+      <c r="K8" s="134"/>
+    </row>
+    <row r="9" spans="1:11" s="132" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="132" t="s">
+        <v>375</v>
+      </c>
+      <c r="B9" s="134"/>
+      <c r="C9" s="134"/>
+      <c r="D9" s="134"/>
+      <c r="E9" s="134"/>
+      <c r="F9" s="134"/>
+      <c r="G9" s="134"/>
+      <c r="H9" s="134"/>
+      <c r="I9" s="134"/>
+      <c r="J9" s="134"/>
+      <c r="K9" s="134"/>
+    </row>
+    <row r="10" spans="1:11" s="132" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="134"/>
+      <c r="C10" s="134"/>
+      <c r="D10" s="134"/>
+      <c r="E10" s="134"/>
+      <c r="F10" s="134"/>
+      <c r="G10" s="134"/>
+      <c r="H10" s="134"/>
+      <c r="I10" s="134"/>
+      <c r="J10" s="134"/>
+      <c r="K10" s="134"/>
+    </row>
+    <row r="11" spans="1:11" s="132" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="134"/>
+      <c r="C11" s="134"/>
+      <c r="D11" s="134"/>
+      <c r="E11" s="134"/>
+      <c r="F11" s="134"/>
+      <c r="G11" s="134"/>
+      <c r="H11" s="134"/>
+      <c r="I11" s="134"/>
+      <c r="J11" s="134"/>
+      <c r="K11" s="134"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B7:K7"/>
+    <mergeCell ref="B8:K8"/>
+    <mergeCell ref="B9:K9"/>
+    <mergeCell ref="B10:K10"/>
+    <mergeCell ref="B11:K11"/>
+    <mergeCell ref="B5:K5"/>
+    <mergeCell ref="B6:K6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="54" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>